<commit_message>
Changed image background in message from dean and principal section
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Microsoft One Drive\OneDrive\Desktop\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F9BDBE31-1E6C-4877-8BF3-DA25418B039F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{248929BC-7291-4CA9-AAA2-270484AC0911}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="33">
   <si>
     <t>Name</t>
   </si>
@@ -77,9 +77,6 @@
     <t>M. Tech., Ph.D.</t>
   </si>
   <si>
-    <t>Interest details...</t>
-  </si>
-  <si>
     <t>Research</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
     <t>Image Src</t>
   </si>
   <si>
-    <t>Teaching details...</t>
-  </si>
-  <si>
     <t>abc@example.com</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>Algorithm, Machine Learning, Data Structure</t>
   </si>
   <si>
-    <t>Teching a</t>
-  </si>
-  <si>
     <t>faculty_image\AvaniKhokhariya.webp</t>
   </si>
   <si>
@@ -132,6 +123,9 @@
   </si>
   <si>
     <t>https://www.charusat.ac.in/cspit/index.html</t>
+  </si>
+  <si>
+    <t>Project details...</t>
   </si>
 </sst>
 </file>
@@ -520,7 +514,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K5"/>
+      <selection activeCell="D3" sqref="D2:D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -545,25 +539,25 @@
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>30</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="2" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -576,29 +570,29 @@
       <c r="C2" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="5" t="s">
-        <v>16</v>
+      <c r="D2" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="E2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K2" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -618,22 +612,22 @@
         <v>9</v>
       </c>
       <c r="F3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="72" x14ac:dyDescent="0.3">
@@ -653,57 +647,57 @@
         <v>13</v>
       </c>
       <c r="F4" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K4" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="72" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B5" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="2" t="s">
+      <c r="F5" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="H5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K5" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="I5" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="K5" s="6" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Changes discussed in todays meeting
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -1818,8 +1818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="E97" sqref="E97"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E94" sqref="E94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Faculty image src path updated in excel sheet
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA929819-038D-47B9-A817-034C94EAE295}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EB5BB14-BF3F-4385-A9FC-0F160BCD86BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1007">
   <si>
     <t>Name</t>
   </si>
@@ -1841,102 +1841,30 @@
     <t>https://vidwan.inflibnet.ac.in/profile/161331</t>
   </si>
   <si>
-    <t>https://placehold.co/400x601</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x603</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x606</t>
   </si>
   <si>
-    <t>https://placehold.co/400x607</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x609</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x611</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x613</t>
   </si>
   <si>
-    <t>https://placehold.co/400x616</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x617</t>
   </si>
   <si>
     <t>https://placehold.co/400x618</t>
   </si>
   <si>
-    <t>https://placehold.co/400x620</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x622</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x624</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x629</t>
   </si>
   <si>
-    <t>https://placehold.co/400x630</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x634</t>
   </si>
   <si>
-    <t>https://placehold.co/400x635</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x639</t>
   </si>
   <si>
-    <t>https://placehold.co/400x644</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x645</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x646</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x647</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x648</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x649</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x651</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x652</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x653</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x654</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x655</t>
   </si>
   <si>
-    <t>https://placehold.co/400x659</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x662</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x663</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x664</t>
   </si>
   <si>
@@ -1946,9 +1874,6 @@
     <t>https://placehold.co/400x667</t>
   </si>
   <si>
-    <t>https://placehold.co/400x670</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x676</t>
   </si>
   <si>
@@ -1958,36 +1883,21 @@
     <t>https://placehold.co/400x681</t>
   </si>
   <si>
-    <t>https://placehold.co/400x682</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x683</t>
   </si>
   <si>
     <t>https://placehold.co/400x684</t>
   </si>
   <si>
-    <t>https://placehold.co/400x686</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x687</t>
   </si>
   <si>
-    <t>https://placehold.co/400x688</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x689</t>
   </si>
   <si>
     <t>https://placehold.co/400x691</t>
   </si>
   <si>
-    <t>https://placehold.co/400x694</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x695</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x696</t>
   </si>
   <si>
@@ -2013,12 +1923,6 @@
   </si>
   <si>
     <t>https://placehold.co/400x710</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x712</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x714</t>
   </si>
   <si>
     <t>https://www.linkedin.com/in/arpitajshah/</t>
@@ -3223,6 +3127,99 @@
   </si>
   <si>
     <t>CSPIT_Faculty\CSE\VIDISHA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\ABHISHEK_s.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\AKASH.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\ANAND.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\ANKURBHAI.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\BHAVIN.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\DATTATRAYA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\DHARA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\DHARMENDRASINH.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\GAJANAN.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\HARMISH.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\JIGNESHKUMAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\JIVANADHAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\KAMLESH.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\KANWAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\RANDHAWA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\KILLOL.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\KUNDAN.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\MADHAV.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\IT\MADHAV.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\MAHAMMADSOAIB.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\CE\MAYURI.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\MAYURKUMAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\MIHIR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\MIHIR_SIDDHARTH.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\NILAYKUMAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\PRATIK.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\PUNIT.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\IT\RAJNIK.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\SAGAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\VIKAS.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\VIRAL.webp</t>
   </si>
 </sst>
 </file>
@@ -3720,8 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A109" workbookViewId="0">
-      <selection activeCell="E111" sqref="E111"/>
+    <sheetView tabSelected="1" topLeftCell="A113" zoomScale="80" workbookViewId="0">
+      <selection activeCell="D116" sqref="D116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3754,7 +3751,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>944</v>
+        <v>912</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -3772,13 +3769,13 @@
         <v>11</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>751</v>
+        <v>719</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>864</v>
+        <v>832</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>943</v>
+        <v>911</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -3795,7 +3792,7 @@
         <v>229</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>968</v>
+        <v>936</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>357</v>
@@ -3810,13 +3807,13 @@
         <v>253</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>947</v>
+        <v>915</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>752</v>
+        <v>720</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>470</v>
@@ -3839,7 +3836,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>562</v>
+        <v>976</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>358</v>
@@ -3854,19 +3851,19 @@
         <v>255</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>948</v>
+        <v>916</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>753</v>
+        <v>721</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>471</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>907</v>
+        <v>875</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -3877,13 +3874,13 @@
         <v>223</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>995</v>
+        <v>963</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>359</v>
@@ -3898,13 +3895,13 @@
         <v>254</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>949</v>
+        <v>917</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>710</v>
+        <v>678</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>754</v>
+        <v>722</v>
       </c>
       <c r="M4" s="9" t="s">
         <v>472</v>
@@ -3927,7 +3924,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>563</v>
+        <v>977</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>360</v>
@@ -3942,13 +3939,13 @@
         <v>256</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>946</v>
+        <v>914</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>755</v>
+        <v>723</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>473</v>
@@ -3971,7 +3968,7 @@
         <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>996</v>
+        <v>964</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>361</v>
@@ -3986,13 +3983,13 @@
         <v>257</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>945</v>
+        <v>913</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>756</v>
+        <v>724</v>
       </c>
       <c r="M6" s="9" t="s">
         <v>474</v>
@@ -4015,7 +4012,7 @@
         <v>230</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>997</v>
+        <v>965</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>362</v>
@@ -4030,19 +4027,19 @@
         <v>259</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>950</v>
+        <v>918</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>757</v>
+        <v>725</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>475</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>908</v>
+        <v>876</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -4059,7 +4056,7 @@
         <v>231</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>363</v>
@@ -4074,13 +4071,13 @@
         <v>258</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>951</v>
+        <v>919</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>758</v>
+        <v>726</v>
       </c>
       <c r="M8" s="10" t="s">
         <v>110</v>
@@ -4097,13 +4094,13 @@
         <v>223</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>734</v>
+        <v>702</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>565</v>
+        <v>978</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>364</v>
@@ -4118,19 +4115,19 @@
         <v>260</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>952</v>
+        <v>920</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>759</v>
+        <v>727</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>476</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>909</v>
+        <v>877</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -4147,7 +4144,7 @@
         <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>969</v>
+        <v>937</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>365</v>
@@ -4162,13 +4159,13 @@
         <v>261</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>953</v>
+        <v>921</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>760</v>
+        <v>728</v>
       </c>
       <c r="M10" s="9" t="s">
         <v>477</v>
@@ -4185,16 +4182,16 @@
         <v>223</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>232</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>566</v>
+        <v>979</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>872</v>
+        <v>840</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>110</v>
@@ -4209,10 +4206,10 @@
         <v>104</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>711</v>
+        <v>679</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>761</v>
+        <v>729</v>
       </c>
       <c r="M11" s="9" t="s">
         <v>477</v>
@@ -4235,7 +4232,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>970</v>
+        <v>938</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>366</v>
@@ -4244,25 +4241,25 @@
         <v>110</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>882</v>
+        <v>850</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>743</v>
+        <v>711</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>622</v>
+        <v>590</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>762</v>
+        <v>730</v>
       </c>
       <c r="M12" s="9" t="s">
         <v>478</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>910</v>
+        <v>878</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="105.6" x14ac:dyDescent="0.3">
@@ -4279,7 +4276,7 @@
         <v>85</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>567</v>
+        <v>938</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>367</v>
@@ -4291,7 +4288,7 @@
         <v>462</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>744</v>
+        <v>712</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>104</v>
@@ -4300,13 +4297,13 @@
         <v>110</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>763</v>
+        <v>731</v>
       </c>
       <c r="M13" s="9" t="s">
         <v>477</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>911</v>
+        <v>879</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -4323,7 +4320,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>971</v>
+        <v>939</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>368</v>
@@ -4332,25 +4329,25 @@
         <v>110</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>883</v>
+        <v>851</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>263</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>623</v>
+        <v>591</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>764</v>
+        <v>732</v>
       </c>
       <c r="M14" s="9" t="s">
         <v>479</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>912</v>
+        <v>880</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -4361,13 +4358,13 @@
         <v>223</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>90</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>568</v>
+        <v>563</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>369</v>
@@ -4382,13 +4379,13 @@
         <v>264</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>624</v>
+        <v>592</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>765</v>
+        <v>733</v>
       </c>
       <c r="M15" s="9" t="s">
         <v>480</v>
@@ -4411,7 +4408,7 @@
         <v>233</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>998</v>
+        <v>966</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>370</v>
@@ -4426,7 +4423,7 @@
         <v>265</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>625</v>
+        <v>593</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>110</v>
@@ -4449,22 +4446,22 @@
         <v>223</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>954</v>
+        <v>922</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>873</v>
+        <v>841</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>110</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>884</v>
+        <v>852</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>110</v>
@@ -4476,13 +4473,13 @@
         <v>110</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>766</v>
+        <v>734</v>
       </c>
       <c r="M17" s="9" t="s">
         <v>481</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>913</v>
+        <v>881</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
@@ -4499,7 +4496,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>569</v>
+        <v>980</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>371</v>
@@ -4514,19 +4511,19 @@
         <v>266</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>626</v>
+        <v>594</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>767</v>
+        <v>735</v>
       </c>
       <c r="M18" s="9" t="s">
         <v>482</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>914</v>
+        <v>882</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -4543,7 +4540,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>372</v>
@@ -4558,19 +4555,19 @@
         <v>267</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>627</v>
+        <v>595</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>768</v>
+        <v>736</v>
       </c>
       <c r="M19" s="9" t="s">
         <v>483</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>915</v>
+        <v>883</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -4587,7 +4584,7 @@
         <v>73</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>373</v>
@@ -4602,13 +4599,13 @@
         <v>268</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>628</v>
+        <v>596</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>769</v>
+        <v>737</v>
       </c>
       <c r="M20" s="9" t="s">
         <v>477</v>
@@ -4631,7 +4628,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>999</v>
+        <v>967</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>374</v>
@@ -4646,13 +4643,13 @@
         <v>269</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>629</v>
+        <v>597</v>
       </c>
       <c r="K21" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>770</v>
+        <v>738</v>
       </c>
       <c r="M21" s="9" t="s">
         <v>484</v>
@@ -4675,10 +4672,10 @@
         <v>50</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>572</v>
+        <v>981</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>874</v>
+        <v>842</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>110</v>
@@ -4696,7 +4693,7 @@
         <v>110</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>771</v>
+        <v>739</v>
       </c>
       <c r="M22" s="9" t="s">
         <v>485</v>
@@ -4719,7 +4716,7 @@
         <v>28</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>972</v>
+        <v>940</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>375</v>
@@ -4734,19 +4731,19 @@
         <v>271</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>630</v>
+        <v>598</v>
       </c>
       <c r="K23" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>772</v>
+        <v>740</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>486</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>916</v>
+        <v>884</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="211.2" x14ac:dyDescent="0.3">
@@ -4757,13 +4754,13 @@
         <v>223</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>573</v>
+        <v>982</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>376</v>
@@ -4778,13 +4775,13 @@
         <v>272</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>631</v>
+        <v>599</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>773</v>
+        <v>741</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>487</v>
@@ -4807,7 +4804,7 @@
         <v>234</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>1000</v>
+        <v>968</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>377</v>
@@ -4819,22 +4816,22 @@
         <v>110</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>745</v>
+        <v>713</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>632</v>
+        <v>600</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>712</v>
+        <v>680</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>774</v>
+        <v>742</v>
       </c>
       <c r="M25" s="10" t="s">
         <v>110</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>917</v>
+        <v>885</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -4851,7 +4848,7 @@
         <v>55</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>574</v>
+        <v>983</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>378</v>
@@ -4860,19 +4857,19 @@
         <v>110</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>885</v>
+        <v>853</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>273</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>633</v>
+        <v>601</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>713</v>
+        <v>681</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>775</v>
+        <v>743</v>
       </c>
       <c r="M26" s="9" t="s">
         <v>488</v>
@@ -4889,13 +4886,13 @@
         <v>223</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>1001</v>
+        <v>969</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>379</v>
@@ -4910,19 +4907,19 @@
         <v>274</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>634</v>
+        <v>602</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>714</v>
+        <v>682</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>776</v>
+        <v>744</v>
       </c>
       <c r="M27" s="9" t="s">
         <v>489</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>918</v>
+        <v>886</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -4939,7 +4936,7 @@
         <v>46</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>973</v>
+        <v>941</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>380</v>
@@ -4951,22 +4948,22 @@
         <v>110</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>746</v>
+        <v>714</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>635</v>
+        <v>603</v>
       </c>
       <c r="K28" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>777</v>
+        <v>745</v>
       </c>
       <c r="M28" s="9" t="s">
         <v>478</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>919</v>
+        <v>887</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
@@ -4977,13 +4974,13 @@
         <v>223</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>974</v>
+        <v>942</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>381</v>
@@ -4995,16 +4992,16 @@
         <v>110</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>747</v>
+        <v>715</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>636</v>
+        <v>604</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>778</v>
+        <v>746</v>
       </c>
       <c r="M29" s="9" t="s">
         <v>490</v>
@@ -5027,7 +5024,7 @@
         <v>235</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>955</v>
+        <v>923</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>382</v>
@@ -5042,13 +5039,13 @@
         <v>275</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>637</v>
+        <v>605</v>
       </c>
       <c r="K30" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>779</v>
+        <v>747</v>
       </c>
       <c r="M30" s="17">
         <v>583944</v>
@@ -5071,7 +5068,7 @@
         <v>236</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>575</v>
+        <v>566</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>383</v>
@@ -5080,19 +5077,19 @@
         <v>110</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>886</v>
+        <v>854</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>276</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>638</v>
+        <v>606</v>
       </c>
       <c r="K31" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>780</v>
+        <v>748</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>491</v>
@@ -5115,7 +5112,7 @@
         <v>39</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>576</v>
+        <v>984</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>384</v>
@@ -5130,16 +5127,16 @@
         <v>277</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>639</v>
+        <v>607</v>
       </c>
       <c r="K32" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>781</v>
+        <v>749</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>861</v>
+        <v>829</v>
       </c>
       <c r="N32" s="10" t="s">
         <v>110</v>
@@ -5159,7 +5156,7 @@
         <v>237</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>984</v>
+        <v>952</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>385</v>
@@ -5174,19 +5171,19 @@
         <v>278</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>640</v>
+        <v>608</v>
       </c>
       <c r="K33" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>782</v>
+        <v>750</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>862</v>
+        <v>830</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>920</v>
+        <v>888</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -5203,7 +5200,7 @@
         <v>70</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>956</v>
+        <v>924</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>386</v>
@@ -5212,19 +5209,19 @@
         <v>110</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>887</v>
+        <v>855</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>279</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>641</v>
+        <v>609</v>
       </c>
       <c r="K34" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>783</v>
+        <v>751</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>492</v>
@@ -5247,7 +5244,7 @@
         <v>35</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>957</v>
+        <v>925</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>387</v>
@@ -5262,7 +5259,7 @@
         <v>280</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>642</v>
+        <v>610</v>
       </c>
       <c r="K35" s="14" t="s">
         <v>110</v>
@@ -5288,10 +5285,10 @@
         <v>5</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>865</v>
+        <v>833</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>577</v>
+        <v>567</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>388</v>
@@ -5306,19 +5303,19 @@
         <v>281</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>643</v>
+        <v>611</v>
       </c>
       <c r="K36" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>784</v>
+        <v>752</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>494</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>921</v>
+        <v>889</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -5335,7 +5332,7 @@
         <v>98</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>578</v>
+        <v>985</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>389</v>
@@ -5350,13 +5347,13 @@
         <v>282</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>644</v>
+        <v>612</v>
       </c>
       <c r="K37" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>785</v>
+        <v>753</v>
       </c>
       <c r="M37" s="9" t="s">
         <v>495</v>
@@ -5373,16 +5370,16 @@
         <v>223</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>1002</v>
+        <v>970</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>875</v>
+        <v>843</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>110</v>
@@ -5394,13 +5391,13 @@
         <v>283</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>645</v>
+        <v>613</v>
       </c>
       <c r="K38" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>786</v>
+        <v>754</v>
       </c>
       <c r="M38" s="9" t="s">
         <v>496</v>
@@ -5417,13 +5414,13 @@
         <v>223</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>1003</v>
+        <v>971</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>390</v>
@@ -5438,13 +5435,13 @@
         <v>284</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>646</v>
+        <v>614</v>
       </c>
       <c r="K39" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>787</v>
+        <v>755</v>
       </c>
       <c r="M39" s="10" t="s">
         <v>110</v>
@@ -5467,7 +5464,7 @@
         <v>81</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>985</v>
+        <v>953</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>391</v>
@@ -5482,13 +5479,13 @@
         <v>110</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>647</v>
+        <v>615</v>
       </c>
       <c r="K40" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>788</v>
+        <v>756</v>
       </c>
       <c r="M40" s="9" t="s">
         <v>497</v>
@@ -5505,13 +5502,13 @@
         <v>223</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>63</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>579</v>
+        <v>568</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>392</v>
@@ -5520,19 +5517,19 @@
         <v>110</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>888</v>
+        <v>856</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>285</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>648</v>
+        <v>616</v>
       </c>
       <c r="K41" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>789</v>
+        <v>757</v>
       </c>
       <c r="M41" s="9" t="s">
         <v>498</v>
@@ -5555,7 +5552,7 @@
         <v>52</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>958</v>
+        <v>926</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>393</v>
@@ -5570,13 +5567,13 @@
         <v>286</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>649</v>
+        <v>617</v>
       </c>
       <c r="K42" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>790</v>
+        <v>758</v>
       </c>
       <c r="M42" s="9" t="s">
         <v>499</v>
@@ -5593,13 +5590,13 @@
         <v>223</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>74</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>987</v>
+        <v>955</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>394</v>
@@ -5614,19 +5611,19 @@
         <v>287</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>650</v>
+        <v>618</v>
       </c>
       <c r="K43" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>791</v>
+        <v>759</v>
       </c>
       <c r="M43" s="9" t="s">
         <v>500</v>
       </c>
       <c r="N43" s="10" t="s">
-        <v>922</v>
+        <v>890</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -5643,7 +5640,7 @@
         <v>94</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>986</v>
+        <v>954</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>395</v>
@@ -5658,13 +5655,13 @@
         <v>288</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>651</v>
+        <v>619</v>
       </c>
       <c r="K44" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>792</v>
+        <v>760</v>
       </c>
       <c r="M44" s="9" t="s">
         <v>501</v>
@@ -5687,7 +5684,7 @@
         <v>86</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>1004</v>
+        <v>972</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>396</v>
@@ -5702,13 +5699,13 @@
         <v>289</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>652</v>
+        <v>620</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>715</v>
+        <v>683</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>793</v>
+        <v>761</v>
       </c>
       <c r="M45" s="9" t="s">
         <v>502</v>
@@ -5725,13 +5722,13 @@
         <v>223</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>736</v>
+        <v>704</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>580</v>
+        <v>986</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>397</v>
@@ -5752,7 +5749,7 @@
         <v>110</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>794</v>
+        <v>762</v>
       </c>
       <c r="M46" s="9" t="s">
         <v>503</v>
@@ -5775,7 +5772,7 @@
         <v>92</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>581</v>
+        <v>987</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>398</v>
@@ -5790,13 +5787,13 @@
         <v>291</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>653</v>
+        <v>621</v>
       </c>
       <c r="K47" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L47" s="9" t="s">
-        <v>795</v>
+        <v>763</v>
       </c>
       <c r="M47" s="10" t="s">
         <v>110</v>
@@ -5819,7 +5816,7 @@
         <v>66</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>582</v>
+        <v>988</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>399</v>
@@ -5840,7 +5837,7 @@
         <v>110</v>
       </c>
       <c r="L48" s="9" t="s">
-        <v>796</v>
+        <v>764</v>
       </c>
       <c r="M48" s="9" t="s">
         <v>477</v>
@@ -5863,7 +5860,7 @@
         <v>20</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>583</v>
+        <v>989</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>400</v>
@@ -5875,22 +5872,22 @@
         <v>110</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>748</v>
+        <v>716</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>654</v>
+        <v>622</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>716</v>
+        <v>684</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>797</v>
+        <v>765</v>
       </c>
       <c r="M49" s="9" t="s">
         <v>504</v>
       </c>
       <c r="N49" s="10" t="s">
-        <v>923</v>
+        <v>891</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
@@ -5907,7 +5904,7 @@
         <v>26</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>584</v>
+        <v>990</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>401</v>
@@ -5916,25 +5913,25 @@
         <v>110</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>889</v>
+        <v>857</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>293</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>655</v>
+        <v>623</v>
       </c>
       <c r="K50" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L50" s="9" t="s">
-        <v>798</v>
+        <v>766</v>
       </c>
       <c r="M50" s="9" t="s">
         <v>505</v>
       </c>
       <c r="N50" s="10" t="s">
-        <v>924</v>
+        <v>892</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -5948,10 +5945,10 @@
         <v>5</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>866</v>
+        <v>834</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>585</v>
+        <v>991</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>402</v>
@@ -5960,7 +5957,7 @@
         <v>110</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>890</v>
+        <v>858</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>294</v>
@@ -5972,7 +5969,7 @@
         <v>110</v>
       </c>
       <c r="L51" s="9" t="s">
-        <v>799</v>
+        <v>767</v>
       </c>
       <c r="M51" s="9" t="s">
         <v>477</v>
@@ -5995,7 +5992,7 @@
         <v>30</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>975</v>
+        <v>943</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>403</v>
@@ -6010,13 +6007,13 @@
         <v>295</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>656</v>
+        <v>624</v>
       </c>
       <c r="K52" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L52" s="9" t="s">
-        <v>800</v>
+        <v>768</v>
       </c>
       <c r="M52" s="10" t="s">
         <v>110</v>
@@ -6039,7 +6036,7 @@
         <v>58</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>586</v>
+        <v>992</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>404</v>
@@ -6054,13 +6051,13 @@
         <v>296</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>657</v>
+        <v>625</v>
       </c>
       <c r="K53" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L53" s="9" t="s">
-        <v>801</v>
+        <v>769</v>
       </c>
       <c r="M53" s="9" t="s">
         <v>506</v>
@@ -6083,7 +6080,7 @@
         <v>62</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>587</v>
+        <v>993</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>405</v>
@@ -6092,19 +6089,19 @@
         <v>110</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>891</v>
+        <v>859</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>298</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>658</v>
+        <v>626</v>
       </c>
       <c r="K54" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L54" s="9" t="s">
-        <v>802</v>
+        <v>770</v>
       </c>
       <c r="M54" s="9" t="s">
         <v>507</v>
@@ -6121,13 +6118,13 @@
         <v>223</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>238</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>588</v>
+        <v>994</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>406</v>
@@ -6136,7 +6133,7 @@
         <v>110</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>892</v>
+        <v>860</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>297</v>
@@ -6148,13 +6145,13 @@
         <v>110</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>803</v>
+        <v>771</v>
       </c>
       <c r="M55" s="9" t="s">
         <v>508</v>
       </c>
       <c r="N55" s="10" t="s">
-        <v>925</v>
+        <v>893</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -6165,16 +6162,16 @@
         <v>223</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>736</v>
+        <v>704</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>589</v>
+        <v>995</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>876</v>
+        <v>844</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>110</v>
@@ -6192,7 +6189,7 @@
         <v>110</v>
       </c>
       <c r="L56" s="9" t="s">
-        <v>804</v>
+        <v>772</v>
       </c>
       <c r="M56" s="9" t="s">
         <v>509</v>
@@ -6212,10 +6209,10 @@
         <v>5</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>867</v>
+        <v>835</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>590</v>
+        <v>569</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>407</v>
@@ -6224,25 +6221,25 @@
         <v>110</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>893</v>
+        <v>861</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>300</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>659</v>
+        <v>627</v>
       </c>
       <c r="K57" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L57" s="9" t="s">
-        <v>805</v>
+        <v>773</v>
       </c>
       <c r="M57" s="9" t="s">
         <v>510</v>
       </c>
       <c r="N57" s="10" t="s">
-        <v>926</v>
+        <v>894</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -6259,7 +6256,7 @@
         <v>239</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>976</v>
+        <v>944</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>408</v>
@@ -6268,19 +6265,19 @@
         <v>110</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>894</v>
+        <v>862</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>301</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>660</v>
+        <v>628</v>
       </c>
       <c r="K58" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L58" s="9" t="s">
-        <v>806</v>
+        <v>774</v>
       </c>
       <c r="M58" s="9" t="s">
         <v>511</v>
@@ -6297,13 +6294,13 @@
         <v>223</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>734</v>
+        <v>702</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>83</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>959</v>
+        <v>927</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>409</v>
@@ -6312,19 +6309,19 @@
         <v>110</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>895</v>
+        <v>863</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>302</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>661</v>
+        <v>629</v>
       </c>
       <c r="K59" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L59" s="9" t="s">
-        <v>807</v>
+        <v>775</v>
       </c>
       <c r="M59" s="9" t="s">
         <v>512</v>
@@ -6347,7 +6344,7 @@
         <v>240</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>959</v>
+        <v>996</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>410</v>
@@ -6362,19 +6359,19 @@
         <v>303</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>662</v>
+        <v>630</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>717</v>
+        <v>685</v>
       </c>
       <c r="L60" s="9" t="s">
-        <v>808</v>
+        <v>776</v>
       </c>
       <c r="M60" s="9" t="s">
         <v>513</v>
       </c>
       <c r="N60" s="10" t="s">
-        <v>927</v>
+        <v>895</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -6391,28 +6388,28 @@
         <v>68</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>591</v>
+        <v>997</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>877</v>
+        <v>845</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>110</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>896</v>
+        <v>864</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>304</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>663</v>
+        <v>631</v>
       </c>
       <c r="K61" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L61" s="9" t="s">
-        <v>809</v>
+        <v>777</v>
       </c>
       <c r="M61" s="9" t="s">
         <v>514</v>
@@ -6429,13 +6426,13 @@
         <v>223</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>65</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>988</v>
+        <v>956</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>411</v>
@@ -6456,7 +6453,7 @@
         <v>110</v>
       </c>
       <c r="L62" s="9" t="s">
-        <v>810</v>
+        <v>778</v>
       </c>
       <c r="M62" s="9" t="s">
         <v>515</v>
@@ -6476,10 +6473,10 @@
         <v>4</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>868</v>
+        <v>836</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>989</v>
+        <v>957</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>412</v>
@@ -6494,13 +6491,13 @@
         <v>306</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>664</v>
+        <v>632</v>
       </c>
       <c r="K63" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L63" s="9" t="s">
-        <v>811</v>
+        <v>779</v>
       </c>
       <c r="M63" s="9" t="s">
         <v>516</v>
@@ -6523,7 +6520,7 @@
         <v>78</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>592</v>
+        <v>998</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>413</v>
@@ -6538,19 +6535,19 @@
         <v>307</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>665</v>
+        <v>633</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>718</v>
+        <v>686</v>
       </c>
       <c r="L64" s="9" t="s">
-        <v>812</v>
+        <v>780</v>
       </c>
       <c r="M64" s="9" t="s">
         <v>477</v>
       </c>
       <c r="N64" s="10" t="s">
-        <v>919</v>
+        <v>887</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
@@ -6561,13 +6558,13 @@
         <v>223</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>737</v>
+        <v>705</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>69</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>593</v>
+        <v>999</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>414</v>
@@ -6576,19 +6573,19 @@
         <v>110</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>897</v>
+        <v>865</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>308</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>666</v>
+        <v>634</v>
       </c>
       <c r="K65" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L65" s="9" t="s">
-        <v>813</v>
+        <v>781</v>
       </c>
       <c r="M65" s="9" t="s">
         <v>517</v>
@@ -6611,7 +6608,7 @@
         <v>99</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>594</v>
+        <v>570</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>415</v>
@@ -6626,19 +6623,19 @@
         <v>309</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>667</v>
+        <v>635</v>
       </c>
       <c r="K66" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L66" s="9" t="s">
-        <v>814</v>
+        <v>782</v>
       </c>
       <c r="M66" s="9" t="s">
         <v>518</v>
       </c>
       <c r="N66" s="10" t="s">
-        <v>928</v>
+        <v>896</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="277.2" x14ac:dyDescent="0.3">
@@ -6655,7 +6652,7 @@
         <v>38</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>595</v>
+        <v>571</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>416</v>
@@ -6664,19 +6661,19 @@
         <v>110</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>898</v>
+        <v>866</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>310</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>668</v>
+        <v>636</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>719</v>
+        <v>687</v>
       </c>
       <c r="L67" s="9" t="s">
-        <v>815</v>
+        <v>783</v>
       </c>
       <c r="M67" s="9" t="s">
         <v>519</v>
@@ -6699,7 +6696,7 @@
         <v>23</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>977</v>
+        <v>945</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>417</v>
@@ -6714,13 +6711,13 @@
         <v>311</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>669</v>
+        <v>637</v>
       </c>
       <c r="K68" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L68" s="9" t="s">
-        <v>816</v>
+        <v>784</v>
       </c>
       <c r="M68" s="9" t="s">
         <v>520</v>
@@ -6743,7 +6740,7 @@
         <v>241</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>596</v>
+        <v>572</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>418</v>
@@ -6758,7 +6755,7 @@
         <v>312</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>670</v>
+        <v>638</v>
       </c>
       <c r="K69" s="14" t="s">
         <v>110</v>
@@ -6787,10 +6784,10 @@
         <v>49</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>990</v>
+        <v>958</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>878</v>
+        <v>846</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>110</v>
@@ -6802,19 +6799,19 @@
         <v>313</v>
       </c>
       <c r="J70" s="9" t="s">
-        <v>671</v>
+        <v>639</v>
       </c>
       <c r="K70" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L70" s="9" t="s">
-        <v>817</v>
+        <v>785</v>
       </c>
       <c r="M70" s="9" t="s">
         <v>521</v>
       </c>
       <c r="N70" s="10" t="s">
-        <v>929</v>
+        <v>897</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -6828,10 +6825,10 @@
         <v>5</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>869</v>
+        <v>837</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>978</v>
+        <v>946</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>419</v>
@@ -6846,13 +6843,13 @@
         <v>314</v>
       </c>
       <c r="J71" s="9" t="s">
-        <v>672</v>
+        <v>640</v>
       </c>
       <c r="K71" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L71" s="9" t="s">
-        <v>818</v>
+        <v>786</v>
       </c>
       <c r="M71" s="9" t="s">
         <v>522</v>
@@ -6875,7 +6872,7 @@
         <v>16</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>597</v>
+        <v>1000</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>420</v>
@@ -6884,19 +6881,19 @@
         <v>110</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>899</v>
+        <v>867</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>315</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>673</v>
+        <v>641</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>720</v>
+        <v>688</v>
       </c>
       <c r="L72" s="9" t="s">
-        <v>819</v>
+        <v>787</v>
       </c>
       <c r="M72" s="9" t="s">
         <v>523</v>
@@ -6919,7 +6916,7 @@
         <v>242</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>960</v>
+        <v>928</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>421</v>
@@ -6928,25 +6925,25 @@
         <v>110</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>900</v>
+        <v>868</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>316</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>674</v>
+        <v>642</v>
       </c>
       <c r="K73" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L73" s="9" t="s">
-        <v>820</v>
+        <v>788</v>
       </c>
       <c r="M73" s="9" t="s">
         <v>524</v>
       </c>
       <c r="N73" s="10" t="s">
-        <v>930</v>
+        <v>898</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -6963,10 +6960,10 @@
         <v>96</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>991</v>
+        <v>959</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>879</v>
+        <v>847</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>110</v>
@@ -6978,19 +6975,19 @@
         <v>317</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>675</v>
+        <v>643</v>
       </c>
       <c r="K74" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L74" s="10" t="s">
-        <v>821</v>
+        <v>789</v>
       </c>
       <c r="M74" s="9" t="s">
         <v>525</v>
       </c>
       <c r="N74" s="10" t="s">
-        <v>926</v>
+        <v>894</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -7007,7 +7004,7 @@
         <v>71</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>961</v>
+        <v>929</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>422</v>
@@ -7022,13 +7019,13 @@
         <v>318</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>676</v>
+        <v>644</v>
       </c>
       <c r="K75" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L75" s="9" t="s">
-        <v>822</v>
+        <v>790</v>
       </c>
       <c r="M75" s="9" t="s">
         <v>477</v>
@@ -7051,7 +7048,7 @@
         <v>243</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>963</v>
+        <v>931</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>423</v>
@@ -7066,19 +7063,19 @@
         <v>319</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>677</v>
+        <v>645</v>
       </c>
       <c r="K76" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L76" s="9" t="s">
-        <v>823</v>
+        <v>791</v>
       </c>
       <c r="M76" s="9" t="s">
         <v>526</v>
       </c>
       <c r="N76" s="10" t="s">
-        <v>931</v>
+        <v>899</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -7095,7 +7092,7 @@
         <v>37</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>962</v>
+        <v>930</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>424</v>
@@ -7110,7 +7107,7 @@
         <v>320</v>
       </c>
       <c r="J77" s="9" t="s">
-        <v>678</v>
+        <v>646</v>
       </c>
       <c r="K77" s="14" t="s">
         <v>110</v>
@@ -7133,13 +7130,13 @@
         <v>223</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>598</v>
+        <v>573</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>425</v>
@@ -7154,7 +7151,7 @@
         <v>321</v>
       </c>
       <c r="J78" s="9" t="s">
-        <v>679</v>
+        <v>647</v>
       </c>
       <c r="K78" s="10" t="s">
         <v>110</v>
@@ -7180,10 +7177,10 @@
         <v>5</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>870</v>
+        <v>838</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>964</v>
+        <v>932</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>426</v>
@@ -7198,13 +7195,13 @@
         <v>322</v>
       </c>
       <c r="J79" s="9" t="s">
-        <v>680</v>
+        <v>648</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>721</v>
+        <v>689</v>
       </c>
       <c r="L79" s="9" t="s">
-        <v>824</v>
+        <v>792</v>
       </c>
       <c r="M79" s="9" t="s">
         <v>528</v>
@@ -7227,7 +7224,7 @@
         <v>33</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>965</v>
+        <v>933</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>427</v>
@@ -7265,16 +7262,16 @@
         <v>223</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>992</v>
+        <v>960</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>880</v>
+        <v>848</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>110</v>
@@ -7292,13 +7289,13 @@
         <v>110</v>
       </c>
       <c r="L81" s="9" t="s">
-        <v>825</v>
+        <v>793</v>
       </c>
       <c r="M81" s="9" t="s">
         <v>530</v>
       </c>
       <c r="N81" s="10" t="s">
-        <v>932</v>
+        <v>900</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -7309,13 +7306,13 @@
         <v>223</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>738</v>
+        <v>706</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>244</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>599</v>
+        <v>574</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>428</v>
@@ -7336,7 +7333,7 @@
         <v>110</v>
       </c>
       <c r="L82" s="9" t="s">
-        <v>826</v>
+        <v>794</v>
       </c>
       <c r="M82" s="9" t="s">
         <v>531</v>
@@ -7359,7 +7356,7 @@
         <v>18</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>600</v>
+        <v>575</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>429</v>
@@ -7374,13 +7371,13 @@
         <v>326</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>681</v>
+        <v>649</v>
       </c>
       <c r="K83" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L83" s="9" t="s">
-        <v>827</v>
+        <v>795</v>
       </c>
       <c r="M83" s="9" t="s">
         <v>532</v>
@@ -7397,13 +7394,13 @@
         <v>223</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>80</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>601</v>
+        <v>1001</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>430</v>
@@ -7418,13 +7415,13 @@
         <v>327</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>682</v>
+        <v>650</v>
       </c>
       <c r="K84" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L84" s="9" t="s">
-        <v>828</v>
+        <v>796</v>
       </c>
       <c r="M84" s="9" t="s">
         <v>533</v>
@@ -7447,7 +7444,7 @@
         <v>245</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>602</v>
+        <v>576</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>431</v>
@@ -7462,13 +7459,13 @@
         <v>110</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>683</v>
+        <v>651</v>
       </c>
       <c r="K85" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L85" s="9" t="s">
-        <v>829</v>
+        <v>797</v>
       </c>
       <c r="M85" s="9" t="s">
         <v>534</v>
@@ -7477,7 +7474,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="330" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="343.2" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>192</v>
       </c>
@@ -7491,7 +7488,7 @@
         <v>31</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>603</v>
+        <v>577</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>432</v>
@@ -7509,16 +7506,16 @@
         <v>101</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>722</v>
+        <v>690</v>
       </c>
       <c r="L86" s="9" t="s">
-        <v>830</v>
+        <v>798</v>
       </c>
       <c r="M86" s="9" t="s">
         <v>535</v>
       </c>
       <c r="N86" s="10" t="s">
-        <v>933</v>
+        <v>901</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -7535,7 +7532,7 @@
         <v>97</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>966</v>
+        <v>934</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>433</v>
@@ -7544,25 +7541,25 @@
         <v>110</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>901</v>
+        <v>869</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>329</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>684</v>
+        <v>652</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>723</v>
+        <v>691</v>
       </c>
       <c r="L87" s="9" t="s">
+        <v>799</v>
+      </c>
+      <c r="M87" s="9" t="s">
         <v>831</v>
       </c>
-      <c r="M87" s="9" t="s">
-        <v>863</v>
-      </c>
       <c r="N87" s="10" t="s">
-        <v>934</v>
+        <v>902</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -7573,13 +7570,13 @@
         <v>223</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>246</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>604</v>
+        <v>1002</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>434</v>
@@ -7600,7 +7597,7 @@
         <v>110</v>
       </c>
       <c r="L88" s="9" t="s">
-        <v>832</v>
+        <v>800</v>
       </c>
       <c r="M88" s="9" t="s">
         <v>536</v>
@@ -7623,7 +7620,7 @@
         <v>95</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>605</v>
+        <v>578</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>435</v>
@@ -7638,13 +7635,13 @@
         <v>331</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>685</v>
+        <v>653</v>
       </c>
       <c r="K89" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L89" s="9" t="s">
-        <v>833</v>
+        <v>801</v>
       </c>
       <c r="M89" s="9" t="s">
         <v>537</v>
@@ -7667,7 +7664,7 @@
         <v>56</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>606</v>
+        <v>1003</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>436</v>
@@ -7679,22 +7676,22 @@
         <v>110</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>749</v>
+        <v>717</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>686</v>
+        <v>654</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>724</v>
+        <v>692</v>
       </c>
       <c r="L90" s="9" t="s">
-        <v>834</v>
+        <v>802</v>
       </c>
       <c r="M90" s="9" t="s">
         <v>538</v>
       </c>
       <c r="N90" s="10" t="s">
-        <v>935</v>
+        <v>903</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -7711,7 +7708,7 @@
         <v>24</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>607</v>
+        <v>579</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>437</v>
@@ -7720,19 +7717,19 @@
         <v>110</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>902</v>
+        <v>870</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>332</v>
       </c>
       <c r="J91" s="9" t="s">
-        <v>687</v>
+        <v>655</v>
       </c>
       <c r="K91" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L91" s="9" t="s">
-        <v>835</v>
+        <v>803</v>
       </c>
       <c r="M91" s="9" t="s">
         <v>539</v>
@@ -7755,7 +7752,7 @@
         <v>21</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>979</v>
+        <v>947</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>438</v>
@@ -7770,13 +7767,13 @@
         <v>333</v>
       </c>
       <c r="J92" s="9" t="s">
-        <v>688</v>
+        <v>656</v>
       </c>
       <c r="K92" s="9" t="s">
-        <v>725</v>
+        <v>693</v>
       </c>
       <c r="L92" s="9" t="s">
-        <v>836</v>
+        <v>804</v>
       </c>
       <c r="M92" s="9" t="s">
         <v>540</v>
@@ -7799,7 +7796,7 @@
         <v>247</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>608</v>
+        <v>580</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>439</v>
@@ -7808,25 +7805,25 @@
         <v>110</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>903</v>
+        <v>871</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>334</v>
       </c>
       <c r="J93" s="9" t="s">
-        <v>689</v>
+        <v>657</v>
       </c>
       <c r="K93" s="9" t="s">
-        <v>726</v>
+        <v>694</v>
       </c>
       <c r="L93" s="9" t="s">
-        <v>837</v>
+        <v>805</v>
       </c>
       <c r="M93" s="9" t="s">
         <v>541</v>
       </c>
       <c r="N93" s="10" t="s">
-        <v>936</v>
+        <v>904</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
@@ -7843,7 +7840,7 @@
         <v>89</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>980</v>
+        <v>948</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>440</v>
@@ -7861,10 +7858,10 @@
         <v>108</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>727</v>
+        <v>695</v>
       </c>
       <c r="L94" s="9" t="s">
-        <v>838</v>
+        <v>806</v>
       </c>
       <c r="M94" s="9" t="s">
         <v>542</v>
@@ -7887,7 +7884,7 @@
         <v>25</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>981</v>
+        <v>949</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>441</v>
@@ -7902,19 +7899,19 @@
         <v>336</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>690</v>
+        <v>658</v>
       </c>
       <c r="K95" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L95" s="9" t="s">
-        <v>839</v>
+        <v>807</v>
       </c>
       <c r="M95" s="9" t="s">
         <v>543</v>
       </c>
       <c r="N95" s="10" t="s">
-        <v>937</v>
+        <v>905</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -7931,7 +7928,7 @@
         <v>79</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>609</v>
+        <v>1004</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>442</v>
@@ -7940,25 +7937,25 @@
         <v>110</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>904</v>
+        <v>872</v>
       </c>
       <c r="I96" s="4" t="s">
         <v>337</v>
       </c>
       <c r="J96" s="9" t="s">
-        <v>691</v>
+        <v>659</v>
       </c>
       <c r="K96" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L96" s="9" t="s">
-        <v>840</v>
+        <v>808</v>
       </c>
       <c r="M96" s="9" t="s">
         <v>544</v>
       </c>
       <c r="N96" s="10" t="s">
-        <v>938</v>
+        <v>906</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -7975,7 +7972,7 @@
         <v>47</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>610</v>
+        <v>1004</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>443</v>
@@ -7984,25 +7981,25 @@
         <v>110</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>905</v>
+        <v>873</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>338</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>692</v>
+        <v>660</v>
       </c>
       <c r="K97" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L97" s="9" t="s">
-        <v>841</v>
+        <v>809</v>
       </c>
       <c r="M97" s="9" t="s">
         <v>545</v>
       </c>
       <c r="N97" s="10" t="s">
-        <v>926</v>
+        <v>894</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -8019,7 +8016,7 @@
         <v>57</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>611</v>
+        <v>581</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>444</v>
@@ -8034,19 +8031,19 @@
         <v>339</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>693</v>
+        <v>661</v>
       </c>
       <c r="K98" s="9" t="s">
-        <v>728</v>
+        <v>696</v>
       </c>
       <c r="L98" s="9" t="s">
-        <v>842</v>
+        <v>810</v>
       </c>
       <c r="M98" s="9" t="s">
         <v>546</v>
       </c>
       <c r="N98" s="10" t="s">
-        <v>939</v>
+        <v>907</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -8057,13 +8054,13 @@
         <v>223</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>612</v>
+        <v>582</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>445</v>
@@ -8084,7 +8081,7 @@
         <v>110</v>
       </c>
       <c r="L99" s="9" t="s">
-        <v>843</v>
+        <v>811</v>
       </c>
       <c r="M99" s="9" t="s">
         <v>547</v>
@@ -8101,13 +8098,13 @@
         <v>223</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>248</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>613</v>
+        <v>583</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>446</v>
@@ -8122,13 +8119,13 @@
         <v>341</v>
       </c>
       <c r="J100" s="9" t="s">
-        <v>694</v>
+        <v>662</v>
       </c>
       <c r="K100" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L100" s="9" t="s">
-        <v>844</v>
+        <v>812</v>
       </c>
       <c r="M100" s="9" t="s">
         <v>548</v>
@@ -8151,7 +8148,7 @@
         <v>43</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>982</v>
+        <v>950</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>447</v>
@@ -8166,13 +8163,13 @@
         <v>342</v>
       </c>
       <c r="J101" s="9" t="s">
-        <v>695</v>
+        <v>663</v>
       </c>
       <c r="K101" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L101" s="9" t="s">
-        <v>845</v>
+        <v>813</v>
       </c>
       <c r="M101" s="9" t="s">
         <v>549</v>
@@ -8189,13 +8186,13 @@
         <v>223</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>739</v>
+        <v>707</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>967</v>
+        <v>935</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>448</v>
@@ -8210,13 +8207,13 @@
         <v>343</v>
       </c>
       <c r="J102" s="9" t="s">
-        <v>696</v>
+        <v>664</v>
       </c>
       <c r="K102" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L102" s="9" t="s">
-        <v>846</v>
+        <v>814</v>
       </c>
       <c r="M102" s="9" t="s">
         <v>550</v>
@@ -8239,7 +8236,7 @@
         <v>88</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>1005</v>
+        <v>973</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>449</v>
@@ -8254,13 +8251,13 @@
         <v>344</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>697</v>
+        <v>665</v>
       </c>
       <c r="K103" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L103" s="9" t="s">
-        <v>847</v>
+        <v>815</v>
       </c>
       <c r="M103" s="10" t="s">
         <v>110</v>
@@ -8277,13 +8274,13 @@
         <v>223</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>740</v>
+        <v>708</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>614</v>
+        <v>584</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>450</v>
@@ -8298,13 +8295,13 @@
         <v>110</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>698</v>
+        <v>666</v>
       </c>
       <c r="K104" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L104" s="9" t="s">
-        <v>848</v>
+        <v>816</v>
       </c>
       <c r="M104" s="9" t="s">
         <v>551</v>
@@ -8321,13 +8318,13 @@
         <v>223</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>615</v>
+        <v>585</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>451</v>
@@ -8342,13 +8339,13 @@
         <v>345</v>
       </c>
       <c r="J105" s="9" t="s">
-        <v>699</v>
+        <v>667</v>
       </c>
       <c r="K105" s="9" t="s">
-        <v>729</v>
+        <v>697</v>
       </c>
       <c r="L105" s="9" t="s">
-        <v>849</v>
+        <v>817</v>
       </c>
       <c r="M105" s="9" t="s">
         <v>552</v>
@@ -8371,7 +8368,7 @@
         <v>22</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>616</v>
+        <v>586</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>452</v>
@@ -8389,10 +8386,10 @@
         <v>100</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>730</v>
+        <v>698</v>
       </c>
       <c r="L106" s="9" t="s">
-        <v>850</v>
+        <v>818</v>
       </c>
       <c r="M106" s="9" t="s">
         <v>553</v>
@@ -8415,7 +8412,7 @@
         <v>249</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>617</v>
+        <v>587</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>453</v>
@@ -8430,19 +8427,19 @@
         <v>347</v>
       </c>
       <c r="J107" s="9" t="s">
-        <v>700</v>
+        <v>668</v>
       </c>
       <c r="K107" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L107" s="9" t="s">
-        <v>851</v>
+        <v>819</v>
       </c>
       <c r="M107" s="9" t="s">
         <v>554</v>
       </c>
       <c r="N107" s="10" t="s">
-        <v>940</v>
+        <v>908</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -8459,7 +8456,7 @@
         <v>250</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>1006</v>
+        <v>974</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>454</v>
@@ -8474,13 +8471,13 @@
         <v>348</v>
       </c>
       <c r="J108" s="9" t="s">
-        <v>701</v>
+        <v>669</v>
       </c>
       <c r="K108" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L108" s="9" t="s">
-        <v>852</v>
+        <v>820</v>
       </c>
       <c r="M108" s="9" t="s">
         <v>555</v>
@@ -8503,7 +8500,7 @@
         <v>75</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>983</v>
+        <v>951</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>75</v>
@@ -8518,13 +8515,13 @@
         <v>349</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>702</v>
+        <v>670</v>
       </c>
       <c r="K109" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L109" s="9" t="s">
-        <v>853</v>
+        <v>821</v>
       </c>
       <c r="M109" s="9" t="s">
         <v>556</v>
@@ -8541,13 +8538,13 @@
         <v>223</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>741</v>
+        <v>709</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>618</v>
+        <v>588</v>
       </c>
       <c r="F110" s="6" t="s">
         <v>455</v>
@@ -8562,19 +8559,19 @@
         <v>350</v>
       </c>
       <c r="J110" s="9" t="s">
-        <v>703</v>
+        <v>671</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>731</v>
+        <v>699</v>
       </c>
       <c r="L110" s="9" t="s">
-        <v>854</v>
+        <v>822</v>
       </c>
       <c r="M110" s="9" t="s">
         <v>557</v>
       </c>
       <c r="N110" s="10" t="s">
-        <v>941</v>
+        <v>909</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -8585,13 +8582,13 @@
         <v>223</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>733</v>
+        <v>701</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>1007</v>
+        <v>975</v>
       </c>
       <c r="F111" s="6" t="s">
         <v>456</v>
@@ -8606,13 +8603,13 @@
         <v>351</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>704</v>
+        <v>672</v>
       </c>
       <c r="K111" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L111" s="9" t="s">
-        <v>855</v>
+        <v>823</v>
       </c>
       <c r="M111" s="9" t="s">
         <v>558</v>
@@ -8635,7 +8632,7 @@
         <v>64</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>619</v>
+        <v>589</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>457</v>
@@ -8644,19 +8641,19 @@
         <v>110</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>906</v>
+        <v>874</v>
       </c>
       <c r="I112" s="4" t="s">
         <v>352</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>705</v>
+        <v>673</v>
       </c>
       <c r="K112" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L112" s="10" t="s">
-        <v>856</v>
+        <v>824</v>
       </c>
       <c r="M112" s="9" t="s">
         <v>559</v>
@@ -8679,7 +8676,7 @@
         <v>77</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>993</v>
+        <v>961</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>458</v>
@@ -8694,19 +8691,19 @@
         <v>353</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>706</v>
+        <v>674</v>
       </c>
       <c r="K113" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L113" s="10" t="s">
-        <v>857</v>
+        <v>825</v>
       </c>
       <c r="M113" s="17" t="s">
         <v>559</v>
       </c>
       <c r="N113" s="10" t="s">
-        <v>942</v>
+        <v>910</v>
       </c>
     </row>
     <row r="114" spans="1:14" ht="184.8" x14ac:dyDescent="0.3">
@@ -8717,13 +8714,13 @@
         <v>223</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>620</v>
+        <v>1005</v>
       </c>
       <c r="F114" s="6" t="s">
         <v>459</v>
@@ -8738,13 +8735,13 @@
         <v>354</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>707</v>
+        <v>675</v>
       </c>
       <c r="K114" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L114" s="9" t="s">
-        <v>858</v>
+        <v>826</v>
       </c>
       <c r="M114" s="9" t="s">
         <v>560</v>
@@ -8761,16 +8758,16 @@
         <v>223</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>735</v>
+        <v>703</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>251</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>994</v>
+        <v>962</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>881</v>
+        <v>849</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>110</v>
@@ -8782,13 +8779,13 @@
         <v>355</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>708</v>
+        <v>676</v>
       </c>
       <c r="K115" s="10" t="s">
         <v>111</v>
       </c>
       <c r="L115" s="9" t="s">
-        <v>859</v>
+        <v>827</v>
       </c>
       <c r="M115" s="9" t="s">
         <v>477</v>
@@ -8805,13 +8802,13 @@
         <v>223</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>734</v>
+        <v>702</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>252</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>621</v>
+        <v>1006</v>
       </c>
       <c r="F116" s="6" t="s">
         <v>460</v>
@@ -8826,13 +8823,13 @@
         <v>356</v>
       </c>
       <c r="J116" s="9" t="s">
-        <v>709</v>
+        <v>677</v>
       </c>
       <c r="K116" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L116" s="9" t="s">
-        <v>860</v>
+        <v>828</v>
       </c>
       <c r="M116" s="9" t="s">
         <v>561</v>
@@ -8843,16 +8840,16 @@
     </row>
     <row r="117" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A117" s="16" t="s">
-        <v>732</v>
+        <v>700</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>223</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>742</v>
+        <v>710</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>871</v>
+        <v>839</v>
       </c>
       <c r="F117" s="16" t="s">
         <v>110</v>
@@ -8861,7 +8858,7 @@
         <v>110</v>
       </c>
       <c r="I117" s="16" t="s">
-        <v>750</v>
+        <v>718</v>
       </c>
       <c r="J117" s="11" t="s">
         <v>110</v>
@@ -8883,461 +8880,462 @@
   <phoneticPr fontId="4" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{A62FB5FE-12B7-435E-B3DF-DE702ECD1D4C}"/>
-    <hyperlink ref="E3" r:id="rId2" display="https://placehold.co/400x600" xr:uid="{B0FAAFEF-605D-4098-8F11-6FC6A0E9E0D6}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{B0FAAFEF-605D-4098-8F11-6FC6A0E9E0D6}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{AB4A22E1-9601-4D07-8888-34F1D29BD46A}"/>
     <hyperlink ref="E6" r:id="rId4" xr:uid="{D5047CB0-F6D4-4475-9DBF-0B83B4DAEAB4}"/>
     <hyperlink ref="E8" r:id="rId5" display="https://placehold.co/400x600" xr:uid="{341347BE-FDF4-47C3-A9AA-7BF0532F61DB}"/>
     <hyperlink ref="E10" r:id="rId6" xr:uid="{CE30ABE6-4735-49AC-9E38-986CD096C5BF}"/>
     <hyperlink ref="E12" r:id="rId7" xr:uid="{17D5C088-BD3A-4E75-8035-22B027942A64}"/>
     <hyperlink ref="E14" r:id="rId8" xr:uid="{6815D31E-1624-40E4-AD43-8FB5276A3E13}"/>
-    <hyperlink ref="E18" r:id="rId9" display="https://placehold.co/400x600" xr:uid="{D37B5237-F7AD-4C72-A4B8-18846345A20A}"/>
+    <hyperlink ref="E18" r:id="rId9" xr:uid="{D37B5237-F7AD-4C72-A4B8-18846345A20A}"/>
     <hyperlink ref="E20" r:id="rId10" display="https://placehold.co/400x600" xr:uid="{455E2F96-6FCE-4ED2-9C3B-2E6E7249AE44}"/>
-    <hyperlink ref="E22" r:id="rId11" display="https://placehold.co/400x600" xr:uid="{77807312-4DCC-424A-9227-0205668D168B}"/>
-    <hyperlink ref="E24" r:id="rId12" display="https://placehold.co/400x600" xr:uid="{8AAD6443-2520-4082-8EC0-C46B0A509927}"/>
-    <hyperlink ref="E26" r:id="rId13" display="https://placehold.co/400x600" xr:uid="{5B8C9469-79CD-4130-A71A-FB9845883315}"/>
+    <hyperlink ref="E22" r:id="rId11" xr:uid="{77807312-4DCC-424A-9227-0205668D168B}"/>
+    <hyperlink ref="E24" r:id="rId12" xr:uid="{8AAD6443-2520-4082-8EC0-C46B0A509927}"/>
+    <hyperlink ref="E26" r:id="rId13" xr:uid="{5B8C9469-79CD-4130-A71A-FB9845883315}"/>
     <hyperlink ref="E28" r:id="rId14" xr:uid="{C6FD206E-083A-424A-BEB2-E5FA5EA1028A}"/>
     <hyperlink ref="E30" r:id="rId15" xr:uid="{3C06105A-95B0-486E-B562-804FA49B279E}"/>
-    <hyperlink ref="E32" r:id="rId16" display="https://placehold.co/400x600" xr:uid="{445C6875-08FB-4A0D-945E-88ACC5B3E36F}"/>
+    <hyperlink ref="E32" r:id="rId16" xr:uid="{445C6875-08FB-4A0D-945E-88ACC5B3E36F}"/>
     <hyperlink ref="E34" r:id="rId17" xr:uid="{65D66EC6-EE19-4700-A25B-1483B78EB1EF}"/>
     <hyperlink ref="E36" r:id="rId18" display="https://placehold.co/400x600" xr:uid="{2E844F72-E0A3-4D15-89E8-4C62C40B0097}"/>
     <hyperlink ref="E38" r:id="rId19" xr:uid="{15AC029B-EF8F-4E8F-BB97-C5EC917FD18C}"/>
     <hyperlink ref="E40" r:id="rId20" xr:uid="{5FE82AD6-8780-451F-B565-3C9E2036135F}"/>
     <hyperlink ref="E42" r:id="rId21" xr:uid="{F7983BF9-576C-4FA2-B35A-DFA749ACF1B5}"/>
     <hyperlink ref="E44" r:id="rId22" xr:uid="{DF66767C-72DE-4D71-B54F-89D37A2B3207}"/>
-    <hyperlink ref="E46" r:id="rId23" display="https://placehold.co/400x600" xr:uid="{E6907F0E-8A63-42E5-881D-83BE98378391}"/>
-    <hyperlink ref="E48" r:id="rId24" display="https://placehold.co/400x600" xr:uid="{BF819DDD-F33C-4323-B234-FA5AEFEBF540}"/>
-    <hyperlink ref="E50" r:id="rId25" display="https://placehold.co/400x600" xr:uid="{B4631102-EF86-443A-975E-E151B867331C}"/>
+    <hyperlink ref="E46" r:id="rId23" xr:uid="{E6907F0E-8A63-42E5-881D-83BE98378391}"/>
+    <hyperlink ref="E48" r:id="rId24" xr:uid="{BF819DDD-F33C-4323-B234-FA5AEFEBF540}"/>
+    <hyperlink ref="E50" r:id="rId25" xr:uid="{B4631102-EF86-443A-975E-E151B867331C}"/>
     <hyperlink ref="E52" r:id="rId26" xr:uid="{D0C8995E-2389-436D-96F9-0ECFED635D2D}"/>
-    <hyperlink ref="E54" r:id="rId27" display="https://placehold.co/400x600" xr:uid="{41208DE8-410A-4988-814F-34D6808B3973}"/>
-    <hyperlink ref="E56" r:id="rId28" display="https://placehold.co/400x600" xr:uid="{D60F983F-3A4A-4B45-A5A9-1CBD13CCBAB1}"/>
-    <hyperlink ref="E58" r:id="rId29" xr:uid="{DDB2A0FD-936A-490E-BE1E-1762A651B20C}"/>
-    <hyperlink ref="E62" r:id="rId30" xr:uid="{5E732335-693B-490D-844A-64351A2B11C7}"/>
-    <hyperlink ref="E64" r:id="rId31" display="https://placehold.co/400x600" xr:uid="{B032BBB6-4D16-4E33-A3F0-D7039E10D767}"/>
-    <hyperlink ref="E66" r:id="rId32" display="https://placehold.co/400x600" xr:uid="{C71F9231-ACA2-46E1-BE2F-462475789CDA}"/>
-    <hyperlink ref="E68" r:id="rId33" xr:uid="{6DAF2527-3F52-4351-90EE-F788A7836287}"/>
-    <hyperlink ref="E70" r:id="rId34" xr:uid="{C213B07F-FB90-4578-BA40-CB5277C5E9F8}"/>
-    <hyperlink ref="E72" r:id="rId35" display="https://placehold.co/400x600" xr:uid="{B6B3C0BC-449F-4D5F-8991-2960BC1E1B95}"/>
-    <hyperlink ref="E74" r:id="rId36" xr:uid="{12F3E568-1027-43BC-89EA-C5D4D2C3F3B1}"/>
-    <hyperlink ref="E76" r:id="rId37" xr:uid="{9BCFDA15-C8D8-41F6-B5C1-8DB9E3F54F38}"/>
-    <hyperlink ref="E78" r:id="rId38" display="https://placehold.co/400x600" xr:uid="{5074351A-0735-4679-AE99-F1F491EAD66F}"/>
-    <hyperlink ref="E80" r:id="rId39" xr:uid="{797A27FB-9286-43BA-A3D3-06E0B7DF57C7}"/>
-    <hyperlink ref="E82" r:id="rId40" display="https://placehold.co/400x600" xr:uid="{E22D4C78-609C-4F6C-902E-67DDEA2AEC08}"/>
-    <hyperlink ref="E84" r:id="rId41" display="https://placehold.co/400x600" xr:uid="{689543FA-D772-478F-B75B-353A8D5F5A0F}"/>
-    <hyperlink ref="E86" r:id="rId42" display="https://placehold.co/400x600" xr:uid="{6F1B4F40-1347-45F9-B0B9-89687F77E0B0}"/>
-    <hyperlink ref="E88" r:id="rId43" display="https://placehold.co/400x600" xr:uid="{269A95A2-A318-4245-8364-07E925D041A6}"/>
-    <hyperlink ref="E90" r:id="rId44" display="https://placehold.co/400x600" xr:uid="{BC5C79FD-42B9-4F63-B259-53ADA917C149}"/>
-    <hyperlink ref="E92" r:id="rId45" xr:uid="{F219C840-96AC-40EA-9D7B-C09CBA360D2A}"/>
-    <hyperlink ref="E94" r:id="rId46" xr:uid="{E85B62E0-66A6-4BDE-AB82-B3F3885FF25D}"/>
-    <hyperlink ref="E96" r:id="rId47" display="https://placehold.co/400x600" xr:uid="{F685C903-F46A-4AEA-A4B6-30F5F5C38E02}"/>
-    <hyperlink ref="E98" r:id="rId48" display="https://placehold.co/400x600" xr:uid="{34A32507-5178-4AE2-8923-C76F8834EAC3}"/>
-    <hyperlink ref="E100" r:id="rId49" display="https://placehold.co/400x600" xr:uid="{316F114E-DC59-4C12-AAE4-7C561A6A4A37}"/>
-    <hyperlink ref="E102" r:id="rId50" xr:uid="{E6C4E1E9-ADFC-463C-BA35-72BF5470C0FC}"/>
-    <hyperlink ref="E104" r:id="rId51" display="https://placehold.co/400x600" xr:uid="{5C2E1F62-17AE-4C61-86CF-CFAADD48E3DA}"/>
-    <hyperlink ref="E106" r:id="rId52" display="https://placehold.co/400x600" xr:uid="{EB2D28AA-5611-4D14-B6D8-65655568052B}"/>
-    <hyperlink ref="E108" r:id="rId53" xr:uid="{1A1FF6C3-6CA4-4205-87F4-FFA4C505FE05}"/>
-    <hyperlink ref="E110" r:id="rId54" display="https://placehold.co/400x600" xr:uid="{D5F8DE7D-9A2E-4EB2-AD3E-1B6347BBB03A}"/>
-    <hyperlink ref="E112" r:id="rId55" display="https://placehold.co/400x600" xr:uid="{72604405-579A-4D04-AD70-2F433C2E73DD}"/>
-    <hyperlink ref="E114" r:id="rId56" display="https://placehold.co/400x600" xr:uid="{F52A7ADE-923C-4FC0-835C-C78BE5475FD1}"/>
-    <hyperlink ref="E116" r:id="rId57" display="https://placehold.co/400x600" xr:uid="{88BB9B9A-193B-430A-8A94-9996D9F8B858}"/>
-    <hyperlink ref="E5" r:id="rId58" display="https://placehold.co/400x600" xr:uid="{673B2D9E-5CEE-40DD-A0A2-66025584E8C2}"/>
-    <hyperlink ref="E7" r:id="rId59" xr:uid="{20202916-CECB-497F-BB8D-D7E09DCEC193}"/>
-    <hyperlink ref="E9" r:id="rId60" display="https://placehold.co/400x600" xr:uid="{E7773CE7-BD5F-4624-B940-0E795B4A4E30}"/>
-    <hyperlink ref="E11" r:id="rId61" display="https://placehold.co/400x600" xr:uid="{93DA058C-7CEC-4BA2-9D33-5FB8B5E88910}"/>
-    <hyperlink ref="E13" r:id="rId62" display="https://placehold.co/400x600" xr:uid="{8F788626-64E7-4F1D-A12D-F2E9D916467C}"/>
-    <hyperlink ref="E15" r:id="rId63" display="https://placehold.co/400x600" xr:uid="{8AD2972F-0CB2-4DCE-8821-C56F9057AD5B}"/>
-    <hyperlink ref="E19" r:id="rId64" display="https://placehold.co/400x600" xr:uid="{D4698768-8DC5-407A-B6F4-C1C875BFB78D}"/>
-    <hyperlink ref="E21" r:id="rId65" xr:uid="{13DD67BA-1FCB-43E0-A39C-FFE32E5D3954}"/>
-    <hyperlink ref="E23" r:id="rId66" xr:uid="{90D0F56C-C7DB-4632-B91C-EF74541F5FEA}"/>
-    <hyperlink ref="E25" r:id="rId67" xr:uid="{F6A0C9FE-D2B9-4181-8F81-93868F3E313C}"/>
-    <hyperlink ref="E27" r:id="rId68" xr:uid="{848B184F-1DE9-469A-9D63-F5CDEBF10D7A}"/>
-    <hyperlink ref="E29" r:id="rId69" xr:uid="{1AF17D20-76D5-4714-B7E2-2D8B8CB9ADC3}"/>
-    <hyperlink ref="E31" r:id="rId70" display="https://placehold.co/400x600" xr:uid="{22DD1D25-8288-4AC9-A5FC-D9B7B89B515C}"/>
-    <hyperlink ref="E33" r:id="rId71" xr:uid="{01F92761-8D63-4A2C-8713-25D41165DB40}"/>
-    <hyperlink ref="E35" r:id="rId72" xr:uid="{FFD57A2F-B179-4903-B296-F8069D1F1332}"/>
-    <hyperlink ref="E37" r:id="rId73" display="https://placehold.co/400x600" xr:uid="{291A37C6-A686-4CDE-9352-CAE725E23B11}"/>
-    <hyperlink ref="E39" r:id="rId74" xr:uid="{6ECECF25-2624-4D12-A089-9B4C4DBCF38B}"/>
-    <hyperlink ref="E41" r:id="rId75" display="https://placehold.co/400x600" xr:uid="{B8267D85-A691-4187-91DB-27E364616A8C}"/>
-    <hyperlink ref="E43" r:id="rId76" xr:uid="{AA69E1F0-E88A-495C-A844-C33C82F6CE26}"/>
-    <hyperlink ref="E45" r:id="rId77" xr:uid="{269F03E1-526C-4849-A6D5-8276665E4485}"/>
-    <hyperlink ref="E47" r:id="rId78" display="https://placehold.co/400x600" xr:uid="{D722AC52-912D-4A3F-8560-FAA4DCA60A56}"/>
-    <hyperlink ref="E49" r:id="rId79" display="https://placehold.co/400x600" xr:uid="{6ED9D463-8E32-4780-942A-C1EC9D07542B}"/>
-    <hyperlink ref="E51" r:id="rId80" display="https://placehold.co/400x600" xr:uid="{FAAE2569-D069-46B3-A7AA-6969338A4AFF}"/>
-    <hyperlink ref="E53" r:id="rId81" display="https://placehold.co/400x600" xr:uid="{919767C3-0A6A-4A63-9549-0F7B3A7EE7DF}"/>
-    <hyperlink ref="E55" r:id="rId82" display="https://placehold.co/400x600" xr:uid="{BD76B93C-ACC1-4CF1-A623-39E4FAFED853}"/>
-    <hyperlink ref="E57" r:id="rId83" display="https://placehold.co/400x600" xr:uid="{7964589D-7453-4997-AC7B-F98F5B5B7029}"/>
-    <hyperlink ref="E59" r:id="rId84" xr:uid="{F72D2D0A-AD07-45DC-AA3D-223C36C995AB}"/>
-    <hyperlink ref="E61" r:id="rId85" display="https://placehold.co/400x600" xr:uid="{D79CAE5D-C5B6-4B75-8261-008B5374EBDB}"/>
-    <hyperlink ref="E63" r:id="rId86" xr:uid="{75C81E45-FAA6-4175-A2FE-BA7C7F71F6F3}"/>
-    <hyperlink ref="E65" r:id="rId87" display="https://placehold.co/400x600" xr:uid="{2A43A7D2-0D9B-42A8-8E87-E447ECDB9951}"/>
-    <hyperlink ref="E67" r:id="rId88" display="https://placehold.co/400x600" xr:uid="{F199289C-0CB7-41CD-95E9-D9C97B86A7E7}"/>
-    <hyperlink ref="E69" r:id="rId89" display="https://placehold.co/400x600" xr:uid="{E4715AC6-7D6D-4434-A585-79B8F25233F6}"/>
-    <hyperlink ref="E71" r:id="rId90" xr:uid="{CFD1BDC4-A848-4998-9430-C29DB079EED4}"/>
-    <hyperlink ref="E73" r:id="rId91" xr:uid="{DEC62E70-AB7A-4365-B90A-11A1D549F375}"/>
-    <hyperlink ref="E75" r:id="rId92" xr:uid="{A925F566-676A-47EA-9068-3A8AC9C78A71}"/>
-    <hyperlink ref="E77" r:id="rId93" xr:uid="{826BB4FF-EF4E-4C68-AE45-B4C9CEE10FB5}"/>
-    <hyperlink ref="E79" r:id="rId94" xr:uid="{D55B186E-0A96-4185-9D34-01F9C47E843E}"/>
-    <hyperlink ref="E81" r:id="rId95" xr:uid="{AC60663B-FB99-47D2-A9DA-11C43648559B}"/>
-    <hyperlink ref="E83" r:id="rId96" display="https://placehold.co/400x600" xr:uid="{F83899A5-222C-48AC-9ABC-BC254C3600A8}"/>
-    <hyperlink ref="E85" r:id="rId97" display="https://placehold.co/400x600" xr:uid="{2EE015AD-95D3-42D3-9727-0C2D20C22B2D}"/>
-    <hyperlink ref="E87" r:id="rId98" xr:uid="{1E9351A5-5685-4A61-91E2-9C72A14FBA45}"/>
-    <hyperlink ref="E89" r:id="rId99" display="https://placehold.co/400x600" xr:uid="{DA14C2E4-99E6-4273-B1C6-88E4314A2B53}"/>
-    <hyperlink ref="E91" r:id="rId100" display="https://placehold.co/400x600" xr:uid="{CED33FAF-E705-4A0E-B5BA-28AC459A08F9}"/>
-    <hyperlink ref="E93" r:id="rId101" display="https://placehold.co/400x600" xr:uid="{69683834-3F44-4B9E-879F-17C7B3985064}"/>
-    <hyperlink ref="E95" r:id="rId102" xr:uid="{6706B29D-6B9E-414D-A766-C429245D96A7}"/>
-    <hyperlink ref="E97" r:id="rId103" display="https://placehold.co/400x600" xr:uid="{B8549196-6B30-41D5-B870-CDF1F6C0AE2B}"/>
-    <hyperlink ref="E99" r:id="rId104" display="https://placehold.co/400x600" xr:uid="{70722206-091E-437D-B026-345C8CDB5176}"/>
-    <hyperlink ref="E101" r:id="rId105" xr:uid="{EF057E02-0A38-4475-84BA-2BC1ED64BA7D}"/>
-    <hyperlink ref="E103" r:id="rId106" xr:uid="{F307B800-2CAD-4E08-A635-F4AD9976A897}"/>
-    <hyperlink ref="E105" r:id="rId107" display="https://placehold.co/400x600" xr:uid="{42F0B609-7315-4192-A377-FDEDE5FDDF8B}"/>
-    <hyperlink ref="E107" r:id="rId108" display="https://placehold.co/400x600" xr:uid="{0BBF4990-1413-476C-AFE7-EC34A9F113B0}"/>
-    <hyperlink ref="E109" r:id="rId109" xr:uid="{43D0B648-1D21-45A3-A6E9-CB546100DAA2}"/>
-    <hyperlink ref="E111" r:id="rId110" xr:uid="{3BF79D70-269C-4AB5-B83F-712DABFF4480}"/>
-    <hyperlink ref="E113" r:id="rId111" xr:uid="{622A2536-A959-42B4-B4F9-EE23F2A44517}"/>
-    <hyperlink ref="E115" r:id="rId112" xr:uid="{7690046C-47D4-4A7B-8DBE-6704DCCAE9C8}"/>
-    <hyperlink ref="J72" r:id="rId113" display="https://www.linkedin.com/in/dr-nilay-patel-106bab14/" xr:uid="{B2E17E23-9358-429B-BBF9-5EE4C8E363CB}"/>
-    <hyperlink ref="J83" r:id="rId114" display="https://www.linkedin.com/in/poonam-thanki-b112a6a2/" xr:uid="{BB16F397-78CE-4DBD-8BE4-13D65525672B}"/>
-    <hyperlink ref="J57" r:id="rId115" display="https://www.linkedin.com/in/dr-manthan-s-manavadaria-2a222219/" xr:uid="{4954A101-EA09-4BF1-8202-A72F86653038}"/>
-    <hyperlink ref="J18" r:id="rId116" display="https://www.linkedin.com/in/bhavin-mehta-86b47795/" xr:uid="{DB7D7CE8-51EF-48EE-BFBF-A021321BDC5F}"/>
-    <hyperlink ref="J49" r:id="rId117" display="https://www.linkedin.com/in/dr-kanwar-preet-kaur-bamrah-64a3a221/" xr:uid="{53166117-8C5A-4AB4-89B7-C2E8B83BC5A5}"/>
-    <hyperlink ref="J92" r:id="rId118" display="https://www.linkedin.com/in/rikita-chokshi-44bb65263/" xr:uid="{184885D3-531C-43E9-853D-5C2EAF6E7696}"/>
-    <hyperlink ref="J106" r:id="rId119" xr:uid="{FBE16C58-F91B-4934-8550-681C7F68CFE1}"/>
-    <hyperlink ref="J68" r:id="rId120" display="https://www.linkedin.com/in/mrugendrasinh-rahevar/" xr:uid="{F0663F50-387A-4315-8A34-03206888175F}"/>
-    <hyperlink ref="J91" r:id="rId121" display="https://www.linkedin.com/in/ravi-patel-13686b19/" xr:uid="{FC6DE30F-2E95-4AA2-B879-8CEAD23CEEC4}"/>
-    <hyperlink ref="J95" r:id="rId122" display="https://www.linkedin.com/in/ronak-patel-63663613a/" xr:uid="{EB8CC283-1781-41D5-BE2D-3C04AED15B01}"/>
-    <hyperlink ref="J50" r:id="rId123" display="https://www.linkedin.com/in/dr-kawaljitsingh-randhawa-96816064/" xr:uid="{4AE0FF76-EF4F-45C3-A542-A7D876A7DA2C}"/>
-    <hyperlink ref="J19" r:id="rId124" display="http://linkedin.com/in/bimal-patel-b7504849" xr:uid="{B02CE38D-7D41-45E6-8D0A-5F0FCF595503}"/>
-    <hyperlink ref="J71" r:id="rId125" display="https://www.linkedin.com/in/nikita-bhatt-ce/?originalSubdomain=in" xr:uid="{9EC6AE06-F884-4149-B7FC-88140006B7F4}"/>
-    <hyperlink ref="J23" r:id="rId126" display="https://www.linkedin.com/in/deep-kothadiya-phd-70983a86/" xr:uid="{8691FEB4-6E3B-4049-9588-FC79EAF0F2EC}"/>
-    <hyperlink ref="J78" r:id="rId127" display="https://www.linkedin.com/in/parmanand-patel-1269016b/" xr:uid="{53EDE3BB-D85D-4DAD-A587-55DA1C805D27}"/>
-    <hyperlink ref="J52" r:id="rId128" display="https://www.linkedin.com/in/krunal-maheriya-aba5681a1/" xr:uid="{9D29078E-A414-4A64-86B1-F77733FF0F8A}"/>
-    <hyperlink ref="J86" r:id="rId129" xr:uid="{21E8E151-1B01-486F-A7D7-4BE4F0BC0B27}"/>
-    <hyperlink ref="J36" r:id="rId130" display="https://www.linkedin.com/in/dr-hardik-modi-181035b/" xr:uid="{F7F908AF-23C0-42F7-8AFE-DF52AF52580B}"/>
-    <hyperlink ref="J14" r:id="rId131" display="http://hlinkedin.com/in/dr-ashwin-makwana-9a6688112" xr:uid="{3D2F3A09-18C9-4E22-B6FA-494330FEF01E}"/>
-    <hyperlink ref="J80" r:id="rId132" xr:uid="{4DA1EB91-0A15-4D6C-9213-F6D1EE675204}"/>
-    <hyperlink ref="J17" r:id="rId133" xr:uid="{8E63BCC9-6C05-45B8-8789-EBB4905292F2}"/>
-    <hyperlink ref="J35" r:id="rId134" display="https://www.linkedin.com/in/gaurav-kumar1582/" xr:uid="{BF49CFFA-7535-44BB-8F9A-67BEFFD957B6}"/>
-    <hyperlink ref="J29" r:id="rId135" display="https://www.linkedin.com/in/dhaval-patel-481b0885/" xr:uid="{5704F17D-173C-4E5E-89CF-B8F7987D86F5}"/>
-    <hyperlink ref="J77" r:id="rId136" display="https://www.linkedin.com/me?trk=p_mwlite_profile_self-secondary_nav" xr:uid="{6148FF48-4942-4818-844D-79919D56DB98}"/>
-    <hyperlink ref="J67" r:id="rId137" display="https://www.linkedin.com/in/dr-miral-desai-245448a2/" xr:uid="{D2BE1269-3E17-415C-B581-A936373A624C}"/>
-    <hyperlink ref="J32" r:id="rId138" display="https://www.linkedin.com/in/gajanan-patange-05ba2219/overlay/about-this-profile/?lipi=urn%3Ali%3Apage%3Ad_flagship3_profile_view_base%3BEvV8mS8jTpy2mGfBhro1og%3D%3D" xr:uid="{CDEEC399-875E-4DDA-A567-6EFC42A0F87E}"/>
-    <hyperlink ref="J114" r:id="rId139" display="https://www.linkedin.com/in/vikas-panchal-873277251/" xr:uid="{A3606037-07FB-4104-B411-BA37A6E2F3CA}"/>
-    <hyperlink ref="J101" r:id="rId140" display="https://www.linkedin.com/in/sneha-padhiar-4aaa17146/" xr:uid="{8CF4272D-E96D-4E1C-80AD-5D3F2F554C53}"/>
-    <hyperlink ref="J38" r:id="rId141" display="https://www.linkedin.com/in/harshul-yagnik-81a6a022/" xr:uid="{683E4E91-B763-4226-99B6-F3E30837AD4B}"/>
-    <hyperlink ref="J21" r:id="rId142" display="https://www.linkedin.com/in/brinda-patel-652073252" xr:uid="{791133CF-E0A2-4B6D-8618-AC19B4D3A9FA}"/>
-    <hyperlink ref="J28" r:id="rId143" xr:uid="{F8104DB3-2B23-47B7-B622-17690E08D84A}"/>
-    <hyperlink ref="J97" r:id="rId144" display="https://www.linkedin.com/in/sagarkumar-patel-0bb94bb5/" xr:uid="{B357E631-0C5E-406B-9B45-A421DE003AD4}"/>
-    <hyperlink ref="J70" r:id="rId145" display="http://www.linkedin.com/in/neha-chauhan22" xr:uid="{E7A9417A-8B16-4D59-A23C-B258564D85D5}"/>
-    <hyperlink ref="J22" r:id="rId146" xr:uid="{895691E5-0B23-47DD-9A36-18923B4FD652}"/>
-    <hyperlink ref="J39" r:id="rId147" display="https://www.linkedin.com/public-profile/settings?trk=d_flagship3_profile_self_view_public_profile" xr:uid="{E4C32594-CCCB-41B2-AE51-AE67F83944BE}"/>
-    <hyperlink ref="J42" r:id="rId148" display="https://www.linkedin.com/in/jalpa-ardeshana-381496b7/" xr:uid="{67C7A4AD-28FD-4291-92FB-A9C4AA0671B4}"/>
-    <hyperlink ref="J102" r:id="rId149" display="https://www.linkedin.com/in/dr-spoorthy-v-10ab3813a/" xr:uid="{EDA5921D-C45B-4D8B-B9FA-3205F4F396D6}"/>
-    <hyperlink ref="J24" r:id="rId150" display="https://www.linkedin.com/in/dhara-patel-839488138" xr:uid="{27C9FC8C-0A44-49AE-8688-8690C8579833}"/>
-    <hyperlink ref="J26" r:id="rId151" display="https://www.linkedin.com/in/dharmendrasinh-chauhan-073a491a4/" xr:uid="{D50E69C7-4F51-4D1B-90EC-FE9F9A44906E}"/>
-    <hyperlink ref="J90" r:id="rId152" display="https://www.linkedin.com/in/rajnik-katriya/" xr:uid="{3AEC1C40-35D9-4AE3-A7E8-9E58FA2C8E43}"/>
-    <hyperlink ref="J98" r:id="rId153" display="https://www.linkedin.com/in/sanket-suthar-544a69210/" xr:uid="{6137F2DC-1F93-4037-B861-A959BDB6DCE6}"/>
-    <hyperlink ref="J53" r:id="rId154" display="http://www.linkedin.com/in/kundan-patel-b9508b27b" xr:uid="{D4BB537A-7CA1-4F2B-9985-F5921034561E}"/>
-    <hyperlink ref="J81" r:id="rId155" xr:uid="{BFFCC995-B6DF-474C-93AA-BDF180E05422}"/>
-    <hyperlink ref="J111" r:id="rId156" display="https://www.linkedin.com/in/vidisha-pradhan-733a1b63/" xr:uid="{06E43119-E5BC-45C4-9126-F192D3006C5B}"/>
-    <hyperlink ref="J27" r:id="rId157" display="https://www.linkedin.com/in/dharmendrasinh-rathod-4482a2a4/" xr:uid="{3BDD0888-FF6F-403B-8A93-FD5176D0DA38}"/>
-    <hyperlink ref="J54" r:id="rId158" display="http://www.linkedin.com/in/madhav-oza-60bb5650" xr:uid="{24641904-0D92-4561-9EC0-14DC5197E375}"/>
-    <hyperlink ref="J41" r:id="rId159" xr:uid="{10BD029B-F728-4FEF-934E-F502C3B3ECDD}"/>
-    <hyperlink ref="J112" r:id="rId160" display="https://www.linkedin.com/in/dr-vijay-chaudhary-12769b311/" xr:uid="{B15A7FAF-9082-4A84-BAA5-265E44F10859}"/>
-    <hyperlink ref="J62" r:id="rId161" display="http://inkedin.com/in/mjdesai/?original_referer=https%3A%2F%2Fwww%2Egoogle%2Ecom%2F&amp;originalSubdomain=in" xr:uid="{58387078-A78B-4059-8DB7-2DA181BAC97F}"/>
-    <hyperlink ref="J48" r:id="rId162" xr:uid="{F61EBA1D-096B-4367-83C7-464D0E0332DE}"/>
-    <hyperlink ref="J51" r:id="rId163" xr:uid="{A7C5CA17-C1E0-4B34-9F67-339F0FC32426}"/>
-    <hyperlink ref="J65" r:id="rId164" display="https://www.linkedin.com/in/mihirmehta-educational-project-and-placements/" xr:uid="{1EF2631D-C319-4F6C-9AF3-9E886A6E863A}"/>
-    <hyperlink ref="J34" r:id="rId165" display="https://www.linkedin.com/in/gaurang-patel-a99266119/" xr:uid="{4A4B2655-5B11-4CEB-8516-A9D046224C31}"/>
-    <hyperlink ref="J75" r:id="rId166" display="http://www.linkedin.com/in/nishant-koshti-52b68b8b" xr:uid="{2E5CF16C-0D7F-4454-B4F7-592A3EC43855}"/>
-    <hyperlink ref="J20" r:id="rId167" display="https://www.linkedin.com/in/brijesh-kundaliya-552b7722/" xr:uid="{FC5C15E0-2AD1-4E2F-8F1E-F2F96829A7A6}"/>
-    <hyperlink ref="J43" r:id="rId168" display="https://www.linkedin.com/in/jalpesh-vasa/" xr:uid="{6768F239-6E23-4A84-8C3E-45670A76F700}"/>
-    <hyperlink ref="J109" r:id="rId169" display="https://www.linkedin.com/in/vaishali-mewada-7a619053/" xr:uid="{DEFB6E16-7F29-44C5-ACAD-D6B1E16E6C24}"/>
-    <hyperlink ref="J46" r:id="rId170" xr:uid="{CCF872D9-BD3F-4521-9093-8C3148DBAC43}"/>
-    <hyperlink ref="J113" r:id="rId171" display="http://www.linkedin.com/in/vijaykumar-panchal-631852280" xr:uid="{2810BDF3-4A14-413D-B157-AF8059E92C49}"/>
-    <hyperlink ref="J64" r:id="rId172" display="https://www.linkedin.com/in/dr-mihir-bhatt-806a85aa/" xr:uid="{AA93D706-7CF6-45C4-B768-B797EB6775B7}"/>
-    <hyperlink ref="J96" r:id="rId173" display="https://www.linkedin.com/in/dr-sagar-chokshi-8646601a/" xr:uid="{35109E28-E96A-4139-B689-0AB43FF55E92}"/>
-    <hyperlink ref="J84" r:id="rId174" display="http://www.linkedin.com/in/pratik-panchal-a35b325a" xr:uid="{6FB924B7-EDB2-44F0-B0D7-E78551105315}"/>
-    <hyperlink ref="J40" r:id="rId175" display="https://www.linkedin.com/in/hemangi-oza-60a189190/" xr:uid="{AC43F6B8-459E-4FF0-82E4-75F8CDE25269}"/>
-    <hyperlink ref="J110" r:id="rId176" display="http://linkedin.com/in/vibha-parmar-81b3045b" xr:uid="{9792CDE9-6059-48ED-AD46-8BECFEF07152}"/>
-    <hyperlink ref="J59" r:id="rId177" display="http://www.linkedin.com/in/maulik-shah-30b483119" xr:uid="{E23FB3E1-55AD-4659-9463-2B3E19FC5E7D}"/>
-    <hyperlink ref="J99" r:id="rId178" display="http://www.linkedin.com/in/saritavisavalia" xr:uid="{3504F31F-4BD3-4D8B-B727-C2FF9DDFF1EA}"/>
-    <hyperlink ref="J13" r:id="rId179" xr:uid="{ACF63811-234F-442B-91D8-C6863212F92A}"/>
-    <hyperlink ref="J45" r:id="rId180" display="https://www.linkedin.com/in/dr-jigar-sarda-00384414/" xr:uid="{0EFC12BA-8B5C-4E86-968D-797B0D43FD98}"/>
-    <hyperlink ref="J105" r:id="rId181" display="https://www.linkedin.com/in/trusha-patel-gajjar" xr:uid="{98AA2D43-F8B2-4B29-93BA-7A9CCA8109B2}"/>
-    <hyperlink ref="J103" r:id="rId182" display="https://www.linkedin.com/in/srushti-gajjar-92b829142?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app" xr:uid="{544D82DB-5386-42AC-B979-94C259CA9E97}"/>
-    <hyperlink ref="J94" r:id="rId183" xr:uid="{F1631FCD-D701-415F-89D8-AB6A7D513AC5}"/>
-    <hyperlink ref="J15" r:id="rId184" display="https://www.linkedin.com/in/asifiqbal-thakor-56949b237/" xr:uid="{3A40B3CD-F1BE-4530-B451-07DF410D1272}"/>
-    <hyperlink ref="J56" r:id="rId185" xr:uid="{99110411-88B4-4B0C-9258-D7E7320C877C}"/>
-    <hyperlink ref="J47" r:id="rId186" display="https://www.linkedin.com/in/jivanadhar-joshi-a76a12ab/" xr:uid="{ED0C7354-C517-49E0-BDF5-C6BF1EC0A53C}"/>
-    <hyperlink ref="J104" r:id="rId187" display="https://in.linkedin.com/in/dr-tigmanshu-patel-b3252639" xr:uid="{8223C32D-E35E-4436-B593-C54F5FEED7DB}"/>
-    <hyperlink ref="J44" r:id="rId188" display="http://linkedin.com/in/jay-bhavsar-a4a9646a" xr:uid="{A3106519-72EE-423E-976E-09F1FD98B248}"/>
-    <hyperlink ref="J89" r:id="rId189" display="http://www.linkedin.com/in/purvi-prajapati-37ba6651" xr:uid="{7A2661BA-3D20-4DF8-8332-CC5726684DD1}"/>
-    <hyperlink ref="J74" r:id="rId190" display="https://www.linkedin.com/in/nirpex-patel-508956119/" xr:uid="{8BF234A3-EF12-4093-8EAF-09B2432506EF}"/>
-    <hyperlink ref="J87" r:id="rId191" display="https://www.linkedin.com/in/priyanka-patel-ph-d-00403393/" xr:uid="{8D6AEC45-7FD5-4128-9D12-F2A6CBB1E864}"/>
-    <hyperlink ref="J63" r:id="rId192" display="https://www.linkedin.com/in/mehulkumar-katakiya-029357b8/" xr:uid="{D058A74D-8E61-413C-9B75-7FF7917660C9}"/>
-    <hyperlink ref="J37" r:id="rId193" display="https://www.linkedin.com/in/harmish-bhatt-88581510a/" xr:uid="{7CC36C27-9781-439B-A945-9C1160C69911}"/>
-    <hyperlink ref="J66" r:id="rId194" display="https://www.linkedin.com/in/mikin-patel-24191386/" xr:uid="{3AEB0F01-575C-4799-B7A0-11A1F0947768}"/>
-    <hyperlink ref="J107" r:id="rId195" display="https://www.linkedin.com/in/dr-upesh-patel-875878138/" xr:uid="{5D7DA379-79C5-410F-9398-20936275BC46}"/>
-    <hyperlink ref="J58" r:id="rId196" xr:uid="{509B130C-6A0C-4944-BFE2-75F1FDF097C4}"/>
-    <hyperlink ref="J69" r:id="rId197" display="https://www.linkedin.com/in/muskan-dave-023197162/" xr:uid="{C8C7BB25-838D-4DFF-B4BD-F8943C06375E}"/>
-    <hyperlink ref="J73" r:id="rId198" display="https://www.linkedin.com/in/dr-nirav-bhatt/" xr:uid="{3F4736BB-5DB7-48E0-ABC4-5DBB591E1122}"/>
-    <hyperlink ref="J11" r:id="rId199" xr:uid="{714022ED-2EC9-40BB-978A-F936135E18E1}"/>
-    <hyperlink ref="J93" r:id="rId200" display="https://www.linkedin.com/in/ritesh-patel-462b0b11" xr:uid="{F4558EEF-FFB0-474A-8E3E-CEBF9566FCDB}"/>
-    <hyperlink ref="J116" r:id="rId201" display="http://www.linkedin.com/in/viral-panara-773877201" xr:uid="{4FB52C9B-4BDB-4971-A78B-1CD2EE789E52}"/>
-    <hyperlink ref="J79" r:id="rId202" display="https://www.linkedin.com/in/shah-parth-d/" xr:uid="{A61E294E-BDA5-4C2E-BA18-BA2B9C98C973}"/>
-    <hyperlink ref="J33" r:id="rId203" display="https://www.linkedin.com/in/gargi-ray-983a8522/" xr:uid="{0C76E47F-7D1B-4E1C-A88F-86156C9D1D6E}"/>
-    <hyperlink ref="J100" r:id="rId204" display="http://www.linkedin.com/in/satayu-travadi-9aab0919" xr:uid="{A79F3F36-387F-427F-848C-3BB8A221E707}"/>
-    <hyperlink ref="J88" r:id="rId205" xr:uid="{A7A467B8-5468-4830-9ADC-34F28E8899B5}"/>
-    <hyperlink ref="J30" r:id="rId206" display="https://www.linkedin.com/in/dheeraj-kumar-shringi-030586107?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app" xr:uid="{D1B60D12-635A-4E71-93D8-B47244D1EF44}"/>
-    <hyperlink ref="J85" r:id="rId207" display="https://in.linkedin.com/in/pratik-mochi-09764b102?original_referer=https%3A%2F%2Fwww.google.com%2F" xr:uid="{CD8066BB-0BA9-4FA9-88DB-0C291F6209A7}"/>
-    <hyperlink ref="J108" r:id="rId208" display="https://www.linkedin.com/in/vaibhavi-patel-67b035224/" xr:uid="{51D509E7-546B-4519-845F-AF5DC77392B9}"/>
-    <hyperlink ref="J60" r:id="rId209" display="http://www.linkedin.com/in/mayuri-popat-213852b1" xr:uid="{336D4B2F-0BBF-4ADA-8647-F20659482547}"/>
-    <hyperlink ref="J55" r:id="rId210" display="http://www.linkedin.com/in/madhavajwalia" xr:uid="{8DE9B663-AD20-42DB-A7F0-4FD167AD95E8}"/>
-    <hyperlink ref="J115" r:id="rId211" display="https://www.linkedin.com/in/vipul-vyas-19214bab/" xr:uid="{00F74D28-7144-4D8C-9870-393AE49126D5}"/>
-    <hyperlink ref="J31" r:id="rId212" display="http://www.linkedin.com/in/dipalkumar-patel-4b97997" xr:uid="{CFB485EB-93AC-436E-BD76-13F13D42FA00}"/>
-    <hyperlink ref="J76" r:id="rId213" display="https://www.linkedin.com/in/nishat-shaikh-b7446019a/" xr:uid="{45535606-CAE7-44BB-B1C5-622D742D5E66}"/>
-    <hyperlink ref="J16" r:id="rId214" display="https://www.linkedin.com/in/avani-khokhariya/" xr:uid="{F2664F6A-73CC-4DAD-982B-E296BD77DF0A}"/>
-    <hyperlink ref="J82" r:id="rId215" xr:uid="{2C60818F-B78B-4EC2-9BA4-C7D88C933280}"/>
-    <hyperlink ref="J25" r:id="rId216" display="https://www.linkedin.com/in/dhara-s-032a6a24/" xr:uid="{4FE7FF63-A73E-4E09-94C4-E2CD5FE6F81D}"/>
-    <hyperlink ref="K72" r:id="rId217" xr:uid="{E7CCB95C-4D9A-474B-9296-0EE719EC4AB3}"/>
-    <hyperlink ref="K92" r:id="rId218" xr:uid="{92D21BA9-793A-4610-9A6A-641322C6CC28}"/>
-    <hyperlink ref="K106" r:id="rId219" xr:uid="{2E05A515-7245-4DDB-9E9C-D041E881E2BF}"/>
-    <hyperlink ref="K86" r:id="rId220" xr:uid="{8C1C3B99-0196-4695-95EB-EEFEEA76042B}"/>
-    <hyperlink ref="K67" r:id="rId221" xr:uid="{4C2AA447-E23D-4BD3-8516-CF8A69E7C676}"/>
-    <hyperlink ref="K90" r:id="rId222" xr:uid="{68D88C01-9035-44B0-9EAE-4AE7236572CC}"/>
-    <hyperlink ref="K98" r:id="rId223" xr:uid="{B89BB500-5F1B-4985-B0B7-D69D9B22538C}"/>
-    <hyperlink ref="K27" r:id="rId224" xr:uid="{461288D1-54CE-41D7-ACBC-4EB753D35618}"/>
-    <hyperlink ref="K64" r:id="rId225" display="https://sites.google.com/a/charusat.ac.in/mihir-bhatt-ee/home/about-me?pli=1" xr:uid="{DD66FE1D-24F8-42A6-8DDC-651F08933CB6}"/>
-    <hyperlink ref="K45" r:id="rId226" xr:uid="{185428FC-1CEB-406E-A327-B537B63CC062}"/>
-    <hyperlink ref="K105" r:id="rId227" xr:uid="{6E3402FB-A293-4394-A12F-C9CE90A43581}"/>
-    <hyperlink ref="K94" r:id="rId228" display="https://sites.google.com/view/ronak-patel/" xr:uid="{30BB4B45-BE3C-4B51-8751-F1166793B9D8}"/>
-    <hyperlink ref="K87" r:id="rId229" display="https://sites.google.com/a/charusat.ac.in/priyanka-patel/about-me" xr:uid="{2F80CF65-0198-4866-9245-0932E2D2E991}"/>
-    <hyperlink ref="K11" r:id="rId230" xr:uid="{B7911887-1D4E-4149-9255-34290DE15C67}"/>
-    <hyperlink ref="K93" r:id="rId231" xr:uid="{CC19190B-EF5A-4030-970E-47B4649A66EC}"/>
-    <hyperlink ref="K79" r:id="rId232" display="http://learnwithparth.in/" xr:uid="{0D098BA1-951E-49B0-BA34-5489DFACFB69}"/>
-    <hyperlink ref="K60" r:id="rId233" display="https://sites.google.com/charusat.ac.in/mayuri-popat/home/academic-experience?authuser=0" xr:uid="{CD111632-8632-4F99-808E-7B0BA423BCF0}"/>
-    <hyperlink ref="K25" r:id="rId234" display="http://https/www.simpldhara.github.io" xr:uid="{1B0FEF49-7DD4-45B9-B1E6-577EDB068225}"/>
-    <hyperlink ref="K4" r:id="rId235" xr:uid="{A55ED677-5A40-43B5-A2E0-3934032012FA}"/>
-    <hyperlink ref="I12" r:id="rId236" xr:uid="{559F5BE6-A98D-4918-9ADE-3B5DB2AC1B24}"/>
-    <hyperlink ref="I13" r:id="rId237" xr:uid="{B5B2A2F7-DD9E-4163-AECE-07D5742E906D}"/>
-    <hyperlink ref="I49" r:id="rId238" xr:uid="{2DF8A589-77D3-487D-9871-F11C086009D1}"/>
-    <hyperlink ref="I82" r:id="rId239" xr:uid="{4F6BB86B-ECFA-4396-9D2B-715AF4C8A22C}"/>
-    <hyperlink ref="I50" r:id="rId240" xr:uid="{C80EDEE3-BA73-444F-89E4-2007846DC254}"/>
-    <hyperlink ref="I90" r:id="rId241" xr:uid="{E27523F8-498C-4ABD-8999-7C5FE36E5CA5}"/>
-    <hyperlink ref="L72" r:id="rId242" xr:uid="{948CADBD-38FA-4A43-B789-35C5FE176C3F}"/>
-    <hyperlink ref="L3" r:id="rId243" xr:uid="{F46A9101-D683-4CCF-9110-8584476B2BA9}"/>
-    <hyperlink ref="L83" r:id="rId244" xr:uid="{6E19F5D8-BA05-4C24-BFED-0131679AE1A3}"/>
-    <hyperlink ref="L57" r:id="rId245" xr:uid="{15D92DD2-9C84-4024-BCB0-89C6EAD615FB}"/>
-    <hyperlink ref="L18" r:id="rId246" xr:uid="{E24865B7-0C5D-46C6-8B52-CB38271DBD7E}"/>
-    <hyperlink ref="L49" r:id="rId247" xr:uid="{4D2C143E-EFF2-43ED-8C1B-94D7326ABF76}"/>
-    <hyperlink ref="L92" r:id="rId248" xr:uid="{22687922-AA0C-441B-A3FA-FB8732C6A78E}"/>
-    <hyperlink ref="L106" r:id="rId249" display="https://scholar.google.com/citations?user=Gzsxo-oAAAAJ&amp;hl=en&amp;oi=ao" xr:uid="{FF9B096B-7991-46C3-B06A-152491BA6C90}"/>
-    <hyperlink ref="L68" r:id="rId250" xr:uid="{690AB285-269F-47C4-BA46-90F767A79CC1}"/>
-    <hyperlink ref="L91" r:id="rId251" xr:uid="{9AF26C9F-30B4-4DAE-A809-C138362FFD00}"/>
-    <hyperlink ref="L95" r:id="rId252" xr:uid="{8D4A0E6E-AA77-4CD4-AA54-DEC95D5CF09E}"/>
-    <hyperlink ref="L50" r:id="rId253" xr:uid="{A64FDC24-6D97-4969-AC20-BF200CE32B3A}"/>
-    <hyperlink ref="L19" r:id="rId254" xr:uid="{2DF7625D-5BDC-4383-BFF5-27331B9E27C1}"/>
-    <hyperlink ref="L71" r:id="rId255" display="https://scholar.google.co.in/citations?user=9PPA-6oAAAAJ&amp;hl=en" xr:uid="{38968AA0-46FD-46B0-84CD-C755BCC30A99}"/>
-    <hyperlink ref="L23" r:id="rId256" xr:uid="{4FF8802A-1D76-4C6B-91B4-17C781B102D6}"/>
-    <hyperlink ref="L52" r:id="rId257" xr:uid="{8365015A-789A-4D2C-9684-352B6CC70A5E}"/>
-    <hyperlink ref="L86" r:id="rId258" xr:uid="{BD03203D-E2A2-453C-8DB9-B1F0B5A13124}"/>
-    <hyperlink ref="L36" r:id="rId259" display="https://scholar.google.com/citations?user=ay8-QY0AAAAJ&amp;hl=en&amp;oi=ao" xr:uid="{CEA8B045-C60C-4ADA-9F10-8B980373388F}"/>
-    <hyperlink ref="L14" r:id="rId260" display="https://scholar.google.com/citations?user=TCsNw-YAAAAJ&amp;hl=en" xr:uid="{D0B58B70-976E-4FD0-A498-4FE5480744DA}"/>
-    <hyperlink ref="L17" r:id="rId261" xr:uid="{19EAA634-8BE7-4A2F-8B30-8A424E254965}"/>
-    <hyperlink ref="L29" r:id="rId262" xr:uid="{3D65CD0F-C15B-4E98-9324-C36FAB47EBC4}"/>
-    <hyperlink ref="L67" r:id="rId263" xr:uid="{264FF3AA-8D89-41E4-9DA6-521BD58711A9}"/>
-    <hyperlink ref="L32" r:id="rId264" display="https://www.bing.com/ck/a?!&amp;&amp;p=6a7ac5a017a1300aJmltdHM9MTcyOTQ2ODgwMCZpZ3VpZD0wMDExMmIyNS1kMzQ5LTY3MTItMmE4My0zZTA1ZDI1NjY2MWEmaW5zaWQ9NTE5NQ&amp;ptn=3&amp;ver=2&amp;hsh=3&amp;fclid=00112b25-d349-6712-2a83-3e05d256661a&amp;psq=google+scholer+gajanan+patange&amp;u=a1aHR0cHM6Ly9zY2hvbGFyLmdvb2dsZS5wbC9jaXRhdGlvbnM_dXNlcj1fRDRISUhjQUFBQUomaGw9ZW4&amp;ntb=1" xr:uid="{275A790E-9657-41D9-B9F2-78D3822C4310}"/>
-    <hyperlink ref="L9" r:id="rId265" xr:uid="{758E6349-E050-42DF-B5C3-FBA97B821030}"/>
-    <hyperlink ref="L114" r:id="rId266" xr:uid="{9ACD46AD-FE8F-41CE-9823-5DC65F691D5B}"/>
-    <hyperlink ref="L4" r:id="rId267" xr:uid="{9B291D90-C0E1-493C-9E5E-17CAF2B7D2F2}"/>
-    <hyperlink ref="L12" r:id="rId268" xr:uid="{8C6729CD-380A-483D-A997-7DBCBA390939}"/>
-    <hyperlink ref="L101" r:id="rId269" xr:uid="{C07AED6D-34B0-40AA-B65E-C9BFB9F1574D}"/>
-    <hyperlink ref="L38" r:id="rId270" display="https://scholar.google.com/citations?user=6d-aVTEAAAAJ&amp;hl=en" xr:uid="{EBC010F8-7D12-4DC1-9FDA-49EFC51EFF71}"/>
-    <hyperlink ref="L21" r:id="rId271" xr:uid="{0DDB7A07-865A-4AD7-986A-DE5D031FFBD0}"/>
-    <hyperlink ref="L28" r:id="rId272" xr:uid="{E6ABE8A4-4EFC-489A-B104-3BCC2E998A7B}"/>
-    <hyperlink ref="L97" r:id="rId273" xr:uid="{ABDCFD31-BA21-4022-B6C1-EDDD441956ED}"/>
-    <hyperlink ref="L6" r:id="rId274" xr:uid="{591DF322-16B2-4785-A83C-3147BF3D09D2}"/>
-    <hyperlink ref="L70" r:id="rId275" xr:uid="{BB403419-C3FE-440B-B0A2-AF35C3C2E8E3}"/>
-    <hyperlink ref="L22" r:id="rId276" xr:uid="{A227399F-9975-4976-9597-2D3E6151DCB8}"/>
-    <hyperlink ref="L39" r:id="rId277" xr:uid="{535A1FEE-65AB-4486-BF0D-ADD9A3382AFB}"/>
-    <hyperlink ref="L42" r:id="rId278" display="https://scholar.google.com/citations?hl=en&amp;user=geQ-r_QAAAAJ" xr:uid="{36509863-135E-43CA-B732-4C0DEFDDC2FC}"/>
-    <hyperlink ref="L102" r:id="rId279" xr:uid="{7F8D3F89-D92D-4081-B489-E387250A10BD}"/>
-    <hyperlink ref="L24" r:id="rId280" xr:uid="{B4A03D8A-649C-469B-B24A-E9F9B481D48B}"/>
-    <hyperlink ref="L26" r:id="rId281" xr:uid="{D3034C74-7237-42E2-A6B8-CD4BA8BBBF41}"/>
-    <hyperlink ref="L90" r:id="rId282" xr:uid="{53AE3D77-EDB3-413A-8D8F-16969CBE8103}"/>
-    <hyperlink ref="L98" r:id="rId283" xr:uid="{76D99C50-072C-40D7-BDEB-328FCCB109D9}"/>
-    <hyperlink ref="L53" r:id="rId284" xr:uid="{CD634DA2-F1A0-45FA-A86C-61D935383D2E}"/>
-    <hyperlink ref="L81" r:id="rId285" xr:uid="{F6874B5E-545B-4745-A546-56B6FD5105E9}"/>
-    <hyperlink ref="L111" r:id="rId286" xr:uid="{C22F05F4-D13D-45A5-A5B0-3237064F3209}"/>
-    <hyperlink ref="L27" r:id="rId287" xr:uid="{32CD251C-92CC-42C2-865F-89BE3026727C}"/>
-    <hyperlink ref="L54" r:id="rId288" xr:uid="{287D782E-D3CC-498E-B117-EBE696C4D447}"/>
-    <hyperlink ref="L41" r:id="rId289" xr:uid="{B241D450-267C-40BF-9C45-8957239BDD86}"/>
-    <hyperlink ref="L62" r:id="rId290" xr:uid="{AA7AD692-35BE-48A4-AF46-1B6413916E3B}"/>
-    <hyperlink ref="L48" r:id="rId291" display="https://scholar.google.co.in/citations?user=EdcH-Y0AAAAJ&amp;hl=en" xr:uid="{CE335172-93AC-45C2-9068-7C9C19F220C4}"/>
-    <hyperlink ref="L10" r:id="rId292" xr:uid="{A33E4A1F-E63E-4F7D-9DC5-3C5AB6E82811}"/>
-    <hyperlink ref="L51" r:id="rId293" xr:uid="{027764B5-CA65-453C-BFB6-EE555AA7BF1B}"/>
-    <hyperlink ref="L61" r:id="rId294" xr:uid="{E2F70942-EACF-4A90-B18A-A80CB466AAE7}"/>
-    <hyperlink ref="L65" r:id="rId295" xr:uid="{5645BFE0-C2D6-4EED-AFCB-0EF806CC91E9}"/>
-    <hyperlink ref="L34" r:id="rId296" xr:uid="{EE598F68-E624-44F6-B4DD-8299C007487F}"/>
-    <hyperlink ref="L75" r:id="rId297" display="https://scholar.google.com/citations?hl=en&amp;authuser=1&amp;user=-9-RhBoAAAAJ" xr:uid="{E935D410-8781-42B6-B609-E835354DEBBB}"/>
-    <hyperlink ref="L5" r:id="rId298" display="https://scholar.google.co.in/citations?user=cVv-kdYAAAAJ&amp;hl=en" xr:uid="{746C1EFC-2FA9-49B1-AFB8-1C7FCA47096B}"/>
-    <hyperlink ref="L20" r:id="rId299" display="https://scholar.google.com/citations?user=dHkQ5D4AAAAJ&amp;hl=en" xr:uid="{25860FE4-2E75-42A8-BFFE-3AA02DEED40F}"/>
-    <hyperlink ref="L43" r:id="rId300" xr:uid="{5A9FF0C8-1A53-40E2-BF07-8AE47CB6B984}"/>
-    <hyperlink ref="L109" r:id="rId301" xr:uid="{5C89C29F-A386-4BBA-9788-4CB223E1744F}"/>
-    <hyperlink ref="L46" r:id="rId302" xr:uid="{63EFEA34-4397-48CB-B385-33D61D726E20}"/>
-    <hyperlink ref="L64" r:id="rId303" xr:uid="{0A4BFD56-8B2D-444E-8903-49F5DC5883A4}"/>
-    <hyperlink ref="L96" r:id="rId304" display="https://scholar.google.com/citations?hl=en&amp;user=utk-ZT0AAAAJ" xr:uid="{501E8FB4-1DC4-4EBD-A3BE-50F19352C1F0}"/>
-    <hyperlink ref="L84" r:id="rId305" xr:uid="{37E9CEEB-DC2C-46A2-BCF4-5A9521147A39}"/>
-    <hyperlink ref="L40" r:id="rId306" xr:uid="{EEF5DC34-1243-4468-B6B1-D9059ADE8AB0}"/>
-    <hyperlink ref="L110" r:id="rId307" display="https://scholar.google.com/citations?view_op=list_works&amp;hl=en&amp;hl=en&amp;user=HDdsZFsAAAAJ&amp;scilu=&amp;scisig=AJY4_hMAAAAAZxidz75RZUbVraeNHOVGYgbAfP0&amp;gmla=ALUCkoUwv9xfR7EENoQtBn_aiKaqTyzZ1X2kORl9--L4aBw5WcKwjoDCVXVaogYeCbraaig0PTa5IzrpT_DyD12Vlt-ODcDk1Nt3fM0&amp;sciund=7577126703303180020" xr:uid="{197DCE6B-BB53-49E3-9D84-78838F524694}"/>
-    <hyperlink ref="L59" r:id="rId308" xr:uid="{B559F61A-BA8D-4A15-AF94-270FD8E6EE0D}"/>
-    <hyperlink ref="L99" r:id="rId309" xr:uid="{BDF263A7-4F8B-46B8-BBE8-705BBF9DE738}"/>
-    <hyperlink ref="L13" r:id="rId310" xr:uid="{7649604F-C033-4670-9F95-0C2C5AC47C84}"/>
-    <hyperlink ref="L45" r:id="rId311" xr:uid="{035221F3-6BA9-41F1-A09D-0FD648704591}"/>
-    <hyperlink ref="L105" r:id="rId312" xr:uid="{1CDECF45-D107-4A0E-A561-5D783437E97C}"/>
-    <hyperlink ref="L103" r:id="rId313" xr:uid="{B653EAA6-C485-435F-854D-438BD267A19D}"/>
-    <hyperlink ref="L94" r:id="rId314" xr:uid="{BAF6ABB2-16F7-4B7A-8AC8-F52F94951E56}"/>
-    <hyperlink ref="L15" r:id="rId315" xr:uid="{F38927F1-EEEB-453A-8636-E6644582D973}"/>
-    <hyperlink ref="L56" r:id="rId316" xr:uid="{9E4C99F0-F427-4B73-88C1-9DDF17D8ABDE}"/>
-    <hyperlink ref="L47" r:id="rId317" xr:uid="{4048416A-0F5D-4582-8A3D-08AFC13874F9}"/>
-    <hyperlink ref="L104" r:id="rId318" xr:uid="{8400FD3C-B4D9-436A-8179-88B2F74CE3F2}"/>
-    <hyperlink ref="L44" r:id="rId319" xr:uid="{201F5259-DE23-43B6-A300-CE6428FFA5ED}"/>
-    <hyperlink ref="L89" r:id="rId320" xr:uid="{31420B66-56AB-4794-90CA-5F5AFEE32FDC}"/>
-    <hyperlink ref="L87" r:id="rId321" xr:uid="{C4F50DBC-0BFE-4509-9E86-8433559B0E5F}"/>
-    <hyperlink ref="L63" r:id="rId322" xr:uid="{90FCCA59-114D-4A5C-9409-D7A92B5C554D}"/>
-    <hyperlink ref="L37" r:id="rId323" xr:uid="{86700D43-54F6-409C-AA74-11A10CF95742}"/>
-    <hyperlink ref="L66" r:id="rId324" xr:uid="{C018FF9B-EED7-4A65-95FA-780ACBBA2D7E}"/>
-    <hyperlink ref="L107" r:id="rId325" xr:uid="{60A89811-803F-44C1-9C4C-03400FFC3370}"/>
-    <hyperlink ref="L58" r:id="rId326" display="https://scholar.google.com/citations?user=D-wd8QgAAAAJ&amp;hl=en" xr:uid="{FEE2843B-8463-42EA-93D3-8C0055A27E1B}"/>
-    <hyperlink ref="L73" r:id="rId327" xr:uid="{D89F1643-F631-4232-BD92-A17AB43537BB}"/>
-    <hyperlink ref="L2" r:id="rId328" xr:uid="{FA588FCD-5B5F-455C-A8F1-363E48BF4B34}"/>
-    <hyperlink ref="L11" r:id="rId329" xr:uid="{75F0D2F4-DBF8-4BC0-81C8-E510EB404F91}"/>
-    <hyperlink ref="L93" r:id="rId330" xr:uid="{4B1641D3-9830-41C6-9804-FD4F1CAA246E}"/>
-    <hyperlink ref="L116" r:id="rId331" xr:uid="{187B270B-DD03-4B4E-A0EC-FA089BBBF941}"/>
-    <hyperlink ref="L79" r:id="rId332" xr:uid="{09000797-9862-4D17-81A3-8BF615CB0D28}"/>
-    <hyperlink ref="L33" r:id="rId333" xr:uid="{30E40F4D-0941-4C35-B988-415178726C05}"/>
-    <hyperlink ref="L100" r:id="rId334" xr:uid="{2A5203BE-43E1-47B8-B2C4-1CC37588A5AB}"/>
-    <hyperlink ref="L88" r:id="rId335" xr:uid="{570C26B0-6EF3-40AB-BBA0-06474B8C9E9F}"/>
-    <hyperlink ref="L30" r:id="rId336" xr:uid="{8315B941-53AD-4CC4-8A93-715BF028D5D6}"/>
-    <hyperlink ref="L85" r:id="rId337" xr:uid="{A11BA51D-FBB4-444E-9239-AD5CA8BDA6AA}"/>
-    <hyperlink ref="L108" r:id="rId338" xr:uid="{BD6653EC-2D4F-4519-B739-A572013209E8}"/>
-    <hyperlink ref="L60" r:id="rId339" xr:uid="{FCDEB08A-0CA4-4598-B598-28FC8001225C}"/>
-    <hyperlink ref="L55" r:id="rId340" xr:uid="{21317881-56A9-411E-B0E0-953DFEB53FB5}"/>
-    <hyperlink ref="L115" r:id="rId341" xr:uid="{2C2ECFF6-DA6C-4C65-B48D-83C8B953A10F}"/>
-    <hyperlink ref="L7" r:id="rId342" xr:uid="{AC52BE48-B1BC-4E71-B6C1-88AF068D6F7B}"/>
-    <hyperlink ref="L31" r:id="rId343" xr:uid="{7701D08D-592D-4F08-8A1D-722D9125A481}"/>
-    <hyperlink ref="L76" r:id="rId344" xr:uid="{08A9DD36-F049-430E-ACEE-0254B9EB019D}"/>
-    <hyperlink ref="L82" r:id="rId345" xr:uid="{69BD5E03-494B-42BC-B711-BD56B50C14BD}"/>
-    <hyperlink ref="L8" r:id="rId346" display="https://scholar.google.com/citations?user=49QO52oAAAAJ&amp;hl=en&amp;citsig=ADIE8snLeq6YPks1Pa9NqbNhY8-8" xr:uid="{597E11F7-5E1F-4746-9B2D-F0B3CE2DAADD}"/>
-    <hyperlink ref="M72" r:id="rId347" display="https://vidwan.inflibnet.ac.in/profile/161243/MTYxMjQz" xr:uid="{377E489A-5F66-4D39-9D16-5A09C06888BF}"/>
-    <hyperlink ref="M3" r:id="rId348" xr:uid="{969CA3F3-003E-45D0-B448-786C1B45A99B}"/>
-    <hyperlink ref="M83" r:id="rId349" xr:uid="{FCF270CA-7E29-44DE-9B34-531A560121D2}"/>
-    <hyperlink ref="M57" r:id="rId350" xr:uid="{27A56F3E-3B7A-497C-B419-6D4EB0B36DFE}"/>
-    <hyperlink ref="M18" r:id="rId351" xr:uid="{A8B03D72-4F58-488B-AA71-6FE545C4F974}"/>
-    <hyperlink ref="M49" r:id="rId352" xr:uid="{46B27430-2CB4-4571-B683-C90BDB1A869A}"/>
-    <hyperlink ref="M92" r:id="rId353" xr:uid="{B3372949-44D6-47D3-93F5-F231A1194C2D}"/>
-    <hyperlink ref="M106" r:id="rId354" xr:uid="{BD564D33-09CC-4E3F-8665-C7CC006586D4}"/>
-    <hyperlink ref="M68" r:id="rId355" xr:uid="{46D7BE4E-C50A-4838-A0D5-A66608E30FB1}"/>
-    <hyperlink ref="M91" r:id="rId356" xr:uid="{49346F82-88CD-458B-9055-E1D237495067}"/>
-    <hyperlink ref="M95" r:id="rId357" xr:uid="{275EA512-D486-4AA6-B9C6-EDFD8EB5E681}"/>
-    <hyperlink ref="M50" r:id="rId358" xr:uid="{F1370FFD-2A24-4E0D-842E-D15A59048874}"/>
-    <hyperlink ref="M19" r:id="rId359" xr:uid="{B079BDCE-9644-48D8-ADB9-55246D89BB3B}"/>
-    <hyperlink ref="M71" r:id="rId360" xr:uid="{21DA9F6E-42F2-4C08-8BCC-45E0F47AC02F}"/>
-    <hyperlink ref="M23" r:id="rId361" display="https://vidwan.inflibnet.ac.in/profile/162290/MTYyMjkw" xr:uid="{C5101B56-8150-4439-9561-ADE65CCB8626}"/>
-    <hyperlink ref="M78" r:id="rId362" xr:uid="{FA23B353-3F9D-46B1-82DA-820AA4FBE86D}"/>
-    <hyperlink ref="M86" r:id="rId363" xr:uid="{680496D4-6792-4688-B37B-3D2836A2CBB1}"/>
-    <hyperlink ref="M36" r:id="rId364" xr:uid="{C295F105-2491-4119-851F-B09A35F5D83B}"/>
-    <hyperlink ref="M14" r:id="rId365" xr:uid="{C6A42F1F-C70B-482C-BAF5-08E29835556D}"/>
-    <hyperlink ref="M80" r:id="rId366" xr:uid="{D12744D8-8D17-44EF-A69E-A1A202FA6698}"/>
-    <hyperlink ref="M17" r:id="rId367" xr:uid="{026E65A7-E47E-491B-A07D-37EBD353FD4E}"/>
-    <hyperlink ref="M35" r:id="rId368" xr:uid="{5D0B8227-026E-47C4-897D-D449D1EA7349}"/>
-    <hyperlink ref="M29" r:id="rId369" xr:uid="{02E7C489-97EB-4764-B304-885B559F8C0E}"/>
-    <hyperlink ref="M67" r:id="rId370" xr:uid="{7BCC998C-8FF9-4866-BDE0-4E618132491D}"/>
-    <hyperlink ref="M9" r:id="rId371" xr:uid="{91B9619A-0474-417B-A83E-F1ACC0AF0CEC}"/>
-    <hyperlink ref="M114" r:id="rId372" xr:uid="{9DC7345F-59EF-46AB-AFF8-A485034FCFB5}"/>
-    <hyperlink ref="M4" r:id="rId373" xr:uid="{C24F8B1B-E131-406E-8B92-980981B7F2F8}"/>
-    <hyperlink ref="M12" r:id="rId374" xr:uid="{BBE0AFF3-0C87-45BA-B244-2EBD516259AE}"/>
-    <hyperlink ref="M101" r:id="rId375" xr:uid="{36A3294C-FBE9-4AE5-B367-A4F7EB299507}"/>
-    <hyperlink ref="M38" r:id="rId376" xr:uid="{CC9655FE-1EDD-46F8-BE5B-9E92C5013680}"/>
-    <hyperlink ref="M21" r:id="rId377" xr:uid="{47BBD086-2D33-4012-A8B6-B4A4E0F676C3}"/>
-    <hyperlink ref="M28" r:id="rId378" xr:uid="{D9812B9F-31E0-4DAD-8A1E-6460EF4BE795}"/>
-    <hyperlink ref="M97" r:id="rId379" xr:uid="{194FE3FD-0EF9-46C4-B769-B4AAF95E0018}"/>
-    <hyperlink ref="M6" r:id="rId380" xr:uid="{3C597F50-A6C7-4686-85A0-F6E6694F57E3}"/>
-    <hyperlink ref="M70" r:id="rId381" xr:uid="{A87D811B-910D-45F2-BF34-A478CD7D8B09}"/>
-    <hyperlink ref="M22" r:id="rId382" xr:uid="{686F19E9-9FDF-4E88-8243-D809ABB3FE79}"/>
-    <hyperlink ref="M42" r:id="rId383" xr:uid="{FB2FC638-1D01-4122-BA7D-9717BC8B2EF3}"/>
-    <hyperlink ref="M102" r:id="rId384" xr:uid="{F0E56AD7-3828-45B1-A3E4-95B4E7B7495F}"/>
-    <hyperlink ref="M24" r:id="rId385" xr:uid="{5E6A27FA-6F1B-4920-AF3A-0018DC331E36}"/>
-    <hyperlink ref="M26" r:id="rId386" xr:uid="{758E2E1D-BBB4-4F0B-A1FA-EB3E5DE2D156}"/>
-    <hyperlink ref="M90" r:id="rId387" xr:uid="{1C320BD2-5251-44A7-81C2-D89E208736CC}"/>
-    <hyperlink ref="M98" r:id="rId388" xr:uid="{4BF3D2D2-9743-494B-A7D1-9EEF7423F2B3}"/>
-    <hyperlink ref="M53" r:id="rId389" xr:uid="{642FC8EF-95E5-4804-8108-73A9ADB45FBB}"/>
-    <hyperlink ref="M81" r:id="rId390" xr:uid="{6069906B-85A1-4520-B697-E8420F4D518A}"/>
-    <hyperlink ref="M111" r:id="rId391" xr:uid="{45C10A27-1AD3-4A6F-966C-946B5F9ECB83}"/>
-    <hyperlink ref="M27" r:id="rId392" xr:uid="{F2CE36A5-3E73-43DE-A91D-5D1E2781384A}"/>
-    <hyperlink ref="M54" r:id="rId393" xr:uid="{6815F862-B01A-4FF2-B310-DDE65D78FBDB}"/>
-    <hyperlink ref="M41" r:id="rId394" xr:uid="{2167CAC5-42F7-48BE-A140-282801D50406}"/>
-    <hyperlink ref="M112" r:id="rId395" xr:uid="{2D0BE123-EDFD-4091-BCF0-204188FF3B30}"/>
-    <hyperlink ref="M62" r:id="rId396" xr:uid="{7A45E352-1CCC-4E30-B5C0-2C2507845C07}"/>
-    <hyperlink ref="M48" r:id="rId397" xr:uid="{D69AB844-8B39-4156-9897-B02CB20CA4D5}"/>
-    <hyperlink ref="M10" r:id="rId398" xr:uid="{04F1C981-8348-4D72-8A69-A692D3062D64}"/>
-    <hyperlink ref="M51" r:id="rId399" xr:uid="{65DE02F5-B84D-45D0-9DC1-F7808BDFD38D}"/>
-    <hyperlink ref="M61" r:id="rId400" xr:uid="{C49314E6-1B8D-41D3-8824-C6AE59F00DDA}"/>
-    <hyperlink ref="M65" r:id="rId401" xr:uid="{22CCAF6F-639B-4091-91C4-0D9E09A79A31}"/>
-    <hyperlink ref="M34" r:id="rId402" xr:uid="{9E6DCF4C-EA31-4D9D-AE0D-50C83C0347DE}"/>
-    <hyperlink ref="M75" r:id="rId403" xr:uid="{D71D3644-6845-46C5-83D7-DA2B52AF5733}"/>
-    <hyperlink ref="M5" r:id="rId404" xr:uid="{7687E521-D8FB-41F5-A5E6-AE953D92E830}"/>
-    <hyperlink ref="M20" r:id="rId405" xr:uid="{4DDDF623-882B-481C-A6D6-41041F349837}"/>
-    <hyperlink ref="M43" r:id="rId406" xr:uid="{52C3C99B-42C3-444C-A194-78CDBDAFC9CB}"/>
-    <hyperlink ref="M109" r:id="rId407" display="https://vidwan.inflibnet.ac.in/profile/161344" xr:uid="{FE2BA8E6-DD6C-4A10-91F1-326AA51E88D5}"/>
-    <hyperlink ref="M46" r:id="rId408" xr:uid="{2FFD071F-CF1A-4200-989A-978DBA72FD44}"/>
-    <hyperlink ref="M64" r:id="rId409" xr:uid="{E4C6C757-CD64-47C7-8F12-6CE6B9FFD60C}"/>
-    <hyperlink ref="M96" r:id="rId410" xr:uid="{722D10A1-25FB-4CE7-9F0B-C75508E442CE}"/>
-    <hyperlink ref="M84" r:id="rId411" xr:uid="{32A836FB-CB40-470F-B02E-7B6392FD539D}"/>
-    <hyperlink ref="M40" r:id="rId412" location="other_information_panel" display="https://vidwan.inflibnet.ac.in/myprofile - other_information_panel" xr:uid="{FE644920-561A-44DA-A700-34ED8EB7963F}"/>
-    <hyperlink ref="M110" r:id="rId413" xr:uid="{2C076003-CA45-4492-A114-A44CC1E60BF2}"/>
-    <hyperlink ref="M59" r:id="rId414" xr:uid="{BC2FF260-09A4-4D46-81FB-823835AD57DA}"/>
-    <hyperlink ref="M99" r:id="rId415" xr:uid="{B2860DA1-1C8E-403D-9E1C-CE3896F91BFD}"/>
-    <hyperlink ref="M13" r:id="rId416" xr:uid="{2DE04985-AB3C-4D4B-BCEE-EF8C728199F4}"/>
-    <hyperlink ref="M45" r:id="rId417" xr:uid="{546046AA-45E7-4EDD-81FB-A6648B9BB595}"/>
-    <hyperlink ref="M105" r:id="rId418" xr:uid="{7330EFFC-2F12-4EFE-BF25-3D30861E8775}"/>
-    <hyperlink ref="M94" r:id="rId419" xr:uid="{4F8D1CF8-D215-443F-8914-E091AFB2DBAE}"/>
-    <hyperlink ref="M15" r:id="rId420" xr:uid="{4CD74FA1-A139-4BCD-9CB7-1D7091E614B9}"/>
-    <hyperlink ref="M56" r:id="rId421" xr:uid="{EAABDC46-8B1B-482C-B7D7-E6E7C16FB647}"/>
-    <hyperlink ref="M104" r:id="rId422" xr:uid="{ACDF2E56-83C7-477F-A573-2B4112936AD3}"/>
-    <hyperlink ref="M44" r:id="rId423" xr:uid="{B502A1CE-A61F-4999-A855-F6ECA908B905}"/>
-    <hyperlink ref="M89" r:id="rId424" xr:uid="{EF82DFB8-BEB4-47BB-B28B-AF5A4CDD6891}"/>
-    <hyperlink ref="M74" r:id="rId425" xr:uid="{6D71EE52-86C9-4EE0-A55D-7B9652B864FF}"/>
-    <hyperlink ref="M87" r:id="rId426" xr:uid="{C073950A-A28A-4ED8-B9C1-BD3B160FAEF3}"/>
-    <hyperlink ref="M63" r:id="rId427" xr:uid="{958C1C19-9C17-41E8-ADC4-BAB91255F382}"/>
-    <hyperlink ref="M37" r:id="rId428" xr:uid="{0CC98B27-C0DC-4F81-A868-5BC7C0784B50}"/>
-    <hyperlink ref="M66" r:id="rId429" xr:uid="{B86191A1-65D6-4540-845F-518E32A64FBF}"/>
-    <hyperlink ref="M107" r:id="rId430" xr:uid="{47889514-AB9C-4B04-95A5-1CCA3A0DFCA8}"/>
-    <hyperlink ref="M58" r:id="rId431" xr:uid="{36AE2A42-0E80-4A5F-8FB0-4EAB2AEA8C36}"/>
-    <hyperlink ref="M69" r:id="rId432" xr:uid="{7FE7C886-2B29-491F-8C86-5526A33F7121}"/>
-    <hyperlink ref="M73" r:id="rId433" xr:uid="{FDFB0EA9-AD4D-43E9-BEF9-C60B9531C82F}"/>
-    <hyperlink ref="M2" r:id="rId434" xr:uid="{251C34E0-B509-4755-B850-FDEB3B770405}"/>
-    <hyperlink ref="M11" r:id="rId435" xr:uid="{3203A1D8-1572-4E08-ADEF-54F74525E87A}"/>
-    <hyperlink ref="M93" r:id="rId436" xr:uid="{28CD01ED-234C-4911-A047-12722FE76C1F}"/>
-    <hyperlink ref="M116" r:id="rId437" xr:uid="{82D93DAC-CF9F-4D41-B8C8-5AE08EA58BAA}"/>
-    <hyperlink ref="M79" r:id="rId438" xr:uid="{68120C28-52E3-4EC9-9F3E-EB5A3578A3BD}"/>
-    <hyperlink ref="M33" r:id="rId439" display="https://vidwan.inflibnet.ac.in/profile/161755-" xr:uid="{B87FE430-1CFA-4F98-A7E4-77FBF96BA37F}"/>
-    <hyperlink ref="M100" r:id="rId440" xr:uid="{649E7EFF-CC71-476F-9A81-1581EC34CD48}"/>
-    <hyperlink ref="M88" r:id="rId441" xr:uid="{1C9375D7-8EF5-40A1-914C-C5A7CD3188FB}"/>
-    <hyperlink ref="M85" r:id="rId442" xr:uid="{66509B53-066F-4635-85A6-6E99D5FE0B3E}"/>
-    <hyperlink ref="M108" r:id="rId443" xr:uid="{775D1521-4736-4C73-BB71-31FD5AD1E561}"/>
-    <hyperlink ref="M60" r:id="rId444" xr:uid="{A128A132-518A-476D-BCF8-6D3638CE18D6}"/>
-    <hyperlink ref="M55" r:id="rId445" xr:uid="{A1AFE28A-9643-4A4A-95E8-53E1C4380AAE}"/>
-    <hyperlink ref="M115" r:id="rId446" xr:uid="{6A1A9D4D-97FF-42A2-B2EA-85F3F7E515C2}"/>
-    <hyperlink ref="M7" r:id="rId447" xr:uid="{BA494279-5FA7-4467-ACAA-FFA1824DB9F7}"/>
-    <hyperlink ref="M31" r:id="rId448" xr:uid="{43BBD922-4BE8-457C-9F25-7684B0D6F35B}"/>
-    <hyperlink ref="M76" r:id="rId449" xr:uid="{C2281EE1-00E4-42D3-875C-3C9C699518DB}"/>
-    <hyperlink ref="M82" r:id="rId450" xr:uid="{3C1D1058-7762-4D63-9FB9-41A44D4AB1F3}"/>
-    <hyperlink ref="E16:E17" r:id="rId451" display="https://placehold.co/400x600" xr:uid="{18BA32A8-6934-421F-9831-28D4907FFF98}"/>
-    <hyperlink ref="E17" r:id="rId452" xr:uid="{7510203D-B2F6-44B8-BB79-8C3F26D4C98A}"/>
+    <hyperlink ref="E56" r:id="rId27" xr:uid="{D60F983F-3A4A-4B45-A5A9-1CBD13CCBAB1}"/>
+    <hyperlink ref="E58" r:id="rId28" xr:uid="{DDB2A0FD-936A-490E-BE1E-1762A651B20C}"/>
+    <hyperlink ref="E62" r:id="rId29" xr:uid="{5E732335-693B-490D-844A-64351A2B11C7}"/>
+    <hyperlink ref="E64" r:id="rId30" xr:uid="{B032BBB6-4D16-4E33-A3F0-D7039E10D767}"/>
+    <hyperlink ref="E66" r:id="rId31" display="https://placehold.co/400x600" xr:uid="{C71F9231-ACA2-46E1-BE2F-462475789CDA}"/>
+    <hyperlink ref="E68" r:id="rId32" xr:uid="{6DAF2527-3F52-4351-90EE-F788A7836287}"/>
+    <hyperlink ref="E70" r:id="rId33" xr:uid="{C213B07F-FB90-4578-BA40-CB5277C5E9F8}"/>
+    <hyperlink ref="E72" r:id="rId34" xr:uid="{B6B3C0BC-449F-4D5F-8991-2960BC1E1B95}"/>
+    <hyperlink ref="E74" r:id="rId35" xr:uid="{12F3E568-1027-43BC-89EA-C5D4D2C3F3B1}"/>
+    <hyperlink ref="E76" r:id="rId36" xr:uid="{9BCFDA15-C8D8-41F6-B5C1-8DB9E3F54F38}"/>
+    <hyperlink ref="E78" r:id="rId37" display="https://placehold.co/400x600" xr:uid="{5074351A-0735-4679-AE99-F1F491EAD66F}"/>
+    <hyperlink ref="E80" r:id="rId38" xr:uid="{797A27FB-9286-43BA-A3D3-06E0B7DF57C7}"/>
+    <hyperlink ref="E82" r:id="rId39" display="https://placehold.co/400x600" xr:uid="{E22D4C78-609C-4F6C-902E-67DDEA2AEC08}"/>
+    <hyperlink ref="E84" r:id="rId40" xr:uid="{689543FA-D772-478F-B75B-353A8D5F5A0F}"/>
+    <hyperlink ref="E86" r:id="rId41" display="https://placehold.co/400x600" xr:uid="{6F1B4F40-1347-45F9-B0B9-89687F77E0B0}"/>
+    <hyperlink ref="E88" r:id="rId42" xr:uid="{269A95A2-A318-4245-8364-07E925D041A6}"/>
+    <hyperlink ref="E90" r:id="rId43" xr:uid="{BC5C79FD-42B9-4F63-B259-53ADA917C149}"/>
+    <hyperlink ref="E92" r:id="rId44" xr:uid="{F219C840-96AC-40EA-9D7B-C09CBA360D2A}"/>
+    <hyperlink ref="E94" r:id="rId45" xr:uid="{E85B62E0-66A6-4BDE-AB82-B3F3885FF25D}"/>
+    <hyperlink ref="E96" r:id="rId46" xr:uid="{F685C903-F46A-4AEA-A4B6-30F5F5C38E02}"/>
+    <hyperlink ref="E98" r:id="rId47" display="https://placehold.co/400x600" xr:uid="{34A32507-5178-4AE2-8923-C76F8834EAC3}"/>
+    <hyperlink ref="E100" r:id="rId48" display="https://placehold.co/400x600" xr:uid="{316F114E-DC59-4C12-AAE4-7C561A6A4A37}"/>
+    <hyperlink ref="E102" r:id="rId49" xr:uid="{E6C4E1E9-ADFC-463C-BA35-72BF5470C0FC}"/>
+    <hyperlink ref="E104" r:id="rId50" display="https://placehold.co/400x600" xr:uid="{5C2E1F62-17AE-4C61-86CF-CFAADD48E3DA}"/>
+    <hyperlink ref="E106" r:id="rId51" display="https://placehold.co/400x600" xr:uid="{EB2D28AA-5611-4D14-B6D8-65655568052B}"/>
+    <hyperlink ref="E108" r:id="rId52" xr:uid="{1A1FF6C3-6CA4-4205-87F4-FFA4C505FE05}"/>
+    <hyperlink ref="E110" r:id="rId53" display="https://placehold.co/400x600" xr:uid="{D5F8DE7D-9A2E-4EB2-AD3E-1B6347BBB03A}"/>
+    <hyperlink ref="E114" r:id="rId54" xr:uid="{F52A7ADE-923C-4FC0-835C-C78BE5475FD1}"/>
+    <hyperlink ref="E116" r:id="rId55" xr:uid="{88BB9B9A-193B-430A-8A94-9996D9F8B858}"/>
+    <hyperlink ref="E5" r:id="rId56" xr:uid="{673B2D9E-5CEE-40DD-A0A2-66025584E8C2}"/>
+    <hyperlink ref="E7" r:id="rId57" xr:uid="{20202916-CECB-497F-BB8D-D7E09DCEC193}"/>
+    <hyperlink ref="E9" r:id="rId58" xr:uid="{E7773CE7-BD5F-4624-B940-0E795B4A4E30}"/>
+    <hyperlink ref="E11" r:id="rId59" xr:uid="{93DA058C-7CEC-4BA2-9D33-5FB8B5E88910}"/>
+    <hyperlink ref="E13" r:id="rId60" xr:uid="{8F788626-64E7-4F1D-A12D-F2E9D916467C}"/>
+    <hyperlink ref="E15" r:id="rId61" display="https://placehold.co/400x600" xr:uid="{8AD2972F-0CB2-4DCE-8821-C56F9057AD5B}"/>
+    <hyperlink ref="E19" r:id="rId62" display="https://placehold.co/400x600" xr:uid="{D4698768-8DC5-407A-B6F4-C1C875BFB78D}"/>
+    <hyperlink ref="E21" r:id="rId63" xr:uid="{13DD67BA-1FCB-43E0-A39C-FFE32E5D3954}"/>
+    <hyperlink ref="E23" r:id="rId64" xr:uid="{90D0F56C-C7DB-4632-B91C-EF74541F5FEA}"/>
+    <hyperlink ref="E25" r:id="rId65" xr:uid="{F6A0C9FE-D2B9-4181-8F81-93868F3E313C}"/>
+    <hyperlink ref="E27" r:id="rId66" xr:uid="{848B184F-1DE9-469A-9D63-F5CDEBF10D7A}"/>
+    <hyperlink ref="E29" r:id="rId67" xr:uid="{1AF17D20-76D5-4714-B7E2-2D8B8CB9ADC3}"/>
+    <hyperlink ref="E31" r:id="rId68" display="https://placehold.co/400x600" xr:uid="{22DD1D25-8288-4AC9-A5FC-D9B7B89B515C}"/>
+    <hyperlink ref="E33" r:id="rId69" xr:uid="{01F92761-8D63-4A2C-8713-25D41165DB40}"/>
+    <hyperlink ref="E35" r:id="rId70" xr:uid="{FFD57A2F-B179-4903-B296-F8069D1F1332}"/>
+    <hyperlink ref="E37" r:id="rId71" xr:uid="{291A37C6-A686-4CDE-9352-CAE725E23B11}"/>
+    <hyperlink ref="E39" r:id="rId72" xr:uid="{6ECECF25-2624-4D12-A089-9B4C4DBCF38B}"/>
+    <hyperlink ref="E41" r:id="rId73" display="https://placehold.co/400x600" xr:uid="{B8267D85-A691-4187-91DB-27E364616A8C}"/>
+    <hyperlink ref="E43" r:id="rId74" xr:uid="{AA69E1F0-E88A-495C-A844-C33C82F6CE26}"/>
+    <hyperlink ref="E45" r:id="rId75" xr:uid="{269F03E1-526C-4849-A6D5-8276665E4485}"/>
+    <hyperlink ref="E47" r:id="rId76" xr:uid="{D722AC52-912D-4A3F-8560-FAA4DCA60A56}"/>
+    <hyperlink ref="E49" r:id="rId77" xr:uid="{6ED9D463-8E32-4780-942A-C1EC9D07542B}"/>
+    <hyperlink ref="E51" r:id="rId78" xr:uid="{FAAE2569-D069-46B3-A7AA-6969338A4AFF}"/>
+    <hyperlink ref="E53" r:id="rId79" xr:uid="{919767C3-0A6A-4A63-9549-0F7B3A7EE7DF}"/>
+    <hyperlink ref="E55" r:id="rId80" xr:uid="{BD76B93C-ACC1-4CF1-A623-39E4FAFED853}"/>
+    <hyperlink ref="E57" r:id="rId81" display="https://placehold.co/400x600" xr:uid="{7964589D-7453-4997-AC7B-F98F5B5B7029}"/>
+    <hyperlink ref="E59" r:id="rId82" xr:uid="{F72D2D0A-AD07-45DC-AA3D-223C36C995AB}"/>
+    <hyperlink ref="E61" r:id="rId83" xr:uid="{D79CAE5D-C5B6-4B75-8261-008B5374EBDB}"/>
+    <hyperlink ref="E63" r:id="rId84" xr:uid="{75C81E45-FAA6-4175-A2FE-BA7C7F71F6F3}"/>
+    <hyperlink ref="E67" r:id="rId85" display="https://placehold.co/400x600" xr:uid="{F199289C-0CB7-41CD-95E9-D9C97B86A7E7}"/>
+    <hyperlink ref="E69" r:id="rId86" display="https://placehold.co/400x600" xr:uid="{E4715AC6-7D6D-4434-A585-79B8F25233F6}"/>
+    <hyperlink ref="E71" r:id="rId87" xr:uid="{CFD1BDC4-A848-4998-9430-C29DB079EED4}"/>
+    <hyperlink ref="E73" r:id="rId88" xr:uid="{DEC62E70-AB7A-4365-B90A-11A1D549F375}"/>
+    <hyperlink ref="E75" r:id="rId89" xr:uid="{A925F566-676A-47EA-9068-3A8AC9C78A71}"/>
+    <hyperlink ref="E77" r:id="rId90" xr:uid="{826BB4FF-EF4E-4C68-AE45-B4C9CEE10FB5}"/>
+    <hyperlink ref="E79" r:id="rId91" xr:uid="{D55B186E-0A96-4185-9D34-01F9C47E843E}"/>
+    <hyperlink ref="E81" r:id="rId92" xr:uid="{AC60663B-FB99-47D2-A9DA-11C43648559B}"/>
+    <hyperlink ref="E83" r:id="rId93" display="https://placehold.co/400x600" xr:uid="{F83899A5-222C-48AC-9ABC-BC254C3600A8}"/>
+    <hyperlink ref="E85" r:id="rId94" display="https://placehold.co/400x600" xr:uid="{2EE015AD-95D3-42D3-9727-0C2D20C22B2D}"/>
+    <hyperlink ref="E87" r:id="rId95" xr:uid="{1E9351A5-5685-4A61-91E2-9C72A14FBA45}"/>
+    <hyperlink ref="E89" r:id="rId96" display="https://placehold.co/400x600" xr:uid="{DA14C2E4-99E6-4273-B1C6-88E4314A2B53}"/>
+    <hyperlink ref="E91" r:id="rId97" display="https://placehold.co/400x600" xr:uid="{CED33FAF-E705-4A0E-B5BA-28AC459A08F9}"/>
+    <hyperlink ref="E93" r:id="rId98" display="https://placehold.co/400x600" xr:uid="{69683834-3F44-4B9E-879F-17C7B3985064}"/>
+    <hyperlink ref="E95" r:id="rId99" xr:uid="{6706B29D-6B9E-414D-A766-C429245D96A7}"/>
+    <hyperlink ref="E97" r:id="rId100" xr:uid="{B8549196-6B30-41D5-B870-CDF1F6C0AE2B}"/>
+    <hyperlink ref="E99" r:id="rId101" display="https://placehold.co/400x600" xr:uid="{70722206-091E-437D-B026-345C8CDB5176}"/>
+    <hyperlink ref="E101" r:id="rId102" xr:uid="{EF057E02-0A38-4475-84BA-2BC1ED64BA7D}"/>
+    <hyperlink ref="E103" r:id="rId103" xr:uid="{F307B800-2CAD-4E08-A635-F4AD9976A897}"/>
+    <hyperlink ref="E105" r:id="rId104" display="https://placehold.co/400x600" xr:uid="{42F0B609-7315-4192-A377-FDEDE5FDDF8B}"/>
+    <hyperlink ref="E107" r:id="rId105" display="https://placehold.co/400x600" xr:uid="{0BBF4990-1413-476C-AFE7-EC34A9F113B0}"/>
+    <hyperlink ref="E109" r:id="rId106" xr:uid="{43D0B648-1D21-45A3-A6E9-CB546100DAA2}"/>
+    <hyperlink ref="E111" r:id="rId107" xr:uid="{3BF79D70-269C-4AB5-B83F-712DABFF4480}"/>
+    <hyperlink ref="E113" r:id="rId108" xr:uid="{622A2536-A959-42B4-B4F9-EE23F2A44517}"/>
+    <hyperlink ref="E115" r:id="rId109" xr:uid="{7690046C-47D4-4A7B-8DBE-6704DCCAE9C8}"/>
+    <hyperlink ref="J72" r:id="rId110" display="https://www.linkedin.com/in/dr-nilay-patel-106bab14/" xr:uid="{B2E17E23-9358-429B-BBF9-5EE4C8E363CB}"/>
+    <hyperlink ref="J83" r:id="rId111" display="https://www.linkedin.com/in/poonam-thanki-b112a6a2/" xr:uid="{BB16F397-78CE-4DBD-8BE4-13D65525672B}"/>
+    <hyperlink ref="J57" r:id="rId112" display="https://www.linkedin.com/in/dr-manthan-s-manavadaria-2a222219/" xr:uid="{4954A101-EA09-4BF1-8202-A72F86653038}"/>
+    <hyperlink ref="J18" r:id="rId113" display="https://www.linkedin.com/in/bhavin-mehta-86b47795/" xr:uid="{DB7D7CE8-51EF-48EE-BFBF-A021321BDC5F}"/>
+    <hyperlink ref="J49" r:id="rId114" display="https://www.linkedin.com/in/dr-kanwar-preet-kaur-bamrah-64a3a221/" xr:uid="{53166117-8C5A-4AB4-89B7-C2E8B83BC5A5}"/>
+    <hyperlink ref="J92" r:id="rId115" display="https://www.linkedin.com/in/rikita-chokshi-44bb65263/" xr:uid="{184885D3-531C-43E9-853D-5C2EAF6E7696}"/>
+    <hyperlink ref="J106" r:id="rId116" xr:uid="{FBE16C58-F91B-4934-8550-681C7F68CFE1}"/>
+    <hyperlink ref="J68" r:id="rId117" display="https://www.linkedin.com/in/mrugendrasinh-rahevar/" xr:uid="{F0663F50-387A-4315-8A34-03206888175F}"/>
+    <hyperlink ref="J91" r:id="rId118" display="https://www.linkedin.com/in/ravi-patel-13686b19/" xr:uid="{FC6DE30F-2E95-4AA2-B879-8CEAD23CEEC4}"/>
+    <hyperlink ref="J95" r:id="rId119" display="https://www.linkedin.com/in/ronak-patel-63663613a/" xr:uid="{EB8CC283-1781-41D5-BE2D-3C04AED15B01}"/>
+    <hyperlink ref="J50" r:id="rId120" display="https://www.linkedin.com/in/dr-kawaljitsingh-randhawa-96816064/" xr:uid="{4AE0FF76-EF4F-45C3-A542-A7D876A7DA2C}"/>
+    <hyperlink ref="J19" r:id="rId121" display="http://linkedin.com/in/bimal-patel-b7504849" xr:uid="{B02CE38D-7D41-45E6-8D0A-5F0FCF595503}"/>
+    <hyperlink ref="J71" r:id="rId122" display="https://www.linkedin.com/in/nikita-bhatt-ce/?originalSubdomain=in" xr:uid="{9EC6AE06-F884-4149-B7FC-88140006B7F4}"/>
+    <hyperlink ref="J23" r:id="rId123" display="https://www.linkedin.com/in/deep-kothadiya-phd-70983a86/" xr:uid="{8691FEB4-6E3B-4049-9588-FC79EAF0F2EC}"/>
+    <hyperlink ref="J78" r:id="rId124" display="https://www.linkedin.com/in/parmanand-patel-1269016b/" xr:uid="{53EDE3BB-D85D-4DAD-A587-55DA1C805D27}"/>
+    <hyperlink ref="J52" r:id="rId125" display="https://www.linkedin.com/in/krunal-maheriya-aba5681a1/" xr:uid="{9D29078E-A414-4A64-86B1-F77733FF0F8A}"/>
+    <hyperlink ref="J86" r:id="rId126" xr:uid="{21E8E151-1B01-486F-A7D7-4BE4F0BC0B27}"/>
+    <hyperlink ref="J36" r:id="rId127" display="https://www.linkedin.com/in/dr-hardik-modi-181035b/" xr:uid="{F7F908AF-23C0-42F7-8AFE-DF52AF52580B}"/>
+    <hyperlink ref="J14" r:id="rId128" display="http://hlinkedin.com/in/dr-ashwin-makwana-9a6688112" xr:uid="{3D2F3A09-18C9-4E22-B6FA-494330FEF01E}"/>
+    <hyperlink ref="J80" r:id="rId129" xr:uid="{4DA1EB91-0A15-4D6C-9213-F6D1EE675204}"/>
+    <hyperlink ref="J17" r:id="rId130" xr:uid="{8E63BCC9-6C05-45B8-8789-EBB4905292F2}"/>
+    <hyperlink ref="J35" r:id="rId131" display="https://www.linkedin.com/in/gaurav-kumar1582/" xr:uid="{BF49CFFA-7535-44BB-8F9A-67BEFFD957B6}"/>
+    <hyperlink ref="J29" r:id="rId132" display="https://www.linkedin.com/in/dhaval-patel-481b0885/" xr:uid="{5704F17D-173C-4E5E-89CF-B8F7987D86F5}"/>
+    <hyperlink ref="J77" r:id="rId133" display="https://www.linkedin.com/me?trk=p_mwlite_profile_self-secondary_nav" xr:uid="{6148FF48-4942-4818-844D-79919D56DB98}"/>
+    <hyperlink ref="J67" r:id="rId134" display="https://www.linkedin.com/in/dr-miral-desai-245448a2/" xr:uid="{D2BE1269-3E17-415C-B581-A936373A624C}"/>
+    <hyperlink ref="J32" r:id="rId135" display="https://www.linkedin.com/in/gajanan-patange-05ba2219/overlay/about-this-profile/?lipi=urn%3Ali%3Apage%3Ad_flagship3_profile_view_base%3BEvV8mS8jTpy2mGfBhro1og%3D%3D" xr:uid="{CDEEC399-875E-4DDA-A567-6EFC42A0F87E}"/>
+    <hyperlink ref="J114" r:id="rId136" display="https://www.linkedin.com/in/vikas-panchal-873277251/" xr:uid="{A3606037-07FB-4104-B411-BA37A6E2F3CA}"/>
+    <hyperlink ref="J101" r:id="rId137" display="https://www.linkedin.com/in/sneha-padhiar-4aaa17146/" xr:uid="{8CF4272D-E96D-4E1C-80AD-5D3F2F554C53}"/>
+    <hyperlink ref="J38" r:id="rId138" display="https://www.linkedin.com/in/harshul-yagnik-81a6a022/" xr:uid="{683E4E91-B763-4226-99B6-F3E30837AD4B}"/>
+    <hyperlink ref="J21" r:id="rId139" display="https://www.linkedin.com/in/brinda-patel-652073252" xr:uid="{791133CF-E0A2-4B6D-8618-AC19B4D3A9FA}"/>
+    <hyperlink ref="J28" r:id="rId140" xr:uid="{F8104DB3-2B23-47B7-B622-17690E08D84A}"/>
+    <hyperlink ref="J97" r:id="rId141" display="https://www.linkedin.com/in/sagarkumar-patel-0bb94bb5/" xr:uid="{B357E631-0C5E-406B-9B45-A421DE003AD4}"/>
+    <hyperlink ref="J70" r:id="rId142" display="http://www.linkedin.com/in/neha-chauhan22" xr:uid="{E7A9417A-8B16-4D59-A23C-B258564D85D5}"/>
+    <hyperlink ref="J22" r:id="rId143" xr:uid="{895691E5-0B23-47DD-9A36-18923B4FD652}"/>
+    <hyperlink ref="J39" r:id="rId144" display="https://www.linkedin.com/public-profile/settings?trk=d_flagship3_profile_self_view_public_profile" xr:uid="{E4C32594-CCCB-41B2-AE51-AE67F83944BE}"/>
+    <hyperlink ref="J42" r:id="rId145" display="https://www.linkedin.com/in/jalpa-ardeshana-381496b7/" xr:uid="{67C7A4AD-28FD-4291-92FB-A9C4AA0671B4}"/>
+    <hyperlink ref="J102" r:id="rId146" display="https://www.linkedin.com/in/dr-spoorthy-v-10ab3813a/" xr:uid="{EDA5921D-C45B-4D8B-B9FA-3205F4F396D6}"/>
+    <hyperlink ref="J24" r:id="rId147" display="https://www.linkedin.com/in/dhara-patel-839488138" xr:uid="{27C9FC8C-0A44-49AE-8688-8690C8579833}"/>
+    <hyperlink ref="J26" r:id="rId148" display="https://www.linkedin.com/in/dharmendrasinh-chauhan-073a491a4/" xr:uid="{D50E69C7-4F51-4D1B-90EC-FE9F9A44906E}"/>
+    <hyperlink ref="J90" r:id="rId149" display="https://www.linkedin.com/in/rajnik-katriya/" xr:uid="{3AEC1C40-35D9-4AE3-A7E8-9E58FA2C8E43}"/>
+    <hyperlink ref="J98" r:id="rId150" display="https://www.linkedin.com/in/sanket-suthar-544a69210/" xr:uid="{6137F2DC-1F93-4037-B861-A959BDB6DCE6}"/>
+    <hyperlink ref="J53" r:id="rId151" display="http://www.linkedin.com/in/kundan-patel-b9508b27b" xr:uid="{D4BB537A-7CA1-4F2B-9985-F5921034561E}"/>
+    <hyperlink ref="J81" r:id="rId152" xr:uid="{BFFCC995-B6DF-474C-93AA-BDF180E05422}"/>
+    <hyperlink ref="J111" r:id="rId153" display="https://www.linkedin.com/in/vidisha-pradhan-733a1b63/" xr:uid="{06E43119-E5BC-45C4-9126-F192D3006C5B}"/>
+    <hyperlink ref="J27" r:id="rId154" display="https://www.linkedin.com/in/dharmendrasinh-rathod-4482a2a4/" xr:uid="{3BDD0888-FF6F-403B-8A93-FD5176D0DA38}"/>
+    <hyperlink ref="J54" r:id="rId155" display="http://www.linkedin.com/in/madhav-oza-60bb5650" xr:uid="{24641904-0D92-4561-9EC0-14DC5197E375}"/>
+    <hyperlink ref="J41" r:id="rId156" xr:uid="{10BD029B-F728-4FEF-934E-F502C3B3ECDD}"/>
+    <hyperlink ref="J112" r:id="rId157" display="https://www.linkedin.com/in/dr-vijay-chaudhary-12769b311/" xr:uid="{B15A7FAF-9082-4A84-BAA5-265E44F10859}"/>
+    <hyperlink ref="J62" r:id="rId158" display="http://inkedin.com/in/mjdesai/?original_referer=https%3A%2F%2Fwww%2Egoogle%2Ecom%2F&amp;originalSubdomain=in" xr:uid="{58387078-A78B-4059-8DB7-2DA181BAC97F}"/>
+    <hyperlink ref="J48" r:id="rId159" xr:uid="{F61EBA1D-096B-4367-83C7-464D0E0332DE}"/>
+    <hyperlink ref="J51" r:id="rId160" xr:uid="{A7C5CA17-C1E0-4B34-9F67-339F0FC32426}"/>
+    <hyperlink ref="J65" r:id="rId161" display="https://www.linkedin.com/in/mihirmehta-educational-project-and-placements/" xr:uid="{1EF2631D-C319-4F6C-9AF3-9E886A6E863A}"/>
+    <hyperlink ref="J34" r:id="rId162" display="https://www.linkedin.com/in/gaurang-patel-a99266119/" xr:uid="{4A4B2655-5B11-4CEB-8516-A9D046224C31}"/>
+    <hyperlink ref="J75" r:id="rId163" display="http://www.linkedin.com/in/nishant-koshti-52b68b8b" xr:uid="{2E5CF16C-0D7F-4454-B4F7-592A3EC43855}"/>
+    <hyperlink ref="J20" r:id="rId164" display="https://www.linkedin.com/in/brijesh-kundaliya-552b7722/" xr:uid="{FC5C15E0-2AD1-4E2F-8F1E-F2F96829A7A6}"/>
+    <hyperlink ref="J43" r:id="rId165" display="https://www.linkedin.com/in/jalpesh-vasa/" xr:uid="{6768F239-6E23-4A84-8C3E-45670A76F700}"/>
+    <hyperlink ref="J109" r:id="rId166" display="https://www.linkedin.com/in/vaishali-mewada-7a619053/" xr:uid="{DEFB6E16-7F29-44C5-ACAD-D6B1E16E6C24}"/>
+    <hyperlink ref="J46" r:id="rId167" xr:uid="{CCF872D9-BD3F-4521-9093-8C3148DBAC43}"/>
+    <hyperlink ref="J113" r:id="rId168" display="http://www.linkedin.com/in/vijaykumar-panchal-631852280" xr:uid="{2810BDF3-4A14-413D-B157-AF8059E92C49}"/>
+    <hyperlink ref="J64" r:id="rId169" display="https://www.linkedin.com/in/dr-mihir-bhatt-806a85aa/" xr:uid="{AA93D706-7CF6-45C4-B768-B797EB6775B7}"/>
+    <hyperlink ref="J96" r:id="rId170" display="https://www.linkedin.com/in/dr-sagar-chokshi-8646601a/" xr:uid="{35109E28-E96A-4139-B689-0AB43FF55E92}"/>
+    <hyperlink ref="J84" r:id="rId171" display="http://www.linkedin.com/in/pratik-panchal-a35b325a" xr:uid="{6FB924B7-EDB2-44F0-B0D7-E78551105315}"/>
+    <hyperlink ref="J40" r:id="rId172" display="https://www.linkedin.com/in/hemangi-oza-60a189190/" xr:uid="{AC43F6B8-459E-4FF0-82E4-75F8CDE25269}"/>
+    <hyperlink ref="J110" r:id="rId173" display="http://linkedin.com/in/vibha-parmar-81b3045b" xr:uid="{9792CDE9-6059-48ED-AD46-8BECFEF07152}"/>
+    <hyperlink ref="J59" r:id="rId174" display="http://www.linkedin.com/in/maulik-shah-30b483119" xr:uid="{E23FB3E1-55AD-4659-9463-2B3E19FC5E7D}"/>
+    <hyperlink ref="J99" r:id="rId175" display="http://www.linkedin.com/in/saritavisavalia" xr:uid="{3504F31F-4BD3-4D8B-B727-C2FF9DDFF1EA}"/>
+    <hyperlink ref="J13" r:id="rId176" xr:uid="{ACF63811-234F-442B-91D8-C6863212F92A}"/>
+    <hyperlink ref="J45" r:id="rId177" display="https://www.linkedin.com/in/dr-jigar-sarda-00384414/" xr:uid="{0EFC12BA-8B5C-4E86-968D-797B0D43FD98}"/>
+    <hyperlink ref="J105" r:id="rId178" display="https://www.linkedin.com/in/trusha-patel-gajjar" xr:uid="{98AA2D43-F8B2-4B29-93BA-7A9CCA8109B2}"/>
+    <hyperlink ref="J103" r:id="rId179" display="https://www.linkedin.com/in/srushti-gajjar-92b829142?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app" xr:uid="{544D82DB-5386-42AC-B979-94C259CA9E97}"/>
+    <hyperlink ref="J94" r:id="rId180" xr:uid="{F1631FCD-D701-415F-89D8-AB6A7D513AC5}"/>
+    <hyperlink ref="J15" r:id="rId181" display="https://www.linkedin.com/in/asifiqbal-thakor-56949b237/" xr:uid="{3A40B3CD-F1BE-4530-B451-07DF410D1272}"/>
+    <hyperlink ref="J56" r:id="rId182" xr:uid="{99110411-88B4-4B0C-9258-D7E7320C877C}"/>
+    <hyperlink ref="J47" r:id="rId183" display="https://www.linkedin.com/in/jivanadhar-joshi-a76a12ab/" xr:uid="{ED0C7354-C517-49E0-BDF5-C6BF1EC0A53C}"/>
+    <hyperlink ref="J104" r:id="rId184" display="https://in.linkedin.com/in/dr-tigmanshu-patel-b3252639" xr:uid="{8223C32D-E35E-4436-B593-C54F5FEED7DB}"/>
+    <hyperlink ref="J44" r:id="rId185" display="http://linkedin.com/in/jay-bhavsar-a4a9646a" xr:uid="{A3106519-72EE-423E-976E-09F1FD98B248}"/>
+    <hyperlink ref="J89" r:id="rId186" display="http://www.linkedin.com/in/purvi-prajapati-37ba6651" xr:uid="{7A2661BA-3D20-4DF8-8332-CC5726684DD1}"/>
+    <hyperlink ref="J74" r:id="rId187" display="https://www.linkedin.com/in/nirpex-patel-508956119/" xr:uid="{8BF234A3-EF12-4093-8EAF-09B2432506EF}"/>
+    <hyperlink ref="J87" r:id="rId188" display="https://www.linkedin.com/in/priyanka-patel-ph-d-00403393/" xr:uid="{8D6AEC45-7FD5-4128-9D12-F2A6CBB1E864}"/>
+    <hyperlink ref="J63" r:id="rId189" display="https://www.linkedin.com/in/mehulkumar-katakiya-029357b8/" xr:uid="{D058A74D-8E61-413C-9B75-7FF7917660C9}"/>
+    <hyperlink ref="J37" r:id="rId190" display="https://www.linkedin.com/in/harmish-bhatt-88581510a/" xr:uid="{7CC36C27-9781-439B-A945-9C1160C69911}"/>
+    <hyperlink ref="J66" r:id="rId191" display="https://www.linkedin.com/in/mikin-patel-24191386/" xr:uid="{3AEB0F01-575C-4799-B7A0-11A1F0947768}"/>
+    <hyperlink ref="J107" r:id="rId192" display="https://www.linkedin.com/in/dr-upesh-patel-875878138/" xr:uid="{5D7DA379-79C5-410F-9398-20936275BC46}"/>
+    <hyperlink ref="J58" r:id="rId193" xr:uid="{509B130C-6A0C-4944-BFE2-75F1FDF097C4}"/>
+    <hyperlink ref="J69" r:id="rId194" display="https://www.linkedin.com/in/muskan-dave-023197162/" xr:uid="{C8C7BB25-838D-4DFF-B4BD-F8943C06375E}"/>
+    <hyperlink ref="J73" r:id="rId195" display="https://www.linkedin.com/in/dr-nirav-bhatt/" xr:uid="{3F4736BB-5DB7-48E0-ABC4-5DBB591E1122}"/>
+    <hyperlink ref="J11" r:id="rId196" xr:uid="{714022ED-2EC9-40BB-978A-F936135E18E1}"/>
+    <hyperlink ref="J93" r:id="rId197" display="https://www.linkedin.com/in/ritesh-patel-462b0b11" xr:uid="{F4558EEF-FFB0-474A-8E3E-CEBF9566FCDB}"/>
+    <hyperlink ref="J116" r:id="rId198" display="http://www.linkedin.com/in/viral-panara-773877201" xr:uid="{4FB52C9B-4BDB-4971-A78B-1CD2EE789E52}"/>
+    <hyperlink ref="J79" r:id="rId199" display="https://www.linkedin.com/in/shah-parth-d/" xr:uid="{A61E294E-BDA5-4C2E-BA18-BA2B9C98C973}"/>
+    <hyperlink ref="J33" r:id="rId200" display="https://www.linkedin.com/in/gargi-ray-983a8522/" xr:uid="{0C76E47F-7D1B-4E1C-A88F-86156C9D1D6E}"/>
+    <hyperlink ref="J100" r:id="rId201" display="http://www.linkedin.com/in/satayu-travadi-9aab0919" xr:uid="{A79F3F36-387F-427F-848C-3BB8A221E707}"/>
+    <hyperlink ref="J88" r:id="rId202" xr:uid="{A7A467B8-5468-4830-9ADC-34F28E8899B5}"/>
+    <hyperlink ref="J30" r:id="rId203" display="https://www.linkedin.com/in/dheeraj-kumar-shringi-030586107?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app" xr:uid="{D1B60D12-635A-4E71-93D8-B47244D1EF44}"/>
+    <hyperlink ref="J85" r:id="rId204" display="https://in.linkedin.com/in/pratik-mochi-09764b102?original_referer=https%3A%2F%2Fwww.google.com%2F" xr:uid="{CD8066BB-0BA9-4FA9-88DB-0C291F6209A7}"/>
+    <hyperlink ref="J108" r:id="rId205" display="https://www.linkedin.com/in/vaibhavi-patel-67b035224/" xr:uid="{51D509E7-546B-4519-845F-AF5DC77392B9}"/>
+    <hyperlink ref="J60" r:id="rId206" display="http://www.linkedin.com/in/mayuri-popat-213852b1" xr:uid="{336D4B2F-0BBF-4ADA-8647-F20659482547}"/>
+    <hyperlink ref="J55" r:id="rId207" display="http://www.linkedin.com/in/madhavajwalia" xr:uid="{8DE9B663-AD20-42DB-A7F0-4FD167AD95E8}"/>
+    <hyperlink ref="J115" r:id="rId208" display="https://www.linkedin.com/in/vipul-vyas-19214bab/" xr:uid="{00F74D28-7144-4D8C-9870-393AE49126D5}"/>
+    <hyperlink ref="J31" r:id="rId209" display="http://www.linkedin.com/in/dipalkumar-patel-4b97997" xr:uid="{CFB485EB-93AC-436E-BD76-13F13D42FA00}"/>
+    <hyperlink ref="J76" r:id="rId210" display="https://www.linkedin.com/in/nishat-shaikh-b7446019a/" xr:uid="{45535606-CAE7-44BB-B1C5-622D742D5E66}"/>
+    <hyperlink ref="J16" r:id="rId211" display="https://www.linkedin.com/in/avani-khokhariya/" xr:uid="{F2664F6A-73CC-4DAD-982B-E296BD77DF0A}"/>
+    <hyperlink ref="J82" r:id="rId212" xr:uid="{2C60818F-B78B-4EC2-9BA4-C7D88C933280}"/>
+    <hyperlink ref="J25" r:id="rId213" display="https://www.linkedin.com/in/dhara-s-032a6a24/" xr:uid="{4FE7FF63-A73E-4E09-94C4-E2CD5FE6F81D}"/>
+    <hyperlink ref="K72" r:id="rId214" xr:uid="{E7CCB95C-4D9A-474B-9296-0EE719EC4AB3}"/>
+    <hyperlink ref="K92" r:id="rId215" xr:uid="{92D21BA9-793A-4610-9A6A-641322C6CC28}"/>
+    <hyperlink ref="K106" r:id="rId216" xr:uid="{2E05A515-7245-4DDB-9E9C-D041E881E2BF}"/>
+    <hyperlink ref="K86" r:id="rId217" xr:uid="{8C1C3B99-0196-4695-95EB-EEFEEA76042B}"/>
+    <hyperlink ref="K67" r:id="rId218" xr:uid="{4C2AA447-E23D-4BD3-8516-CF8A69E7C676}"/>
+    <hyperlink ref="K90" r:id="rId219" xr:uid="{68D88C01-9035-44B0-9EAE-4AE7236572CC}"/>
+    <hyperlink ref="K98" r:id="rId220" xr:uid="{B89BB500-5F1B-4985-B0B7-D69D9B22538C}"/>
+    <hyperlink ref="K27" r:id="rId221" xr:uid="{461288D1-54CE-41D7-ACBC-4EB753D35618}"/>
+    <hyperlink ref="K64" r:id="rId222" display="https://sites.google.com/a/charusat.ac.in/mihir-bhatt-ee/home/about-me?pli=1" xr:uid="{DD66FE1D-24F8-42A6-8DDC-651F08933CB6}"/>
+    <hyperlink ref="K45" r:id="rId223" xr:uid="{185428FC-1CEB-406E-A327-B537B63CC062}"/>
+    <hyperlink ref="K105" r:id="rId224" xr:uid="{6E3402FB-A293-4394-A12F-C9CE90A43581}"/>
+    <hyperlink ref="K94" r:id="rId225" display="https://sites.google.com/view/ronak-patel/" xr:uid="{30BB4B45-BE3C-4B51-8751-F1166793B9D8}"/>
+    <hyperlink ref="K87" r:id="rId226" display="https://sites.google.com/a/charusat.ac.in/priyanka-patel/about-me" xr:uid="{2F80CF65-0198-4866-9245-0932E2D2E991}"/>
+    <hyperlink ref="K11" r:id="rId227" xr:uid="{B7911887-1D4E-4149-9255-34290DE15C67}"/>
+    <hyperlink ref="K93" r:id="rId228" xr:uid="{CC19190B-EF5A-4030-970E-47B4649A66EC}"/>
+    <hyperlink ref="K79" r:id="rId229" display="http://learnwithparth.in/" xr:uid="{0D098BA1-951E-49B0-BA34-5489DFACFB69}"/>
+    <hyperlink ref="K60" r:id="rId230" display="https://sites.google.com/charusat.ac.in/mayuri-popat/home/academic-experience?authuser=0" xr:uid="{CD111632-8632-4F99-808E-7B0BA423BCF0}"/>
+    <hyperlink ref="K25" r:id="rId231" display="http://https/www.simpldhara.github.io" xr:uid="{1B0FEF49-7DD4-45B9-B1E6-577EDB068225}"/>
+    <hyperlink ref="K4" r:id="rId232" xr:uid="{A55ED677-5A40-43B5-A2E0-3934032012FA}"/>
+    <hyperlink ref="I12" r:id="rId233" xr:uid="{559F5BE6-A98D-4918-9ADE-3B5DB2AC1B24}"/>
+    <hyperlink ref="I13" r:id="rId234" xr:uid="{B5B2A2F7-DD9E-4163-AECE-07D5742E906D}"/>
+    <hyperlink ref="I49" r:id="rId235" xr:uid="{2DF8A589-77D3-487D-9871-F11C086009D1}"/>
+    <hyperlink ref="I82" r:id="rId236" xr:uid="{4F6BB86B-ECFA-4396-9D2B-715AF4C8A22C}"/>
+    <hyperlink ref="I50" r:id="rId237" xr:uid="{C80EDEE3-BA73-444F-89E4-2007846DC254}"/>
+    <hyperlink ref="I90" r:id="rId238" xr:uid="{E27523F8-498C-4ABD-8999-7C5FE36E5CA5}"/>
+    <hyperlink ref="L72" r:id="rId239" xr:uid="{948CADBD-38FA-4A43-B789-35C5FE176C3F}"/>
+    <hyperlink ref="L3" r:id="rId240" xr:uid="{F46A9101-D683-4CCF-9110-8584476B2BA9}"/>
+    <hyperlink ref="L83" r:id="rId241" xr:uid="{6E19F5D8-BA05-4C24-BFED-0131679AE1A3}"/>
+    <hyperlink ref="L57" r:id="rId242" xr:uid="{15D92DD2-9C84-4024-BCB0-89C6EAD615FB}"/>
+    <hyperlink ref="L18" r:id="rId243" xr:uid="{E24865B7-0C5D-46C6-8B52-CB38271DBD7E}"/>
+    <hyperlink ref="L49" r:id="rId244" xr:uid="{4D2C143E-EFF2-43ED-8C1B-94D7326ABF76}"/>
+    <hyperlink ref="L92" r:id="rId245" xr:uid="{22687922-AA0C-441B-A3FA-FB8732C6A78E}"/>
+    <hyperlink ref="L106" r:id="rId246" display="https://scholar.google.com/citations?user=Gzsxo-oAAAAJ&amp;hl=en&amp;oi=ao" xr:uid="{FF9B096B-7991-46C3-B06A-152491BA6C90}"/>
+    <hyperlink ref="L68" r:id="rId247" xr:uid="{690AB285-269F-47C4-BA46-90F767A79CC1}"/>
+    <hyperlink ref="L91" r:id="rId248" xr:uid="{9AF26C9F-30B4-4DAE-A809-C138362FFD00}"/>
+    <hyperlink ref="L95" r:id="rId249" xr:uid="{8D4A0E6E-AA77-4CD4-AA54-DEC95D5CF09E}"/>
+    <hyperlink ref="L50" r:id="rId250" xr:uid="{A64FDC24-6D97-4969-AC20-BF200CE32B3A}"/>
+    <hyperlink ref="L19" r:id="rId251" xr:uid="{2DF7625D-5BDC-4383-BFF5-27331B9E27C1}"/>
+    <hyperlink ref="L71" r:id="rId252" display="https://scholar.google.co.in/citations?user=9PPA-6oAAAAJ&amp;hl=en" xr:uid="{38968AA0-46FD-46B0-84CD-C755BCC30A99}"/>
+    <hyperlink ref="L23" r:id="rId253" xr:uid="{4FF8802A-1D76-4C6B-91B4-17C781B102D6}"/>
+    <hyperlink ref="L52" r:id="rId254" xr:uid="{8365015A-789A-4D2C-9684-352B6CC70A5E}"/>
+    <hyperlink ref="L86" r:id="rId255" xr:uid="{BD03203D-E2A2-453C-8DB9-B1F0B5A13124}"/>
+    <hyperlink ref="L36" r:id="rId256" display="https://scholar.google.com/citations?user=ay8-QY0AAAAJ&amp;hl=en&amp;oi=ao" xr:uid="{CEA8B045-C60C-4ADA-9F10-8B980373388F}"/>
+    <hyperlink ref="L14" r:id="rId257" display="https://scholar.google.com/citations?user=TCsNw-YAAAAJ&amp;hl=en" xr:uid="{D0B58B70-976E-4FD0-A498-4FE5480744DA}"/>
+    <hyperlink ref="L17" r:id="rId258" xr:uid="{19EAA634-8BE7-4A2F-8B30-8A424E254965}"/>
+    <hyperlink ref="L29" r:id="rId259" xr:uid="{3D65CD0F-C15B-4E98-9324-C36FAB47EBC4}"/>
+    <hyperlink ref="L67" r:id="rId260" xr:uid="{264FF3AA-8D89-41E4-9DA6-521BD58711A9}"/>
+    <hyperlink ref="L32" r:id="rId261" display="https://www.bing.com/ck/a?!&amp;&amp;p=6a7ac5a017a1300aJmltdHM9MTcyOTQ2ODgwMCZpZ3VpZD0wMDExMmIyNS1kMzQ5LTY3MTItMmE4My0zZTA1ZDI1NjY2MWEmaW5zaWQ9NTE5NQ&amp;ptn=3&amp;ver=2&amp;hsh=3&amp;fclid=00112b25-d349-6712-2a83-3e05d256661a&amp;psq=google+scholer+gajanan+patange&amp;u=a1aHR0cHM6Ly9zY2hvbGFyLmdvb2dsZS5wbC9jaXRhdGlvbnM_dXNlcj1fRDRISUhjQUFBQUomaGw9ZW4&amp;ntb=1" xr:uid="{275A790E-9657-41D9-B9F2-78D3822C4310}"/>
+    <hyperlink ref="L9" r:id="rId262" xr:uid="{758E6349-E050-42DF-B5C3-FBA97B821030}"/>
+    <hyperlink ref="L114" r:id="rId263" xr:uid="{9ACD46AD-FE8F-41CE-9823-5DC65F691D5B}"/>
+    <hyperlink ref="L4" r:id="rId264" xr:uid="{9B291D90-C0E1-493C-9E5E-17CAF2B7D2F2}"/>
+    <hyperlink ref="L12" r:id="rId265" xr:uid="{8C6729CD-380A-483D-A997-7DBCBA390939}"/>
+    <hyperlink ref="L101" r:id="rId266" xr:uid="{C07AED6D-34B0-40AA-B65E-C9BFB9F1574D}"/>
+    <hyperlink ref="L38" r:id="rId267" display="https://scholar.google.com/citations?user=6d-aVTEAAAAJ&amp;hl=en" xr:uid="{EBC010F8-7D12-4DC1-9FDA-49EFC51EFF71}"/>
+    <hyperlink ref="L21" r:id="rId268" xr:uid="{0DDB7A07-865A-4AD7-986A-DE5D031FFBD0}"/>
+    <hyperlink ref="L28" r:id="rId269" xr:uid="{E6ABE8A4-4EFC-489A-B104-3BCC2E998A7B}"/>
+    <hyperlink ref="L97" r:id="rId270" xr:uid="{ABDCFD31-BA21-4022-B6C1-EDDD441956ED}"/>
+    <hyperlink ref="L6" r:id="rId271" xr:uid="{591DF322-16B2-4785-A83C-3147BF3D09D2}"/>
+    <hyperlink ref="L70" r:id="rId272" xr:uid="{BB403419-C3FE-440B-B0A2-AF35C3C2E8E3}"/>
+    <hyperlink ref="L22" r:id="rId273" xr:uid="{A227399F-9975-4976-9597-2D3E6151DCB8}"/>
+    <hyperlink ref="L39" r:id="rId274" xr:uid="{535A1FEE-65AB-4486-BF0D-ADD9A3382AFB}"/>
+    <hyperlink ref="L42" r:id="rId275" display="https://scholar.google.com/citations?hl=en&amp;user=geQ-r_QAAAAJ" xr:uid="{36509863-135E-43CA-B732-4C0DEFDDC2FC}"/>
+    <hyperlink ref="L102" r:id="rId276" xr:uid="{7F8D3F89-D92D-4081-B489-E387250A10BD}"/>
+    <hyperlink ref="L24" r:id="rId277" xr:uid="{B4A03D8A-649C-469B-B24A-E9F9B481D48B}"/>
+    <hyperlink ref="L26" r:id="rId278" xr:uid="{D3034C74-7237-42E2-A6B8-CD4BA8BBBF41}"/>
+    <hyperlink ref="L90" r:id="rId279" xr:uid="{53AE3D77-EDB3-413A-8D8F-16969CBE8103}"/>
+    <hyperlink ref="L98" r:id="rId280" xr:uid="{76D99C50-072C-40D7-BDEB-328FCCB109D9}"/>
+    <hyperlink ref="L53" r:id="rId281" xr:uid="{CD634DA2-F1A0-45FA-A86C-61D935383D2E}"/>
+    <hyperlink ref="L81" r:id="rId282" xr:uid="{F6874B5E-545B-4745-A546-56B6FD5105E9}"/>
+    <hyperlink ref="L111" r:id="rId283" xr:uid="{C22F05F4-D13D-45A5-A5B0-3237064F3209}"/>
+    <hyperlink ref="L27" r:id="rId284" xr:uid="{32CD251C-92CC-42C2-865F-89BE3026727C}"/>
+    <hyperlink ref="L54" r:id="rId285" xr:uid="{287D782E-D3CC-498E-B117-EBE696C4D447}"/>
+    <hyperlink ref="L41" r:id="rId286" xr:uid="{B241D450-267C-40BF-9C45-8957239BDD86}"/>
+    <hyperlink ref="L62" r:id="rId287" xr:uid="{AA7AD692-35BE-48A4-AF46-1B6413916E3B}"/>
+    <hyperlink ref="L48" r:id="rId288" display="https://scholar.google.co.in/citations?user=EdcH-Y0AAAAJ&amp;hl=en" xr:uid="{CE335172-93AC-45C2-9068-7C9C19F220C4}"/>
+    <hyperlink ref="L10" r:id="rId289" xr:uid="{A33E4A1F-E63E-4F7D-9DC5-3C5AB6E82811}"/>
+    <hyperlink ref="L51" r:id="rId290" xr:uid="{027764B5-CA65-453C-BFB6-EE555AA7BF1B}"/>
+    <hyperlink ref="L61" r:id="rId291" xr:uid="{E2F70942-EACF-4A90-B18A-A80CB466AAE7}"/>
+    <hyperlink ref="L65" r:id="rId292" xr:uid="{5645BFE0-C2D6-4EED-AFCB-0EF806CC91E9}"/>
+    <hyperlink ref="L34" r:id="rId293" xr:uid="{EE598F68-E624-44F6-B4DD-8299C007487F}"/>
+    <hyperlink ref="L75" r:id="rId294" display="https://scholar.google.com/citations?hl=en&amp;authuser=1&amp;user=-9-RhBoAAAAJ" xr:uid="{E935D410-8781-42B6-B609-E835354DEBBB}"/>
+    <hyperlink ref="L5" r:id="rId295" display="https://scholar.google.co.in/citations?user=cVv-kdYAAAAJ&amp;hl=en" xr:uid="{746C1EFC-2FA9-49B1-AFB8-1C7FCA47096B}"/>
+    <hyperlink ref="L20" r:id="rId296" display="https://scholar.google.com/citations?user=dHkQ5D4AAAAJ&amp;hl=en" xr:uid="{25860FE4-2E75-42A8-BFFE-3AA02DEED40F}"/>
+    <hyperlink ref="L43" r:id="rId297" xr:uid="{5A9FF0C8-1A53-40E2-BF07-8AE47CB6B984}"/>
+    <hyperlink ref="L109" r:id="rId298" xr:uid="{5C89C29F-A386-4BBA-9788-4CB223E1744F}"/>
+    <hyperlink ref="L46" r:id="rId299" xr:uid="{63EFEA34-4397-48CB-B385-33D61D726E20}"/>
+    <hyperlink ref="L64" r:id="rId300" xr:uid="{0A4BFD56-8B2D-444E-8903-49F5DC5883A4}"/>
+    <hyperlink ref="L96" r:id="rId301" display="https://scholar.google.com/citations?hl=en&amp;user=utk-ZT0AAAAJ" xr:uid="{501E8FB4-1DC4-4EBD-A3BE-50F19352C1F0}"/>
+    <hyperlink ref="L84" r:id="rId302" xr:uid="{37E9CEEB-DC2C-46A2-BCF4-5A9521147A39}"/>
+    <hyperlink ref="L40" r:id="rId303" xr:uid="{EEF5DC34-1243-4468-B6B1-D9059ADE8AB0}"/>
+    <hyperlink ref="L110" r:id="rId304" display="https://scholar.google.com/citations?view_op=list_works&amp;hl=en&amp;hl=en&amp;user=HDdsZFsAAAAJ&amp;scilu=&amp;scisig=AJY4_hMAAAAAZxidz75RZUbVraeNHOVGYgbAfP0&amp;gmla=ALUCkoUwv9xfR7EENoQtBn_aiKaqTyzZ1X2kORl9--L4aBw5WcKwjoDCVXVaogYeCbraaig0PTa5IzrpT_DyD12Vlt-ODcDk1Nt3fM0&amp;sciund=7577126703303180020" xr:uid="{197DCE6B-BB53-49E3-9D84-78838F524694}"/>
+    <hyperlink ref="L59" r:id="rId305" xr:uid="{B559F61A-BA8D-4A15-AF94-270FD8E6EE0D}"/>
+    <hyperlink ref="L99" r:id="rId306" xr:uid="{BDF263A7-4F8B-46B8-BBE8-705BBF9DE738}"/>
+    <hyperlink ref="L13" r:id="rId307" xr:uid="{7649604F-C033-4670-9F95-0C2C5AC47C84}"/>
+    <hyperlink ref="L45" r:id="rId308" xr:uid="{035221F3-6BA9-41F1-A09D-0FD648704591}"/>
+    <hyperlink ref="L105" r:id="rId309" xr:uid="{1CDECF45-D107-4A0E-A561-5D783437E97C}"/>
+    <hyperlink ref="L103" r:id="rId310" xr:uid="{B653EAA6-C485-435F-854D-438BD267A19D}"/>
+    <hyperlink ref="L94" r:id="rId311" xr:uid="{BAF6ABB2-16F7-4B7A-8AC8-F52F94951E56}"/>
+    <hyperlink ref="L15" r:id="rId312" xr:uid="{F38927F1-EEEB-453A-8636-E6644582D973}"/>
+    <hyperlink ref="L56" r:id="rId313" xr:uid="{9E4C99F0-F427-4B73-88C1-9DDF17D8ABDE}"/>
+    <hyperlink ref="L47" r:id="rId314" xr:uid="{4048416A-0F5D-4582-8A3D-08AFC13874F9}"/>
+    <hyperlink ref="L104" r:id="rId315" xr:uid="{8400FD3C-B4D9-436A-8179-88B2F74CE3F2}"/>
+    <hyperlink ref="L44" r:id="rId316" xr:uid="{201F5259-DE23-43B6-A300-CE6428FFA5ED}"/>
+    <hyperlink ref="L89" r:id="rId317" xr:uid="{31420B66-56AB-4794-90CA-5F5AFEE32FDC}"/>
+    <hyperlink ref="L87" r:id="rId318" xr:uid="{C4F50DBC-0BFE-4509-9E86-8433559B0E5F}"/>
+    <hyperlink ref="L63" r:id="rId319" xr:uid="{90FCCA59-114D-4A5C-9409-D7A92B5C554D}"/>
+    <hyperlink ref="L37" r:id="rId320" xr:uid="{86700D43-54F6-409C-AA74-11A10CF95742}"/>
+    <hyperlink ref="L66" r:id="rId321" xr:uid="{C018FF9B-EED7-4A65-95FA-780ACBBA2D7E}"/>
+    <hyperlink ref="L107" r:id="rId322" xr:uid="{60A89811-803F-44C1-9C4C-03400FFC3370}"/>
+    <hyperlink ref="L58" r:id="rId323" display="https://scholar.google.com/citations?user=D-wd8QgAAAAJ&amp;hl=en" xr:uid="{FEE2843B-8463-42EA-93D3-8C0055A27E1B}"/>
+    <hyperlink ref="L73" r:id="rId324" xr:uid="{D89F1643-F631-4232-BD92-A17AB43537BB}"/>
+    <hyperlink ref="L2" r:id="rId325" xr:uid="{FA588FCD-5B5F-455C-A8F1-363E48BF4B34}"/>
+    <hyperlink ref="L11" r:id="rId326" xr:uid="{75F0D2F4-DBF8-4BC0-81C8-E510EB404F91}"/>
+    <hyperlink ref="L93" r:id="rId327" xr:uid="{4B1641D3-9830-41C6-9804-FD4F1CAA246E}"/>
+    <hyperlink ref="L116" r:id="rId328" xr:uid="{187B270B-DD03-4B4E-A0EC-FA089BBBF941}"/>
+    <hyperlink ref="L79" r:id="rId329" xr:uid="{09000797-9862-4D17-81A3-8BF615CB0D28}"/>
+    <hyperlink ref="L33" r:id="rId330" xr:uid="{30E40F4D-0941-4C35-B988-415178726C05}"/>
+    <hyperlink ref="L100" r:id="rId331" xr:uid="{2A5203BE-43E1-47B8-B2C4-1CC37588A5AB}"/>
+    <hyperlink ref="L88" r:id="rId332" xr:uid="{570C26B0-6EF3-40AB-BBA0-06474B8C9E9F}"/>
+    <hyperlink ref="L30" r:id="rId333" xr:uid="{8315B941-53AD-4CC4-8A93-715BF028D5D6}"/>
+    <hyperlink ref="L85" r:id="rId334" xr:uid="{A11BA51D-FBB4-444E-9239-AD5CA8BDA6AA}"/>
+    <hyperlink ref="L108" r:id="rId335" xr:uid="{BD6653EC-2D4F-4519-B739-A572013209E8}"/>
+    <hyperlink ref="L60" r:id="rId336" xr:uid="{FCDEB08A-0CA4-4598-B598-28FC8001225C}"/>
+    <hyperlink ref="L55" r:id="rId337" xr:uid="{21317881-56A9-411E-B0E0-953DFEB53FB5}"/>
+    <hyperlink ref="L115" r:id="rId338" xr:uid="{2C2ECFF6-DA6C-4C65-B48D-83C8B953A10F}"/>
+    <hyperlink ref="L7" r:id="rId339" xr:uid="{AC52BE48-B1BC-4E71-B6C1-88AF068D6F7B}"/>
+    <hyperlink ref="L31" r:id="rId340" xr:uid="{7701D08D-592D-4F08-8A1D-722D9125A481}"/>
+    <hyperlink ref="L76" r:id="rId341" xr:uid="{08A9DD36-F049-430E-ACEE-0254B9EB019D}"/>
+    <hyperlink ref="L82" r:id="rId342" xr:uid="{69BD5E03-494B-42BC-B711-BD56B50C14BD}"/>
+    <hyperlink ref="L8" r:id="rId343" display="https://scholar.google.com/citations?user=49QO52oAAAAJ&amp;hl=en&amp;citsig=ADIE8snLeq6YPks1Pa9NqbNhY8-8" xr:uid="{597E11F7-5E1F-4746-9B2D-F0B3CE2DAADD}"/>
+    <hyperlink ref="M72" r:id="rId344" display="https://vidwan.inflibnet.ac.in/profile/161243/MTYxMjQz" xr:uid="{377E489A-5F66-4D39-9D16-5A09C06888BF}"/>
+    <hyperlink ref="M3" r:id="rId345" xr:uid="{969CA3F3-003E-45D0-B448-786C1B45A99B}"/>
+    <hyperlink ref="M83" r:id="rId346" xr:uid="{FCF270CA-7E29-44DE-9B34-531A560121D2}"/>
+    <hyperlink ref="M57" r:id="rId347" xr:uid="{27A56F3E-3B7A-497C-B419-6D4EB0B36DFE}"/>
+    <hyperlink ref="M18" r:id="rId348" xr:uid="{A8B03D72-4F58-488B-AA71-6FE545C4F974}"/>
+    <hyperlink ref="M49" r:id="rId349" xr:uid="{46B27430-2CB4-4571-B683-C90BDB1A869A}"/>
+    <hyperlink ref="M92" r:id="rId350" xr:uid="{B3372949-44D6-47D3-93F5-F231A1194C2D}"/>
+    <hyperlink ref="M106" r:id="rId351" xr:uid="{BD564D33-09CC-4E3F-8665-C7CC006586D4}"/>
+    <hyperlink ref="M68" r:id="rId352" xr:uid="{46D7BE4E-C50A-4838-A0D5-A66608E30FB1}"/>
+    <hyperlink ref="M91" r:id="rId353" xr:uid="{49346F82-88CD-458B-9055-E1D237495067}"/>
+    <hyperlink ref="M95" r:id="rId354" xr:uid="{275EA512-D486-4AA6-B9C6-EDFD8EB5E681}"/>
+    <hyperlink ref="M50" r:id="rId355" xr:uid="{F1370FFD-2A24-4E0D-842E-D15A59048874}"/>
+    <hyperlink ref="M19" r:id="rId356" xr:uid="{B079BDCE-9644-48D8-ADB9-55246D89BB3B}"/>
+    <hyperlink ref="M71" r:id="rId357" xr:uid="{21DA9F6E-42F2-4C08-8BCC-45E0F47AC02F}"/>
+    <hyperlink ref="M23" r:id="rId358" display="https://vidwan.inflibnet.ac.in/profile/162290/MTYyMjkw" xr:uid="{C5101B56-8150-4439-9561-ADE65CCB8626}"/>
+    <hyperlink ref="M78" r:id="rId359" xr:uid="{FA23B353-3F9D-46B1-82DA-820AA4FBE86D}"/>
+    <hyperlink ref="M86" r:id="rId360" xr:uid="{680496D4-6792-4688-B37B-3D2836A2CBB1}"/>
+    <hyperlink ref="M36" r:id="rId361" xr:uid="{C295F105-2491-4119-851F-B09A35F5D83B}"/>
+    <hyperlink ref="M14" r:id="rId362" xr:uid="{C6A42F1F-C70B-482C-BAF5-08E29835556D}"/>
+    <hyperlink ref="M80" r:id="rId363" xr:uid="{D12744D8-8D17-44EF-A69E-A1A202FA6698}"/>
+    <hyperlink ref="M17" r:id="rId364" xr:uid="{026E65A7-E47E-491B-A07D-37EBD353FD4E}"/>
+    <hyperlink ref="M35" r:id="rId365" xr:uid="{5D0B8227-026E-47C4-897D-D449D1EA7349}"/>
+    <hyperlink ref="M29" r:id="rId366" xr:uid="{02E7C489-97EB-4764-B304-885B559F8C0E}"/>
+    <hyperlink ref="M67" r:id="rId367" xr:uid="{7BCC998C-8FF9-4866-BDE0-4E618132491D}"/>
+    <hyperlink ref="M9" r:id="rId368" xr:uid="{91B9619A-0474-417B-A83E-F1ACC0AF0CEC}"/>
+    <hyperlink ref="M114" r:id="rId369" xr:uid="{9DC7345F-59EF-46AB-AFF8-A485034FCFB5}"/>
+    <hyperlink ref="M4" r:id="rId370" xr:uid="{C24F8B1B-E131-406E-8B92-980981B7F2F8}"/>
+    <hyperlink ref="M12" r:id="rId371" xr:uid="{BBE0AFF3-0C87-45BA-B244-2EBD516259AE}"/>
+    <hyperlink ref="M101" r:id="rId372" xr:uid="{36A3294C-FBE9-4AE5-B367-A4F7EB299507}"/>
+    <hyperlink ref="M38" r:id="rId373" xr:uid="{CC9655FE-1EDD-46F8-BE5B-9E92C5013680}"/>
+    <hyperlink ref="M21" r:id="rId374" xr:uid="{47BBD086-2D33-4012-A8B6-B4A4E0F676C3}"/>
+    <hyperlink ref="M28" r:id="rId375" xr:uid="{D9812B9F-31E0-4DAD-8A1E-6460EF4BE795}"/>
+    <hyperlink ref="M97" r:id="rId376" xr:uid="{194FE3FD-0EF9-46C4-B769-B4AAF95E0018}"/>
+    <hyperlink ref="M6" r:id="rId377" xr:uid="{3C597F50-A6C7-4686-85A0-F6E6694F57E3}"/>
+    <hyperlink ref="M70" r:id="rId378" xr:uid="{A87D811B-910D-45F2-BF34-A478CD7D8B09}"/>
+    <hyperlink ref="M22" r:id="rId379" xr:uid="{686F19E9-9FDF-4E88-8243-D809ABB3FE79}"/>
+    <hyperlink ref="M42" r:id="rId380" xr:uid="{FB2FC638-1D01-4122-BA7D-9717BC8B2EF3}"/>
+    <hyperlink ref="M102" r:id="rId381" xr:uid="{F0E56AD7-3828-45B1-A3E4-95B4E7B7495F}"/>
+    <hyperlink ref="M24" r:id="rId382" xr:uid="{5E6A27FA-6F1B-4920-AF3A-0018DC331E36}"/>
+    <hyperlink ref="M26" r:id="rId383" xr:uid="{758E2E1D-BBB4-4F0B-A1FA-EB3E5DE2D156}"/>
+    <hyperlink ref="M90" r:id="rId384" xr:uid="{1C320BD2-5251-44A7-81C2-D89E208736CC}"/>
+    <hyperlink ref="M98" r:id="rId385" xr:uid="{4BF3D2D2-9743-494B-A7D1-9EEF7423F2B3}"/>
+    <hyperlink ref="M53" r:id="rId386" xr:uid="{642FC8EF-95E5-4804-8108-73A9ADB45FBB}"/>
+    <hyperlink ref="M81" r:id="rId387" xr:uid="{6069906B-85A1-4520-B697-E8420F4D518A}"/>
+    <hyperlink ref="M111" r:id="rId388" xr:uid="{45C10A27-1AD3-4A6F-966C-946B5F9ECB83}"/>
+    <hyperlink ref="M27" r:id="rId389" xr:uid="{F2CE36A5-3E73-43DE-A91D-5D1E2781384A}"/>
+    <hyperlink ref="M54" r:id="rId390" xr:uid="{6815F862-B01A-4FF2-B310-DDE65D78FBDB}"/>
+    <hyperlink ref="M41" r:id="rId391" xr:uid="{2167CAC5-42F7-48BE-A140-282801D50406}"/>
+    <hyperlink ref="M112" r:id="rId392" xr:uid="{2D0BE123-EDFD-4091-BCF0-204188FF3B30}"/>
+    <hyperlink ref="M62" r:id="rId393" xr:uid="{7A45E352-1CCC-4E30-B5C0-2C2507845C07}"/>
+    <hyperlink ref="M48" r:id="rId394" xr:uid="{D69AB844-8B39-4156-9897-B02CB20CA4D5}"/>
+    <hyperlink ref="M10" r:id="rId395" xr:uid="{04F1C981-8348-4D72-8A69-A692D3062D64}"/>
+    <hyperlink ref="M51" r:id="rId396" xr:uid="{65DE02F5-B84D-45D0-9DC1-F7808BDFD38D}"/>
+    <hyperlink ref="M61" r:id="rId397" xr:uid="{C49314E6-1B8D-41D3-8824-C6AE59F00DDA}"/>
+    <hyperlink ref="M65" r:id="rId398" xr:uid="{22CCAF6F-639B-4091-91C4-0D9E09A79A31}"/>
+    <hyperlink ref="M34" r:id="rId399" xr:uid="{9E6DCF4C-EA31-4D9D-AE0D-50C83C0347DE}"/>
+    <hyperlink ref="M75" r:id="rId400" xr:uid="{D71D3644-6845-46C5-83D7-DA2B52AF5733}"/>
+    <hyperlink ref="M5" r:id="rId401" xr:uid="{7687E521-D8FB-41F5-A5E6-AE953D92E830}"/>
+    <hyperlink ref="M20" r:id="rId402" xr:uid="{4DDDF623-882B-481C-A6D6-41041F349837}"/>
+    <hyperlink ref="M43" r:id="rId403" xr:uid="{52C3C99B-42C3-444C-A194-78CDBDAFC9CB}"/>
+    <hyperlink ref="M109" r:id="rId404" display="https://vidwan.inflibnet.ac.in/profile/161344" xr:uid="{FE2BA8E6-DD6C-4A10-91F1-326AA51E88D5}"/>
+    <hyperlink ref="M46" r:id="rId405" xr:uid="{2FFD071F-CF1A-4200-989A-978DBA72FD44}"/>
+    <hyperlink ref="M64" r:id="rId406" xr:uid="{E4C6C757-CD64-47C7-8F12-6CE6B9FFD60C}"/>
+    <hyperlink ref="M96" r:id="rId407" xr:uid="{722D10A1-25FB-4CE7-9F0B-C75508E442CE}"/>
+    <hyperlink ref="M84" r:id="rId408" xr:uid="{32A836FB-CB40-470F-B02E-7B6392FD539D}"/>
+    <hyperlink ref="M40" r:id="rId409" location="other_information_panel" display="https://vidwan.inflibnet.ac.in/myprofile - other_information_panel" xr:uid="{FE644920-561A-44DA-A700-34ED8EB7963F}"/>
+    <hyperlink ref="M110" r:id="rId410" xr:uid="{2C076003-CA45-4492-A114-A44CC1E60BF2}"/>
+    <hyperlink ref="M59" r:id="rId411" xr:uid="{BC2FF260-09A4-4D46-81FB-823835AD57DA}"/>
+    <hyperlink ref="M99" r:id="rId412" xr:uid="{B2860DA1-1C8E-403D-9E1C-CE3896F91BFD}"/>
+    <hyperlink ref="M13" r:id="rId413" xr:uid="{2DE04985-AB3C-4D4B-BCEE-EF8C728199F4}"/>
+    <hyperlink ref="M45" r:id="rId414" xr:uid="{546046AA-45E7-4EDD-81FB-A6648B9BB595}"/>
+    <hyperlink ref="M105" r:id="rId415" xr:uid="{7330EFFC-2F12-4EFE-BF25-3D30861E8775}"/>
+    <hyperlink ref="M94" r:id="rId416" xr:uid="{4F8D1CF8-D215-443F-8914-E091AFB2DBAE}"/>
+    <hyperlink ref="M15" r:id="rId417" xr:uid="{4CD74FA1-A139-4BCD-9CB7-1D7091E614B9}"/>
+    <hyperlink ref="M56" r:id="rId418" xr:uid="{EAABDC46-8B1B-482C-B7D7-E6E7C16FB647}"/>
+    <hyperlink ref="M104" r:id="rId419" xr:uid="{ACDF2E56-83C7-477F-A573-2B4112936AD3}"/>
+    <hyperlink ref="M44" r:id="rId420" xr:uid="{B502A1CE-A61F-4999-A855-F6ECA908B905}"/>
+    <hyperlink ref="M89" r:id="rId421" xr:uid="{EF82DFB8-BEB4-47BB-B28B-AF5A4CDD6891}"/>
+    <hyperlink ref="M74" r:id="rId422" xr:uid="{6D71EE52-86C9-4EE0-A55D-7B9652B864FF}"/>
+    <hyperlink ref="M87" r:id="rId423" xr:uid="{C073950A-A28A-4ED8-B9C1-BD3B160FAEF3}"/>
+    <hyperlink ref="M63" r:id="rId424" xr:uid="{958C1C19-9C17-41E8-ADC4-BAB91255F382}"/>
+    <hyperlink ref="M37" r:id="rId425" xr:uid="{0CC98B27-C0DC-4F81-A868-5BC7C0784B50}"/>
+    <hyperlink ref="M66" r:id="rId426" xr:uid="{B86191A1-65D6-4540-845F-518E32A64FBF}"/>
+    <hyperlink ref="M107" r:id="rId427" xr:uid="{47889514-AB9C-4B04-95A5-1CCA3A0DFCA8}"/>
+    <hyperlink ref="M58" r:id="rId428" xr:uid="{36AE2A42-0E80-4A5F-8FB0-4EAB2AEA8C36}"/>
+    <hyperlink ref="M69" r:id="rId429" xr:uid="{7FE7C886-2B29-491F-8C86-5526A33F7121}"/>
+    <hyperlink ref="M73" r:id="rId430" xr:uid="{FDFB0EA9-AD4D-43E9-BEF9-C60B9531C82F}"/>
+    <hyperlink ref="M2" r:id="rId431" xr:uid="{251C34E0-B509-4755-B850-FDEB3B770405}"/>
+    <hyperlink ref="M11" r:id="rId432" xr:uid="{3203A1D8-1572-4E08-ADEF-54F74525E87A}"/>
+    <hyperlink ref="M93" r:id="rId433" xr:uid="{28CD01ED-234C-4911-A047-12722FE76C1F}"/>
+    <hyperlink ref="M116" r:id="rId434" xr:uid="{82D93DAC-CF9F-4D41-B8C8-5AE08EA58BAA}"/>
+    <hyperlink ref="M79" r:id="rId435" xr:uid="{68120C28-52E3-4EC9-9F3E-EB5A3578A3BD}"/>
+    <hyperlink ref="M33" r:id="rId436" display="https://vidwan.inflibnet.ac.in/profile/161755-" xr:uid="{B87FE430-1CFA-4F98-A7E4-77FBF96BA37F}"/>
+    <hyperlink ref="M100" r:id="rId437" xr:uid="{649E7EFF-CC71-476F-9A81-1581EC34CD48}"/>
+    <hyperlink ref="M88" r:id="rId438" xr:uid="{1C9375D7-8EF5-40A1-914C-C5A7CD3188FB}"/>
+    <hyperlink ref="M85" r:id="rId439" xr:uid="{66509B53-066F-4635-85A6-6E99D5FE0B3E}"/>
+    <hyperlink ref="M108" r:id="rId440" xr:uid="{775D1521-4736-4C73-BB71-31FD5AD1E561}"/>
+    <hyperlink ref="M60" r:id="rId441" xr:uid="{A128A132-518A-476D-BCF8-6D3638CE18D6}"/>
+    <hyperlink ref="M55" r:id="rId442" xr:uid="{A1AFE28A-9643-4A4A-95E8-53E1C4380AAE}"/>
+    <hyperlink ref="M115" r:id="rId443" xr:uid="{6A1A9D4D-97FF-42A2-B2EA-85F3F7E515C2}"/>
+    <hyperlink ref="M7" r:id="rId444" xr:uid="{BA494279-5FA7-4467-ACAA-FFA1824DB9F7}"/>
+    <hyperlink ref="M31" r:id="rId445" xr:uid="{43BBD922-4BE8-457C-9F25-7684B0D6F35B}"/>
+    <hyperlink ref="M76" r:id="rId446" xr:uid="{C2281EE1-00E4-42D3-875C-3C9C699518DB}"/>
+    <hyperlink ref="M82" r:id="rId447" xr:uid="{3C1D1058-7762-4D63-9FB9-41A44D4AB1F3}"/>
+    <hyperlink ref="E16:E17" r:id="rId448" display="https://placehold.co/400x600" xr:uid="{18BA32A8-6934-421F-9831-28D4907FFF98}"/>
+    <hyperlink ref="E17" r:id="rId449" xr:uid="{7510203D-B2F6-44B8-BB79-8C3F26D4C98A}"/>
+    <hyperlink ref="E16" r:id="rId450" xr:uid="{7C7925F6-A06D-4A2F-A60E-DE952DACBD81}"/>
+    <hyperlink ref="E54" r:id="rId451" xr:uid="{41208DE8-410A-4988-814F-34D6808B3973}"/>
+    <hyperlink ref="E65" r:id="rId452" xr:uid="{2A43A7D2-0D9B-42A8-8E87-E447ECDB9951}"/>
     <hyperlink ref="E60" r:id="rId453" xr:uid="{6FED2870-0657-4424-9493-C87C5558030E}"/>
-    <hyperlink ref="E16" r:id="rId454" xr:uid="{7C7925F6-A06D-4A2F-A60E-DE952DACBD81}"/>
+    <hyperlink ref="E112" r:id="rId454" display="https://placehold.co/400x600" xr:uid="{72604405-579A-4D04-AD70-2F433C2E73DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId455"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Faculty image path updated in excel sheet
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11040E03-D95F-42DF-8913-CF8A97CA1F18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEFFBE3-4932-4796-B960-524E7FDE92F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1008">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1007">
   <si>
     <t>Name</t>
   </si>
@@ -1844,85 +1844,16 @@
     <t>https://placehold.co/400x606</t>
   </si>
   <si>
-    <t>https://placehold.co/400x613</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x617</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x618</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x629</t>
   </si>
   <si>
-    <t>https://placehold.co/400x634</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x639</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x655</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x664</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x665</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x667</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x676</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x680</t>
   </si>
   <si>
-    <t>https://placehold.co/400x681</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x683</t>
   </si>
   <si>
-    <t>https://placehold.co/400x684</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x687</t>
-  </si>
-  <si>
     <t>https://placehold.co/400x689</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x691</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x696</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x697</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x698</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x702</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x703</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x704</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x705</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x708</t>
-  </si>
-  <si>
-    <t>https://placehold.co/400x710</t>
   </si>
   <si>
     <t>https://www.linkedin.com/in/arpitajshah/</t>
@@ -3223,6 +3154,72 @@
   </si>
   <si>
     <t>CSPIT_Faculty\Electronics\ARPITA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\CE\ASIFIQBAL YAVARMIYA THAKOR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\IT\BIMAL HARIVADAN PATEL.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\BRIJESH LAXMANBHAI KUNDALIYA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\HARDIK P MODI.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\MANTHAN SUDHIRBHAI MANAVADARIA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\IT\MIKINKBHAI RAKESHBHAI PATEL.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\MIRAL MUKESHBHAI DESAI.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\CE\MUSKAN CHANDRAKANT DAVE.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\IT\HEMANT NANDLALBHAI YADAV.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\CE\PARMANANDKUMAR SAHDEVBHAI PATEL.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\POONAM.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\IT\PRITESHKUMAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\IT\PURVI.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\CE\RITESH.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\IT\SANKETKUMAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\CE\SARITA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\SATAYU.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\TIGMANSHU.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\CE\TRUSHA.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\TRUSHIT.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\UPESH.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electrical\VIBHABEN.webp</t>
   </si>
 </sst>
 </file>
@@ -3720,8 +3717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="80" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="80" workbookViewId="0">
+      <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3754,7 +3751,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>912</v>
+        <v>889</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -3772,13 +3769,13 @@
         <v>11</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>719</v>
+        <v>696</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>832</v>
+        <v>809</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>911</v>
+        <v>888</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -3795,7 +3792,7 @@
         <v>229</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>936</v>
+        <v>913</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>357</v>
@@ -3810,13 +3807,13 @@
         <v>253</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>915</v>
+        <v>892</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>720</v>
+        <v>697</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>470</v>
@@ -3839,7 +3836,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>976</v>
+        <v>953</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>358</v>
@@ -3854,19 +3851,19 @@
         <v>255</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>916</v>
+        <v>893</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>721</v>
+        <v>698</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>471</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>875</v>
+        <v>852</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -3877,13 +3874,13 @@
         <v>223</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>963</v>
+        <v>940</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>359</v>
@@ -3898,13 +3895,13 @@
         <v>254</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>917</v>
+        <v>894</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>678</v>
+        <v>655</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>722</v>
+        <v>699</v>
       </c>
       <c r="M4" s="9" t="s">
         <v>472</v>
@@ -3927,7 +3924,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>977</v>
+        <v>954</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>360</v>
@@ -3942,13 +3939,13 @@
         <v>256</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>914</v>
+        <v>891</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>723</v>
+        <v>700</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>473</v>
@@ -3971,7 +3968,7 @@
         <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>964</v>
+        <v>941</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>361</v>
@@ -3986,13 +3983,13 @@
         <v>257</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>913</v>
+        <v>890</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>724</v>
+        <v>701</v>
       </c>
       <c r="M6" s="9" t="s">
         <v>474</v>
@@ -4015,7 +4012,7 @@
         <v>230</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>965</v>
+        <v>942</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>362</v>
@@ -4030,19 +4027,19 @@
         <v>259</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>918</v>
+        <v>895</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>725</v>
+        <v>702</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>475</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>876</v>
+        <v>853</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -4074,13 +4071,13 @@
         <v>258</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>919</v>
+        <v>896</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>726</v>
+        <v>703</v>
       </c>
       <c r="M8" s="10" t="s">
         <v>110</v>
@@ -4097,13 +4094,13 @@
         <v>223</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>702</v>
+        <v>679</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>978</v>
+        <v>955</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>364</v>
@@ -4118,19 +4115,19 @@
         <v>260</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>920</v>
+        <v>897</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>727</v>
+        <v>704</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>476</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>877</v>
+        <v>854</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -4147,7 +4144,7 @@
         <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>937</v>
+        <v>914</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>365</v>
@@ -4162,13 +4159,13 @@
         <v>261</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>921</v>
+        <v>898</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>728</v>
+        <v>705</v>
       </c>
       <c r="M10" s="9" t="s">
         <v>477</v>
@@ -4185,16 +4182,16 @@
         <v>223</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>232</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>979</v>
+        <v>956</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>840</v>
+        <v>817</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>110</v>
@@ -4209,10 +4206,10 @@
         <v>104</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>679</v>
+        <v>656</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>729</v>
+        <v>706</v>
       </c>
       <c r="M11" s="9" t="s">
         <v>477</v>
@@ -4235,7 +4232,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>938</v>
+        <v>915</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>366</v>
@@ -4244,25 +4241,25 @@
         <v>110</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>850</v>
+        <v>827</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>711</v>
+        <v>688</v>
       </c>
       <c r="J12" s="9" t="s">
-        <v>590</v>
+        <v>567</v>
       </c>
       <c r="K12" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>730</v>
+        <v>707</v>
       </c>
       <c r="M12" s="9" t="s">
         <v>478</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>878</v>
+        <v>855</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="105.6" x14ac:dyDescent="0.3">
@@ -4279,7 +4276,7 @@
         <v>85</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>1007</v>
+        <v>984</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>367</v>
@@ -4291,7 +4288,7 @@
         <v>462</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>712</v>
+        <v>689</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>104</v>
@@ -4300,13 +4297,13 @@
         <v>110</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>731</v>
+        <v>708</v>
       </c>
       <c r="M13" s="9" t="s">
         <v>477</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>879</v>
+        <v>856</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -4323,7 +4320,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>939</v>
+        <v>916</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>368</v>
@@ -4332,25 +4329,25 @@
         <v>110</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>851</v>
+        <v>828</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>263</v>
       </c>
       <c r="J14" s="9" t="s">
-        <v>591</v>
+        <v>568</v>
       </c>
       <c r="K14" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>732</v>
+        <v>709</v>
       </c>
       <c r="M14" s="9" t="s">
         <v>479</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>880</v>
+        <v>857</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -4361,13 +4358,13 @@
         <v>223</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>90</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>563</v>
+        <v>985</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>369</v>
@@ -4382,13 +4379,13 @@
         <v>264</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>592</v>
+        <v>569</v>
       </c>
       <c r="K15" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>733</v>
+        <v>710</v>
       </c>
       <c r="M15" s="9" t="s">
         <v>480</v>
@@ -4411,7 +4408,7 @@
         <v>233</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>966</v>
+        <v>943</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>370</v>
@@ -4426,7 +4423,7 @@
         <v>265</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>593</v>
+        <v>570</v>
       </c>
       <c r="K16" s="10" t="s">
         <v>110</v>
@@ -4449,22 +4446,22 @@
         <v>223</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>922</v>
+        <v>899</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>841</v>
+        <v>818</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>110</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>852</v>
+        <v>829</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>110</v>
@@ -4476,13 +4473,13 @@
         <v>110</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>734</v>
+        <v>711</v>
       </c>
       <c r="M17" s="9" t="s">
         <v>481</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>881</v>
+        <v>858</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
@@ -4499,7 +4496,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>980</v>
+        <v>957</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>371</v>
@@ -4514,19 +4511,19 @@
         <v>266</v>
       </c>
       <c r="J18" s="9" t="s">
-        <v>594</v>
+        <v>571</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>735</v>
+        <v>712</v>
       </c>
       <c r="M18" s="9" t="s">
         <v>482</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>882</v>
+        <v>859</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -4543,7 +4540,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>564</v>
+        <v>986</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>372</v>
@@ -4558,19 +4555,19 @@
         <v>267</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>595</v>
+        <v>572</v>
       </c>
       <c r="K19" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>736</v>
+        <v>713</v>
       </c>
       <c r="M19" s="9" t="s">
         <v>483</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>883</v>
+        <v>860</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -4587,7 +4584,7 @@
         <v>73</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>565</v>
+        <v>987</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>373</v>
@@ -4602,13 +4599,13 @@
         <v>268</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>596</v>
+        <v>573</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>737</v>
+        <v>714</v>
       </c>
       <c r="M20" s="9" t="s">
         <v>477</v>
@@ -4631,7 +4628,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>967</v>
+        <v>944</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>374</v>
@@ -4646,13 +4643,13 @@
         <v>269</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>597</v>
+        <v>574</v>
       </c>
       <c r="K21" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>738</v>
+        <v>715</v>
       </c>
       <c r="M21" s="9" t="s">
         <v>484</v>
@@ -4675,10 +4672,10 @@
         <v>50</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>981</v>
+        <v>958</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>842</v>
+        <v>819</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>110</v>
@@ -4696,7 +4693,7 @@
         <v>110</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>739</v>
+        <v>716</v>
       </c>
       <c r="M22" s="9" t="s">
         <v>485</v>
@@ -4719,7 +4716,7 @@
         <v>28</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>940</v>
+        <v>917</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>375</v>
@@ -4734,19 +4731,19 @@
         <v>271</v>
       </c>
       <c r="J23" s="9" t="s">
-        <v>598</v>
+        <v>575</v>
       </c>
       <c r="K23" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>740</v>
+        <v>717</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>486</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>884</v>
+        <v>861</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="211.2" x14ac:dyDescent="0.3">
@@ -4757,13 +4754,13 @@
         <v>223</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>982</v>
+        <v>959</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>376</v>
@@ -4778,13 +4775,13 @@
         <v>272</v>
       </c>
       <c r="J24" s="9" t="s">
-        <v>599</v>
+        <v>576</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>741</v>
+        <v>718</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>487</v>
@@ -4807,7 +4804,7 @@
         <v>234</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>968</v>
+        <v>945</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>377</v>
@@ -4819,22 +4816,22 @@
         <v>110</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>713</v>
+        <v>690</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>600</v>
+        <v>577</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>680</v>
+        <v>657</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>742</v>
+        <v>719</v>
       </c>
       <c r="M25" s="10" t="s">
         <v>110</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>885</v>
+        <v>862</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -4851,7 +4848,7 @@
         <v>55</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>983</v>
+        <v>960</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>378</v>
@@ -4860,19 +4857,19 @@
         <v>110</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>853</v>
+        <v>830</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>273</v>
       </c>
       <c r="J26" s="9" t="s">
-        <v>601</v>
+        <v>578</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>681</v>
+        <v>658</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>743</v>
+        <v>720</v>
       </c>
       <c r="M26" s="9" t="s">
         <v>488</v>
@@ -4889,13 +4886,13 @@
         <v>223</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>969</v>
+        <v>946</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>379</v>
@@ -4910,19 +4907,19 @@
         <v>274</v>
       </c>
       <c r="J27" s="9" t="s">
-        <v>602</v>
+        <v>579</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>682</v>
+        <v>659</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>744</v>
+        <v>721</v>
       </c>
       <c r="M27" s="9" t="s">
         <v>489</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>886</v>
+        <v>863</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -4939,7 +4936,7 @@
         <v>46</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>941</v>
+        <v>918</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>380</v>
@@ -4951,22 +4948,22 @@
         <v>110</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>714</v>
+        <v>691</v>
       </c>
       <c r="J28" s="9" t="s">
-        <v>603</v>
+        <v>580</v>
       </c>
       <c r="K28" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>745</v>
+        <v>722</v>
       </c>
       <c r="M28" s="9" t="s">
         <v>478</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>887</v>
+        <v>864</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
@@ -4977,13 +4974,13 @@
         <v>223</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>942</v>
+        <v>919</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>381</v>
@@ -4995,16 +4992,16 @@
         <v>110</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>715</v>
+        <v>692</v>
       </c>
       <c r="J29" s="9" t="s">
-        <v>604</v>
+        <v>581</v>
       </c>
       <c r="K29" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>746</v>
+        <v>723</v>
       </c>
       <c r="M29" s="9" t="s">
         <v>490</v>
@@ -5027,7 +5024,7 @@
         <v>235</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>923</v>
+        <v>900</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>382</v>
@@ -5042,13 +5039,13 @@
         <v>275</v>
       </c>
       <c r="J30" s="9" t="s">
-        <v>605</v>
+        <v>582</v>
       </c>
       <c r="K30" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>747</v>
+        <v>724</v>
       </c>
       <c r="M30" s="17">
         <v>583944</v>
@@ -5071,7 +5068,7 @@
         <v>236</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>383</v>
@@ -5080,19 +5077,19 @@
         <v>110</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>854</v>
+        <v>831</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>276</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>606</v>
+        <v>583</v>
       </c>
       <c r="K31" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>748</v>
+        <v>725</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>491</v>
@@ -5115,7 +5112,7 @@
         <v>39</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>984</v>
+        <v>961</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>384</v>
@@ -5130,16 +5127,16 @@
         <v>277</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>607</v>
+        <v>584</v>
       </c>
       <c r="K32" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>749</v>
+        <v>726</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>829</v>
+        <v>806</v>
       </c>
       <c r="N32" s="10" t="s">
         <v>110</v>
@@ -5159,7 +5156,7 @@
         <v>237</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>952</v>
+        <v>929</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>385</v>
@@ -5174,19 +5171,19 @@
         <v>278</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>608</v>
+        <v>585</v>
       </c>
       <c r="K33" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>750</v>
+        <v>727</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>830</v>
+        <v>807</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>888</v>
+        <v>865</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -5203,7 +5200,7 @@
         <v>70</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>924</v>
+        <v>901</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>386</v>
@@ -5212,19 +5209,19 @@
         <v>110</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>855</v>
+        <v>832</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>279</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>609</v>
+        <v>586</v>
       </c>
       <c r="K34" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>751</v>
+        <v>728</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>492</v>
@@ -5247,7 +5244,7 @@
         <v>35</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>925</v>
+        <v>902</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>387</v>
@@ -5262,7 +5259,7 @@
         <v>280</v>
       </c>
       <c r="J35" s="9" t="s">
-        <v>610</v>
+        <v>587</v>
       </c>
       <c r="K35" s="14" t="s">
         <v>110</v>
@@ -5288,10 +5285,10 @@
         <v>5</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>833</v>
+        <v>810</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>567</v>
+        <v>988</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>388</v>
@@ -5306,19 +5303,19 @@
         <v>281</v>
       </c>
       <c r="J36" s="9" t="s">
-        <v>611</v>
+        <v>588</v>
       </c>
       <c r="K36" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>752</v>
+        <v>729</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>494</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>889</v>
+        <v>866</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -5335,7 +5332,7 @@
         <v>98</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>985</v>
+        <v>962</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>389</v>
@@ -5350,13 +5347,13 @@
         <v>282</v>
       </c>
       <c r="J37" s="9" t="s">
-        <v>612</v>
+        <v>589</v>
       </c>
       <c r="K37" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>753</v>
+        <v>730</v>
       </c>
       <c r="M37" s="9" t="s">
         <v>495</v>
@@ -5373,16 +5370,16 @@
         <v>223</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>970</v>
+        <v>947</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>843</v>
+        <v>820</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>110</v>
@@ -5394,13 +5391,13 @@
         <v>283</v>
       </c>
       <c r="J38" s="9" t="s">
-        <v>613</v>
+        <v>590</v>
       </c>
       <c r="K38" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>754</v>
+        <v>731</v>
       </c>
       <c r="M38" s="9" t="s">
         <v>496</v>
@@ -5417,13 +5414,13 @@
         <v>223</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>971</v>
+        <v>948</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>390</v>
@@ -5438,13 +5435,13 @@
         <v>284</v>
       </c>
       <c r="J39" s="9" t="s">
-        <v>614</v>
+        <v>591</v>
       </c>
       <c r="K39" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>755</v>
+        <v>732</v>
       </c>
       <c r="M39" s="10" t="s">
         <v>110</v>
@@ -5467,7 +5464,7 @@
         <v>81</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>953</v>
+        <v>930</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>391</v>
@@ -5482,13 +5479,13 @@
         <v>110</v>
       </c>
       <c r="J40" s="9" t="s">
-        <v>615</v>
+        <v>592</v>
       </c>
       <c r="K40" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>756</v>
+        <v>733</v>
       </c>
       <c r="M40" s="9" t="s">
         <v>497</v>
@@ -5505,13 +5502,13 @@
         <v>223</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>63</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>568</v>
+        <v>993</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>392</v>
@@ -5520,19 +5517,19 @@
         <v>110</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>856</v>
+        <v>833</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>285</v>
       </c>
       <c r="J41" s="9" t="s">
-        <v>616</v>
+        <v>593</v>
       </c>
       <c r="K41" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>757</v>
+        <v>734</v>
       </c>
       <c r="M41" s="9" t="s">
         <v>498</v>
@@ -5555,7 +5552,7 @@
         <v>52</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>926</v>
+        <v>903</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>393</v>
@@ -5570,13 +5567,13 @@
         <v>286</v>
       </c>
       <c r="J42" s="9" t="s">
-        <v>617</v>
+        <v>594</v>
       </c>
       <c r="K42" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>758</v>
+        <v>735</v>
       </c>
       <c r="M42" s="9" t="s">
         <v>499</v>
@@ -5593,13 +5590,13 @@
         <v>223</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>74</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>955</v>
+        <v>932</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>394</v>
@@ -5614,19 +5611,19 @@
         <v>287</v>
       </c>
       <c r="J43" s="9" t="s">
-        <v>618</v>
+        <v>595</v>
       </c>
       <c r="K43" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>759</v>
+        <v>736</v>
       </c>
       <c r="M43" s="9" t="s">
         <v>500</v>
       </c>
       <c r="N43" s="10" t="s">
-        <v>890</v>
+        <v>867</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -5643,7 +5640,7 @@
         <v>94</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>954</v>
+        <v>931</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>395</v>
@@ -5658,13 +5655,13 @@
         <v>288</v>
       </c>
       <c r="J44" s="9" t="s">
-        <v>619</v>
+        <v>596</v>
       </c>
       <c r="K44" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>760</v>
+        <v>737</v>
       </c>
       <c r="M44" s="9" t="s">
         <v>501</v>
@@ -5687,7 +5684,7 @@
         <v>86</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>972</v>
+        <v>949</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>396</v>
@@ -5702,13 +5699,13 @@
         <v>289</v>
       </c>
       <c r="J45" s="9" t="s">
-        <v>620</v>
+        <v>597</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>683</v>
+        <v>660</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>761</v>
+        <v>738</v>
       </c>
       <c r="M45" s="9" t="s">
         <v>502</v>
@@ -5725,13 +5722,13 @@
         <v>223</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>704</v>
+        <v>681</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>986</v>
+        <v>963</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>397</v>
@@ -5752,7 +5749,7 @@
         <v>110</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>762</v>
+        <v>739</v>
       </c>
       <c r="M46" s="9" t="s">
         <v>503</v>
@@ -5775,7 +5772,7 @@
         <v>92</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>987</v>
+        <v>964</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>398</v>
@@ -5790,13 +5787,13 @@
         <v>291</v>
       </c>
       <c r="J47" s="9" t="s">
-        <v>621</v>
+        <v>598</v>
       </c>
       <c r="K47" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L47" s="9" t="s">
-        <v>763</v>
+        <v>740</v>
       </c>
       <c r="M47" s="10" t="s">
         <v>110</v>
@@ -5819,7 +5816,7 @@
         <v>66</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>988</v>
+        <v>965</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>399</v>
@@ -5840,7 +5837,7 @@
         <v>110</v>
       </c>
       <c r="L48" s="9" t="s">
-        <v>764</v>
+        <v>741</v>
       </c>
       <c r="M48" s="9" t="s">
         <v>477</v>
@@ -5863,7 +5860,7 @@
         <v>20</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>989</v>
+        <v>966</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>400</v>
@@ -5875,22 +5872,22 @@
         <v>110</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>716</v>
+        <v>693</v>
       </c>
       <c r="J49" s="9" t="s">
-        <v>622</v>
+        <v>599</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>684</v>
+        <v>661</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>765</v>
+        <v>742</v>
       </c>
       <c r="M49" s="9" t="s">
         <v>504</v>
       </c>
       <c r="N49" s="10" t="s">
-        <v>891</v>
+        <v>868</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
@@ -5907,7 +5904,7 @@
         <v>26</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>990</v>
+        <v>967</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>401</v>
@@ -5916,25 +5913,25 @@
         <v>110</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>857</v>
+        <v>834</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>293</v>
       </c>
       <c r="J50" s="9" t="s">
-        <v>623</v>
+        <v>600</v>
       </c>
       <c r="K50" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L50" s="9" t="s">
-        <v>766</v>
+        <v>743</v>
       </c>
       <c r="M50" s="9" t="s">
         <v>505</v>
       </c>
       <c r="N50" s="10" t="s">
-        <v>892</v>
+        <v>869</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -5948,10 +5945,10 @@
         <v>5</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>834</v>
+        <v>811</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>991</v>
+        <v>968</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>402</v>
@@ -5960,7 +5957,7 @@
         <v>110</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>858</v>
+        <v>835</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>294</v>
@@ -5972,7 +5969,7 @@
         <v>110</v>
       </c>
       <c r="L51" s="9" t="s">
-        <v>767</v>
+        <v>744</v>
       </c>
       <c r="M51" s="9" t="s">
         <v>477</v>
@@ -5995,7 +5992,7 @@
         <v>30</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>943</v>
+        <v>920</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>403</v>
@@ -6010,13 +6007,13 @@
         <v>295</v>
       </c>
       <c r="J52" s="9" t="s">
-        <v>624</v>
+        <v>601</v>
       </c>
       <c r="K52" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L52" s="9" t="s">
-        <v>768</v>
+        <v>745</v>
       </c>
       <c r="M52" s="10" t="s">
         <v>110</v>
@@ -6039,7 +6036,7 @@
         <v>58</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>992</v>
+        <v>969</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>404</v>
@@ -6054,13 +6051,13 @@
         <v>296</v>
       </c>
       <c r="J53" s="9" t="s">
-        <v>625</v>
+        <v>602</v>
       </c>
       <c r="K53" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L53" s="9" t="s">
-        <v>769</v>
+        <v>746</v>
       </c>
       <c r="M53" s="9" t="s">
         <v>506</v>
@@ -6083,7 +6080,7 @@
         <v>62</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>993</v>
+        <v>970</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>405</v>
@@ -6092,19 +6089,19 @@
         <v>110</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>859</v>
+        <v>836</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>298</v>
       </c>
       <c r="J54" s="9" t="s">
-        <v>626</v>
+        <v>603</v>
       </c>
       <c r="K54" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L54" s="9" t="s">
-        <v>770</v>
+        <v>747</v>
       </c>
       <c r="M54" s="9" t="s">
         <v>507</v>
@@ -6121,13 +6118,13 @@
         <v>223</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>238</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>994</v>
+        <v>971</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>406</v>
@@ -6136,7 +6133,7 @@
         <v>110</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>860</v>
+        <v>837</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>297</v>
@@ -6148,13 +6145,13 @@
         <v>110</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>771</v>
+        <v>748</v>
       </c>
       <c r="M55" s="9" t="s">
         <v>508</v>
       </c>
       <c r="N55" s="10" t="s">
-        <v>893</v>
+        <v>870</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -6165,16 +6162,16 @@
         <v>223</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>704</v>
+        <v>681</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>995</v>
+        <v>972</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>844</v>
+        <v>821</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>110</v>
@@ -6192,7 +6189,7 @@
         <v>110</v>
       </c>
       <c r="L56" s="9" t="s">
-        <v>772</v>
+        <v>749</v>
       </c>
       <c r="M56" s="9" t="s">
         <v>509</v>
@@ -6212,10 +6209,10 @@
         <v>5</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>835</v>
+        <v>812</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>569</v>
+        <v>989</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>407</v>
@@ -6224,25 +6221,25 @@
         <v>110</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>861</v>
+        <v>838</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>300</v>
       </c>
       <c r="J57" s="9" t="s">
-        <v>627</v>
+        <v>604</v>
       </c>
       <c r="K57" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L57" s="9" t="s">
-        <v>773</v>
+        <v>750</v>
       </c>
       <c r="M57" s="9" t="s">
         <v>510</v>
       </c>
       <c r="N57" s="10" t="s">
-        <v>894</v>
+        <v>871</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -6259,7 +6256,7 @@
         <v>239</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>944</v>
+        <v>921</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>408</v>
@@ -6268,19 +6265,19 @@
         <v>110</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>862</v>
+        <v>839</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>301</v>
       </c>
       <c r="J58" s="9" t="s">
-        <v>628</v>
+        <v>605</v>
       </c>
       <c r="K58" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L58" s="9" t="s">
-        <v>774</v>
+        <v>751</v>
       </c>
       <c r="M58" s="9" t="s">
         <v>511</v>
@@ -6297,13 +6294,13 @@
         <v>223</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>702</v>
+        <v>679</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>83</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>927</v>
+        <v>904</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>409</v>
@@ -6312,19 +6309,19 @@
         <v>110</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>863</v>
+        <v>840</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>302</v>
       </c>
       <c r="J59" s="9" t="s">
-        <v>629</v>
+        <v>606</v>
       </c>
       <c r="K59" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L59" s="9" t="s">
-        <v>775</v>
+        <v>752</v>
       </c>
       <c r="M59" s="9" t="s">
         <v>512</v>
@@ -6347,7 +6344,7 @@
         <v>240</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>996</v>
+        <v>973</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>410</v>
@@ -6362,19 +6359,19 @@
         <v>303</v>
       </c>
       <c r="J60" s="9" t="s">
-        <v>630</v>
+        <v>607</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>685</v>
+        <v>662</v>
       </c>
       <c r="L60" s="9" t="s">
-        <v>776</v>
+        <v>753</v>
       </c>
       <c r="M60" s="9" t="s">
         <v>513</v>
       </c>
       <c r="N60" s="10" t="s">
-        <v>895</v>
+        <v>872</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -6391,28 +6388,28 @@
         <v>68</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>997</v>
+        <v>974</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>845</v>
+        <v>822</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>110</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>864</v>
+        <v>841</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>304</v>
       </c>
       <c r="J61" s="10" t="s">
-        <v>631</v>
+        <v>608</v>
       </c>
       <c r="K61" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L61" s="9" t="s">
-        <v>777</v>
+        <v>754</v>
       </c>
       <c r="M61" s="9" t="s">
         <v>514</v>
@@ -6429,13 +6426,13 @@
         <v>223</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>65</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>956</v>
+        <v>933</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>411</v>
@@ -6456,7 +6453,7 @@
         <v>110</v>
       </c>
       <c r="L62" s="9" t="s">
-        <v>778</v>
+        <v>755</v>
       </c>
       <c r="M62" s="9" t="s">
         <v>515</v>
@@ -6476,10 +6473,10 @@
         <v>4</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>836</v>
+        <v>813</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>957</v>
+        <v>934</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>412</v>
@@ -6494,13 +6491,13 @@
         <v>306</v>
       </c>
       <c r="J63" s="9" t="s">
-        <v>632</v>
+        <v>609</v>
       </c>
       <c r="K63" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L63" s="9" t="s">
-        <v>779</v>
+        <v>756</v>
       </c>
       <c r="M63" s="9" t="s">
         <v>516</v>
@@ -6523,7 +6520,7 @@
         <v>78</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>998</v>
+        <v>975</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>413</v>
@@ -6538,19 +6535,19 @@
         <v>307</v>
       </c>
       <c r="J64" s="9" t="s">
-        <v>633</v>
+        <v>610</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>686</v>
+        <v>663</v>
       </c>
       <c r="L64" s="9" t="s">
-        <v>780</v>
+        <v>757</v>
       </c>
       <c r="M64" s="9" t="s">
         <v>477</v>
       </c>
       <c r="N64" s="10" t="s">
-        <v>887</v>
+        <v>864</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
@@ -6561,13 +6558,13 @@
         <v>223</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>705</v>
+        <v>682</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>69</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>999</v>
+        <v>976</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>414</v>
@@ -6576,19 +6573,19 @@
         <v>110</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>865</v>
+        <v>842</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>308</v>
       </c>
       <c r="J65" s="9" t="s">
-        <v>634</v>
+        <v>611</v>
       </c>
       <c r="K65" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L65" s="9" t="s">
-        <v>781</v>
+        <v>758</v>
       </c>
       <c r="M65" s="9" t="s">
         <v>517</v>
@@ -6611,7 +6608,7 @@
         <v>99</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>570</v>
+        <v>990</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>415</v>
@@ -6626,19 +6623,19 @@
         <v>309</v>
       </c>
       <c r="J66" s="9" t="s">
-        <v>635</v>
+        <v>612</v>
       </c>
       <c r="K66" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L66" s="9" t="s">
-        <v>782</v>
+        <v>759</v>
       </c>
       <c r="M66" s="9" t="s">
         <v>518</v>
       </c>
       <c r="N66" s="10" t="s">
-        <v>896</v>
+        <v>873</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="277.2" x14ac:dyDescent="0.3">
@@ -6655,7 +6652,7 @@
         <v>38</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>571</v>
+        <v>991</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>416</v>
@@ -6664,19 +6661,19 @@
         <v>110</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>866</v>
+        <v>843</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>310</v>
       </c>
       <c r="J67" s="9" t="s">
-        <v>636</v>
+        <v>613</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>687</v>
+        <v>664</v>
       </c>
       <c r="L67" s="9" t="s">
-        <v>783</v>
+        <v>760</v>
       </c>
       <c r="M67" s="9" t="s">
         <v>519</v>
@@ -6699,7 +6696,7 @@
         <v>23</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>945</v>
+        <v>922</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>417</v>
@@ -6714,13 +6711,13 @@
         <v>311</v>
       </c>
       <c r="J68" s="9" t="s">
-        <v>637</v>
+        <v>614</v>
       </c>
       <c r="K68" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L68" s="9" t="s">
-        <v>784</v>
+        <v>761</v>
       </c>
       <c r="M68" s="9" t="s">
         <v>520</v>
@@ -6743,7 +6740,7 @@
         <v>241</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>572</v>
+        <v>992</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>418</v>
@@ -6758,7 +6755,7 @@
         <v>312</v>
       </c>
       <c r="J69" s="9" t="s">
-        <v>638</v>
+        <v>615</v>
       </c>
       <c r="K69" s="14" t="s">
         <v>110</v>
@@ -6787,10 +6784,10 @@
         <v>49</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>958</v>
+        <v>935</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>846</v>
+        <v>823</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>110</v>
@@ -6802,19 +6799,19 @@
         <v>313</v>
       </c>
       <c r="J70" s="9" t="s">
-        <v>639</v>
+        <v>616</v>
       </c>
       <c r="K70" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L70" s="9" t="s">
-        <v>785</v>
+        <v>762</v>
       </c>
       <c r="M70" s="9" t="s">
         <v>521</v>
       </c>
       <c r="N70" s="10" t="s">
-        <v>897</v>
+        <v>874</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -6828,10 +6825,10 @@
         <v>5</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>837</v>
+        <v>814</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>946</v>
+        <v>923</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>419</v>
@@ -6846,13 +6843,13 @@
         <v>314</v>
       </c>
       <c r="J71" s="9" t="s">
-        <v>640</v>
+        <v>617</v>
       </c>
       <c r="K71" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L71" s="9" t="s">
-        <v>786</v>
+        <v>763</v>
       </c>
       <c r="M71" s="9" t="s">
         <v>522</v>
@@ -6875,7 +6872,7 @@
         <v>16</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>1000</v>
+        <v>977</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>420</v>
@@ -6884,19 +6881,19 @@
         <v>110</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>867</v>
+        <v>844</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>315</v>
       </c>
       <c r="J72" s="9" t="s">
-        <v>641</v>
+        <v>618</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>688</v>
+        <v>665</v>
       </c>
       <c r="L72" s="9" t="s">
-        <v>787</v>
+        <v>764</v>
       </c>
       <c r="M72" s="9" t="s">
         <v>523</v>
@@ -6919,7 +6916,7 @@
         <v>242</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>928</v>
+        <v>905</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>421</v>
@@ -6928,25 +6925,25 @@
         <v>110</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>868</v>
+        <v>845</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>316</v>
       </c>
       <c r="J73" s="9" t="s">
-        <v>642</v>
+        <v>619</v>
       </c>
       <c r="K73" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L73" s="9" t="s">
-        <v>788</v>
+        <v>765</v>
       </c>
       <c r="M73" s="9" t="s">
         <v>524</v>
       </c>
       <c r="N73" s="10" t="s">
-        <v>898</v>
+        <v>875</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -6963,10 +6960,10 @@
         <v>96</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>959</v>
+        <v>936</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>847</v>
+        <v>824</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>110</v>
@@ -6978,19 +6975,19 @@
         <v>317</v>
       </c>
       <c r="J74" s="9" t="s">
-        <v>643</v>
+        <v>620</v>
       </c>
       <c r="K74" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L74" s="10" t="s">
-        <v>789</v>
+        <v>766</v>
       </c>
       <c r="M74" s="9" t="s">
         <v>525</v>
       </c>
       <c r="N74" s="10" t="s">
-        <v>894</v>
+        <v>871</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -7007,7 +7004,7 @@
         <v>71</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>929</v>
+        <v>906</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>422</v>
@@ -7022,13 +7019,13 @@
         <v>318</v>
       </c>
       <c r="J75" s="9" t="s">
-        <v>644</v>
+        <v>621</v>
       </c>
       <c r="K75" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L75" s="9" t="s">
-        <v>790</v>
+        <v>767</v>
       </c>
       <c r="M75" s="9" t="s">
         <v>477</v>
@@ -7051,7 +7048,7 @@
         <v>243</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>931</v>
+        <v>908</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>423</v>
@@ -7066,19 +7063,19 @@
         <v>319</v>
       </c>
       <c r="J76" s="9" t="s">
-        <v>645</v>
+        <v>622</v>
       </c>
       <c r="K76" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L76" s="9" t="s">
-        <v>791</v>
+        <v>768</v>
       </c>
       <c r="M76" s="9" t="s">
         <v>526</v>
       </c>
       <c r="N76" s="10" t="s">
-        <v>899</v>
+        <v>876</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -7095,7 +7092,7 @@
         <v>37</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>930</v>
+        <v>907</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>424</v>
@@ -7110,7 +7107,7 @@
         <v>320</v>
       </c>
       <c r="J77" s="9" t="s">
-        <v>646</v>
+        <v>623</v>
       </c>
       <c r="K77" s="14" t="s">
         <v>110</v>
@@ -7133,13 +7130,13 @@
         <v>223</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>573</v>
+        <v>994</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>425</v>
@@ -7154,7 +7151,7 @@
         <v>321</v>
       </c>
       <c r="J78" s="9" t="s">
-        <v>647</v>
+        <v>624</v>
       </c>
       <c r="K78" s="10" t="s">
         <v>110</v>
@@ -7180,10 +7177,10 @@
         <v>5</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>838</v>
+        <v>815</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>932</v>
+        <v>909</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>426</v>
@@ -7198,13 +7195,13 @@
         <v>322</v>
       </c>
       <c r="J79" s="9" t="s">
-        <v>648</v>
+        <v>625</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>689</v>
+        <v>666</v>
       </c>
       <c r="L79" s="9" t="s">
-        <v>792</v>
+        <v>769</v>
       </c>
       <c r="M79" s="9" t="s">
         <v>528</v>
@@ -7227,7 +7224,7 @@
         <v>33</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>933</v>
+        <v>910</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>427</v>
@@ -7265,16 +7262,16 @@
         <v>223</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>960</v>
+        <v>937</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>848</v>
+        <v>825</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>110</v>
@@ -7292,13 +7289,13 @@
         <v>110</v>
       </c>
       <c r="L81" s="9" t="s">
-        <v>793</v>
+        <v>770</v>
       </c>
       <c r="M81" s="9" t="s">
         <v>530</v>
       </c>
       <c r="N81" s="10" t="s">
-        <v>900</v>
+        <v>877</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -7309,13 +7306,13 @@
         <v>223</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>706</v>
+        <v>683</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>244</v>
       </c>
       <c r="E82" s="2" t="s">
-        <v>574</v>
+        <v>564</v>
       </c>
       <c r="F82" s="6" t="s">
         <v>428</v>
@@ -7336,7 +7333,7 @@
         <v>110</v>
       </c>
       <c r="L82" s="9" t="s">
-        <v>794</v>
+        <v>771</v>
       </c>
       <c r="M82" s="9" t="s">
         <v>531</v>
@@ -7359,7 +7356,7 @@
         <v>18</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>575</v>
+        <v>995</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>429</v>
@@ -7374,13 +7371,13 @@
         <v>326</v>
       </c>
       <c r="J83" s="9" t="s">
-        <v>649</v>
+        <v>626</v>
       </c>
       <c r="K83" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L83" s="9" t="s">
-        <v>795</v>
+        <v>772</v>
       </c>
       <c r="M83" s="9" t="s">
         <v>532</v>
@@ -7397,13 +7394,13 @@
         <v>223</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>80</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>1001</v>
+        <v>978</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>430</v>
@@ -7418,13 +7415,13 @@
         <v>327</v>
       </c>
       <c r="J84" s="9" t="s">
-        <v>650</v>
+        <v>627</v>
       </c>
       <c r="K84" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L84" s="9" t="s">
-        <v>796</v>
+        <v>773</v>
       </c>
       <c r="M84" s="9" t="s">
         <v>533</v>
@@ -7447,7 +7444,7 @@
         <v>245</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>576</v>
+        <v>565</v>
       </c>
       <c r="F85" s="6" t="s">
         <v>431</v>
@@ -7462,13 +7459,13 @@
         <v>110</v>
       </c>
       <c r="J85" s="9" t="s">
-        <v>651</v>
+        <v>628</v>
       </c>
       <c r="K85" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L85" s="9" t="s">
-        <v>797</v>
+        <v>774</v>
       </c>
       <c r="M85" s="9" t="s">
         <v>534</v>
@@ -7477,7 +7474,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="330" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="343.2" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>192</v>
       </c>
@@ -7491,7 +7488,7 @@
         <v>31</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>577</v>
+        <v>996</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>432</v>
@@ -7509,16 +7506,16 @@
         <v>101</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>690</v>
+        <v>667</v>
       </c>
       <c r="L86" s="9" t="s">
-        <v>798</v>
+        <v>775</v>
       </c>
       <c r="M86" s="9" t="s">
         <v>535</v>
       </c>
       <c r="N86" s="10" t="s">
-        <v>901</v>
+        <v>878</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -7535,7 +7532,7 @@
         <v>97</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>934</v>
+        <v>911</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>433</v>
@@ -7544,25 +7541,25 @@
         <v>110</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>869</v>
+        <v>846</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>329</v>
       </c>
       <c r="J87" s="9" t="s">
-        <v>652</v>
+        <v>629</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>691</v>
+        <v>668</v>
       </c>
       <c r="L87" s="9" t="s">
-        <v>799</v>
+        <v>776</v>
       </c>
       <c r="M87" s="9" t="s">
-        <v>831</v>
+        <v>808</v>
       </c>
       <c r="N87" s="10" t="s">
-        <v>902</v>
+        <v>879</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -7573,13 +7570,13 @@
         <v>223</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>246</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>1002</v>
+        <v>979</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>434</v>
@@ -7600,7 +7597,7 @@
         <v>110</v>
       </c>
       <c r="L88" s="9" t="s">
-        <v>800</v>
+        <v>777</v>
       </c>
       <c r="M88" s="9" t="s">
         <v>536</v>
@@ -7623,7 +7620,7 @@
         <v>95</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>578</v>
+        <v>997</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>435</v>
@@ -7638,13 +7635,13 @@
         <v>331</v>
       </c>
       <c r="J89" s="9" t="s">
-        <v>653</v>
+        <v>630</v>
       </c>
       <c r="K89" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L89" s="9" t="s">
-        <v>801</v>
+        <v>778</v>
       </c>
       <c r="M89" s="9" t="s">
         <v>537</v>
@@ -7667,7 +7664,7 @@
         <v>56</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>1003</v>
+        <v>980</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>436</v>
@@ -7679,22 +7676,22 @@
         <v>110</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>717</v>
+        <v>694</v>
       </c>
       <c r="J90" s="9" t="s">
-        <v>654</v>
+        <v>631</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>692</v>
+        <v>669</v>
       </c>
       <c r="L90" s="9" t="s">
-        <v>802</v>
+        <v>779</v>
       </c>
       <c r="M90" s="9" t="s">
         <v>538</v>
       </c>
       <c r="N90" s="10" t="s">
-        <v>903</v>
+        <v>880</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -7711,7 +7708,7 @@
         <v>24</v>
       </c>
       <c r="E91" s="2" t="s">
-        <v>579</v>
+        <v>566</v>
       </c>
       <c r="F91" s="6" t="s">
         <v>437</v>
@@ -7720,19 +7717,19 @@
         <v>110</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>870</v>
+        <v>847</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>332</v>
       </c>
       <c r="J91" s="9" t="s">
-        <v>655</v>
+        <v>632</v>
       </c>
       <c r="K91" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L91" s="9" t="s">
-        <v>803</v>
+        <v>780</v>
       </c>
       <c r="M91" s="9" t="s">
         <v>539</v>
@@ -7755,7 +7752,7 @@
         <v>21</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>947</v>
+        <v>924</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>438</v>
@@ -7770,13 +7767,13 @@
         <v>333</v>
       </c>
       <c r="J92" s="9" t="s">
-        <v>656</v>
+        <v>633</v>
       </c>
       <c r="K92" s="9" t="s">
-        <v>693</v>
+        <v>670</v>
       </c>
       <c r="L92" s="9" t="s">
-        <v>804</v>
+        <v>781</v>
       </c>
       <c r="M92" s="9" t="s">
         <v>540</v>
@@ -7799,7 +7796,7 @@
         <v>247</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>580</v>
+        <v>998</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>439</v>
@@ -7808,25 +7805,25 @@
         <v>110</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>871</v>
+        <v>848</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>334</v>
       </c>
       <c r="J93" s="9" t="s">
-        <v>657</v>
+        <v>634</v>
       </c>
       <c r="K93" s="9" t="s">
-        <v>694</v>
+        <v>671</v>
       </c>
       <c r="L93" s="9" t="s">
-        <v>805</v>
+        <v>782</v>
       </c>
       <c r="M93" s="9" t="s">
         <v>541</v>
       </c>
       <c r="N93" s="10" t="s">
-        <v>904</v>
+        <v>881</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
@@ -7843,7 +7840,7 @@
         <v>89</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>948</v>
+        <v>925</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>440</v>
@@ -7861,10 +7858,10 @@
         <v>108</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>695</v>
+        <v>672</v>
       </c>
       <c r="L94" s="9" t="s">
-        <v>806</v>
+        <v>783</v>
       </c>
       <c r="M94" s="9" t="s">
         <v>542</v>
@@ -7887,7 +7884,7 @@
         <v>25</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>949</v>
+        <v>926</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>441</v>
@@ -7902,19 +7899,19 @@
         <v>336</v>
       </c>
       <c r="J95" s="9" t="s">
-        <v>658</v>
+        <v>635</v>
       </c>
       <c r="K95" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L95" s="9" t="s">
-        <v>807</v>
+        <v>784</v>
       </c>
       <c r="M95" s="9" t="s">
         <v>543</v>
       </c>
       <c r="N95" s="10" t="s">
-        <v>905</v>
+        <v>882</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -7931,7 +7928,7 @@
         <v>79</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>1004</v>
+        <v>981</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>442</v>
@@ -7940,25 +7937,25 @@
         <v>110</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>872</v>
+        <v>849</v>
       </c>
       <c r="I96" s="4" t="s">
         <v>337</v>
       </c>
       <c r="J96" s="9" t="s">
-        <v>659</v>
+        <v>636</v>
       </c>
       <c r="K96" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L96" s="9" t="s">
-        <v>808</v>
+        <v>785</v>
       </c>
       <c r="M96" s="9" t="s">
         <v>544</v>
       </c>
       <c r="N96" s="10" t="s">
-        <v>906</v>
+        <v>883</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -7975,7 +7972,7 @@
         <v>47</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>1004</v>
+        <v>981</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>443</v>
@@ -7984,25 +7981,25 @@
         <v>110</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>873</v>
+        <v>850</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>338</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>660</v>
+        <v>637</v>
       </c>
       <c r="K97" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L97" s="9" t="s">
-        <v>809</v>
+        <v>786</v>
       </c>
       <c r="M97" s="9" t="s">
         <v>545</v>
       </c>
       <c r="N97" s="10" t="s">
-        <v>894</v>
+        <v>871</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -8019,7 +8016,7 @@
         <v>57</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>581</v>
+        <v>999</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>444</v>
@@ -8034,19 +8031,19 @@
         <v>339</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>661</v>
+        <v>638</v>
       </c>
       <c r="K98" s="9" t="s">
-        <v>696</v>
+        <v>673</v>
       </c>
       <c r="L98" s="9" t="s">
-        <v>810</v>
+        <v>787</v>
       </c>
       <c r="M98" s="9" t="s">
         <v>546</v>
       </c>
       <c r="N98" s="10" t="s">
-        <v>907</v>
+        <v>884</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -8057,13 +8054,13 @@
         <v>223</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>582</v>
+        <v>1000</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>445</v>
@@ -8084,7 +8081,7 @@
         <v>110</v>
       </c>
       <c r="L99" s="9" t="s">
-        <v>811</v>
+        <v>788</v>
       </c>
       <c r="M99" s="9" t="s">
         <v>547</v>
@@ -8101,13 +8098,13 @@
         <v>223</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>248</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>583</v>
+        <v>1001</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>446</v>
@@ -8122,13 +8119,13 @@
         <v>341</v>
       </c>
       <c r="J100" s="9" t="s">
-        <v>662</v>
+        <v>639</v>
       </c>
       <c r="K100" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L100" s="9" t="s">
-        <v>812</v>
+        <v>789</v>
       </c>
       <c r="M100" s="9" t="s">
         <v>548</v>
@@ -8151,7 +8148,7 @@
         <v>43</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>950</v>
+        <v>927</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>447</v>
@@ -8166,13 +8163,13 @@
         <v>342</v>
       </c>
       <c r="J101" s="9" t="s">
-        <v>663</v>
+        <v>640</v>
       </c>
       <c r="K101" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L101" s="9" t="s">
-        <v>813</v>
+        <v>790</v>
       </c>
       <c r="M101" s="9" t="s">
         <v>549</v>
@@ -8189,13 +8186,13 @@
         <v>223</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>707</v>
+        <v>684</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>935</v>
+        <v>912</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>448</v>
@@ -8210,13 +8207,13 @@
         <v>343</v>
       </c>
       <c r="J102" s="9" t="s">
-        <v>664</v>
+        <v>641</v>
       </c>
       <c r="K102" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L102" s="9" t="s">
-        <v>814</v>
+        <v>791</v>
       </c>
       <c r="M102" s="9" t="s">
         <v>550</v>
@@ -8239,7 +8236,7 @@
         <v>88</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>973</v>
+        <v>950</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>449</v>
@@ -8254,13 +8251,13 @@
         <v>344</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>665</v>
+        <v>642</v>
       </c>
       <c r="K103" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L103" s="9" t="s">
-        <v>815</v>
+        <v>792</v>
       </c>
       <c r="M103" s="10" t="s">
         <v>110</v>
@@ -8277,13 +8274,13 @@
         <v>223</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>708</v>
+        <v>685</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>584</v>
+        <v>1002</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>450</v>
@@ -8298,13 +8295,13 @@
         <v>110</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>666</v>
+        <v>643</v>
       </c>
       <c r="K104" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L104" s="9" t="s">
-        <v>816</v>
+        <v>793</v>
       </c>
       <c r="M104" s="9" t="s">
         <v>551</v>
@@ -8321,13 +8318,13 @@
         <v>223</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>585</v>
+        <v>1003</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>451</v>
@@ -8342,13 +8339,13 @@
         <v>345</v>
       </c>
       <c r="J105" s="9" t="s">
-        <v>667</v>
+        <v>644</v>
       </c>
       <c r="K105" s="9" t="s">
-        <v>697</v>
+        <v>674</v>
       </c>
       <c r="L105" s="9" t="s">
-        <v>817</v>
+        <v>794</v>
       </c>
       <c r="M105" s="9" t="s">
         <v>552</v>
@@ -8371,7 +8368,7 @@
         <v>22</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>586</v>
+        <v>1004</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>452</v>
@@ -8389,10 +8386,10 @@
         <v>100</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>698</v>
+        <v>675</v>
       </c>
       <c r="L106" s="9" t="s">
-        <v>818</v>
+        <v>795</v>
       </c>
       <c r="M106" s="9" t="s">
         <v>553</v>
@@ -8415,7 +8412,7 @@
         <v>249</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>587</v>
+        <v>1005</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>453</v>
@@ -8430,19 +8427,19 @@
         <v>347</v>
       </c>
       <c r="J107" s="9" t="s">
-        <v>668</v>
+        <v>645</v>
       </c>
       <c r="K107" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L107" s="9" t="s">
-        <v>819</v>
+        <v>796</v>
       </c>
       <c r="M107" s="9" t="s">
         <v>554</v>
       </c>
       <c r="N107" s="10" t="s">
-        <v>908</v>
+        <v>885</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -8459,7 +8456,7 @@
         <v>250</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>974</v>
+        <v>951</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>454</v>
@@ -8474,13 +8471,13 @@
         <v>348</v>
       </c>
       <c r="J108" s="9" t="s">
-        <v>669</v>
+        <v>646</v>
       </c>
       <c r="K108" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L108" s="9" t="s">
-        <v>820</v>
+        <v>797</v>
       </c>
       <c r="M108" s="9" t="s">
         <v>555</v>
@@ -8503,7 +8500,7 @@
         <v>75</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>951</v>
+        <v>928</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>75</v>
@@ -8518,13 +8515,13 @@
         <v>349</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>670</v>
+        <v>647</v>
       </c>
       <c r="K109" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L109" s="9" t="s">
-        <v>821</v>
+        <v>798</v>
       </c>
       <c r="M109" s="9" t="s">
         <v>556</v>
@@ -8541,13 +8538,13 @@
         <v>223</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>709</v>
+        <v>686</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>588</v>
+        <v>1006</v>
       </c>
       <c r="F110" s="6" t="s">
         <v>455</v>
@@ -8562,19 +8559,19 @@
         <v>350</v>
       </c>
       <c r="J110" s="9" t="s">
-        <v>671</v>
+        <v>648</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>699</v>
+        <v>676</v>
       </c>
       <c r="L110" s="9" t="s">
-        <v>822</v>
+        <v>799</v>
       </c>
       <c r="M110" s="9" t="s">
         <v>557</v>
       </c>
       <c r="N110" s="10" t="s">
-        <v>909</v>
+        <v>886</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -8585,13 +8582,13 @@
         <v>223</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>701</v>
+        <v>678</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>975</v>
+        <v>952</v>
       </c>
       <c r="F111" s="6" t="s">
         <v>456</v>
@@ -8606,13 +8603,13 @@
         <v>351</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>672</v>
+        <v>649</v>
       </c>
       <c r="K111" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L111" s="9" t="s">
-        <v>823</v>
+        <v>800</v>
       </c>
       <c r="M111" s="9" t="s">
         <v>558</v>
@@ -8635,7 +8632,7 @@
         <v>64</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>589</v>
+        <v>938</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>457</v>
@@ -8644,19 +8641,19 @@
         <v>110</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>874</v>
+        <v>851</v>
       </c>
       <c r="I112" s="4" t="s">
         <v>352</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>673</v>
+        <v>650</v>
       </c>
       <c r="K112" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L112" s="10" t="s">
-        <v>824</v>
+        <v>801</v>
       </c>
       <c r="M112" s="9" t="s">
         <v>559</v>
@@ -8679,7 +8676,7 @@
         <v>77</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>961</v>
+        <v>938</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>458</v>
@@ -8694,19 +8691,19 @@
         <v>353</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>674</v>
+        <v>651</v>
       </c>
       <c r="K113" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L113" s="10" t="s">
-        <v>825</v>
+        <v>802</v>
       </c>
       <c r="M113" s="17" t="s">
         <v>559</v>
       </c>
       <c r="N113" s="10" t="s">
-        <v>910</v>
+        <v>887</v>
       </c>
     </row>
     <row r="114" spans="1:14" ht="184.8" x14ac:dyDescent="0.3">
@@ -8717,13 +8714,13 @@
         <v>223</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>1005</v>
+        <v>982</v>
       </c>
       <c r="F114" s="6" t="s">
         <v>459</v>
@@ -8738,13 +8735,13 @@
         <v>354</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>675</v>
+        <v>652</v>
       </c>
       <c r="K114" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L114" s="9" t="s">
-        <v>826</v>
+        <v>803</v>
       </c>
       <c r="M114" s="9" t="s">
         <v>560</v>
@@ -8761,16 +8758,16 @@
         <v>223</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>703</v>
+        <v>680</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>251</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>962</v>
+        <v>939</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>849</v>
+        <v>826</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>110</v>
@@ -8782,13 +8779,13 @@
         <v>355</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>676</v>
+        <v>653</v>
       </c>
       <c r="K115" s="10" t="s">
         <v>111</v>
       </c>
       <c r="L115" s="9" t="s">
-        <v>827</v>
+        <v>804</v>
       </c>
       <c r="M115" s="9" t="s">
         <v>477</v>
@@ -8805,13 +8802,13 @@
         <v>223</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>702</v>
+        <v>679</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>252</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>1006</v>
+        <v>983</v>
       </c>
       <c r="F116" s="6" t="s">
         <v>460</v>
@@ -8826,13 +8823,13 @@
         <v>356</v>
       </c>
       <c r="J116" s="9" t="s">
-        <v>677</v>
+        <v>654</v>
       </c>
       <c r="K116" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L116" s="9" t="s">
-        <v>828</v>
+        <v>805</v>
       </c>
       <c r="M116" s="9" t="s">
         <v>561</v>
@@ -8843,16 +8840,16 @@
     </row>
     <row r="117" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A117" s="16" t="s">
-        <v>700</v>
+        <v>677</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>223</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>710</v>
+        <v>687</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>839</v>
+        <v>816</v>
       </c>
       <c r="F117" s="16" t="s">
         <v>110</v>
@@ -8861,7 +8858,7 @@
         <v>110</v>
       </c>
       <c r="I117" s="16" t="s">
-        <v>718</v>
+        <v>695</v>
       </c>
       <c r="J117" s="11" t="s">
         <v>110</v>
@@ -8891,7 +8888,7 @@
     <hyperlink ref="E12" r:id="rId7" xr:uid="{17D5C088-BD3A-4E75-8035-22B027942A64}"/>
     <hyperlink ref="E14" r:id="rId8" xr:uid="{6815D31E-1624-40E4-AD43-8FB5276A3E13}"/>
     <hyperlink ref="E18" r:id="rId9" xr:uid="{D37B5237-F7AD-4C72-A4B8-18846345A20A}"/>
-    <hyperlink ref="E20" r:id="rId10" display="https://placehold.co/400x600" xr:uid="{455E2F96-6FCE-4ED2-9C3B-2E6E7249AE44}"/>
+    <hyperlink ref="E20" r:id="rId10" xr:uid="{455E2F96-6FCE-4ED2-9C3B-2E6E7249AE44}"/>
     <hyperlink ref="E22" r:id="rId11" xr:uid="{77807312-4DCC-424A-9227-0205668D168B}"/>
     <hyperlink ref="E24" r:id="rId12" xr:uid="{8AAD6443-2520-4082-8EC0-C46B0A509927}"/>
     <hyperlink ref="E26" r:id="rId13" xr:uid="{5B8C9469-79CD-4130-A71A-FB9845883315}"/>
@@ -8899,7 +8896,7 @@
     <hyperlink ref="E30" r:id="rId15" xr:uid="{3C06105A-95B0-486E-B562-804FA49B279E}"/>
     <hyperlink ref="E32" r:id="rId16" xr:uid="{445C6875-08FB-4A0D-945E-88ACC5B3E36F}"/>
     <hyperlink ref="E34" r:id="rId17" xr:uid="{65D66EC6-EE19-4700-A25B-1483B78EB1EF}"/>
-    <hyperlink ref="E36" r:id="rId18" display="https://placehold.co/400x600" xr:uid="{2E844F72-E0A3-4D15-89E8-4C62C40B0097}"/>
+    <hyperlink ref="E36" r:id="rId18" xr:uid="{2E844F72-E0A3-4D15-89E8-4C62C40B0097}"/>
     <hyperlink ref="E38" r:id="rId19" xr:uid="{15AC029B-EF8F-4E8F-BB97-C5EC917FD18C}"/>
     <hyperlink ref="E40" r:id="rId20" xr:uid="{5FE82AD6-8780-451F-B565-3C9E2036135F}"/>
     <hyperlink ref="E42" r:id="rId21" xr:uid="{F7983BF9-576C-4FA2-B35A-DFA749ACF1B5}"/>
@@ -8912,29 +8909,29 @@
     <hyperlink ref="E58" r:id="rId28" xr:uid="{DDB2A0FD-936A-490E-BE1E-1762A651B20C}"/>
     <hyperlink ref="E62" r:id="rId29" xr:uid="{5E732335-693B-490D-844A-64351A2B11C7}"/>
     <hyperlink ref="E64" r:id="rId30" xr:uid="{B032BBB6-4D16-4E33-A3F0-D7039E10D767}"/>
-    <hyperlink ref="E66" r:id="rId31" display="https://placehold.co/400x600" xr:uid="{C71F9231-ACA2-46E1-BE2F-462475789CDA}"/>
+    <hyperlink ref="E66" r:id="rId31" xr:uid="{C71F9231-ACA2-46E1-BE2F-462475789CDA}"/>
     <hyperlink ref="E68" r:id="rId32" xr:uid="{6DAF2527-3F52-4351-90EE-F788A7836287}"/>
     <hyperlink ref="E70" r:id="rId33" xr:uid="{C213B07F-FB90-4578-BA40-CB5277C5E9F8}"/>
     <hyperlink ref="E72" r:id="rId34" xr:uid="{B6B3C0BC-449F-4D5F-8991-2960BC1E1B95}"/>
     <hyperlink ref="E74" r:id="rId35" xr:uid="{12F3E568-1027-43BC-89EA-C5D4D2C3F3B1}"/>
     <hyperlink ref="E76" r:id="rId36" xr:uid="{9BCFDA15-C8D8-41F6-B5C1-8DB9E3F54F38}"/>
-    <hyperlink ref="E78" r:id="rId37" display="https://placehold.co/400x600" xr:uid="{5074351A-0735-4679-AE99-F1F491EAD66F}"/>
+    <hyperlink ref="E78" r:id="rId37" xr:uid="{5074351A-0735-4679-AE99-F1F491EAD66F}"/>
     <hyperlink ref="E80" r:id="rId38" xr:uid="{797A27FB-9286-43BA-A3D3-06E0B7DF57C7}"/>
     <hyperlink ref="E82" r:id="rId39" display="https://placehold.co/400x600" xr:uid="{E22D4C78-609C-4F6C-902E-67DDEA2AEC08}"/>
     <hyperlink ref="E84" r:id="rId40" xr:uid="{689543FA-D772-478F-B75B-353A8D5F5A0F}"/>
-    <hyperlink ref="E86" r:id="rId41" display="https://placehold.co/400x600" xr:uid="{6F1B4F40-1347-45F9-B0B9-89687F77E0B0}"/>
+    <hyperlink ref="E86" r:id="rId41" xr:uid="{6F1B4F40-1347-45F9-B0B9-89687F77E0B0}"/>
     <hyperlink ref="E88" r:id="rId42" xr:uid="{269A95A2-A318-4245-8364-07E925D041A6}"/>
     <hyperlink ref="E90" r:id="rId43" xr:uid="{BC5C79FD-42B9-4F63-B259-53ADA917C149}"/>
     <hyperlink ref="E92" r:id="rId44" xr:uid="{F219C840-96AC-40EA-9D7B-C09CBA360D2A}"/>
     <hyperlink ref="E94" r:id="rId45" xr:uid="{E85B62E0-66A6-4BDE-AB82-B3F3885FF25D}"/>
     <hyperlink ref="E96" r:id="rId46" xr:uid="{F685C903-F46A-4AEA-A4B6-30F5F5C38E02}"/>
-    <hyperlink ref="E98" r:id="rId47" display="https://placehold.co/400x600" xr:uid="{34A32507-5178-4AE2-8923-C76F8834EAC3}"/>
-    <hyperlink ref="E100" r:id="rId48" display="https://placehold.co/400x600" xr:uid="{316F114E-DC59-4C12-AAE4-7C561A6A4A37}"/>
+    <hyperlink ref="E98" r:id="rId47" xr:uid="{34A32507-5178-4AE2-8923-C76F8834EAC3}"/>
+    <hyperlink ref="E100" r:id="rId48" xr:uid="{316F114E-DC59-4C12-AAE4-7C561A6A4A37}"/>
     <hyperlink ref="E102" r:id="rId49" xr:uid="{E6C4E1E9-ADFC-463C-BA35-72BF5470C0FC}"/>
-    <hyperlink ref="E104" r:id="rId50" display="https://placehold.co/400x600" xr:uid="{5C2E1F62-17AE-4C61-86CF-CFAADD48E3DA}"/>
-    <hyperlink ref="E106" r:id="rId51" display="https://placehold.co/400x600" xr:uid="{EB2D28AA-5611-4D14-B6D8-65655568052B}"/>
+    <hyperlink ref="E104" r:id="rId50" xr:uid="{5C2E1F62-17AE-4C61-86CF-CFAADD48E3DA}"/>
+    <hyperlink ref="E106" r:id="rId51" xr:uid="{EB2D28AA-5611-4D14-B6D8-65655568052B}"/>
     <hyperlink ref="E108" r:id="rId52" xr:uid="{1A1FF6C3-6CA4-4205-87F4-FFA4C505FE05}"/>
-    <hyperlink ref="E110" r:id="rId53" display="https://placehold.co/400x600" xr:uid="{D5F8DE7D-9A2E-4EB2-AD3E-1B6347BBB03A}"/>
+    <hyperlink ref="E110" r:id="rId53" xr:uid="{D5F8DE7D-9A2E-4EB2-AD3E-1B6347BBB03A}"/>
     <hyperlink ref="E114" r:id="rId54" xr:uid="{F52A7ADE-923C-4FC0-835C-C78BE5475FD1}"/>
     <hyperlink ref="E116" r:id="rId55" xr:uid="{88BB9B9A-193B-430A-8A94-9996D9F8B858}"/>
     <hyperlink ref="E5" r:id="rId56" xr:uid="{673B2D9E-5CEE-40DD-A0A2-66025584E8C2}"/>
@@ -8942,8 +8939,8 @@
     <hyperlink ref="E9" r:id="rId58" xr:uid="{E7773CE7-BD5F-4624-B940-0E795B4A4E30}"/>
     <hyperlink ref="E11" r:id="rId59" xr:uid="{93DA058C-7CEC-4BA2-9D33-5FB8B5E88910}"/>
     <hyperlink ref="E13" r:id="rId60" xr:uid="{8F788626-64E7-4F1D-A12D-F2E9D916467C}"/>
-    <hyperlink ref="E15" r:id="rId61" display="https://placehold.co/400x600" xr:uid="{8AD2972F-0CB2-4DCE-8821-C56F9057AD5B}"/>
-    <hyperlink ref="E19" r:id="rId62" display="https://placehold.co/400x600" xr:uid="{D4698768-8DC5-407A-B6F4-C1C875BFB78D}"/>
+    <hyperlink ref="E15" r:id="rId61" xr:uid="{8AD2972F-0CB2-4DCE-8821-C56F9057AD5B}"/>
+    <hyperlink ref="E19" r:id="rId62" xr:uid="{D4698768-8DC5-407A-B6F4-C1C875BFB78D}"/>
     <hyperlink ref="E21" r:id="rId63" xr:uid="{13DD67BA-1FCB-43E0-A39C-FFE32E5D3954}"/>
     <hyperlink ref="E23" r:id="rId64" xr:uid="{90D0F56C-C7DB-4632-B91C-EF74541F5FEA}"/>
     <hyperlink ref="E25" r:id="rId65" xr:uid="{F6A0C9FE-D2B9-4181-8F81-93868F3E313C}"/>
@@ -8954,7 +8951,7 @@
     <hyperlink ref="E35" r:id="rId70" xr:uid="{FFD57A2F-B179-4903-B296-F8069D1F1332}"/>
     <hyperlink ref="E37" r:id="rId71" xr:uid="{291A37C6-A686-4CDE-9352-CAE725E23B11}"/>
     <hyperlink ref="E39" r:id="rId72" xr:uid="{6ECECF25-2624-4D12-A089-9B4C4DBCF38B}"/>
-    <hyperlink ref="E41" r:id="rId73" display="https://placehold.co/400x600" xr:uid="{B8267D85-A691-4187-91DB-27E364616A8C}"/>
+    <hyperlink ref="E41" r:id="rId73" xr:uid="{B8267D85-A691-4187-91DB-27E364616A8C}"/>
     <hyperlink ref="E43" r:id="rId74" xr:uid="{AA69E1F0-E88A-495C-A844-C33C82F6CE26}"/>
     <hyperlink ref="E45" r:id="rId75" xr:uid="{269F03E1-526C-4849-A6D5-8276665E4485}"/>
     <hyperlink ref="E47" r:id="rId76" xr:uid="{D722AC52-912D-4A3F-8560-FAA4DCA60A56}"/>
@@ -8962,31 +8959,31 @@
     <hyperlink ref="E51" r:id="rId78" xr:uid="{FAAE2569-D069-46B3-A7AA-6969338A4AFF}"/>
     <hyperlink ref="E53" r:id="rId79" xr:uid="{919767C3-0A6A-4A63-9549-0F7B3A7EE7DF}"/>
     <hyperlink ref="E55" r:id="rId80" xr:uid="{BD76B93C-ACC1-4CF1-A623-39E4FAFED853}"/>
-    <hyperlink ref="E57" r:id="rId81" display="https://placehold.co/400x600" xr:uid="{7964589D-7453-4997-AC7B-F98F5B5B7029}"/>
+    <hyperlink ref="E57" r:id="rId81" xr:uid="{7964589D-7453-4997-AC7B-F98F5B5B7029}"/>
     <hyperlink ref="E59" r:id="rId82" xr:uid="{F72D2D0A-AD07-45DC-AA3D-223C36C995AB}"/>
     <hyperlink ref="E61" r:id="rId83" xr:uid="{D79CAE5D-C5B6-4B75-8261-008B5374EBDB}"/>
     <hyperlink ref="E63" r:id="rId84" xr:uid="{75C81E45-FAA6-4175-A2FE-BA7C7F71F6F3}"/>
-    <hyperlink ref="E67" r:id="rId85" display="https://placehold.co/400x600" xr:uid="{F199289C-0CB7-41CD-95E9-D9C97B86A7E7}"/>
-    <hyperlink ref="E69" r:id="rId86" display="https://placehold.co/400x600" xr:uid="{E4715AC6-7D6D-4434-A585-79B8F25233F6}"/>
+    <hyperlink ref="E67" r:id="rId85" xr:uid="{F199289C-0CB7-41CD-95E9-D9C97B86A7E7}"/>
+    <hyperlink ref="E69" r:id="rId86" xr:uid="{E4715AC6-7D6D-4434-A585-79B8F25233F6}"/>
     <hyperlink ref="E71" r:id="rId87" xr:uid="{CFD1BDC4-A848-4998-9430-C29DB079EED4}"/>
     <hyperlink ref="E73" r:id="rId88" xr:uid="{DEC62E70-AB7A-4365-B90A-11A1D549F375}"/>
     <hyperlink ref="E75" r:id="rId89" xr:uid="{A925F566-676A-47EA-9068-3A8AC9C78A71}"/>
     <hyperlink ref="E77" r:id="rId90" xr:uid="{826BB4FF-EF4E-4C68-AE45-B4C9CEE10FB5}"/>
     <hyperlink ref="E79" r:id="rId91" xr:uid="{D55B186E-0A96-4185-9D34-01F9C47E843E}"/>
     <hyperlink ref="E81" r:id="rId92" xr:uid="{AC60663B-FB99-47D2-A9DA-11C43648559B}"/>
-    <hyperlink ref="E83" r:id="rId93" display="https://placehold.co/400x600" xr:uid="{F83899A5-222C-48AC-9ABC-BC254C3600A8}"/>
+    <hyperlink ref="E83" r:id="rId93" xr:uid="{F83899A5-222C-48AC-9ABC-BC254C3600A8}"/>
     <hyperlink ref="E85" r:id="rId94" display="https://placehold.co/400x600" xr:uid="{2EE015AD-95D3-42D3-9727-0C2D20C22B2D}"/>
     <hyperlink ref="E87" r:id="rId95" xr:uid="{1E9351A5-5685-4A61-91E2-9C72A14FBA45}"/>
-    <hyperlink ref="E89" r:id="rId96" display="https://placehold.co/400x600" xr:uid="{DA14C2E4-99E6-4273-B1C6-88E4314A2B53}"/>
+    <hyperlink ref="E89" r:id="rId96" xr:uid="{DA14C2E4-99E6-4273-B1C6-88E4314A2B53}"/>
     <hyperlink ref="E91" r:id="rId97" display="https://placehold.co/400x600" xr:uid="{CED33FAF-E705-4A0E-B5BA-28AC459A08F9}"/>
-    <hyperlink ref="E93" r:id="rId98" display="https://placehold.co/400x600" xr:uid="{69683834-3F44-4B9E-879F-17C7B3985064}"/>
+    <hyperlink ref="E93" r:id="rId98" xr:uid="{69683834-3F44-4B9E-879F-17C7B3985064}"/>
     <hyperlink ref="E95" r:id="rId99" xr:uid="{6706B29D-6B9E-414D-A766-C429245D96A7}"/>
     <hyperlink ref="E97" r:id="rId100" xr:uid="{B8549196-6B30-41D5-B870-CDF1F6C0AE2B}"/>
-    <hyperlink ref="E99" r:id="rId101" display="https://placehold.co/400x600" xr:uid="{70722206-091E-437D-B026-345C8CDB5176}"/>
+    <hyperlink ref="E99" r:id="rId101" xr:uid="{70722206-091E-437D-B026-345C8CDB5176}"/>
     <hyperlink ref="E101" r:id="rId102" xr:uid="{EF057E02-0A38-4475-84BA-2BC1ED64BA7D}"/>
     <hyperlink ref="E103" r:id="rId103" xr:uid="{F307B800-2CAD-4E08-A635-F4AD9976A897}"/>
-    <hyperlink ref="E105" r:id="rId104" display="https://placehold.co/400x600" xr:uid="{42F0B609-7315-4192-A377-FDEDE5FDDF8B}"/>
-    <hyperlink ref="E107" r:id="rId105" display="https://placehold.co/400x600" xr:uid="{0BBF4990-1413-476C-AFE7-EC34A9F113B0}"/>
+    <hyperlink ref="E105" r:id="rId104" xr:uid="{42F0B609-7315-4192-A377-FDEDE5FDDF8B}"/>
+    <hyperlink ref="E107" r:id="rId105" xr:uid="{0BBF4990-1413-476C-AFE7-EC34A9F113B0}"/>
     <hyperlink ref="E109" r:id="rId106" xr:uid="{43D0B648-1D21-45A3-A6E9-CB546100DAA2}"/>
     <hyperlink ref="E111" r:id="rId107" xr:uid="{3BF79D70-269C-4AB5-B83F-712DABFF4480}"/>
     <hyperlink ref="E113" r:id="rId108" xr:uid="{622A2536-A959-42B4-B4F9-EE23F2A44517}"/>
@@ -9335,7 +9332,7 @@
     <hyperlink ref="E54" r:id="rId451" xr:uid="{41208DE8-410A-4988-814F-34D6808B3973}"/>
     <hyperlink ref="E65" r:id="rId452" xr:uid="{2A43A7D2-0D9B-42A8-8E87-E447ECDB9951}"/>
     <hyperlink ref="E60" r:id="rId453" xr:uid="{6FED2870-0657-4424-9493-C87C5558030E}"/>
-    <hyperlink ref="E112" r:id="rId454" display="https://placehold.co/400x600" xr:uid="{72604405-579A-4D04-AD70-2F433C2E73DD}"/>
+    <hyperlink ref="E112" r:id="rId454" xr:uid="{72604405-579A-4D04-AD70-2F433C2E73DD}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId455"/>

</xml_diff>

<commit_message>
gradient background in faculty image
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAEFFBE3-4932-4796-B960-524E7FDE92F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4EE2A1-F28D-40DE-AF83-F000130A09F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1007">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="1009">
   <si>
     <t>Name</t>
   </si>
@@ -3220,6 +3220,12 @@
   </si>
   <si>
     <t>CSPIT_Faculty\Electrical\VIBHABEN.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Electronics\SAGARKUMAR.webp</t>
+  </si>
+  <si>
+    <t>CSPIT_Faculty\Mechanical\VIJAYKUMAR.webp</t>
   </si>
 </sst>
 </file>
@@ -3717,7 +3723,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A114" zoomScale="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="115" workbookViewId="0">
       <selection activeCell="E112" sqref="E112"/>
     </sheetView>
   </sheetViews>
@@ -7474,7 +7480,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="86" spans="1:14" ht="343.2" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" ht="330" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>192</v>
       </c>
@@ -7972,7 +7978,7 @@
         <v>47</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>981</v>
+        <v>1007</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>443</v>
@@ -8632,7 +8638,7 @@
         <v>64</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>938</v>
+        <v>1008</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>457</v>

</xml_diff>

<commit_message>
FACULTY details page dont load accordian when no data is available
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4518248c6cd0c0d5/Desktop/CSPIT_NEW_2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB4EE2A1-F28D-40DE-AF83-F000130A09F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="6_{42F40C5C-83DD-423A-A0F7-83E3ED73F5A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A7114F75-8C6F-4D5D-8825-CB85622AF32D}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2066,12 +2066,6 @@
     <t>https://www.linkedin.com/in/drNAsagarNAchokshiNA8646601a/</t>
   </si>
   <si>
-    <t>https://www.linkedin.com/in/sagarkumarNApatelNA0bb94bb5/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/sanketNAsutharNA544a69210/</t>
-  </si>
-  <si>
     <t>www.linkedin.com/in/satayuNAtravadiNA9aab0919</t>
   </si>
   <si>
@@ -3226,6 +3220,12 @@
   </si>
   <si>
     <t>CSPIT_Faculty\Mechanical\VIJAYKUMAR.webp</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sagarkumar-patel-0bb94bb5/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/sanket-suthar-544a69210/</t>
   </si>
 </sst>
 </file>
@@ -3723,8 +3723,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A111" zoomScale="115" workbookViewId="0">
-      <selection activeCell="E112" sqref="E112"/>
+    <sheetView tabSelected="1" topLeftCell="E97" zoomScale="115" workbookViewId="0">
+      <selection activeCell="J98" sqref="J98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3757,7 +3757,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>889</v>
+        <v>887</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>6</v>
@@ -3775,13 +3775,13 @@
         <v>11</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>696</v>
+        <v>694</v>
       </c>
       <c r="M1" s="13" t="s">
-        <v>809</v>
+        <v>807</v>
       </c>
       <c r="N1" s="13" t="s">
-        <v>888</v>
+        <v>886</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -3798,7 +3798,7 @@
         <v>229</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>913</v>
+        <v>911</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>357</v>
@@ -3813,13 +3813,13 @@
         <v>253</v>
       </c>
       <c r="J2" s="9" t="s">
-        <v>892</v>
+        <v>890</v>
       </c>
       <c r="K2" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L2" s="9" t="s">
-        <v>697</v>
+        <v>695</v>
       </c>
       <c r="M2" s="9" t="s">
         <v>470</v>
@@ -3842,7 +3842,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>953</v>
+        <v>951</v>
       </c>
       <c r="F3" s="6" t="s">
         <v>358</v>
@@ -3857,19 +3857,19 @@
         <v>255</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>893</v>
+        <v>891</v>
       </c>
       <c r="K3" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>698</v>
+        <v>696</v>
       </c>
       <c r="M3" s="9" t="s">
         <v>471</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>852</v>
+        <v>850</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -3880,13 +3880,13 @@
         <v>223</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>940</v>
+        <v>938</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>359</v>
@@ -3901,13 +3901,13 @@
         <v>254</v>
       </c>
       <c r="J4" s="9" t="s">
-        <v>894</v>
+        <v>892</v>
       </c>
       <c r="K4" s="9" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>699</v>
+        <v>697</v>
       </c>
       <c r="M4" s="9" t="s">
         <v>472</v>
@@ -3930,7 +3930,7 @@
         <v>72</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>954</v>
+        <v>952</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>360</v>
@@ -3945,13 +3945,13 @@
         <v>256</v>
       </c>
       <c r="J5" s="9" t="s">
-        <v>891</v>
+        <v>889</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>700</v>
+        <v>698</v>
       </c>
       <c r="M5" s="9" t="s">
         <v>473</v>
@@ -3974,7 +3974,7 @@
         <v>48</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>941</v>
+        <v>939</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>361</v>
@@ -3989,13 +3989,13 @@
         <v>257</v>
       </c>
       <c r="J6" s="9" t="s">
-        <v>890</v>
+        <v>888</v>
       </c>
       <c r="K6" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>701</v>
+        <v>699</v>
       </c>
       <c r="M6" s="9" t="s">
         <v>474</v>
@@ -4018,7 +4018,7 @@
         <v>230</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>942</v>
+        <v>940</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>362</v>
@@ -4033,19 +4033,19 @@
         <v>259</v>
       </c>
       <c r="J7" s="9" t="s">
-        <v>895</v>
+        <v>893</v>
       </c>
       <c r="K7" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>702</v>
+        <v>700</v>
       </c>
       <c r="M7" s="9" t="s">
         <v>475</v>
       </c>
       <c r="N7" s="10" t="s">
-        <v>853</v>
+        <v>851</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -4077,13 +4077,13 @@
         <v>258</v>
       </c>
       <c r="J8" s="9" t="s">
-        <v>896</v>
+        <v>894</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>703</v>
+        <v>701</v>
       </c>
       <c r="M8" s="10" t="s">
         <v>110</v>
@@ -4100,13 +4100,13 @@
         <v>223</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>40</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>955</v>
+        <v>953</v>
       </c>
       <c r="F9" s="6" t="s">
         <v>364</v>
@@ -4121,19 +4121,19 @@
         <v>260</v>
       </c>
       <c r="J9" s="9" t="s">
-        <v>897</v>
+        <v>895</v>
       </c>
       <c r="K9" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>704</v>
+        <v>702</v>
       </c>
       <c r="M9" s="9" t="s">
         <v>476</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>854</v>
+        <v>852</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -4150,7 +4150,7 @@
         <v>67</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>914</v>
+        <v>912</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>365</v>
@@ -4165,13 +4165,13 @@
         <v>261</v>
       </c>
       <c r="J10" s="9" t="s">
-        <v>898</v>
+        <v>896</v>
       </c>
       <c r="K10" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>705</v>
+        <v>703</v>
       </c>
       <c r="M10" s="9" t="s">
         <v>477</v>
@@ -4188,16 +4188,16 @@
         <v>223</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>232</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>956</v>
+        <v>954</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>110</v>
@@ -4212,10 +4212,10 @@
         <v>104</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>656</v>
+        <v>654</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>706</v>
+        <v>704</v>
       </c>
       <c r="M11" s="9" t="s">
         <v>477</v>
@@ -4238,7 +4238,7 @@
         <v>42</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>915</v>
+        <v>913</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>366</v>
@@ -4247,10 +4247,10 @@
         <v>110</v>
       </c>
       <c r="H12" s="6" t="s">
-        <v>827</v>
+        <v>825</v>
       </c>
       <c r="I12" s="11" t="s">
-        <v>688</v>
+        <v>686</v>
       </c>
       <c r="J12" s="9" t="s">
         <v>567</v>
@@ -4259,13 +4259,13 @@
         <v>110</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>707</v>
+        <v>705</v>
       </c>
       <c r="M12" s="9" t="s">
         <v>478</v>
       </c>
       <c r="N12" s="10" t="s">
-        <v>855</v>
+        <v>853</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="105.6" x14ac:dyDescent="0.3">
@@ -4282,7 +4282,7 @@
         <v>85</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>984</v>
+        <v>982</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>367</v>
@@ -4294,7 +4294,7 @@
         <v>462</v>
       </c>
       <c r="I13" s="11" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="J13" s="9" t="s">
         <v>104</v>
@@ -4303,13 +4303,13 @@
         <v>110</v>
       </c>
       <c r="L13" s="9" t="s">
-        <v>708</v>
+        <v>706</v>
       </c>
       <c r="M13" s="9" t="s">
         <v>477</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>856</v>
+        <v>854</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -4326,7 +4326,7 @@
         <v>32</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>916</v>
+        <v>914</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>368</v>
@@ -4335,7 +4335,7 @@
         <v>110</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
       <c r="I14" s="4" t="s">
         <v>263</v>
@@ -4347,13 +4347,13 @@
         <v>110</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>709</v>
+        <v>707</v>
       </c>
       <c r="M14" s="9" t="s">
         <v>479</v>
       </c>
       <c r="N14" s="10" t="s">
-        <v>857</v>
+        <v>855</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -4364,13 +4364,13 @@
         <v>223</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>90</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>985</v>
+        <v>983</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>369</v>
@@ -4391,7 +4391,7 @@
         <v>110</v>
       </c>
       <c r="L15" s="9" t="s">
-        <v>710</v>
+        <v>708</v>
       </c>
       <c r="M15" s="9" t="s">
         <v>480</v>
@@ -4414,7 +4414,7 @@
         <v>233</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>943</v>
+        <v>941</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>370</v>
@@ -4452,22 +4452,22 @@
         <v>223</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>34</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>899</v>
+        <v>897</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>818</v>
+        <v>816</v>
       </c>
       <c r="G17" s="4" t="s">
         <v>110</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
       <c r="I17" s="4" t="s">
         <v>110</v>
@@ -4479,13 +4479,13 @@
         <v>110</v>
       </c>
       <c r="L17" s="9" t="s">
-        <v>711</v>
+        <v>709</v>
       </c>
       <c r="M17" s="9" t="s">
         <v>481</v>
       </c>
       <c r="N17" s="10" t="s">
-        <v>858</v>
+        <v>856</v>
       </c>
     </row>
     <row r="18" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
@@ -4502,7 +4502,7 @@
         <v>19</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>957</v>
+        <v>955</v>
       </c>
       <c r="F18" s="6" t="s">
         <v>371</v>
@@ -4523,13 +4523,13 @@
         <v>110</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>712</v>
+        <v>710</v>
       </c>
       <c r="M18" s="9" t="s">
         <v>482</v>
       </c>
       <c r="N18" s="10" t="s">
-        <v>859</v>
+        <v>857</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -4546,7 +4546,7 @@
         <v>27</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>986</v>
+        <v>984</v>
       </c>
       <c r="F19" s="6" t="s">
         <v>372</v>
@@ -4567,13 +4567,13 @@
         <v>110</v>
       </c>
       <c r="L19" s="9" t="s">
-        <v>713</v>
+        <v>711</v>
       </c>
       <c r="M19" s="9" t="s">
         <v>483</v>
       </c>
       <c r="N19" s="10" t="s">
-        <v>860</v>
+        <v>858</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -4590,7 +4590,7 @@
         <v>73</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>987</v>
+        <v>985</v>
       </c>
       <c r="F20" s="6" t="s">
         <v>373</v>
@@ -4611,7 +4611,7 @@
         <v>110</v>
       </c>
       <c r="L20" s="9" t="s">
-        <v>714</v>
+        <v>712</v>
       </c>
       <c r="M20" s="9" t="s">
         <v>477</v>
@@ -4634,7 +4634,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>944</v>
+        <v>942</v>
       </c>
       <c r="F21" s="6" t="s">
         <v>374</v>
@@ -4655,7 +4655,7 @@
         <v>110</v>
       </c>
       <c r="L21" s="9" t="s">
-        <v>715</v>
+        <v>713</v>
       </c>
       <c r="M21" s="9" t="s">
         <v>484</v>
@@ -4678,10 +4678,10 @@
         <v>50</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>958</v>
+        <v>956</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>110</v>
@@ -4699,7 +4699,7 @@
         <v>110</v>
       </c>
       <c r="L22" s="9" t="s">
-        <v>716</v>
+        <v>714</v>
       </c>
       <c r="M22" s="9" t="s">
         <v>485</v>
@@ -4722,7 +4722,7 @@
         <v>28</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>917</v>
+        <v>915</v>
       </c>
       <c r="F23" s="6" t="s">
         <v>375</v>
@@ -4743,13 +4743,13 @@
         <v>110</v>
       </c>
       <c r="L23" s="9" t="s">
-        <v>717</v>
+        <v>715</v>
       </c>
       <c r="M23" s="9" t="s">
         <v>486</v>
       </c>
       <c r="N23" s="10" t="s">
-        <v>861</v>
+        <v>859</v>
       </c>
     </row>
     <row r="24" spans="1:14" ht="211.2" x14ac:dyDescent="0.3">
@@ -4760,13 +4760,13 @@
         <v>223</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>54</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>959</v>
+        <v>957</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>376</v>
@@ -4787,7 +4787,7 @@
         <v>110</v>
       </c>
       <c r="L24" s="9" t="s">
-        <v>718</v>
+        <v>716</v>
       </c>
       <c r="M24" s="9" t="s">
         <v>487</v>
@@ -4810,7 +4810,7 @@
         <v>234</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>945</v>
+        <v>943</v>
       </c>
       <c r="F25" s="6" t="s">
         <v>377</v>
@@ -4822,22 +4822,22 @@
         <v>110</v>
       </c>
       <c r="I25" s="4" t="s">
-        <v>690</v>
+        <v>688</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>577</v>
       </c>
       <c r="K25" s="9" t="s">
-        <v>657</v>
+        <v>655</v>
       </c>
       <c r="L25" s="10" t="s">
-        <v>719</v>
+        <v>717</v>
       </c>
       <c r="M25" s="10" t="s">
         <v>110</v>
       </c>
       <c r="N25" s="10" t="s">
-        <v>862</v>
+        <v>860</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -4854,7 +4854,7 @@
         <v>55</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>960</v>
+        <v>958</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>378</v>
@@ -4863,7 +4863,7 @@
         <v>110</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="I26" s="4" t="s">
         <v>273</v>
@@ -4872,10 +4872,10 @@
         <v>578</v>
       </c>
       <c r="K26" s="10" t="s">
-        <v>658</v>
+        <v>656</v>
       </c>
       <c r="L26" s="9" t="s">
-        <v>720</v>
+        <v>718</v>
       </c>
       <c r="M26" s="9" t="s">
         <v>488</v>
@@ -4892,13 +4892,13 @@
         <v>223</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>61</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>946</v>
+        <v>944</v>
       </c>
       <c r="F27" s="6" t="s">
         <v>379</v>
@@ -4916,16 +4916,16 @@
         <v>579</v>
       </c>
       <c r="K27" s="9" t="s">
-        <v>659</v>
+        <v>657</v>
       </c>
       <c r="L27" s="9" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="M27" s="9" t="s">
         <v>489</v>
       </c>
       <c r="N27" s="10" t="s">
-        <v>863</v>
+        <v>861</v>
       </c>
     </row>
     <row r="28" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -4942,7 +4942,7 @@
         <v>46</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>918</v>
+        <v>916</v>
       </c>
       <c r="F28" s="6" t="s">
         <v>380</v>
@@ -4954,7 +4954,7 @@
         <v>110</v>
       </c>
       <c r="I28" s="4" t="s">
-        <v>691</v>
+        <v>689</v>
       </c>
       <c r="J28" s="9" t="s">
         <v>580</v>
@@ -4963,13 +4963,13 @@
         <v>110</v>
       </c>
       <c r="L28" s="9" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="M28" s="9" t="s">
         <v>478</v>
       </c>
       <c r="N28" s="10" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="29" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
@@ -4980,13 +4980,13 @@
         <v>223</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>36</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>919</v>
+        <v>917</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>381</v>
@@ -4998,7 +4998,7 @@
         <v>110</v>
       </c>
       <c r="I29" s="4" t="s">
-        <v>692</v>
+        <v>690</v>
       </c>
       <c r="J29" s="9" t="s">
         <v>581</v>
@@ -5007,7 +5007,7 @@
         <v>110</v>
       </c>
       <c r="L29" s="9" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="M29" s="9" t="s">
         <v>490</v>
@@ -5030,7 +5030,7 @@
         <v>235</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>900</v>
+        <v>898</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>382</v>
@@ -5051,7 +5051,7 @@
         <v>110</v>
       </c>
       <c r="L30" s="9" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="M30" s="17">
         <v>583944</v>
@@ -5083,7 +5083,7 @@
         <v>110</v>
       </c>
       <c r="H31" s="6" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="I31" s="4" t="s">
         <v>276</v>
@@ -5095,7 +5095,7 @@
         <v>110</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="M31" s="9" t="s">
         <v>491</v>
@@ -5118,7 +5118,7 @@
         <v>39</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>961</v>
+        <v>959</v>
       </c>
       <c r="F32" s="6" t="s">
         <v>384</v>
@@ -5139,10 +5139,10 @@
         <v>110</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="M32" s="9" t="s">
-        <v>806</v>
+        <v>804</v>
       </c>
       <c r="N32" s="10" t="s">
         <v>110</v>
@@ -5162,7 +5162,7 @@
         <v>237</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>929</v>
+        <v>927</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>385</v>
@@ -5183,13 +5183,13 @@
         <v>110</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>727</v>
+        <v>725</v>
       </c>
       <c r="M33" s="9" t="s">
-        <v>807</v>
+        <v>805</v>
       </c>
       <c r="N33" s="10" t="s">
-        <v>865</v>
+        <v>863</v>
       </c>
     </row>
     <row r="34" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -5206,7 +5206,7 @@
         <v>70</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>901</v>
+        <v>899</v>
       </c>
       <c r="F34" s="6" t="s">
         <v>386</v>
@@ -5215,7 +5215,7 @@
         <v>110</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="I34" s="4" t="s">
         <v>279</v>
@@ -5227,7 +5227,7 @@
         <v>110</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="M34" s="9" t="s">
         <v>492</v>
@@ -5250,7 +5250,7 @@
         <v>35</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>902</v>
+        <v>900</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>387</v>
@@ -5291,10 +5291,10 @@
         <v>5</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>988</v>
+        <v>986</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>388</v>
@@ -5315,13 +5315,13 @@
         <v>110</v>
       </c>
       <c r="L36" s="9" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="M36" s="9" t="s">
         <v>494</v>
       </c>
       <c r="N36" s="10" t="s">
-        <v>866</v>
+        <v>864</v>
       </c>
     </row>
     <row r="37" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -5338,7 +5338,7 @@
         <v>98</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>962</v>
+        <v>960</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>389</v>
@@ -5359,7 +5359,7 @@
         <v>110</v>
       </c>
       <c r="L37" s="9" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="M37" s="9" t="s">
         <v>495</v>
@@ -5376,16 +5376,16 @@
         <v>223</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>44</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>947</v>
+        <v>945</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>820</v>
+        <v>818</v>
       </c>
       <c r="G38" s="4" t="s">
         <v>110</v>
@@ -5403,7 +5403,7 @@
         <v>110</v>
       </c>
       <c r="L38" s="9" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="M38" s="9" t="s">
         <v>496</v>
@@ -5420,13 +5420,13 @@
         <v>223</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>51</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>948</v>
+        <v>946</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>390</v>
@@ -5447,7 +5447,7 @@
         <v>110</v>
       </c>
       <c r="L39" s="9" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="M39" s="10" t="s">
         <v>110</v>
@@ -5470,7 +5470,7 @@
         <v>81</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>930</v>
+        <v>928</v>
       </c>
       <c r="F40" s="6" t="s">
         <v>391</v>
@@ -5491,7 +5491,7 @@
         <v>110</v>
       </c>
       <c r="L40" s="9" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="M40" s="9" t="s">
         <v>497</v>
@@ -5508,13 +5508,13 @@
         <v>223</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>63</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>993</v>
+        <v>991</v>
       </c>
       <c r="F41" s="6" t="s">
         <v>392</v>
@@ -5523,7 +5523,7 @@
         <v>110</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>833</v>
+        <v>831</v>
       </c>
       <c r="I41" s="4" t="s">
         <v>285</v>
@@ -5535,7 +5535,7 @@
         <v>110</v>
       </c>
       <c r="L41" s="9" t="s">
-        <v>734</v>
+        <v>732</v>
       </c>
       <c r="M41" s="9" t="s">
         <v>498</v>
@@ -5558,7 +5558,7 @@
         <v>52</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>903</v>
+        <v>901</v>
       </c>
       <c r="F42" s="6" t="s">
         <v>393</v>
@@ -5579,7 +5579,7 @@
         <v>110</v>
       </c>
       <c r="L42" s="9" t="s">
-        <v>735</v>
+        <v>733</v>
       </c>
       <c r="M42" s="9" t="s">
         <v>499</v>
@@ -5596,13 +5596,13 @@
         <v>223</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>74</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>932</v>
+        <v>930</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>394</v>
@@ -5623,13 +5623,13 @@
         <v>110</v>
       </c>
       <c r="L43" s="9" t="s">
-        <v>736</v>
+        <v>734</v>
       </c>
       <c r="M43" s="9" t="s">
         <v>500</v>
       </c>
       <c r="N43" s="10" t="s">
-        <v>867</v>
+        <v>865</v>
       </c>
     </row>
     <row r="44" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -5646,7 +5646,7 @@
         <v>94</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>931</v>
+        <v>929</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>395</v>
@@ -5667,7 +5667,7 @@
         <v>110</v>
       </c>
       <c r="L44" s="9" t="s">
-        <v>737</v>
+        <v>735</v>
       </c>
       <c r="M44" s="9" t="s">
         <v>501</v>
@@ -5690,7 +5690,7 @@
         <v>86</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>949</v>
+        <v>947</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>396</v>
@@ -5708,10 +5708,10 @@
         <v>597</v>
       </c>
       <c r="K45" s="9" t="s">
-        <v>660</v>
+        <v>658</v>
       </c>
       <c r="L45" s="9" t="s">
-        <v>738</v>
+        <v>736</v>
       </c>
       <c r="M45" s="9" t="s">
         <v>502</v>
@@ -5728,13 +5728,13 @@
         <v>223</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>76</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>963</v>
+        <v>961</v>
       </c>
       <c r="F46" s="6" t="s">
         <v>397</v>
@@ -5755,7 +5755,7 @@
         <v>110</v>
       </c>
       <c r="L46" s="9" t="s">
-        <v>739</v>
+        <v>737</v>
       </c>
       <c r="M46" s="9" t="s">
         <v>503</v>
@@ -5778,7 +5778,7 @@
         <v>92</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>964</v>
+        <v>962</v>
       </c>
       <c r="F47" s="6" t="s">
         <v>398</v>
@@ -5799,7 +5799,7 @@
         <v>110</v>
       </c>
       <c r="L47" s="9" t="s">
-        <v>740</v>
+        <v>738</v>
       </c>
       <c r="M47" s="10" t="s">
         <v>110</v>
@@ -5822,7 +5822,7 @@
         <v>66</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>965</v>
+        <v>963</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>399</v>
@@ -5843,7 +5843,7 @@
         <v>110</v>
       </c>
       <c r="L48" s="9" t="s">
-        <v>741</v>
+        <v>739</v>
       </c>
       <c r="M48" s="9" t="s">
         <v>477</v>
@@ -5866,7 +5866,7 @@
         <v>20</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>966</v>
+        <v>964</v>
       </c>
       <c r="F49" s="6" t="s">
         <v>400</v>
@@ -5878,22 +5878,22 @@
         <v>110</v>
       </c>
       <c r="I49" s="11" t="s">
-        <v>693</v>
+        <v>691</v>
       </c>
       <c r="J49" s="9" t="s">
         <v>599</v>
       </c>
       <c r="K49" s="10" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
       <c r="L49" s="9" t="s">
-        <v>742</v>
+        <v>740</v>
       </c>
       <c r="M49" s="9" t="s">
         <v>504</v>
       </c>
       <c r="N49" s="10" t="s">
-        <v>868</v>
+        <v>866</v>
       </c>
     </row>
     <row r="50" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
@@ -5910,7 +5910,7 @@
         <v>26</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>967</v>
+        <v>965</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>401</v>
@@ -5919,7 +5919,7 @@
         <v>110</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>834</v>
+        <v>832</v>
       </c>
       <c r="I50" s="11" t="s">
         <v>293</v>
@@ -5931,13 +5931,13 @@
         <v>110</v>
       </c>
       <c r="L50" s="9" t="s">
-        <v>743</v>
+        <v>741</v>
       </c>
       <c r="M50" s="9" t="s">
         <v>505</v>
       </c>
       <c r="N50" s="10" t="s">
-        <v>869</v>
+        <v>867</v>
       </c>
     </row>
     <row r="51" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -5951,10 +5951,10 @@
         <v>5</v>
       </c>
       <c r="D51" s="6" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="E51" s="2" t="s">
-        <v>968</v>
+        <v>966</v>
       </c>
       <c r="F51" s="6" t="s">
         <v>402</v>
@@ -5963,7 +5963,7 @@
         <v>110</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>835</v>
+        <v>833</v>
       </c>
       <c r="I51" s="4" t="s">
         <v>294</v>
@@ -5975,7 +5975,7 @@
         <v>110</v>
       </c>
       <c r="L51" s="9" t="s">
-        <v>744</v>
+        <v>742</v>
       </c>
       <c r="M51" s="9" t="s">
         <v>477</v>
@@ -5998,7 +5998,7 @@
         <v>30</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>920</v>
+        <v>918</v>
       </c>
       <c r="F52" s="6" t="s">
         <v>403</v>
@@ -6019,7 +6019,7 @@
         <v>110</v>
       </c>
       <c r="L52" s="9" t="s">
-        <v>745</v>
+        <v>743</v>
       </c>
       <c r="M52" s="10" t="s">
         <v>110</v>
@@ -6042,7 +6042,7 @@
         <v>58</v>
       </c>
       <c r="E53" s="2" t="s">
-        <v>969</v>
+        <v>967</v>
       </c>
       <c r="F53" s="6" t="s">
         <v>404</v>
@@ -6063,7 +6063,7 @@
         <v>110</v>
       </c>
       <c r="L53" s="9" t="s">
-        <v>746</v>
+        <v>744</v>
       </c>
       <c r="M53" s="9" t="s">
         <v>506</v>
@@ -6086,7 +6086,7 @@
         <v>62</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>970</v>
+        <v>968</v>
       </c>
       <c r="F54" s="6" t="s">
         <v>405</v>
@@ -6095,7 +6095,7 @@
         <v>110</v>
       </c>
       <c r="H54" s="6" t="s">
-        <v>836</v>
+        <v>834</v>
       </c>
       <c r="I54" s="4" t="s">
         <v>298</v>
@@ -6107,7 +6107,7 @@
         <v>110</v>
       </c>
       <c r="L54" s="9" t="s">
-        <v>747</v>
+        <v>745</v>
       </c>
       <c r="M54" s="9" t="s">
         <v>507</v>
@@ -6124,13 +6124,13 @@
         <v>223</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>238</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>971</v>
+        <v>969</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>406</v>
@@ -6139,7 +6139,7 @@
         <v>110</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>837</v>
+        <v>835</v>
       </c>
       <c r="I55" s="4" t="s">
         <v>297</v>
@@ -6151,13 +6151,13 @@
         <v>110</v>
       </c>
       <c r="L55" s="9" t="s">
-        <v>748</v>
+        <v>746</v>
       </c>
       <c r="M55" s="9" t="s">
         <v>508</v>
       </c>
       <c r="N55" s="10" t="s">
-        <v>870</v>
+        <v>868</v>
       </c>
     </row>
     <row r="56" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
@@ -6168,16 +6168,16 @@
         <v>223</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>681</v>
+        <v>679</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>91</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>972</v>
+        <v>970</v>
       </c>
       <c r="F56" s="6" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="G56" s="4" t="s">
         <v>110</v>
@@ -6195,7 +6195,7 @@
         <v>110</v>
       </c>
       <c r="L56" s="9" t="s">
-        <v>749</v>
+        <v>747</v>
       </c>
       <c r="M56" s="9" t="s">
         <v>509</v>
@@ -6215,10 +6215,10 @@
         <v>5</v>
       </c>
       <c r="D57" s="6" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>989</v>
+        <v>987</v>
       </c>
       <c r="F57" s="6" t="s">
         <v>407</v>
@@ -6227,7 +6227,7 @@
         <v>110</v>
       </c>
       <c r="H57" s="6" t="s">
-        <v>838</v>
+        <v>836</v>
       </c>
       <c r="I57" s="4" t="s">
         <v>300</v>
@@ -6239,13 +6239,13 @@
         <v>110</v>
       </c>
       <c r="L57" s="9" t="s">
-        <v>750</v>
+        <v>748</v>
       </c>
       <c r="M57" s="9" t="s">
         <v>510</v>
       </c>
       <c r="N57" s="10" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="58" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -6262,7 +6262,7 @@
         <v>239</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>921</v>
+        <v>919</v>
       </c>
       <c r="F58" s="6" t="s">
         <v>408</v>
@@ -6271,7 +6271,7 @@
         <v>110</v>
       </c>
       <c r="H58" s="6" t="s">
-        <v>839</v>
+        <v>837</v>
       </c>
       <c r="I58" s="4" t="s">
         <v>301</v>
@@ -6283,7 +6283,7 @@
         <v>110</v>
       </c>
       <c r="L58" s="9" t="s">
-        <v>751</v>
+        <v>749</v>
       </c>
       <c r="M58" s="9" t="s">
         <v>511</v>
@@ -6300,13 +6300,13 @@
         <v>223</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D59" s="6" t="s">
         <v>83</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>904</v>
+        <v>902</v>
       </c>
       <c r="F59" s="6" t="s">
         <v>409</v>
@@ -6315,7 +6315,7 @@
         <v>110</v>
       </c>
       <c r="H59" s="6" t="s">
-        <v>840</v>
+        <v>838</v>
       </c>
       <c r="I59" s="4" t="s">
         <v>302</v>
@@ -6327,7 +6327,7 @@
         <v>110</v>
       </c>
       <c r="L59" s="9" t="s">
-        <v>752</v>
+        <v>750</v>
       </c>
       <c r="M59" s="9" t="s">
         <v>512</v>
@@ -6350,7 +6350,7 @@
         <v>240</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>973</v>
+        <v>971</v>
       </c>
       <c r="F60" s="6" t="s">
         <v>410</v>
@@ -6368,16 +6368,16 @@
         <v>607</v>
       </c>
       <c r="K60" s="9" t="s">
-        <v>662</v>
+        <v>660</v>
       </c>
       <c r="L60" s="9" t="s">
-        <v>753</v>
+        <v>751</v>
       </c>
       <c r="M60" s="9" t="s">
         <v>513</v>
       </c>
       <c r="N60" s="10" t="s">
-        <v>872</v>
+        <v>870</v>
       </c>
     </row>
     <row r="61" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -6394,16 +6394,16 @@
         <v>68</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>974</v>
+        <v>972</v>
       </c>
       <c r="F61" s="6" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="G61" s="4" t="s">
         <v>110</v>
       </c>
       <c r="H61" s="6" t="s">
-        <v>841</v>
+        <v>839</v>
       </c>
       <c r="I61" s="4" t="s">
         <v>304</v>
@@ -6415,7 +6415,7 @@
         <v>110</v>
       </c>
       <c r="L61" s="9" t="s">
-        <v>754</v>
+        <v>752</v>
       </c>
       <c r="M61" s="9" t="s">
         <v>514</v>
@@ -6432,13 +6432,13 @@
         <v>223</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D62" s="6" t="s">
         <v>65</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>933</v>
+        <v>931</v>
       </c>
       <c r="F62" s="6" t="s">
         <v>411</v>
@@ -6459,7 +6459,7 @@
         <v>110</v>
       </c>
       <c r="L62" s="9" t="s">
-        <v>755</v>
+        <v>753</v>
       </c>
       <c r="M62" s="9" t="s">
         <v>515</v>
@@ -6479,10 +6479,10 @@
         <v>4</v>
       </c>
       <c r="D63" s="6" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>934</v>
+        <v>932</v>
       </c>
       <c r="F63" s="6" t="s">
         <v>412</v>
@@ -6503,7 +6503,7 @@
         <v>110</v>
       </c>
       <c r="L63" s="9" t="s">
-        <v>756</v>
+        <v>754</v>
       </c>
       <c r="M63" s="9" t="s">
         <v>516</v>
@@ -6526,7 +6526,7 @@
         <v>78</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>975</v>
+        <v>973</v>
       </c>
       <c r="F64" s="6" t="s">
         <v>413</v>
@@ -6544,16 +6544,16 @@
         <v>610</v>
       </c>
       <c r="K64" s="9" t="s">
-        <v>663</v>
+        <v>661</v>
       </c>
       <c r="L64" s="9" t="s">
-        <v>757</v>
+        <v>755</v>
       </c>
       <c r="M64" s="9" t="s">
         <v>477</v>
       </c>
       <c r="N64" s="10" t="s">
-        <v>864</v>
+        <v>862</v>
       </c>
     </row>
     <row r="65" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
@@ -6564,13 +6564,13 @@
         <v>223</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>682</v>
+        <v>680</v>
       </c>
       <c r="D65" s="6" t="s">
         <v>69</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>976</v>
+        <v>974</v>
       </c>
       <c r="F65" s="6" t="s">
         <v>414</v>
@@ -6579,7 +6579,7 @@
         <v>110</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>842</v>
+        <v>840</v>
       </c>
       <c r="I65" s="4" t="s">
         <v>308</v>
@@ -6591,7 +6591,7 @@
         <v>110</v>
       </c>
       <c r="L65" s="9" t="s">
-        <v>758</v>
+        <v>756</v>
       </c>
       <c r="M65" s="9" t="s">
         <v>517</v>
@@ -6614,7 +6614,7 @@
         <v>99</v>
       </c>
       <c r="E66" s="2" t="s">
-        <v>990</v>
+        <v>988</v>
       </c>
       <c r="F66" s="6" t="s">
         <v>415</v>
@@ -6635,13 +6635,13 @@
         <v>110</v>
       </c>
       <c r="L66" s="9" t="s">
-        <v>759</v>
+        <v>757</v>
       </c>
       <c r="M66" s="9" t="s">
         <v>518</v>
       </c>
       <c r="N66" s="10" t="s">
-        <v>873</v>
+        <v>871</v>
       </c>
     </row>
     <row r="67" spans="1:14" ht="277.2" x14ac:dyDescent="0.3">
@@ -6658,7 +6658,7 @@
         <v>38</v>
       </c>
       <c r="E67" s="2" t="s">
-        <v>991</v>
+        <v>989</v>
       </c>
       <c r="F67" s="6" t="s">
         <v>416</v>
@@ -6667,7 +6667,7 @@
         <v>110</v>
       </c>
       <c r="H67" s="6" t="s">
-        <v>843</v>
+        <v>841</v>
       </c>
       <c r="I67" s="4" t="s">
         <v>310</v>
@@ -6676,10 +6676,10 @@
         <v>613</v>
       </c>
       <c r="K67" s="9" t="s">
-        <v>664</v>
+        <v>662</v>
       </c>
       <c r="L67" s="9" t="s">
-        <v>760</v>
+        <v>758</v>
       </c>
       <c r="M67" s="9" t="s">
         <v>519</v>
@@ -6702,7 +6702,7 @@
         <v>23</v>
       </c>
       <c r="E68" s="2" t="s">
-        <v>922</v>
+        <v>920</v>
       </c>
       <c r="F68" s="6" t="s">
         <v>417</v>
@@ -6723,7 +6723,7 @@
         <v>110</v>
       </c>
       <c r="L68" s="9" t="s">
-        <v>761</v>
+        <v>759</v>
       </c>
       <c r="M68" s="9" t="s">
         <v>520</v>
@@ -6746,7 +6746,7 @@
         <v>241</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>992</v>
+        <v>990</v>
       </c>
       <c r="F69" s="6" t="s">
         <v>418</v>
@@ -6790,10 +6790,10 @@
         <v>49</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>935</v>
+        <v>933</v>
       </c>
       <c r="F70" s="6" t="s">
-        <v>823</v>
+        <v>821</v>
       </c>
       <c r="G70" s="4" t="s">
         <v>110</v>
@@ -6811,13 +6811,13 @@
         <v>110</v>
       </c>
       <c r="L70" s="9" t="s">
-        <v>762</v>
+        <v>760</v>
       </c>
       <c r="M70" s="9" t="s">
         <v>521</v>
       </c>
       <c r="N70" s="10" t="s">
-        <v>874</v>
+        <v>872</v>
       </c>
     </row>
     <row r="71" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -6831,10 +6831,10 @@
         <v>5</v>
       </c>
       <c r="D71" s="6" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>923</v>
+        <v>921</v>
       </c>
       <c r="F71" s="6" t="s">
         <v>419</v>
@@ -6855,7 +6855,7 @@
         <v>110</v>
       </c>
       <c r="L71" s="9" t="s">
-        <v>763</v>
+        <v>761</v>
       </c>
       <c r="M71" s="9" t="s">
         <v>522</v>
@@ -6878,7 +6878,7 @@
         <v>16</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>977</v>
+        <v>975</v>
       </c>
       <c r="F72" s="6" t="s">
         <v>420</v>
@@ -6887,7 +6887,7 @@
         <v>110</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>844</v>
+        <v>842</v>
       </c>
       <c r="I72" s="4" t="s">
         <v>315</v>
@@ -6896,10 +6896,10 @@
         <v>618</v>
       </c>
       <c r="K72" s="9" t="s">
-        <v>665</v>
+        <v>663</v>
       </c>
       <c r="L72" s="9" t="s">
-        <v>764</v>
+        <v>762</v>
       </c>
       <c r="M72" s="9" t="s">
         <v>523</v>
@@ -6922,7 +6922,7 @@
         <v>242</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>905</v>
+        <v>903</v>
       </c>
       <c r="F73" s="6" t="s">
         <v>421</v>
@@ -6931,7 +6931,7 @@
         <v>110</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>845</v>
+        <v>843</v>
       </c>
       <c r="I73" s="4" t="s">
         <v>316</v>
@@ -6943,13 +6943,13 @@
         <v>110</v>
       </c>
       <c r="L73" s="9" t="s">
-        <v>765</v>
+        <v>763</v>
       </c>
       <c r="M73" s="9" t="s">
         <v>524</v>
       </c>
       <c r="N73" s="10" t="s">
-        <v>875</v>
+        <v>873</v>
       </c>
     </row>
     <row r="74" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
@@ -6966,10 +6966,10 @@
         <v>96</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>936</v>
+        <v>934</v>
       </c>
       <c r="F74" s="6" t="s">
-        <v>824</v>
+        <v>822</v>
       </c>
       <c r="G74" s="4" t="s">
         <v>110</v>
@@ -6987,13 +6987,13 @@
         <v>110</v>
       </c>
       <c r="L74" s="10" t="s">
-        <v>766</v>
+        <v>764</v>
       </c>
       <c r="M74" s="9" t="s">
         <v>525</v>
       </c>
       <c r="N74" s="10" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="75" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -7010,7 +7010,7 @@
         <v>71</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>906</v>
+        <v>904</v>
       </c>
       <c r="F75" s="6" t="s">
         <v>422</v>
@@ -7031,7 +7031,7 @@
         <v>110</v>
       </c>
       <c r="L75" s="9" t="s">
-        <v>767</v>
+        <v>765</v>
       </c>
       <c r="M75" s="9" t="s">
         <v>477</v>
@@ -7054,7 +7054,7 @@
         <v>243</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>908</v>
+        <v>906</v>
       </c>
       <c r="F76" s="6" t="s">
         <v>423</v>
@@ -7075,13 +7075,13 @@
         <v>110</v>
       </c>
       <c r="L76" s="9" t="s">
-        <v>768</v>
+        <v>766</v>
       </c>
       <c r="M76" s="9" t="s">
         <v>526</v>
       </c>
       <c r="N76" s="10" t="s">
-        <v>876</v>
+        <v>874</v>
       </c>
     </row>
     <row r="77" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
@@ -7098,7 +7098,7 @@
         <v>37</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>907</v>
+        <v>905</v>
       </c>
       <c r="F77" s="6" t="s">
         <v>424</v>
@@ -7136,13 +7136,13 @@
         <v>223</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D78" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>994</v>
+        <v>992</v>
       </c>
       <c r="F78" s="6" t="s">
         <v>425</v>
@@ -7183,10 +7183,10 @@
         <v>5</v>
       </c>
       <c r="D79" s="6" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>909</v>
+        <v>907</v>
       </c>
       <c r="F79" s="6" t="s">
         <v>426</v>
@@ -7204,10 +7204,10 @@
         <v>625</v>
       </c>
       <c r="K79" s="9" t="s">
-        <v>666</v>
+        <v>664</v>
       </c>
       <c r="L79" s="9" t="s">
-        <v>769</v>
+        <v>767</v>
       </c>
       <c r="M79" s="9" t="s">
         <v>528</v>
@@ -7230,7 +7230,7 @@
         <v>33</v>
       </c>
       <c r="E80" s="2" t="s">
-        <v>910</v>
+        <v>908</v>
       </c>
       <c r="F80" s="6" t="s">
         <v>427</v>
@@ -7268,16 +7268,16 @@
         <v>223</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D81" s="6" t="s">
         <v>59</v>
       </c>
       <c r="E81" s="2" t="s">
-        <v>937</v>
+        <v>935</v>
       </c>
       <c r="F81" s="6" t="s">
-        <v>825</v>
+        <v>823</v>
       </c>
       <c r="G81" s="4" t="s">
         <v>110</v>
@@ -7295,13 +7295,13 @@
         <v>110</v>
       </c>
       <c r="L81" s="9" t="s">
-        <v>770</v>
+        <v>768</v>
       </c>
       <c r="M81" s="9" t="s">
         <v>530</v>
       </c>
       <c r="N81" s="10" t="s">
-        <v>877</v>
+        <v>875</v>
       </c>
     </row>
     <row r="82" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -7312,7 +7312,7 @@
         <v>223</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>683</v>
+        <v>681</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>244</v>
@@ -7339,7 +7339,7 @@
         <v>110</v>
       </c>
       <c r="L82" s="9" t="s">
-        <v>771</v>
+        <v>769</v>
       </c>
       <c r="M82" s="9" t="s">
         <v>531</v>
@@ -7362,7 +7362,7 @@
         <v>18</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>995</v>
+        <v>993</v>
       </c>
       <c r="F83" s="6" t="s">
         <v>429</v>
@@ -7383,7 +7383,7 @@
         <v>110</v>
       </c>
       <c r="L83" s="9" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="M83" s="9" t="s">
         <v>532</v>
@@ -7400,13 +7400,13 @@
         <v>223</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D84" s="6" t="s">
         <v>80</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>978</v>
+        <v>976</v>
       </c>
       <c r="F84" s="6" t="s">
         <v>430</v>
@@ -7427,7 +7427,7 @@
         <v>110</v>
       </c>
       <c r="L84" s="9" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="M84" s="9" t="s">
         <v>533</v>
@@ -7471,7 +7471,7 @@
         <v>110</v>
       </c>
       <c r="L85" s="9" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="M85" s="9" t="s">
         <v>534</v>
@@ -7494,7 +7494,7 @@
         <v>31</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>996</v>
+        <v>994</v>
       </c>
       <c r="F86" s="6" t="s">
         <v>432</v>
@@ -7512,16 +7512,16 @@
         <v>101</v>
       </c>
       <c r="K86" s="9" t="s">
-        <v>667</v>
+        <v>665</v>
       </c>
       <c r="L86" s="9" t="s">
-        <v>775</v>
+        <v>773</v>
       </c>
       <c r="M86" s="9" t="s">
         <v>535</v>
       </c>
       <c r="N86" s="10" t="s">
-        <v>878</v>
+        <v>876</v>
       </c>
     </row>
     <row r="87" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -7538,7 +7538,7 @@
         <v>97</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>911</v>
+        <v>909</v>
       </c>
       <c r="F87" s="6" t="s">
         <v>433</v>
@@ -7547,7 +7547,7 @@
         <v>110</v>
       </c>
       <c r="H87" s="6" t="s">
-        <v>846</v>
+        <v>844</v>
       </c>
       <c r="I87" s="4" t="s">
         <v>329</v>
@@ -7556,16 +7556,16 @@
         <v>629</v>
       </c>
       <c r="K87" s="9" t="s">
-        <v>668</v>
+        <v>666</v>
       </c>
       <c r="L87" s="9" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="M87" s="9" t="s">
-        <v>808</v>
+        <v>806</v>
       </c>
       <c r="N87" s="10" t="s">
-        <v>879</v>
+        <v>877</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
@@ -7576,13 +7576,13 @@
         <v>223</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D88" s="6" t="s">
         <v>246</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>979</v>
+        <v>977</v>
       </c>
       <c r="F88" s="6" t="s">
         <v>434</v>
@@ -7603,7 +7603,7 @@
         <v>110</v>
       </c>
       <c r="L88" s="9" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="M88" s="9" t="s">
         <v>536</v>
@@ -7626,7 +7626,7 @@
         <v>95</v>
       </c>
       <c r="E89" s="2" t="s">
-        <v>997</v>
+        <v>995</v>
       </c>
       <c r="F89" s="6" t="s">
         <v>435</v>
@@ -7647,7 +7647,7 @@
         <v>110</v>
       </c>
       <c r="L89" s="9" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="M89" s="9" t="s">
         <v>537</v>
@@ -7670,7 +7670,7 @@
         <v>56</v>
       </c>
       <c r="E90" s="2" t="s">
-        <v>980</v>
+        <v>978</v>
       </c>
       <c r="F90" s="6" t="s">
         <v>436</v>
@@ -7682,22 +7682,22 @@
         <v>110</v>
       </c>
       <c r="I90" s="11" t="s">
-        <v>694</v>
+        <v>692</v>
       </c>
       <c r="J90" s="9" t="s">
         <v>631</v>
       </c>
       <c r="K90" s="9" t="s">
-        <v>669</v>
+        <v>667</v>
       </c>
       <c r="L90" s="9" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="M90" s="9" t="s">
         <v>538</v>
       </c>
       <c r="N90" s="10" t="s">
-        <v>880</v>
+        <v>878</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
@@ -7723,7 +7723,7 @@
         <v>110</v>
       </c>
       <c r="H91" s="6" t="s">
-        <v>847</v>
+        <v>845</v>
       </c>
       <c r="I91" s="4" t="s">
         <v>332</v>
@@ -7735,7 +7735,7 @@
         <v>110</v>
       </c>
       <c r="L91" s="9" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="M91" s="9" t="s">
         <v>539</v>
@@ -7758,7 +7758,7 @@
         <v>21</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="F92" s="6" t="s">
         <v>438</v>
@@ -7776,10 +7776,10 @@
         <v>633</v>
       </c>
       <c r="K92" s="9" t="s">
-        <v>670</v>
+        <v>668</v>
       </c>
       <c r="L92" s="9" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="M92" s="9" t="s">
         <v>540</v>
@@ -7802,7 +7802,7 @@
         <v>247</v>
       </c>
       <c r="E93" s="2" t="s">
-        <v>998</v>
+        <v>996</v>
       </c>
       <c r="F93" s="6" t="s">
         <v>439</v>
@@ -7811,7 +7811,7 @@
         <v>110</v>
       </c>
       <c r="H93" s="6" t="s">
-        <v>848</v>
+        <v>846</v>
       </c>
       <c r="I93" s="4" t="s">
         <v>334</v>
@@ -7820,16 +7820,16 @@
         <v>634</v>
       </c>
       <c r="K93" s="9" t="s">
-        <v>671</v>
+        <v>669</v>
       </c>
       <c r="L93" s="9" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="M93" s="9" t="s">
         <v>541</v>
       </c>
       <c r="N93" s="10" t="s">
-        <v>881</v>
+        <v>879</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
@@ -7846,7 +7846,7 @@
         <v>89</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="F94" s="6" t="s">
         <v>440</v>
@@ -7864,10 +7864,10 @@
         <v>108</v>
       </c>
       <c r="K94" s="9" t="s">
-        <v>672</v>
+        <v>670</v>
       </c>
       <c r="L94" s="9" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="M94" s="9" t="s">
         <v>542</v>
@@ -7890,7 +7890,7 @@
         <v>25</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>926</v>
+        <v>924</v>
       </c>
       <c r="F95" s="6" t="s">
         <v>441</v>
@@ -7911,13 +7911,13 @@
         <v>110</v>
       </c>
       <c r="L95" s="9" t="s">
-        <v>784</v>
+        <v>782</v>
       </c>
       <c r="M95" s="9" t="s">
         <v>543</v>
       </c>
       <c r="N95" s="10" t="s">
-        <v>882</v>
+        <v>880</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -7934,7 +7934,7 @@
         <v>79</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>981</v>
+        <v>979</v>
       </c>
       <c r="F96" s="6" t="s">
         <v>442</v>
@@ -7943,7 +7943,7 @@
         <v>110</v>
       </c>
       <c r="H96" s="6" t="s">
-        <v>849</v>
+        <v>847</v>
       </c>
       <c r="I96" s="4" t="s">
         <v>337</v>
@@ -7955,13 +7955,13 @@
         <v>110</v>
       </c>
       <c r="L96" s="9" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="M96" s="9" t="s">
         <v>544</v>
       </c>
       <c r="N96" s="10" t="s">
-        <v>883</v>
+        <v>881</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="132" x14ac:dyDescent="0.3">
@@ -7978,7 +7978,7 @@
         <v>47</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>1007</v>
+        <v>1005</v>
       </c>
       <c r="F97" s="6" t="s">
         <v>443</v>
@@ -7987,25 +7987,25 @@
         <v>110</v>
       </c>
       <c r="H97" s="6" t="s">
-        <v>850</v>
+        <v>848</v>
       </c>
       <c r="I97" s="4" t="s">
         <v>338</v>
       </c>
       <c r="J97" s="9" t="s">
-        <v>637</v>
+        <v>1007</v>
       </c>
       <c r="K97" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L97" s="9" t="s">
-        <v>786</v>
+        <v>784</v>
       </c>
       <c r="M97" s="9" t="s">
         <v>545</v>
       </c>
       <c r="N97" s="10" t="s">
-        <v>871</v>
+        <v>869</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -8022,7 +8022,7 @@
         <v>57</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>999</v>
+        <v>997</v>
       </c>
       <c r="F98" s="6" t="s">
         <v>444</v>
@@ -8037,19 +8037,19 @@
         <v>339</v>
       </c>
       <c r="J98" s="9" t="s">
-        <v>638</v>
+        <v>1008</v>
       </c>
       <c r="K98" s="9" t="s">
-        <v>673</v>
+        <v>671</v>
       </c>
       <c r="L98" s="9" t="s">
-        <v>787</v>
+        <v>785</v>
       </c>
       <c r="M98" s="9" t="s">
         <v>546</v>
       </c>
       <c r="N98" s="10" t="s">
-        <v>884</v>
+        <v>882</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="66" x14ac:dyDescent="0.3">
@@ -8060,13 +8060,13 @@
         <v>223</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D99" s="6" t="s">
         <v>84</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>1000</v>
+        <v>998</v>
       </c>
       <c r="F99" s="6" t="s">
         <v>445</v>
@@ -8087,7 +8087,7 @@
         <v>110</v>
       </c>
       <c r="L99" s="9" t="s">
-        <v>788</v>
+        <v>786</v>
       </c>
       <c r="M99" s="9" t="s">
         <v>547</v>
@@ -8104,13 +8104,13 @@
         <v>223</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D100" s="6" t="s">
         <v>248</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>1001</v>
+        <v>999</v>
       </c>
       <c r="F100" s="6" t="s">
         <v>446</v>
@@ -8125,13 +8125,13 @@
         <v>341</v>
       </c>
       <c r="J100" s="9" t="s">
-        <v>639</v>
+        <v>637</v>
       </c>
       <c r="K100" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L100" s="9" t="s">
-        <v>789</v>
+        <v>787</v>
       </c>
       <c r="M100" s="9" t="s">
         <v>548</v>
@@ -8154,7 +8154,7 @@
         <v>43</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>927</v>
+        <v>925</v>
       </c>
       <c r="F101" s="6" t="s">
         <v>447</v>
@@ -8169,13 +8169,13 @@
         <v>342</v>
       </c>
       <c r="J101" s="9" t="s">
-        <v>640</v>
+        <v>638</v>
       </c>
       <c r="K101" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L101" s="9" t="s">
-        <v>790</v>
+        <v>788</v>
       </c>
       <c r="M101" s="9" t="s">
         <v>549</v>
@@ -8192,13 +8192,13 @@
         <v>223</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>684</v>
+        <v>682</v>
       </c>
       <c r="D102" s="6" t="s">
         <v>53</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>912</v>
+        <v>910</v>
       </c>
       <c r="F102" s="6" t="s">
         <v>448</v>
@@ -8213,13 +8213,13 @@
         <v>343</v>
       </c>
       <c r="J102" s="9" t="s">
-        <v>641</v>
+        <v>639</v>
       </c>
       <c r="K102" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L102" s="9" t="s">
-        <v>791</v>
+        <v>789</v>
       </c>
       <c r="M102" s="9" t="s">
         <v>550</v>
@@ -8242,7 +8242,7 @@
         <v>88</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>950</v>
+        <v>948</v>
       </c>
       <c r="F103" s="6" t="s">
         <v>449</v>
@@ -8257,13 +8257,13 @@
         <v>344</v>
       </c>
       <c r="J103" s="9" t="s">
-        <v>642</v>
+        <v>640</v>
       </c>
       <c r="K103" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L103" s="9" t="s">
-        <v>792</v>
+        <v>790</v>
       </c>
       <c r="M103" s="10" t="s">
         <v>110</v>
@@ -8280,13 +8280,13 @@
         <v>223</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>685</v>
+        <v>683</v>
       </c>
       <c r="D104" s="6" t="s">
         <v>93</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>1002</v>
+        <v>1000</v>
       </c>
       <c r="F104" s="6" t="s">
         <v>450</v>
@@ -8301,13 +8301,13 @@
         <v>110</v>
       </c>
       <c r="J104" s="9" t="s">
-        <v>643</v>
+        <v>641</v>
       </c>
       <c r="K104" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L104" s="9" t="s">
-        <v>793</v>
+        <v>791</v>
       </c>
       <c r="M104" s="9" t="s">
         <v>551</v>
@@ -8324,13 +8324,13 @@
         <v>223</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D105" s="6" t="s">
         <v>87</v>
       </c>
       <c r="E105" s="2" t="s">
-        <v>1003</v>
+        <v>1001</v>
       </c>
       <c r="F105" s="6" t="s">
         <v>451</v>
@@ -8345,13 +8345,13 @@
         <v>345</v>
       </c>
       <c r="J105" s="9" t="s">
-        <v>644</v>
+        <v>642</v>
       </c>
       <c r="K105" s="9" t="s">
-        <v>674</v>
+        <v>672</v>
       </c>
       <c r="L105" s="9" t="s">
-        <v>794</v>
+        <v>792</v>
       </c>
       <c r="M105" s="9" t="s">
         <v>552</v>
@@ -8374,7 +8374,7 @@
         <v>22</v>
       </c>
       <c r="E106" s="2" t="s">
-        <v>1004</v>
+        <v>1002</v>
       </c>
       <c r="F106" s="6" t="s">
         <v>452</v>
@@ -8392,10 +8392,10 @@
         <v>100</v>
       </c>
       <c r="K106" s="9" t="s">
-        <v>675</v>
+        <v>673</v>
       </c>
       <c r="L106" s="9" t="s">
-        <v>795</v>
+        <v>793</v>
       </c>
       <c r="M106" s="9" t="s">
         <v>553</v>
@@ -8418,7 +8418,7 @@
         <v>249</v>
       </c>
       <c r="E107" s="2" t="s">
-        <v>1005</v>
+        <v>1003</v>
       </c>
       <c r="F107" s="6" t="s">
         <v>453</v>
@@ -8433,19 +8433,19 @@
         <v>347</v>
       </c>
       <c r="J107" s="9" t="s">
-        <v>645</v>
+        <v>643</v>
       </c>
       <c r="K107" s="10" t="s">
         <v>110</v>
       </c>
       <c r="L107" s="9" t="s">
-        <v>796</v>
+        <v>794</v>
       </c>
       <c r="M107" s="9" t="s">
         <v>554</v>
       </c>
       <c r="N107" s="10" t="s">
-        <v>885</v>
+        <v>883</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
@@ -8462,7 +8462,7 @@
         <v>250</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>951</v>
+        <v>949</v>
       </c>
       <c r="F108" s="6" t="s">
         <v>454</v>
@@ -8477,13 +8477,13 @@
         <v>348</v>
       </c>
       <c r="J108" s="9" t="s">
-        <v>646</v>
+        <v>644</v>
       </c>
       <c r="K108" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L108" s="9" t="s">
-        <v>797</v>
+        <v>795</v>
       </c>
       <c r="M108" s="9" t="s">
         <v>555</v>
@@ -8506,7 +8506,7 @@
         <v>75</v>
       </c>
       <c r="E109" s="2" t="s">
-        <v>928</v>
+        <v>926</v>
       </c>
       <c r="F109" s="6" t="s">
         <v>75</v>
@@ -8521,13 +8521,13 @@
         <v>349</v>
       </c>
       <c r="J109" s="9" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
       <c r="K109" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L109" s="9" t="s">
-        <v>798</v>
+        <v>796</v>
       </c>
       <c r="M109" s="9" t="s">
         <v>556</v>
@@ -8544,13 +8544,13 @@
         <v>223</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>686</v>
+        <v>684</v>
       </c>
       <c r="D110" s="6" t="s">
         <v>82</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>1006</v>
+        <v>1004</v>
       </c>
       <c r="F110" s="6" t="s">
         <v>455</v>
@@ -8565,19 +8565,19 @@
         <v>350</v>
       </c>
       <c r="J110" s="9" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="K110" s="10" t="s">
-        <v>676</v>
+        <v>674</v>
       </c>
       <c r="L110" s="9" t="s">
-        <v>799</v>
+        <v>797</v>
       </c>
       <c r="M110" s="9" t="s">
         <v>557</v>
       </c>
       <c r="N110" s="10" t="s">
-        <v>886</v>
+        <v>884</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
@@ -8588,13 +8588,13 @@
         <v>223</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>678</v>
+        <v>676</v>
       </c>
       <c r="D111" s="6" t="s">
         <v>60</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>952</v>
+        <v>950</v>
       </c>
       <c r="F111" s="6" t="s">
         <v>456</v>
@@ -8609,13 +8609,13 @@
         <v>351</v>
       </c>
       <c r="J111" s="9" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
       <c r="K111" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L111" s="9" t="s">
-        <v>800</v>
+        <v>798</v>
       </c>
       <c r="M111" s="9" t="s">
         <v>558</v>
@@ -8638,7 +8638,7 @@
         <v>64</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>1008</v>
+        <v>1006</v>
       </c>
       <c r="F112" s="6" t="s">
         <v>457</v>
@@ -8647,19 +8647,19 @@
         <v>110</v>
       </c>
       <c r="H112" s="6" t="s">
-        <v>851</v>
+        <v>849</v>
       </c>
       <c r="I112" s="4" t="s">
         <v>352</v>
       </c>
       <c r="J112" s="9" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="K112" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L112" s="10" t="s">
-        <v>801</v>
+        <v>799</v>
       </c>
       <c r="M112" s="9" t="s">
         <v>559</v>
@@ -8682,7 +8682,7 @@
         <v>77</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>938</v>
+        <v>936</v>
       </c>
       <c r="F113" s="6" t="s">
         <v>458</v>
@@ -8697,19 +8697,19 @@
         <v>353</v>
       </c>
       <c r="J113" s="9" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
       <c r="K113" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L113" s="10" t="s">
-        <v>802</v>
+        <v>800</v>
       </c>
       <c r="M113" s="17" t="s">
         <v>559</v>
       </c>
       <c r="N113" s="10" t="s">
-        <v>887</v>
+        <v>885</v>
       </c>
     </row>
     <row r="114" spans="1:14" ht="184.8" x14ac:dyDescent="0.3">
@@ -8720,13 +8720,13 @@
         <v>223</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D114" s="6" t="s">
         <v>41</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>982</v>
+        <v>980</v>
       </c>
       <c r="F114" s="6" t="s">
         <v>459</v>
@@ -8741,13 +8741,13 @@
         <v>354</v>
       </c>
       <c r="J114" s="9" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
       <c r="K114" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L114" s="9" t="s">
-        <v>803</v>
+        <v>801</v>
       </c>
       <c r="M114" s="9" t="s">
         <v>560</v>
@@ -8764,16 +8764,16 @@
         <v>223</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>680</v>
+        <v>678</v>
       </c>
       <c r="D115" s="6" t="s">
         <v>251</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>939</v>
+        <v>937</v>
       </c>
       <c r="F115" s="6" t="s">
-        <v>826</v>
+        <v>824</v>
       </c>
       <c r="G115" s="4" t="s">
         <v>110</v>
@@ -8785,13 +8785,13 @@
         <v>355</v>
       </c>
       <c r="J115" s="9" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="K115" s="10" t="s">
         <v>111</v>
       </c>
       <c r="L115" s="9" t="s">
-        <v>804</v>
+        <v>802</v>
       </c>
       <c r="M115" s="9" t="s">
         <v>477</v>
@@ -8808,13 +8808,13 @@
         <v>223</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>679</v>
+        <v>677</v>
       </c>
       <c r="D116" s="6" t="s">
         <v>252</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>983</v>
+        <v>981</v>
       </c>
       <c r="F116" s="6" t="s">
         <v>460</v>
@@ -8829,13 +8829,13 @@
         <v>356</v>
       </c>
       <c r="J116" s="9" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="K116" s="14" t="s">
         <v>110</v>
       </c>
       <c r="L116" s="9" t="s">
-        <v>805</v>
+        <v>803</v>
       </c>
       <c r="M116" s="9" t="s">
         <v>561</v>
@@ -8846,16 +8846,16 @@
     </row>
     <row r="117" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A117" s="16" t="s">
-        <v>677</v>
+        <v>675</v>
       </c>
       <c r="B117" s="4" t="s">
         <v>223</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>687</v>
+        <v>685</v>
       </c>
       <c r="D117" s="15" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="F117" s="16" t="s">
         <v>110</v>
@@ -8864,7 +8864,7 @@
         <v>110</v>
       </c>
       <c r="I117" s="16" t="s">
-        <v>695</v>
+        <v>693</v>
       </c>
       <c r="J117" s="11" t="s">
         <v>110</v>
@@ -9025,7 +9025,7 @@
     <hyperlink ref="J38" r:id="rId138" display="https://www.linkedin.com/in/harshul-yagnik-81a6a022/" xr:uid="{683E4E91-B763-4226-99B6-F3E30837AD4B}"/>
     <hyperlink ref="J21" r:id="rId139" display="https://www.linkedin.com/in/brinda-patel-652073252" xr:uid="{791133CF-E0A2-4B6D-8618-AC19B4D3A9FA}"/>
     <hyperlink ref="J28" r:id="rId140" xr:uid="{F8104DB3-2B23-47B7-B622-17690E08D84A}"/>
-    <hyperlink ref="J97" r:id="rId141" display="https://www.linkedin.com/in/sagarkumar-patel-0bb94bb5/" xr:uid="{B357E631-0C5E-406B-9B45-A421DE003AD4}"/>
+    <hyperlink ref="J97" r:id="rId141" xr:uid="{B357E631-0C5E-406B-9B45-A421DE003AD4}"/>
     <hyperlink ref="J70" r:id="rId142" display="http://www.linkedin.com/in/neha-chauhan22" xr:uid="{E7A9417A-8B16-4D59-A23C-B258564D85D5}"/>
     <hyperlink ref="J22" r:id="rId143" xr:uid="{895691E5-0B23-47DD-9A36-18923B4FD652}"/>
     <hyperlink ref="J39" r:id="rId144" display="https://www.linkedin.com/public-profile/settings?trk=d_flagship3_profile_self_view_public_profile" xr:uid="{E4C32594-CCCB-41B2-AE51-AE67F83944BE}"/>
@@ -9034,7 +9034,7 @@
     <hyperlink ref="J24" r:id="rId147" display="https://www.linkedin.com/in/dhara-patel-839488138" xr:uid="{27C9FC8C-0A44-49AE-8688-8690C8579833}"/>
     <hyperlink ref="J26" r:id="rId148" display="https://www.linkedin.com/in/dharmendrasinh-chauhan-073a491a4/" xr:uid="{D50E69C7-4F51-4D1B-90EC-FE9F9A44906E}"/>
     <hyperlink ref="J90" r:id="rId149" display="https://www.linkedin.com/in/rajnik-katriya/" xr:uid="{3AEC1C40-35D9-4AE3-A7E8-9E58FA2C8E43}"/>
-    <hyperlink ref="J98" r:id="rId150" display="https://www.linkedin.com/in/sanket-suthar-544a69210/" xr:uid="{6137F2DC-1F93-4037-B861-A959BDB6DCE6}"/>
+    <hyperlink ref="J98" r:id="rId150" xr:uid="{6137F2DC-1F93-4037-B861-A959BDB6DCE6}"/>
     <hyperlink ref="J53" r:id="rId151" display="http://www.linkedin.com/in/kundan-patel-b9508b27b" xr:uid="{D4BB537A-7CA1-4F2B-9985-F5921034561E}"/>
     <hyperlink ref="J81" r:id="rId152" xr:uid="{BFFCC995-B6DF-474C-93AA-BDF180E05422}"/>
     <hyperlink ref="J111" r:id="rId153" display="https://www.linkedin.com/in/vidisha-pradhan-733a1b63/" xr:uid="{06E43119-E5BC-45C4-9126-F192D3006C5B}"/>

</xml_diff>

<commit_message>
Membership in Prof. Org & Certi. Columns added
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\CSPIT_Main\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C19EE12-9DBC-4A9B-A6D5-84EE6E7D60B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E3FC34-D802-42B5-97D9-49FE93FD7A06}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1631" uniqueCount="1004">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1841" uniqueCount="1105">
   <si>
     <t>Name</t>
   </si>
@@ -3199,12 +3199,351 @@
   <si>
     <t>kunalbhatt.ee@charusat.ac.in</t>
   </si>
+  <si>
+    <t>Membership in Professional Organization / Society</t>
+  </si>
+  <si>
+    <t>Professional Certification Earned</t>
+  </si>
+  <si>
+    <t>SCRS</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>1. IEEE
+2. ISTE</t>
+  </si>
+  <si>
+    <t>1. Microsoft Certified : Azure Fundamentals
+2. Microsoft Certified: Azure AI Fundamentals</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certified Information Security Manager® (CISM®) </t>
+  </si>
+  <si>
+    <t>CSI</t>
+  </si>
+  <si>
+    <t>Microsoft Certified: Azure AI Fundamentals</t>
+  </si>
+  <si>
+    <t>Internal Auditor ISO/IEC 17025-2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISTE, SAEINDIA, </t>
+  </si>
+  <si>
+    <t>FORMULA BHARAT JUDGE</t>
+  </si>
+  <si>
+    <t>ACM</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>IEEE</t>
+  </si>
+  <si>
+    <t>IEEE,ISTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. CSI Associate Life Member, 
+2. ISTD Life Member, 
+3. CII-HR Panel member
+4. CII-Industry Academia Panel member 
+</t>
+  </si>
+  <si>
+    <t>Microsoft Certifed Professional (MCP)</t>
+  </si>
+  <si>
+    <t>ISTE</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>The Institution of Engineers (India)</t>
+  </si>
+  <si>
+    <t>Soft Computing Research Society(SCRS)</t>
+  </si>
+  <si>
+    <t>NPTEL Introduction to Internet of Things</t>
+  </si>
+  <si>
+    <t>ISTE, Soft Computing Research Society</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Networking Fundamental By Microsoft Technology </t>
+  </si>
+  <si>
+    <t>--</t>
+  </si>
+  <si>
+    <t>AWS Cloud Practitioner</t>
+  </si>
+  <si>
+    <t>Microsoft Certified: Azure Fundamentals
+Microsoft Certified: Azure AI Fundamentals</t>
+  </si>
+  <si>
+    <t>IEEE (Professional) and ISTE</t>
+  </si>
+  <si>
+    <t>Microsoft Azure AZ-900</t>
+  </si>
+  <si>
+    <t>nil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">	Life Member Of  Indian Society For Technical Education(LM55005)
+	Life Member Of Indian Institution Of Industrial Engineering LM( 434499)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certified ‘IGBC Accredited Professional – Associate’ by Indian Green Building Council, CII on 
+September 2021 </t>
+  </si>
+  <si>
+    <t>CSWA SOLIDWORKS CAD design Associate</t>
+  </si>
+  <si>
+    <t>Google Business Intelligence</t>
+  </si>
+  <si>
+    <t>International Association of Engineers (IAENG)</t>
+  </si>
+  <si>
+    <t>n.a.</t>
+  </si>
+  <si>
+    <t>3 IEEE and 4. ISTE</t>
+  </si>
+  <si>
+    <t>1. NPTEL certificate 
+subjects:- Applied Natural Language Processing 
+Python for Data Science,	
+Introduction to Research,
+Deep Learning</t>
+  </si>
+  <si>
+    <t>No Membership</t>
+  </si>
+  <si>
+    <t>No certification as such</t>
+  </si>
+  <si>
+    <t>Deep learning Specialization, AWS Academy Machine Learning Foundation, MLOps Specialization</t>
+  </si>
+  <si>
+    <t>SCRS (Soft Computing Research Society) - 2024-04-15-5421</t>
+  </si>
+  <si>
+    <t>AWS cloud Practitioner Certification</t>
+  </si>
+  <si>
+    <t>Laboratory Management System as per ISO/IEC 17025:2017 &amp; Internal Audit</t>
+  </si>
+  <si>
+    <t>IEEE, EuMA, IE, IETE, ISTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Metamaterials and Metasurface using Circuit Theory under CCE-Proficience Programme, IISc Bengaluru </t>
+  </si>
+  <si>
+    <t>Istec Vibration Category 1+ Certification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IEEE, </t>
+  </si>
+  <si>
+    <t>"Certified Blockchain Associate" by Kerala Blockchain Academy, “Certified 365 fundamentals” by Microsoft, “Certified Security, Compliance and Identity Fundamentals” by Microsoft, “Certified Azure Fundamentals” by Microsoft</t>
+  </si>
+  <si>
+    <t>1. IE (India), 2. ISTE, 3. IETE, 4. SAISE</t>
+  </si>
+  <si>
+    <t>1. Google Data Analytics
+2. ARPIT-2020 (Electronic Systems for Sensor Application)
+3. AICTE UHV-I and UHV-II</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Soft Computing Research Society (SCRS) </t>
+  </si>
+  <si>
+    <t>Space Society of Mechanical Engineers (SSME), Society of Automotive Engineers (SAE), Composite Excellence Centre for Asia (CECA), Indian Society for Technical Education (ISTE)</t>
+  </si>
+  <si>
+    <t>Soft Computing Research Society</t>
+  </si>
+  <si>
+    <t>Not Applicable</t>
+  </si>
+  <si>
+    <t>ISTE, AMM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institute of Engineer India, The Indian society for Technical Education, </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certified "IGBC Accredited Professional – Associate’ by Indian Green Building Council, CII </t>
+  </si>
+  <si>
+    <t>1. Laboratory Management System Awareness &amp;  Auditing (As per ISO / IEC  17025 : 2017 &amp; NABL Requirements)
+2. Internal audit as per ISO 9001:2015 Quality management system (QMS)</t>
+  </si>
+  <si>
+    <t>Microsoft Certified: Security, Compliance, and Identity Fundamentals</t>
+  </si>
+  <si>
+    <t>IEEE, ISTE</t>
+  </si>
+  <si>
+    <t>American Concrete Institute (ACI)
+Indian Concrete Institute (ICI)</t>
+  </si>
+  <si>
+    <t>Energy Auditor, Energy Manager</t>
+  </si>
+  <si>
+    <t>1. Oracle Cloud Data Management Certified Foundation Associate.  
+2. Microsoft Technology Associate: Database Administration Fundamentals</t>
+  </si>
+  <si>
+    <t>ISO 9001:2015 Internal Auditor (Quality Management System Training)</t>
+  </si>
+  <si>
+    <t>Red Hat Systems Administration , Microsoft Certified (Azure Fundamentals)</t>
+  </si>
+  <si>
+    <t>AWS Solution Architect Associate, EC Council  Certified Ethical Hacking</t>
+  </si>
+  <si>
+    <t>Salesforce B2C Commerce  Developer</t>
+  </si>
+  <si>
+    <t>Institute of Engineer India, Structural Engineering Forum of India</t>
+  </si>
+  <si>
+    <t>CSI, ISTE, IEEE, IEI</t>
+  </si>
+  <si>
+    <t>ISTE--</t>
+  </si>
+  <si>
+    <t>Renewal Pending in IEEE</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>1. Association for Computing Machinery
+2. South Asia Institute of Science and Engineering
+3. International Association of Engineers</t>
+  </si>
+  <si>
+    <t>1. Certified Cloud Security Engineer by EC-Council
+2. Certified Blockchain Associate by Kerala Blockchain Academy
+3. Microsoft Certified: Security, Compliance, and Identity Fundamentals by Microsoft 
+4. Certified Network Defender by EC-Council
+5. EC-Council Certified Incident Handler by EC-Council 
+6. Computer Hacking Forensic Investigator by EC-Council 
+7. Certified EC-Council Instructor by EC-Council 
+8. Certified Ethical Hacker by EC-Council 
+9. Microsoft Azure Fundamentals by Microsoft 
+10. Google Associate Cloud Engineer by Google 
+11. Oracle Autonomous Database Cloud 2019 Certified Specialist by Oracle
+12. Oracle Cloud Infrastructure Foundations 2020 Certified Associate by Oracle</t>
+  </si>
+  <si>
+    <t>Composites Excellence Center of Asia, International Society for Research and Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ACM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">•	Microsoft Certified Networking Fundamentals ,
+certification on National Programming Aptitude Test </t>
+  </si>
+  <si>
+    <t>NPTEL Certification (Blockchain Technology)</t>
+  </si>
+  <si>
+    <t>IAENG</t>
+  </si>
+  <si>
+    <t>AWS Solution Architecture Associate</t>
+  </si>
+  <si>
+    <t>CSI,IETF</t>
+  </si>
+  <si>
+    <t>CCNA Instructor, CCNSP Instructor</t>
+  </si>
+  <si>
+    <t>NONE</t>
+  </si>
+  <si>
+    <t>ISTE (LM 82407), CECA (20207067)</t>
+  </si>
+  <si>
+    <t>1. IEEE- Senior Member
+2. ISTE</t>
+  </si>
+  <si>
+    <t>AWS cloud practitioner certification, Microsoft Azure Fundamentals</t>
+  </si>
+  <si>
+    <t>Google Advanced Data Analytics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 nptel certification </t>
+  </si>
+  <si>
+    <t>ISTE, ISA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trainer, Automation Technologies, </t>
+  </si>
+  <si>
+    <t>CISCO CERTIFIED NETWORK ASSOCIATE, CISCO CERTIFIED ACADEMY INSTRUCTOR</t>
+  </si>
+  <si>
+    <t>NPTEL-Internet of Things</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ethical Hacking </t>
+  </si>
+  <si>
+    <t>Institution of Engineers (IE), ISTE, AMM, ISRD</t>
+  </si>
+  <si>
+    <t>Autodesk certifications on AutoCAD</t>
+  </si>
+  <si>
+    <t>1. Google Data Analytics 
+2. Google Advanced Data Analytics
+3. Google AI Essentials</t>
+  </si>
+  <si>
+    <t>STRUCTURAL ENGINEERING FORUM OF INDIA [SEFI]</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3276,6 +3615,13 @@
       <sz val="10"/>
       <name val="Roboto"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -3291,7 +3637,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -3314,13 +3660,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -3377,10 +3736,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3696,10 +4080,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N117"/>
+  <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="82" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScale="76" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3713,9 +4097,10 @@
     <col min="12" max="12" width="34.88671875" style="12" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="43.21875" style="12" customWidth="1"/>
     <col min="14" max="14" width="25.88671875" style="12"/>
+    <col min="15" max="16" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="3" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="3" customFormat="1" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3755,11 +4140,17 @@
       <c r="M1" s="13" t="s">
         <v>681</v>
       </c>
-      <c r="N1" s="13" t="s">
+      <c r="N1" s="24" t="s">
         <v>759</v>
       </c>
-    </row>
-    <row r="2" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O1" s="13" t="s">
+        <v>1004</v>
+      </c>
+      <c r="P1" s="13" t="s">
+        <v>1005</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>881</v>
       </c>
@@ -3799,11 +4190,17 @@
       <c r="M2" s="9" t="s">
         <v>352</v>
       </c>
-      <c r="N2" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="3" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="N2" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O2" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P2" s="21" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>994</v>
       </c>
@@ -3843,11 +4240,17 @@
       <c r="M3" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="26" t="s">
         <v>723</v>
       </c>
-    </row>
-    <row r="4" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="O3" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="P3" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>882</v>
       </c>
@@ -3887,11 +4290,17 @@
       <c r="M4" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="N4" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N4" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O4" s="21" t="s">
+        <v>1008</v>
+      </c>
+      <c r="P4" s="21" t="s">
+        <v>1009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>883</v>
       </c>
@@ -3931,11 +4340,17 @@
       <c r="M5" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="N5" s="6" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N5" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O5" s="21" t="s">
+        <v>532</v>
+      </c>
+      <c r="P5" s="21" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>884</v>
       </c>
@@ -3975,11 +4390,17 @@
       <c r="M6" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="N6" s="4" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="N6" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="21" t="s">
+        <v>1010</v>
+      </c>
+      <c r="P6" s="21" t="s">
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>885</v>
       </c>
@@ -4019,11 +4440,17 @@
       <c r="M7" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="N7" s="10" t="s">
+      <c r="N7" s="26" t="s">
         <v>724</v>
       </c>
-    </row>
-    <row r="8" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O7" s="21" t="s">
+        <v>1012</v>
+      </c>
+      <c r="P7" s="21" t="s">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>886</v>
       </c>
@@ -4063,11 +4490,15 @@
       <c r="M8" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="N8" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="O8" s="22"/>
+      <c r="P8" s="21" t="s">
+        <v>1014</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>887</v>
       </c>
@@ -4107,11 +4538,17 @@
       <c r="M9" s="9" t="s">
         <v>358</v>
       </c>
-      <c r="N9" s="10" t="s">
+      <c r="N9" s="26" t="s">
         <v>725</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="O9" s="21" t="s">
+        <v>1015</v>
+      </c>
+      <c r="P9" s="21" t="s">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>888</v>
       </c>
@@ -4151,11 +4588,17 @@
       <c r="M10" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N10" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" ht="145.19999999999999" x14ac:dyDescent="0.3">
+      <c r="N10" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O10" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P10" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>889</v>
       </c>
@@ -4195,11 +4638,17 @@
       <c r="M11" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N11" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" ht="198" x14ac:dyDescent="0.3">
+      <c r="N11" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O11" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P11" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="198" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>890</v>
       </c>
@@ -4239,11 +4688,17 @@
       <c r="M12" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="N12" s="10" t="s">
+      <c r="N12" s="26" t="s">
         <v>726</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" ht="105.6" x14ac:dyDescent="0.3">
+      <c r="O12" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P12" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>891</v>
       </c>
@@ -4283,11 +4738,17 @@
       <c r="M13" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N13" s="10" t="s">
+      <c r="N13" s="26" t="s">
         <v>727</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="O13" s="21" t="s">
+        <v>1020</v>
+      </c>
+      <c r="P13" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>892</v>
       </c>
@@ -4327,11 +4788,17 @@
       <c r="M14" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="N14" s="10" t="s">
+      <c r="N14" s="26" t="s">
         <v>728</v>
       </c>
-    </row>
-    <row r="15" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="O14" s="21" t="s">
+        <v>1021</v>
+      </c>
+      <c r="P14" s="21" t="s">
+        <v>1022</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>893</v>
       </c>
@@ -4371,11 +4838,17 @@
       <c r="M15" s="9" t="s">
         <v>362</v>
       </c>
-      <c r="N15" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N15" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O15" s="21" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P15" s="21" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>894</v>
       </c>
@@ -4415,11 +4888,17 @@
       <c r="M16" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="N16" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14" ht="211.2" x14ac:dyDescent="0.3">
+      <c r="N16" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O16" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="P16" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="211.2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
         <v>895</v>
       </c>
@@ -4459,11 +4938,17 @@
       <c r="M17" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="N17" s="10" t="s">
+      <c r="N17" s="26" t="s">
         <v>729</v>
       </c>
-    </row>
-    <row r="18" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="O17" s="21" t="s">
+        <v>1025</v>
+      </c>
+      <c r="P17" s="21" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>896</v>
       </c>
@@ -4503,11 +4988,15 @@
       <c r="M18" s="9" t="s">
         <v>364</v>
       </c>
-      <c r="N18" s="10" t="s">
+      <c r="N18" s="26" t="s">
         <v>730</v>
       </c>
-    </row>
-    <row r="19" spans="1:14" ht="132" x14ac:dyDescent="0.3">
+      <c r="O18" s="21" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P18" s="21"/>
+    </row>
+    <row r="19" spans="1:16" ht="132" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
         <v>897</v>
       </c>
@@ -4547,11 +5036,17 @@
       <c r="M19" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="N19" s="10" t="s">
+      <c r="N19" s="26" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="20" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="O19" s="21" t="s">
+        <v>1026</v>
+      </c>
+      <c r="P19" s="21" t="s">
+        <v>1027</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
         <v>898</v>
       </c>
@@ -4591,11 +5086,17 @@
       <c r="M20" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N20" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N20" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O20" s="21" t="s">
+        <v>1028</v>
+      </c>
+      <c r="P20" s="21" t="s">
+        <v>1029</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
         <v>899</v>
       </c>
@@ -4635,11 +5136,17 @@
       <c r="M21" s="9" t="s">
         <v>366</v>
       </c>
-      <c r="N21" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N21" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O21" s="21" t="s">
+        <v>1018</v>
+      </c>
+      <c r="P21" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
         <v>900</v>
       </c>
@@ -4679,11 +5186,17 @@
       <c r="M22" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="N22" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N22" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O22" s="21" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P22" s="21" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
         <v>901</v>
       </c>
@@ -4723,11 +5236,17 @@
       <c r="M23" s="9" t="s">
         <v>368</v>
       </c>
-      <c r="N23" s="10" t="s">
+      <c r="N23" s="26" t="s">
         <v>732</v>
       </c>
-    </row>
-    <row r="24" spans="1:14" ht="211.2" x14ac:dyDescent="0.3">
+      <c r="O23" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P23" s="21" t="s">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="211.2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
         <v>902</v>
       </c>
@@ -4767,11 +5286,17 @@
       <c r="M24" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="N24" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="25" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N24" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O24" s="21" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P24" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
         <v>903</v>
       </c>
@@ -4811,11 +5336,17 @@
       <c r="M25" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="N25" s="10" t="s">
+      <c r="N25" s="26" t="s">
         <v>733</v>
       </c>
-    </row>
-    <row r="26" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="O25" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P25" s="21" t="s">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
         <v>993</v>
       </c>
@@ -4855,11 +5386,17 @@
       <c r="M26" s="9" t="s">
         <v>370</v>
       </c>
-      <c r="N26" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="27" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="N26" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O26" s="21" t="s">
+        <v>1033</v>
+      </c>
+      <c r="P26" s="21" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A27" s="4" t="s">
         <v>904</v>
       </c>
@@ -4899,11 +5436,17 @@
       <c r="M27" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="N27" s="10" t="s">
+      <c r="N27" s="26" t="s">
         <v>734</v>
       </c>
-    </row>
-    <row r="28" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="O27" s="21" t="s">
+        <v>1033</v>
+      </c>
+      <c r="P27" s="21" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A28" s="4" t="s">
         <v>905</v>
       </c>
@@ -4943,11 +5486,17 @@
       <c r="M28" s="9" t="s">
         <v>360</v>
       </c>
-      <c r="N28" s="10" t="s">
+      <c r="N28" s="26" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="29" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="O28" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P28" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A29" s="4" t="s">
         <v>906</v>
       </c>
@@ -4987,11 +5536,17 @@
       <c r="M29" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="N29" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="N29" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O29" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P29" s="21" t="s">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A30" s="4" t="s">
         <v>907</v>
       </c>
@@ -5031,11 +5586,17 @@
       <c r="M30" s="17">
         <v>583944</v>
       </c>
-      <c r="N30" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" ht="264" x14ac:dyDescent="0.3">
+      <c r="N30" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O30" s="21" t="s">
+        <v>1035</v>
+      </c>
+      <c r="P30" s="21" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="264" x14ac:dyDescent="0.3">
       <c r="A31" s="4" t="s">
         <v>908</v>
       </c>
@@ -5075,11 +5636,17 @@
       <c r="M31" s="9" t="s">
         <v>678</v>
       </c>
-      <c r="N31" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="32" spans="1:14" ht="198" x14ac:dyDescent="0.3">
+      <c r="N31" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O31" s="23" t="s">
+        <v>1036</v>
+      </c>
+      <c r="P31" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="198" x14ac:dyDescent="0.3">
       <c r="A32" s="4" t="s">
         <v>909</v>
       </c>
@@ -5119,11 +5686,15 @@
       <c r="M32" s="9" t="s">
         <v>679</v>
       </c>
-      <c r="N32" s="10" t="s">
+      <c r="N32" s="26" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="33" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="O32" s="22"/>
+      <c r="P32" s="21" t="s">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A33" s="4" t="s">
         <v>910</v>
       </c>
@@ -5163,11 +5734,15 @@
       <c r="M33" s="9" t="s">
         <v>373</v>
       </c>
-      <c r="N33" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="34" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N33" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21" t="s">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A34" s="4" t="s">
         <v>911</v>
       </c>
@@ -5207,11 +5782,17 @@
       <c r="M34" s="9" t="s">
         <v>374</v>
       </c>
-      <c r="N34" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="35" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="N34" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O34" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="P34" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A35" s="4" t="s">
         <v>992</v>
       </c>
@@ -5251,11 +5832,17 @@
       <c r="M35" s="9" t="s">
         <v>375</v>
       </c>
-      <c r="N35" s="10" t="s">
+      <c r="N35" s="26" t="s">
         <v>737</v>
       </c>
-    </row>
-    <row r="36" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="O35" s="21" t="s">
+        <v>1020</v>
+      </c>
+      <c r="P35" s="21" t="s">
+        <v>1039</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A36" s="4" t="s">
         <v>912</v>
       </c>
@@ -5295,11 +5882,17 @@
       <c r="M36" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="N36" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="37" spans="1:14" ht="132" x14ac:dyDescent="0.3">
+      <c r="N36" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O36" s="21" t="s">
+        <v>1040</v>
+      </c>
+      <c r="P36" s="21" t="s">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="132" x14ac:dyDescent="0.3">
       <c r="A37" s="4" t="s">
         <v>913</v>
       </c>
@@ -5339,11 +5932,17 @@
       <c r="M37" s="9" t="s">
         <v>377</v>
       </c>
-      <c r="N37" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="38" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="N37" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O37" s="21" t="s">
+        <v>1042</v>
+      </c>
+      <c r="P37" s="21" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A38" s="4" t="s">
         <v>914</v>
       </c>
@@ -5383,11 +5982,17 @@
       <c r="M38" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="N38" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N38" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O38" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P38" s="21" t="s">
+        <v>1043</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A39" s="4" t="s">
         <v>915</v>
       </c>
@@ -5427,11 +6032,17 @@
       <c r="M39" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="N39" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="40" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N39" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O39" s="21" t="s">
+        <v>1044</v>
+      </c>
+      <c r="P39" s="21" t="s">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>916</v>
       </c>
@@ -5471,11 +6082,17 @@
       <c r="M40" s="9" t="s">
         <v>379</v>
       </c>
-      <c r="N40" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="41" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N40" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O40" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P40" s="21" t="s">
+        <v>1046</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A41" s="4" t="s">
         <v>917</v>
       </c>
@@ -5515,11 +6132,17 @@
       <c r="M41" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="N41" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N41" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="O41" s="21" t="s">
+        <v>532</v>
+      </c>
+      <c r="P41" s="21" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A42" s="4" t="s">
         <v>918</v>
       </c>
@@ -5559,11 +6182,17 @@
       <c r="M42" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="N42" s="10" t="s">
+      <c r="N42" s="26" t="s">
         <v>738</v>
       </c>
-    </row>
-    <row r="43" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="O42" s="21" t="s">
+        <v>1047</v>
+      </c>
+      <c r="P42" s="21" t="s">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A43" s="4" t="s">
         <v>919</v>
       </c>
@@ -5603,11 +6232,15 @@
       <c r="M43" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="N43" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="44" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N43" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21" t="s">
+        <v>1049</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A44" s="4" t="s">
         <v>920</v>
       </c>
@@ -5647,11 +6280,17 @@
       <c r="M44" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="N44" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="45" spans="1:14" ht="290.39999999999998" x14ac:dyDescent="0.3">
+      <c r="N44" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O44" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P44" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="290.39999999999998" x14ac:dyDescent="0.3">
       <c r="A45" s="4" t="s">
         <v>921</v>
       </c>
@@ -5691,11 +6330,15 @@
       <c r="M45" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="N45" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="N45" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A46" s="4" t="s">
         <v>922</v>
       </c>
@@ -5735,11 +6378,17 @@
       <c r="M46" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="N46" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N46" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O46" s="21" t="s">
+        <v>107</v>
+      </c>
+      <c r="P46" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A47" s="4" t="s">
         <v>923</v>
       </c>
@@ -5779,11 +6428,17 @@
       <c r="M47" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N47" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" ht="105.6" x14ac:dyDescent="0.3">
+      <c r="N47" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O47" s="21" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P47" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="105.6" x14ac:dyDescent="0.3">
       <c r="A48" s="4" t="s">
         <v>924</v>
       </c>
@@ -5823,11 +6478,17 @@
       <c r="M48" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="N48" s="10" t="s">
+      <c r="N48" s="26" t="s">
         <v>739</v>
       </c>
-    </row>
-    <row r="49" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="O48" s="21" t="s">
+        <v>1050</v>
+      </c>
+      <c r="P48" s="21" t="s">
+        <v>1051</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>925</v>
       </c>
@@ -5867,11 +6528,17 @@
       <c r="M49" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="N49" s="10" t="s">
+      <c r="N49" s="26" t="s">
         <v>740</v>
       </c>
-    </row>
-    <row r="50" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="O49" s="21" t="s">
+        <v>1040</v>
+      </c>
+      <c r="P49" s="21" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A50" s="4" t="s">
         <v>926</v>
       </c>
@@ -5911,11 +6578,17 @@
       <c r="M50" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N50" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N50" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O50" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P50" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A51" s="4" t="s">
         <v>1000</v>
       </c>
@@ -5936,7 +6609,7 @@
         <v>106</v>
       </c>
       <c r="H51" s="6"/>
-      <c r="I51" s="21" t="s">
+      <c r="I51" s="20" t="s">
         <v>1003</v>
       </c>
       <c r="J51" s="9"/>
@@ -5945,11 +6618,13 @@
       </c>
       <c r="L51" s="9"/>
       <c r="M51" s="9"/>
-      <c r="N51" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="52" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N51" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+    </row>
+    <row r="52" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="4" t="s">
         <v>927</v>
       </c>
@@ -5989,11 +6664,15 @@
       <c r="M52" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="N52" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="53" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="N52" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O52" s="21"/>
+      <c r="P52" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A53" s="4" t="s">
         <v>928</v>
       </c>
@@ -6033,11 +6712,17 @@
       <c r="M53" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="N53" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="54" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="N53" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O53" s="21" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P53" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A54" s="4" t="s">
         <v>929</v>
       </c>
@@ -6077,11 +6762,17 @@
       <c r="M54" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="N54" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="55" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N54" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O54" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="P54" s="21" t="s">
+        <v>1052</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A55" s="4" t="s">
         <v>930</v>
       </c>
@@ -6121,11 +6812,17 @@
       <c r="M55" s="9" t="s">
         <v>389</v>
       </c>
-      <c r="N55" s="10" t="s">
+      <c r="N55" s="26" t="s">
         <v>741</v>
       </c>
-    </row>
-    <row r="56" spans="1:14" ht="171.6" x14ac:dyDescent="0.3">
+      <c r="O55" s="21" t="s">
+        <v>1053</v>
+      </c>
+      <c r="P55" s="21" t="s">
+        <v>1054</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="171.6" x14ac:dyDescent="0.3">
       <c r="A56" s="4" t="s">
         <v>931</v>
       </c>
@@ -6165,11 +6862,17 @@
       <c r="M56" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="N56" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="57" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="N56" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O56" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P56" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A57" s="4" t="s">
         <v>932</v>
       </c>
@@ -6209,11 +6912,17 @@
       <c r="M57" s="9" t="s">
         <v>391</v>
       </c>
-      <c r="N57" s="10" t="s">
+      <c r="N57" s="26" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="58" spans="1:14" ht="132" x14ac:dyDescent="0.3">
+      <c r="O57" s="21" t="s">
+        <v>1055</v>
+      </c>
+      <c r="P57" s="21" t="s">
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" ht="132" x14ac:dyDescent="0.3">
       <c r="A58" s="4" t="s">
         <v>933</v>
       </c>
@@ -6253,11 +6962,17 @@
       <c r="M58" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="N58" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="59" spans="1:14" ht="356.4" x14ac:dyDescent="0.3">
+      <c r="N58" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O58" s="21" t="s">
+        <v>1057</v>
+      </c>
+      <c r="P58" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="59" spans="1:16" ht="356.4" x14ac:dyDescent="0.3">
       <c r="A59" s="4" t="s">
         <v>934</v>
       </c>
@@ -6297,11 +7012,17 @@
       <c r="M59" s="9" t="s">
         <v>393</v>
       </c>
-      <c r="N59" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="60" spans="1:14" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="N59" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O59" s="21" t="s">
+        <v>1058</v>
+      </c>
+      <c r="P59" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" ht="158.4" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>935</v>
       </c>
@@ -6341,11 +7062,17 @@
       <c r="M60" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="N60" s="10" t="s">
+      <c r="N60" s="26" t="s">
         <v>743</v>
       </c>
-    </row>
-    <row r="61" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="O60" s="21" t="s">
+        <v>1059</v>
+      </c>
+      <c r="P60" s="21" t="s">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>936</v>
       </c>
@@ -6385,11 +7112,17 @@
       <c r="M61" s="9" t="s">
         <v>395</v>
       </c>
-      <c r="N61" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="62" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N61" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O61" s="21" t="s">
+        <v>1061</v>
+      </c>
+      <c r="P61" s="21" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A62" s="4" t="s">
         <v>937</v>
       </c>
@@ -6429,11 +7162,17 @@
       <c r="M62" s="9" t="s">
         <v>396</v>
       </c>
-      <c r="N62" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="63" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N62" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O62" s="21" t="s">
+        <v>1062</v>
+      </c>
+      <c r="P62" s="21" t="s">
+        <v>1063</v>
+      </c>
+    </row>
+    <row r="63" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A63" s="4" t="s">
         <v>938</v>
       </c>
@@ -6473,11 +7212,15 @@
       <c r="M63" s="9" t="s">
         <v>397</v>
       </c>
-      <c r="N63" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="64" spans="1:14" ht="132" x14ac:dyDescent="0.3">
+      <c r="N63" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O63" s="21"/>
+      <c r="P63" s="21" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="132" x14ac:dyDescent="0.3">
       <c r="A64" s="4" t="s">
         <v>939</v>
       </c>
@@ -6517,11 +7260,17 @@
       <c r="M64" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N64" s="10" t="s">
+      <c r="N64" s="26" t="s">
         <v>735</v>
       </c>
-    </row>
-    <row r="65" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="O64" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P64" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="65" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A65" s="4" t="s">
         <v>940</v>
       </c>
@@ -6561,11 +7310,15 @@
       <c r="M65" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="N65" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="66" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N65" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O65" s="21"/>
+      <c r="P65" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="66" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A66" s="4" t="s">
         <v>941</v>
       </c>
@@ -6605,11 +7358,17 @@
       <c r="M66" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="N66" s="10" t="s">
+      <c r="N66" s="26" t="s">
         <v>744</v>
       </c>
-    </row>
-    <row r="67" spans="1:14" ht="277.2" x14ac:dyDescent="0.3">
+      <c r="O66" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P66" s="21" t="s">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="277.2" x14ac:dyDescent="0.3">
       <c r="A67" s="4" t="s">
         <v>942</v>
       </c>
@@ -6649,11 +7408,17 @@
       <c r="M67" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="N67" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="68" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="N67" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O67" s="21" t="s">
+        <v>1066</v>
+      </c>
+      <c r="P67" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="68" spans="1:16" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A68" s="4" t="s">
         <v>943</v>
       </c>
@@ -6693,11 +7458,17 @@
       <c r="M68" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="N68" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="69" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N68" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O68" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P68" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="69" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A69" s="4" t="s">
         <v>944</v>
       </c>
@@ -6737,11 +7508,17 @@
       <c r="M69" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N69" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="70" spans="1:14" ht="184.8" x14ac:dyDescent="0.3">
+      <c r="N69" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O69" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="P69" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="70" spans="1:16" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A70" s="4" t="s">
         <v>945</v>
       </c>
@@ -6781,11 +7558,17 @@
       <c r="M70" s="9" t="s">
         <v>402</v>
       </c>
-      <c r="N70" s="10" t="s">
+      <c r="N70" s="26" t="s">
         <v>745</v>
       </c>
-    </row>
-    <row r="71" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="O70" s="21" t="s">
+        <v>1067</v>
+      </c>
+      <c r="P70" s="21" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A71" s="4" t="s">
         <v>991</v>
       </c>
@@ -6825,11 +7608,17 @@
       <c r="M71" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="N71" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="72" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="N71" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O71" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P71" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A72" s="4" t="s">
         <v>946</v>
       </c>
@@ -6869,11 +7658,17 @@
       <c r="M72" s="9" t="s">
         <v>404</v>
       </c>
-      <c r="N72" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="73" spans="1:14" ht="184.8" x14ac:dyDescent="0.3">
+      <c r="N72" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O72" s="21" t="s">
+        <v>1066</v>
+      </c>
+      <c r="P72" s="21" t="s">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A73" s="4" t="s">
         <v>947</v>
       </c>
@@ -6913,11 +7708,17 @@
       <c r="M73" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="N73" s="10" t="s">
+      <c r="N73" s="26" t="s">
         <v>746</v>
       </c>
-    </row>
-    <row r="74" spans="1:14" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="O73" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P73" s="21" t="s">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="409.6" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>948</v>
       </c>
@@ -6957,11 +7758,15 @@
       <c r="M74" s="9" t="s">
         <v>406</v>
       </c>
-      <c r="N74" s="10" t="s">
+      <c r="N74" s="26" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="75" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="O74" s="21"/>
+      <c r="P74" s="21" t="s">
+        <v>1070</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A75" s="4" t="s">
         <v>949</v>
       </c>
@@ -7001,11 +7806,17 @@
       <c r="M75" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N75" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="76" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N75" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O75" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="P75" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A76" s="4" t="s">
         <v>950</v>
       </c>
@@ -7045,11 +7856,17 @@
       <c r="M76" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="N76" s="10" t="s">
+      <c r="N76" s="26" t="s">
         <v>747</v>
       </c>
-    </row>
-    <row r="77" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="O76" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P76" s="21" t="s">
+        <v>1071</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A77" s="4" t="s">
         <v>951</v>
       </c>
@@ -7089,11 +7906,15 @@
       <c r="M77" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="N77" s="19" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="78" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N77" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="O77" s="21"/>
+      <c r="P77" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A78" s="4" t="s">
         <v>952</v>
       </c>
@@ -7133,11 +7954,15 @@
       <c r="M78" s="9" t="s">
         <v>408</v>
       </c>
-      <c r="N78" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="79" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N78" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O78" s="21"/>
+      <c r="P78" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A79" s="4" t="s">
         <v>990</v>
       </c>
@@ -7177,11 +8002,17 @@
       <c r="M79" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="N79" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="80" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="N79" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O79" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P79" s="21" t="s">
+        <v>1072</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A80" s="4" t="s">
         <v>953</v>
       </c>
@@ -7221,11 +8052,17 @@
       <c r="M80" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="N80" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="81" spans="1:14" ht="145.19999999999999" x14ac:dyDescent="0.3">
+      <c r="N80" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O80" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P80" s="21" t="s">
+        <v>1073</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A81" s="4" t="s">
         <v>954</v>
       </c>
@@ -7265,11 +8102,17 @@
       <c r="M81" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="N81" s="10" t="s">
+      <c r="N81" s="26" t="s">
         <v>748</v>
       </c>
-    </row>
-    <row r="82" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="O81" s="21" t="s">
+        <v>1074</v>
+      </c>
+      <c r="P81" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="82" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A82" s="4" t="s">
         <v>955</v>
       </c>
@@ -7309,11 +8152,17 @@
       <c r="M82" s="9" t="s">
         <v>412</v>
       </c>
-      <c r="N82" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="83" spans="1:14" ht="118.8" x14ac:dyDescent="0.3">
+      <c r="N82" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O82" s="21" t="s">
+        <v>1075</v>
+      </c>
+      <c r="P82" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A83" s="4" t="s">
         <v>989</v>
       </c>
@@ -7353,11 +8202,17 @@
       <c r="M83" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="N83" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="84" spans="1:14" ht="145.19999999999999" x14ac:dyDescent="0.3">
+      <c r="N83" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O83" s="21" t="s">
+        <v>1076</v>
+      </c>
+      <c r="P83" s="21" t="s">
+        <v>1030</v>
+      </c>
+    </row>
+    <row r="84" spans="1:16" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="4" t="s">
         <v>956</v>
       </c>
@@ -7397,11 +8252,17 @@
       <c r="M84" s="9" t="s">
         <v>414</v>
       </c>
-      <c r="N84" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="85" spans="1:14" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="N84" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O84" s="21" t="s">
+        <v>1077</v>
+      </c>
+      <c r="P84" s="21" t="s">
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="85" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="4" t="s">
         <v>957</v>
       </c>
@@ -7441,11 +8302,17 @@
       <c r="M85" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="N85" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="86" spans="1:14" ht="330" x14ac:dyDescent="0.3">
+      <c r="N85" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O85" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P85" s="21" t="s">
+        <v>1078</v>
+      </c>
+    </row>
+    <row r="86" spans="1:16" ht="330" x14ac:dyDescent="0.3">
       <c r="A86" s="4" t="s">
         <v>958</v>
       </c>
@@ -7485,11 +8352,17 @@
       <c r="M86" s="9" t="s">
         <v>416</v>
       </c>
-      <c r="N86" s="10" t="s">
+      <c r="N86" s="26" t="s">
         <v>749</v>
       </c>
-    </row>
-    <row r="87" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="O86" s="21" t="s">
+        <v>1079</v>
+      </c>
+      <c r="P86" s="21" t="s">
+        <v>1080</v>
+      </c>
+    </row>
+    <row r="87" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A87" s="4" t="s">
         <v>959</v>
       </c>
@@ -7529,11 +8402,17 @@
       <c r="M87" s="9" t="s">
         <v>680</v>
       </c>
-      <c r="N87" s="10" t="s">
+      <c r="N87" s="26" t="s">
         <v>750</v>
       </c>
-    </row>
-    <row r="88" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="O87" s="21" t="s">
+        <v>1012</v>
+      </c>
+      <c r="P87" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A88" s="4" t="s">
         <v>960</v>
       </c>
@@ -7573,11 +8452,17 @@
       <c r="M88" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="N88" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="89" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N88" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O88" s="21" t="s">
+        <v>1081</v>
+      </c>
+      <c r="P88" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="89" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A89" s="4" t="s">
         <v>988</v>
       </c>
@@ -7617,11 +8502,17 @@
       <c r="M89" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="N89" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="90" spans="1:14" ht="290.39999999999998" x14ac:dyDescent="0.3">
+      <c r="N89" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O89" s="21" t="s">
+        <v>1082</v>
+      </c>
+      <c r="P89" s="21" t="s">
+        <v>1083</v>
+      </c>
+    </row>
+    <row r="90" spans="1:16" ht="290.39999999999998" x14ac:dyDescent="0.3">
       <c r="A90" s="4" t="s">
         <v>961</v>
       </c>
@@ -7661,11 +8552,17 @@
       <c r="M90" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="N90" s="10" t="s">
+      <c r="N90" s="26" t="s">
         <v>751</v>
       </c>
-    </row>
-    <row r="91" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="O90" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P90" s="21" t="s">
+        <v>1084</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A91" s="4" t="s">
         <v>962</v>
       </c>
@@ -7705,11 +8602,17 @@
       <c r="M91" s="9" t="s">
         <v>420</v>
       </c>
-      <c r="N91" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="92" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N91" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O91" s="21" t="s">
+        <v>1085</v>
+      </c>
+      <c r="P91" s="21" t="s">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="92" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A92" s="4" t="s">
         <v>963</v>
       </c>
@@ -7749,11 +8652,13 @@
       <c r="M92" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="N92" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="93" spans="1:14" ht="250.8" x14ac:dyDescent="0.3">
+      <c r="N92" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O92" s="9"/>
+      <c r="P92" s="9"/>
+    </row>
+    <row r="93" spans="1:16" ht="250.8" x14ac:dyDescent="0.3">
       <c r="A93" s="4" t="s">
         <v>964</v>
       </c>
@@ -7793,11 +8698,17 @@
       <c r="M93" s="9" t="s">
         <v>422</v>
       </c>
-      <c r="N93" s="10" t="s">
+      <c r="N93" s="26" t="s">
         <v>752</v>
       </c>
-    </row>
-    <row r="94" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="O93" s="21" t="s">
+        <v>1087</v>
+      </c>
+      <c r="P93" s="21" t="s">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="94" spans="1:16" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A94" s="4" t="s">
         <v>965</v>
       </c>
@@ -7837,11 +8748,17 @@
       <c r="M94" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="N94" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="95" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N94" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O94" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P94" s="21" t="s">
+        <v>1089</v>
+      </c>
+    </row>
+    <row r="95" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A95" s="4" t="s">
         <v>965</v>
       </c>
@@ -7881,11 +8798,17 @@
       <c r="M95" s="9" t="s">
         <v>424</v>
       </c>
-      <c r="N95" s="10" t="s">
+      <c r="N95" s="26" t="s">
         <v>753</v>
       </c>
-    </row>
-    <row r="96" spans="1:14" ht="132" x14ac:dyDescent="0.3">
+      <c r="O95" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P95" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="96" spans="1:16" ht="132" x14ac:dyDescent="0.3">
       <c r="A96" s="4" t="s">
         <v>966</v>
       </c>
@@ -7925,11 +8848,17 @@
       <c r="M96" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="N96" s="10" t="s">
+      <c r="N96" s="26" t="s">
         <v>754</v>
       </c>
-    </row>
-    <row r="97" spans="1:14" ht="132" x14ac:dyDescent="0.3">
+      <c r="O96" s="21" t="s">
+        <v>1090</v>
+      </c>
+      <c r="P96" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" ht="132" x14ac:dyDescent="0.3">
       <c r="A97" s="4" t="s">
         <v>967</v>
       </c>
@@ -7969,11 +8898,17 @@
       <c r="M97" s="9" t="s">
         <v>426</v>
       </c>
-      <c r="N97" s="10" t="s">
+      <c r="N97" s="26" t="s">
         <v>742</v>
       </c>
-    </row>
-    <row r="98" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="O97" s="21" t="s">
+        <v>1091</v>
+      </c>
+      <c r="P97" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="98" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A98" s="4" t="s">
         <v>968</v>
       </c>
@@ -8013,11 +8948,17 @@
       <c r="M98" s="9" t="s">
         <v>427</v>
       </c>
-      <c r="N98" s="10" t="s">
+      <c r="N98" s="26" t="s">
         <v>755</v>
       </c>
-    </row>
-    <row r="99" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="O98" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P98" s="21" t="s">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A99" s="4" t="s">
         <v>969</v>
       </c>
@@ -8057,11 +8998,17 @@
       <c r="M99" s="9" t="s">
         <v>428</v>
       </c>
-      <c r="N99" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="100" spans="1:14" ht="39.6" x14ac:dyDescent="0.3">
+      <c r="N99" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O99" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P99" s="21" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="100" spans="1:16" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A100" s="4" t="s">
         <v>970</v>
       </c>
@@ -8101,11 +9048,17 @@
       <c r="M100" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="N100" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="101" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N100" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O100" s="21" t="s">
+        <v>106</v>
+      </c>
+      <c r="P100" s="21" t="s">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A101" s="4" t="s">
         <v>971</v>
       </c>
@@ -8145,11 +9098,17 @@
       <c r="M101" s="9" t="s">
         <v>430</v>
       </c>
-      <c r="N101" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="102" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="N101" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O101" s="21" t="s">
+        <v>1006</v>
+      </c>
+      <c r="P101" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A102" s="4" t="s">
         <v>972</v>
       </c>
@@ -8189,11 +9148,17 @@
       <c r="M102" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="N102" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="103" spans="1:14" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="N102" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O102" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P102" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A103" s="4" t="s">
         <v>973</v>
       </c>
@@ -8233,11 +9198,15 @@
       <c r="M103" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="N103" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="104" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N103" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O103" s="21"/>
+      <c r="P103" s="21" t="s">
+        <v>1094</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A104" s="4" t="s">
         <v>974</v>
       </c>
@@ -8277,11 +9246,17 @@
       <c r="M104" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="N104" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="105" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N104" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O104" s="21" t="s">
+        <v>1095</v>
+      </c>
+      <c r="P104" s="21" t="s">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="105" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A105" s="4" t="s">
         <v>975</v>
       </c>
@@ -8321,11 +9296,17 @@
       <c r="M105" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="N105" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="106" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N105" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O105" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P105" s="21" t="s">
+        <v>1007</v>
+      </c>
+    </row>
+    <row r="106" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A106" s="4" t="s">
         <v>976</v>
       </c>
@@ -8365,11 +9346,17 @@
       <c r="M106" s="9" t="s">
         <v>434</v>
       </c>
-      <c r="N106" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="107" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="N106" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O106" s="21" t="s">
+        <v>1066</v>
+      </c>
+      <c r="P106" s="21" t="s">
+        <v>1097</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A107" s="4" t="s">
         <v>977</v>
       </c>
@@ -8409,11 +9396,17 @@
       <c r="M107" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="N107" s="10" t="s">
+      <c r="N107" s="26" t="s">
         <v>756</v>
       </c>
-    </row>
-    <row r="108" spans="1:14" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="O107" s="21" t="s">
+        <v>1019</v>
+      </c>
+      <c r="P107" s="21" t="s">
+        <v>1018</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A108" s="4" t="s">
         <v>978</v>
       </c>
@@ -8453,11 +9446,15 @@
       <c r="M108" s="9" t="s">
         <v>436</v>
       </c>
-      <c r="N108" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="109" spans="1:14" ht="52.8" x14ac:dyDescent="0.3">
+      <c r="N108" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O108" s="22"/>
+      <c r="P108" s="21" t="s">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A109" s="4" t="s">
         <v>979</v>
       </c>
@@ -8497,11 +9494,17 @@
       <c r="M109" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="N109" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="110" spans="1:14" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="N109" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O109" s="21" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P109" s="21" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="110" spans="1:16" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A110" s="4" t="s">
         <v>980</v>
       </c>
@@ -8541,11 +9544,17 @@
       <c r="M110" s="9" t="s">
         <v>438</v>
       </c>
-      <c r="N110" s="10" t="s">
+      <c r="N110" s="26" t="s">
         <v>757</v>
       </c>
-    </row>
-    <row r="111" spans="1:14" ht="92.4" x14ac:dyDescent="0.3">
+      <c r="O110" s="21" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P110" s="21" t="s">
+        <v>1024</v>
+      </c>
+    </row>
+    <row r="111" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A111" s="4" t="s">
         <v>981</v>
       </c>
@@ -8585,11 +9594,15 @@
       <c r="M111" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="N111" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="112" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N111" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O111" s="21"/>
+      <c r="P111" s="21" t="s">
+        <v>1099</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A112" s="4" t="s">
         <v>987</v>
       </c>
@@ -8629,11 +9642,17 @@
       <c r="M112" s="9" t="s">
         <v>440</v>
       </c>
-      <c r="N112" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="113" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N112" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O112" s="21" t="s">
+        <v>1100</v>
+      </c>
+      <c r="P112" s="21" t="s">
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="113" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A113" s="4" t="s">
         <v>982</v>
       </c>
@@ -8673,11 +9692,13 @@
       <c r="M113" s="17" t="s">
         <v>440</v>
       </c>
-      <c r="N113" s="10" t="s">
+      <c r="N113" s="26" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="114" spans="1:14" ht="184.8" x14ac:dyDescent="0.3">
+      <c r="O113" s="17"/>
+      <c r="P113" s="17"/>
+    </row>
+    <row r="114" spans="1:16" ht="184.8" x14ac:dyDescent="0.3">
       <c r="A114" s="4" t="s">
         <v>983</v>
       </c>
@@ -8717,11 +9738,17 @@
       <c r="M114" s="9" t="s">
         <v>441</v>
       </c>
-      <c r="N114" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="115" spans="1:14" ht="66" x14ac:dyDescent="0.3">
+      <c r="N114" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O114" s="21" t="s">
+        <v>1007</v>
+      </c>
+      <c r="P114" s="21" t="s">
+        <v>1102</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A115" s="4" t="s">
         <v>984</v>
       </c>
@@ -8761,11 +9788,17 @@
       <c r="M115" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="N115" s="10" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" ht="79.2" x14ac:dyDescent="0.3">
+      <c r="N115" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="O115" s="21" t="s">
+        <v>1103</v>
+      </c>
+      <c r="P115" s="21" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="116" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A116" s="4" t="s">
         <v>985</v>
       </c>
@@ -8805,11 +9838,15 @@
       <c r="M116" s="9" t="s">
         <v>442</v>
       </c>
-      <c r="N116" s="14" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="117" spans="1:14" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="N116" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="O116" s="22"/>
+      <c r="P116" s="21" t="s">
+        <v>1104</v>
+      </c>
+    </row>
+    <row r="117" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="16" t="s">
         <v>986</v>
       </c>
@@ -8846,9 +9883,11 @@
       <c r="M117" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="N117" s="20" t="s">
-        <v>106</v>
-      </c>
+      <c r="N117" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="O117" s="11"/>
+      <c r="P117" s="11"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>

<commit_message>
Arpita maam photo changed
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4A8D666-D5E0-415D-A1AE-BA85B07325C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72963D7-1F1B-4E2C-8FAB-C5890ED098A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3685,7 +3685,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -3735,19 +3735,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -4096,27 +4095,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M16" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T18" sqref="T18"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="35.6640625" style="19" customWidth="1"/>
-    <col min="2" max="4" width="25.88671875" style="23"/>
-    <col min="5" max="5" width="24.6640625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="25.88671875" style="23"/>
-    <col min="7" max="7" width="8.88671875" style="19"/>
-    <col min="8" max="10" width="25.88671875" style="23"/>
-    <col min="11" max="11" width="24.6640625" style="23" customWidth="1"/>
-    <col min="12" max="12" width="34.88671875" style="23" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.33203125" style="23" customWidth="1"/>
-    <col min="14" max="14" width="25.88671875" style="23"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="4" width="25.88671875" style="22"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" style="22"/>
+    <col min="8" max="10" width="25.88671875" style="22"/>
+    <col min="11" max="11" width="24.6640625" style="22" customWidth="1"/>
+    <col min="12" max="12" width="34.88671875" style="22" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.33203125" style="22" customWidth="1"/>
+    <col min="14" max="14" width="25.88671875" style="22"/>
     <col min="15" max="16" width="27.109375" style="15" customWidth="1"/>
-    <col min="17" max="16384" width="8.88671875" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="22" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" s="21" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
@@ -4156,7 +4153,7 @@
       <c r="M1" s="9" t="s">
         <v>679</v>
       </c>
-      <c r="N1" s="27" t="s">
+      <c r="N1" s="26" t="s">
         <v>757</v>
       </c>
       <c r="O1" s="9" t="s">
@@ -4206,13 +4203,13 @@
       <c r="M2" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="N2" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O2" s="24" t="s">
+      <c r="N2" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O2" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="P2" s="24" t="s">
+      <c r="P2" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4256,13 +4253,13 @@
       <c r="M3" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="N3" s="28" t="s">
         <v>721</v>
       </c>
-      <c r="O3" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P3" s="24" t="s">
+      <c r="O3" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P3" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4306,13 +4303,13 @@
       <c r="M4" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="N4" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O4" s="24" t="s">
+      <c r="N4" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O4" s="23" t="s">
         <v>1014</v>
       </c>
-      <c r="P4" s="24" t="s">
+      <c r="P4" s="23" t="s">
         <v>1015</v>
       </c>
     </row>
@@ -4356,13 +4353,13 @@
       <c r="M5" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="N5" s="30" t="s">
-        <v>106</v>
-      </c>
-      <c r="O5" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P5" s="24" t="s">
+      <c r="N5" s="29" t="s">
+        <v>106</v>
+      </c>
+      <c r="O5" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P5" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4406,13 +4403,13 @@
       <c r="M6" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="N6" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="O6" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P6" s="24" t="s">
+      <c r="N6" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="O6" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P6" s="23" t="s">
         <v>1017</v>
       </c>
     </row>
@@ -4456,13 +4453,13 @@
       <c r="M7" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="N7" s="29" t="s">
+      <c r="N7" s="28" t="s">
         <v>722</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="23" t="s">
         <v>1018</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="23" t="s">
         <v>1019</v>
       </c>
     </row>
@@ -4506,11 +4503,11 @@
       <c r="M8" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="N8" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="O8" s="25"/>
-      <c r="P8" s="24" t="s">
+      <c r="N8" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="O8" s="24"/>
+      <c r="P8" s="23" t="s">
         <v>1020</v>
       </c>
     </row>
@@ -4554,13 +4551,13 @@
       <c r="M9" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="N9" s="29" t="s">
+      <c r="N9" s="28" t="s">
         <v>723</v>
       </c>
-      <c r="O9" s="24" t="s">
+      <c r="O9" s="23" t="s">
         <v>1021</v>
       </c>
-      <c r="P9" s="24" t="s">
+      <c r="P9" s="23" t="s">
         <v>1022</v>
       </c>
     </row>
@@ -4604,13 +4601,13 @@
       <c r="M10" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N10" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O10" s="24" t="s">
+      <c r="N10" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O10" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="P10" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4654,13 +4651,13 @@
       <c r="M11" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N11" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O11" s="24" t="s">
+      <c r="N11" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O11" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P11" s="24" t="s">
+      <c r="P11" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4704,13 +4701,13 @@
       <c r="M12" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="N12" s="29" t="s">
+      <c r="N12" s="28" t="s">
         <v>724</v>
       </c>
-      <c r="O12" s="24" t="s">
+      <c r="O12" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="P12" s="24" t="s">
+      <c r="P12" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4754,13 +4751,13 @@
       <c r="M13" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N13" s="29" t="s">
+      <c r="N13" s="28" t="s">
         <v>725</v>
       </c>
-      <c r="O13" s="24" t="s">
+      <c r="O13" s="23" t="s">
         <v>1026</v>
       </c>
-      <c r="P13" s="24" t="s">
+      <c r="P13" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4804,13 +4801,13 @@
       <c r="M14" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="N14" s="29" t="s">
+      <c r="N14" s="28" t="s">
         <v>726</v>
       </c>
-      <c r="O14" s="24" t="s">
+      <c r="O14" s="23" t="s">
         <v>1027</v>
       </c>
-      <c r="P14" s="24" t="s">
+      <c r="P14" s="23" t="s">
         <v>1028</v>
       </c>
     </row>
@@ -4854,13 +4851,13 @@
       <c r="M15" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="N15" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O15" s="24" t="s">
+      <c r="N15" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O15" s="23" t="s">
         <v>1029</v>
       </c>
-      <c r="P15" s="24" t="s">
+      <c r="P15" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4904,13 +4901,13 @@
       <c r="M16" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="N16" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O16" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P16" s="24" t="s">
+      <c r="N16" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O16" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P16" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -4954,13 +4951,13 @@
       <c r="M17" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="N17" s="29" t="s">
+      <c r="N17" s="28" t="s">
         <v>727</v>
       </c>
-      <c r="O17" s="24" t="s">
+      <c r="O17" s="23" t="s">
         <v>1030</v>
       </c>
-      <c r="P17" s="24" t="s">
+      <c r="P17" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5004,13 +5001,13 @@
       <c r="M18" s="6" t="s">
         <v>364</v>
       </c>
-      <c r="N18" s="29" t="s">
+      <c r="N18" s="28" t="s">
         <v>728</v>
       </c>
-      <c r="O18" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P18" s="24" t="s">
+      <c r="O18" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P18" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5054,13 +5051,13 @@
       <c r="M19" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="N19" s="29" t="s">
+      <c r="N19" s="28" t="s">
         <v>729</v>
       </c>
-      <c r="O19" s="24" t="s">
+      <c r="O19" s="23" t="s">
         <v>1031</v>
       </c>
-      <c r="P19" s="24" t="s">
+      <c r="P19" s="23" t="s">
         <v>1032</v>
       </c>
     </row>
@@ -5104,13 +5101,13 @@
       <c r="M20" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N20" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O20" s="24" t="s">
+      <c r="N20" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O20" s="23" t="s">
         <v>1033</v>
       </c>
-      <c r="P20" s="24" t="s">
+      <c r="P20" s="23" t="s">
         <v>1034</v>
       </c>
     </row>
@@ -5154,13 +5151,13 @@
       <c r="M21" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="N21" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O21" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P21" s="24" t="s">
+      <c r="N21" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O21" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P21" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5204,13 +5201,13 @@
       <c r="M22" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="N22" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O22" s="24" t="s">
+      <c r="N22" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O22" s="23" t="s">
         <v>1029</v>
       </c>
-      <c r="P22" s="24" t="s">
+      <c r="P22" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5254,13 +5251,13 @@
       <c r="M23" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="N23" s="29" t="s">
+      <c r="N23" s="28" t="s">
         <v>730</v>
       </c>
-      <c r="O23" s="24" t="s">
+      <c r="O23" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="P23" s="24" t="s">
+      <c r="P23" s="23" t="s">
         <v>1035</v>
       </c>
     </row>
@@ -5304,13 +5301,13 @@
       <c r="M24" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="N24" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O24" s="24" t="s">
+      <c r="N24" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O24" s="23" t="s">
         <v>1029</v>
       </c>
-      <c r="P24" s="24" t="s">
+      <c r="P24" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5354,13 +5351,13 @@
       <c r="M25" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="N25" s="29" t="s">
+      <c r="N25" s="28" t="s">
         <v>731</v>
       </c>
-      <c r="O25" s="24" t="s">
+      <c r="O25" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P25" s="24" t="s">
+      <c r="P25" s="23" t="s">
         <v>1036</v>
       </c>
     </row>
@@ -5404,13 +5401,13 @@
       <c r="M26" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="N26" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O26" s="24" t="s">
+      <c r="N26" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O26" s="23" t="s">
         <v>1037</v>
       </c>
-      <c r="P26" s="24" t="s">
+      <c r="P26" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5454,13 +5451,13 @@
       <c r="M27" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="N27" s="29" t="s">
+      <c r="N27" s="28" t="s">
         <v>732</v>
       </c>
-      <c r="O27" s="24" t="s">
+      <c r="O27" s="23" t="s">
         <v>1037</v>
       </c>
-      <c r="P27" s="24" t="s">
+      <c r="P27" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5504,13 +5501,13 @@
       <c r="M28" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="N28" s="29" t="s">
+      <c r="N28" s="28" t="s">
         <v>733</v>
       </c>
-      <c r="O28" s="24" t="s">
+      <c r="O28" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="P28" s="24" t="s">
+      <c r="P28" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5554,13 +5551,13 @@
       <c r="M29" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="N29" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O29" s="24" t="s">
+      <c r="N29" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O29" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P29" s="24" t="s">
+      <c r="P29" s="23" t="s">
         <v>1038</v>
       </c>
     </row>
@@ -5604,13 +5601,13 @@
       <c r="M30" s="13">
         <v>583944</v>
       </c>
-      <c r="N30" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O30" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P30" s="24" t="s">
+      <c r="N30" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O30" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P30" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5654,13 +5651,13 @@
       <c r="M31" s="6" t="s">
         <v>676</v>
       </c>
-      <c r="N31" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O31" s="26" t="s">
+      <c r="N31" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O31" s="25" t="s">
         <v>1039</v>
       </c>
-      <c r="P31" s="24" t="s">
+      <c r="P31" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5704,11 +5701,11 @@
       <c r="M32" s="6" t="s">
         <v>677</v>
       </c>
-      <c r="N32" s="29" t="s">
+      <c r="N32" s="28" t="s">
         <v>734</v>
       </c>
-      <c r="O32" s="25"/>
-      <c r="P32" s="24" t="s">
+      <c r="O32" s="24"/>
+      <c r="P32" s="23" t="s">
         <v>1040</v>
       </c>
     </row>
@@ -5752,11 +5749,11 @@
       <c r="M33" s="6" t="s">
         <v>373</v>
       </c>
-      <c r="N33" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O33" s="24"/>
-      <c r="P33" s="24" t="s">
+      <c r="N33" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O33" s="23"/>
+      <c r="P33" s="23" t="s">
         <v>1041</v>
       </c>
     </row>
@@ -5800,13 +5797,13 @@
       <c r="M34" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="N34" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O34" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P34" s="24" t="s">
+      <c r="N34" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O34" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P34" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5850,13 +5847,13 @@
       <c r="M35" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="N35" s="29" t="s">
+      <c r="N35" s="28" t="s">
         <v>735</v>
       </c>
-      <c r="O35" s="24" t="s">
+      <c r="O35" s="23" t="s">
         <v>1026</v>
       </c>
-      <c r="P35" s="24" t="s">
+      <c r="P35" s="23" t="s">
         <v>1042</v>
       </c>
     </row>
@@ -5900,13 +5897,13 @@
       <c r="M36" s="6" t="s">
         <v>376</v>
       </c>
-      <c r="N36" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O36" s="24" t="s">
+      <c r="N36" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O36" s="23" t="s">
         <v>1043</v>
       </c>
-      <c r="P36" s="24" t="s">
+      <c r="P36" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -5950,13 +5947,13 @@
       <c r="M37" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="N37" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O37" s="24" t="s">
+      <c r="N37" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O37" s="23" t="s">
         <v>1044</v>
       </c>
-      <c r="P37" s="24" t="s">
+      <c r="P37" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6000,13 +5997,13 @@
       <c r="M38" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="N38" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O38" s="24" t="s">
+      <c r="N38" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O38" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="P38" s="24" t="s">
+      <c r="P38" s="23" t="s">
         <v>1045</v>
       </c>
     </row>
@@ -6050,13 +6047,13 @@
       <c r="M39" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="N39" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O39" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P39" s="24" t="s">
+      <c r="N39" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O39" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P39" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6100,13 +6097,13 @@
       <c r="M40" s="6" t="s">
         <v>379</v>
       </c>
-      <c r="N40" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O40" s="24" t="s">
+      <c r="N40" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O40" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P40" s="24" t="s">
+      <c r="P40" s="23" t="s">
         <v>1046</v>
       </c>
     </row>
@@ -6150,13 +6147,13 @@
       <c r="M41" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="N41" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="O41" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P41" s="24" t="s">
+      <c r="N41" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="O41" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P41" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6200,13 +6197,13 @@
       <c r="M42" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="N42" s="29" t="s">
+      <c r="N42" s="28" t="s">
         <v>736</v>
       </c>
-      <c r="O42" s="24" t="s">
+      <c r="O42" s="23" t="s">
         <v>1047</v>
       </c>
-      <c r="P42" s="24" t="s">
+      <c r="P42" s="23" t="s">
         <v>1048</v>
       </c>
     </row>
@@ -6250,11 +6247,11 @@
       <c r="M43" s="6" t="s">
         <v>382</v>
       </c>
-      <c r="N43" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O43" s="24"/>
-      <c r="P43" s="24" t="s">
+      <c r="N43" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O43" s="23"/>
+      <c r="P43" s="23" t="s">
         <v>1049</v>
       </c>
     </row>
@@ -6298,13 +6295,13 @@
       <c r="M44" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="N44" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O44" s="24" t="s">
+      <c r="N44" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O44" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P44" s="24" t="s">
+      <c r="P44" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6348,11 +6345,11 @@
       <c r="M45" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="N45" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O45" s="24"/>
-      <c r="P45" s="24" t="s">
+      <c r="N45" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O45" s="23"/>
+      <c r="P45" s="23" t="s">
         <v>1024</v>
       </c>
     </row>
@@ -6396,13 +6393,13 @@
       <c r="M46" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="N46" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O46" s="24" t="s">
+      <c r="N46" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O46" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="P46" s="24" t="s">
+      <c r="P46" s="23" t="s">
         <v>107</v>
       </c>
     </row>
@@ -6446,13 +6443,13 @@
       <c r="M47" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N47" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O47" s="24" t="s">
+      <c r="N47" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O47" s="23" t="s">
         <v>1029</v>
       </c>
-      <c r="P47" s="24" t="s">
+      <c r="P47" s="23" t="s">
         <v>1016</v>
       </c>
     </row>
@@ -6496,13 +6493,13 @@
       <c r="M48" s="6" t="s">
         <v>385</v>
       </c>
-      <c r="N48" s="29" t="s">
+      <c r="N48" s="28" t="s">
         <v>737</v>
       </c>
-      <c r="O48" s="24" t="s">
+      <c r="O48" s="23" t="s">
         <v>1050</v>
       </c>
-      <c r="P48" s="24" t="s">
+      <c r="P48" s="23" t="s">
         <v>1051</v>
       </c>
     </row>
@@ -6546,13 +6543,13 @@
       <c r="M49" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="N49" s="29" t="s">
+      <c r="N49" s="28" t="s">
         <v>738</v>
       </c>
-      <c r="O49" s="24" t="s">
+      <c r="O49" s="23" t="s">
         <v>1043</v>
       </c>
-      <c r="P49" s="24" t="s">
+      <c r="P49" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6596,13 +6593,13 @@
       <c r="M50" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N50" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O50" s="24" t="s">
+      <c r="N50" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O50" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P50" s="24" t="s">
+      <c r="P50" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6636,7 +6633,7 @@
       </c>
       <c r="L51" s="6"/>
       <c r="M51" s="6"/>
-      <c r="N51" s="33"/>
+      <c r="N51" s="32"/>
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
     </row>
@@ -6680,11 +6677,11 @@
       <c r="M52" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="N52" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O52" s="24"/>
-      <c r="P52" s="24" t="s">
+      <c r="N52" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O52" s="23"/>
+      <c r="P52" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6728,13 +6725,13 @@
       <c r="M53" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="N53" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O53" s="24" t="s">
+      <c r="N53" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O53" s="23" t="s">
         <v>1029</v>
       </c>
-      <c r="P53" s="24" t="s">
+      <c r="P53" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6778,13 +6775,13 @@
       <c r="M54" s="6" t="s">
         <v>388</v>
       </c>
-      <c r="N54" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O54" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P54" s="24" t="s">
+      <c r="N54" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O54" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P54" s="23" t="s">
         <v>1052</v>
       </c>
     </row>
@@ -6828,13 +6825,13 @@
       <c r="M55" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="N55" s="29" t="s">
+      <c r="N55" s="28" t="s">
         <v>739</v>
       </c>
-      <c r="O55" s="24" t="s">
+      <c r="O55" s="23" t="s">
         <v>1053</v>
       </c>
-      <c r="P55" s="24" t="s">
+      <c r="P55" s="23" t="s">
         <v>1054</v>
       </c>
     </row>
@@ -6878,13 +6875,13 @@
       <c r="M56" s="6" t="s">
         <v>390</v>
       </c>
-      <c r="N56" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O56" s="24" t="s">
+      <c r="N56" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O56" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P56" s="24" t="s">
+      <c r="P56" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -6928,13 +6925,13 @@
       <c r="M57" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="N57" s="29" t="s">
+      <c r="N57" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="O57" s="24" t="s">
+      <c r="O57" s="23" t="s">
         <v>1055</v>
       </c>
-      <c r="P57" s="24" t="s">
+      <c r="P57" s="23" t="s">
         <v>1056</v>
       </c>
     </row>
@@ -6978,13 +6975,13 @@
       <c r="M58" s="6" t="s">
         <v>392</v>
       </c>
-      <c r="N58" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O58" s="24" t="s">
+      <c r="N58" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O58" s="23" t="s">
         <v>1057</v>
       </c>
-      <c r="P58" s="24" t="s">
+      <c r="P58" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7028,13 +7025,13 @@
       <c r="M59" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="N59" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O59" s="24" t="s">
+      <c r="N59" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O59" s="23" t="s">
         <v>1058</v>
       </c>
-      <c r="P59" s="24" t="s">
+      <c r="P59" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7078,13 +7075,13 @@
       <c r="M60" s="6" t="s">
         <v>394</v>
       </c>
-      <c r="N60" s="29" t="s">
+      <c r="N60" s="28" t="s">
         <v>741</v>
       </c>
-      <c r="O60" s="24" t="s">
+      <c r="O60" s="23" t="s">
         <v>1059</v>
       </c>
-      <c r="P60" s="24" t="s">
+      <c r="P60" s="23" t="s">
         <v>1060</v>
       </c>
     </row>
@@ -7128,13 +7125,13 @@
       <c r="M61" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="N61" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O61" s="24" t="s">
+      <c r="N61" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O61" s="23" t="s">
         <v>1061</v>
       </c>
-      <c r="P61" s="24" t="s">
+      <c r="P61" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7178,13 +7175,13 @@
       <c r="M62" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="N62" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O62" s="24" t="s">
+      <c r="N62" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O62" s="23" t="s">
         <v>1062</v>
       </c>
-      <c r="P62" s="24" t="s">
+      <c r="P62" s="23" t="s">
         <v>1063</v>
       </c>
     </row>
@@ -7228,11 +7225,11 @@
       <c r="M63" s="6" t="s">
         <v>397</v>
       </c>
-      <c r="N63" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O63" s="24"/>
-      <c r="P63" s="24" t="s">
+      <c r="N63" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O63" s="23"/>
+      <c r="P63" s="23" t="s">
         <v>1064</v>
       </c>
     </row>
@@ -7276,13 +7273,13 @@
       <c r="M64" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N64" s="29" t="s">
+      <c r="N64" s="28" t="s">
         <v>733</v>
       </c>
-      <c r="O64" s="24" t="s">
+      <c r="O64" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P64" s="24" t="s">
+      <c r="P64" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7326,11 +7323,11 @@
       <c r="M65" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="N65" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O65" s="24"/>
-      <c r="P65" s="24" t="s">
+      <c r="N65" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O65" s="23"/>
+      <c r="P65" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7374,13 +7371,13 @@
       <c r="M66" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="N66" s="29" t="s">
+      <c r="N66" s="28" t="s">
         <v>742</v>
       </c>
-      <c r="O66" s="24" t="s">
+      <c r="O66" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P66" s="24" t="s">
+      <c r="P66" s="23" t="s">
         <v>1065</v>
       </c>
     </row>
@@ -7424,13 +7421,13 @@
       <c r="M67" s="6" t="s">
         <v>400</v>
       </c>
-      <c r="N67" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O67" s="24" t="s">
+      <c r="N67" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O67" s="23" t="s">
         <v>1066</v>
       </c>
-      <c r="P67" s="24" t="s">
+      <c r="P67" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7474,13 +7471,13 @@
       <c r="M68" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="N68" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O68" s="24" t="s">
+      <c r="N68" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O68" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="P68" s="24" t="s">
+      <c r="P68" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7524,13 +7521,13 @@
       <c r="M69" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N69" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O69" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P69" s="24" t="s">
+      <c r="N69" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O69" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P69" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7574,13 +7571,13 @@
       <c r="M70" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="N70" s="29" t="s">
+      <c r="N70" s="28" t="s">
         <v>743</v>
       </c>
-      <c r="O70" s="24" t="s">
+      <c r="O70" s="23" t="s">
         <v>1067</v>
       </c>
-      <c r="P70" s="24"/>
+      <c r="P70" s="23"/>
     </row>
     <row r="71" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="s">
@@ -7622,13 +7619,13 @@
       <c r="M71" s="6" t="s">
         <v>403</v>
       </c>
-      <c r="N71" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O71" s="24" t="s">
+      <c r="N71" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O71" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P71" s="24"/>
+      <c r="P71" s="23"/>
     </row>
     <row r="72" spans="1:16" ht="118.8" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="s">
@@ -7670,13 +7667,13 @@
       <c r="M72" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="N72" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O72" s="24" t="s">
+      <c r="N72" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O72" s="23" t="s">
         <v>1066</v>
       </c>
-      <c r="P72" s="24" t="s">
+      <c r="P72" s="23" t="s">
         <v>1068</v>
       </c>
     </row>
@@ -7720,13 +7717,13 @@
       <c r="M73" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="N73" s="29" t="s">
+      <c r="N73" s="28" t="s">
         <v>744</v>
       </c>
-      <c r="O73" s="24" t="s">
+      <c r="O73" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P73" s="24" t="s">
+      <c r="P73" s="23" t="s">
         <v>1069</v>
       </c>
     </row>
@@ -7770,11 +7767,11 @@
       <c r="M74" s="6" t="s">
         <v>406</v>
       </c>
-      <c r="N74" s="29" t="s">
+      <c r="N74" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="O74" s="24"/>
-      <c r="P74" s="24" t="s">
+      <c r="O74" s="23"/>
+      <c r="P74" s="23" t="s">
         <v>1070</v>
       </c>
     </row>
@@ -7818,13 +7815,13 @@
       <c r="M75" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N75" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O75" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P75" s="24" t="s">
+      <c r="N75" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O75" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P75" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7868,13 +7865,13 @@
       <c r="M76" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="N76" s="29" t="s">
+      <c r="N76" s="28" t="s">
         <v>745</v>
       </c>
-      <c r="O76" s="24" t="s">
+      <c r="O76" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P76" s="24" t="s">
+      <c r="P76" s="23" t="s">
         <v>1071</v>
       </c>
     </row>
@@ -7918,11 +7915,11 @@
       <c r="M77" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="N77" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="O77" s="24"/>
-      <c r="P77" s="24" t="s">
+      <c r="N77" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="O77" s="23"/>
+      <c r="P77" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -7966,11 +7963,11 @@
       <c r="M78" s="6" t="s">
         <v>408</v>
       </c>
-      <c r="N78" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O78" s="24"/>
-      <c r="P78" s="24" t="s">
+      <c r="N78" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O78" s="23"/>
+      <c r="P78" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -8014,13 +8011,13 @@
       <c r="M79" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="N79" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O79" s="24" t="s">
+      <c r="N79" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O79" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P79" s="24" t="s">
+      <c r="P79" s="23" t="s">
         <v>1072</v>
       </c>
     </row>
@@ -8064,13 +8061,13 @@
       <c r="M80" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="N80" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O80" s="24" t="s">
+      <c r="N80" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O80" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P80" s="24" t="s">
+      <c r="P80" s="23" t="s">
         <v>1073</v>
       </c>
     </row>
@@ -8114,13 +8111,13 @@
       <c r="M81" s="6" t="s">
         <v>411</v>
       </c>
-      <c r="N81" s="29" t="s">
+      <c r="N81" s="28" t="s">
         <v>746</v>
       </c>
-      <c r="O81" s="24" t="s">
+      <c r="O81" s="23" t="s">
         <v>1074</v>
       </c>
-      <c r="P81" s="24"/>
+      <c r="P81" s="23"/>
     </row>
     <row r="82" spans="1:16" ht="66" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="s">
@@ -8162,13 +8159,13 @@
       <c r="M82" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="N82" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O82" s="24" t="s">
+      <c r="N82" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O82" s="23" t="s">
         <v>1075</v>
       </c>
-      <c r="P82" s="24" t="s">
+      <c r="P82" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -8212,13 +8209,13 @@
       <c r="M83" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="N83" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O83" s="24" t="s">
+      <c r="N83" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O83" s="23" t="s">
         <v>1076</v>
       </c>
-      <c r="P83" s="24"/>
+      <c r="P83" s="23"/>
     </row>
     <row r="84" spans="1:16" ht="145.19999999999999" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="s">
@@ -8260,13 +8257,13 @@
       <c r="M84" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="N84" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O84" s="24" t="s">
+      <c r="N84" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O84" s="23" t="s">
         <v>1077</v>
       </c>
-      <c r="P84" s="24"/>
+      <c r="P84" s="23"/>
     </row>
     <row r="85" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="s">
@@ -8308,13 +8305,13 @@
       <c r="M85" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="N85" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O85" s="24" t="s">
+      <c r="N85" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O85" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P85" s="24"/>
+      <c r="P85" s="23"/>
     </row>
     <row r="86" spans="1:16" ht="330" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="s">
@@ -8356,13 +8353,13 @@
       <c r="M86" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="N86" s="29" t="s">
+      <c r="N86" s="28" t="s">
         <v>747</v>
       </c>
-      <c r="O86" s="24" t="s">
+      <c r="O86" s="23" t="s">
         <v>1078</v>
       </c>
-      <c r="P86" s="24" t="s">
+      <c r="P86" s="23" t="s">
         <v>1079</v>
       </c>
     </row>
@@ -8406,13 +8403,13 @@
       <c r="M87" s="6" t="s">
         <v>678</v>
       </c>
-      <c r="N87" s="29" t="s">
+      <c r="N87" s="28" t="s">
         <v>748</v>
       </c>
-      <c r="O87" s="24" t="s">
+      <c r="O87" s="23" t="s">
         <v>1018</v>
       </c>
-      <c r="P87" s="24" t="s">
+      <c r="P87" s="23" t="s">
         <v>1024</v>
       </c>
     </row>
@@ -8456,13 +8453,13 @@
       <c r="M88" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="N88" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O88" s="24" t="s">
+      <c r="N88" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O88" s="23" t="s">
         <v>1080</v>
       </c>
-      <c r="P88" s="24"/>
+      <c r="P88" s="23"/>
     </row>
     <row r="89" spans="1:16" ht="79.2" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="s">
@@ -8504,13 +8501,13 @@
       <c r="M89" s="6" t="s">
         <v>418</v>
       </c>
-      <c r="N89" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O89" s="24" t="s">
+      <c r="N89" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O89" s="23" t="s">
         <v>1081</v>
       </c>
-      <c r="P89" s="24" t="s">
+      <c r="P89" s="23" t="s">
         <v>1082</v>
       </c>
     </row>
@@ -8554,13 +8551,13 @@
       <c r="M90" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="N90" s="29" t="s">
+      <c r="N90" s="28" t="s">
         <v>749</v>
       </c>
-      <c r="O90" s="24" t="s">
+      <c r="O90" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P90" s="24" t="s">
+      <c r="P90" s="23" t="s">
         <v>1083</v>
       </c>
     </row>
@@ -8604,13 +8601,13 @@
       <c r="M91" s="6" t="s">
         <v>420</v>
       </c>
-      <c r="N91" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O91" s="24" t="s">
+      <c r="N91" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O91" s="23" t="s">
         <v>1084</v>
       </c>
-      <c r="P91" s="24" t="s">
+      <c r="P91" s="23" t="s">
         <v>1085</v>
       </c>
     </row>
@@ -8654,7 +8651,7 @@
       <c r="M92" s="6" t="s">
         <v>421</v>
       </c>
-      <c r="N92" s="28" t="s">
+      <c r="N92" s="27" t="s">
         <v>106</v>
       </c>
       <c r="O92" s="6"/>
@@ -8700,13 +8697,13 @@
       <c r="M93" s="6" t="s">
         <v>422</v>
       </c>
-      <c r="N93" s="29" t="s">
+      <c r="N93" s="28" t="s">
         <v>750</v>
       </c>
-      <c r="O93" s="24" t="s">
+      <c r="O93" s="23" t="s">
         <v>1086</v>
       </c>
-      <c r="P93" s="24" t="s">
+      <c r="P93" s="23" t="s">
         <v>1087</v>
       </c>
     </row>
@@ -8750,13 +8747,13 @@
       <c r="M94" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="N94" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O94" s="24" t="s">
+      <c r="N94" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O94" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P94" s="24"/>
+      <c r="P94" s="23"/>
     </row>
     <row r="95" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="s">
@@ -8798,13 +8795,13 @@
       <c r="M95" s="6" t="s">
         <v>424</v>
       </c>
-      <c r="N95" s="29" t="s">
+      <c r="N95" s="28" t="s">
         <v>751</v>
       </c>
-      <c r="O95" s="24" t="s">
+      <c r="O95" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="P95" s="24" t="s">
+      <c r="P95" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -8848,13 +8845,13 @@
       <c r="M96" s="6" t="s">
         <v>425</v>
       </c>
-      <c r="N96" s="29" t="s">
+      <c r="N96" s="28" t="s">
         <v>752</v>
       </c>
-      <c r="O96" s="24" t="s">
+      <c r="O96" s="23" t="s">
         <v>1088</v>
       </c>
-      <c r="P96" s="24" t="s">
+      <c r="P96" s="23" t="s">
         <v>1024</v>
       </c>
     </row>
@@ -8898,13 +8895,13 @@
       <c r="M97" s="6" t="s">
         <v>426</v>
       </c>
-      <c r="N97" s="29" t="s">
+      <c r="N97" s="28" t="s">
         <v>740</v>
       </c>
-      <c r="O97" s="24" t="s">
+      <c r="O97" s="23" t="s">
         <v>1089</v>
       </c>
-      <c r="P97" s="24"/>
+      <c r="P97" s="23"/>
     </row>
     <row r="98" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="s">
@@ -8946,13 +8943,13 @@
       <c r="M98" s="6" t="s">
         <v>427</v>
       </c>
-      <c r="N98" s="29" t="s">
+      <c r="N98" s="28" t="s">
         <v>753</v>
       </c>
-      <c r="O98" s="24" t="s">
+      <c r="O98" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P98" s="24" t="s">
+      <c r="P98" s="23" t="s">
         <v>1090</v>
       </c>
     </row>
@@ -8996,13 +8993,13 @@
       <c r="M99" s="6" t="s">
         <v>428</v>
       </c>
-      <c r="N99" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O99" s="24" t="s">
+      <c r="N99" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O99" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P99" s="24"/>
+      <c r="P99" s="23"/>
     </row>
     <row r="100" spans="1:16" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="s">
@@ -9044,13 +9041,13 @@
       <c r="M100" s="6" t="s">
         <v>429</v>
       </c>
-      <c r="N100" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O100" s="24" t="s">
-        <v>106</v>
-      </c>
-      <c r="P100" s="24" t="s">
+      <c r="N100" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O100" s="23" t="s">
+        <v>106</v>
+      </c>
+      <c r="P100" s="23" t="s">
         <v>1091</v>
       </c>
     </row>
@@ -9094,13 +9091,13 @@
       <c r="M101" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="N101" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O101" s="24" t="s">
+      <c r="N101" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O101" s="23" t="s">
         <v>1013</v>
       </c>
-      <c r="P101" s="24" t="s">
+      <c r="P101" s="23" t="s">
         <v>1024</v>
       </c>
     </row>
@@ -9144,13 +9141,13 @@
       <c r="M102" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="N102" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O102" s="24" t="s">
+      <c r="N102" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O102" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P102" s="24" t="s">
+      <c r="P102" s="23" t="s">
         <v>1024</v>
       </c>
     </row>
@@ -9194,11 +9191,11 @@
       <c r="M103" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="N103" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O103" s="24"/>
-      <c r="P103" s="24" t="s">
+      <c r="N103" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O103" s="23"/>
+      <c r="P103" s="23" t="s">
         <v>1092</v>
       </c>
     </row>
@@ -9242,13 +9239,13 @@
       <c r="M104" s="6" t="s">
         <v>432</v>
       </c>
-      <c r="N104" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O104" s="24" t="s">
+      <c r="N104" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O104" s="23" t="s">
         <v>1093</v>
       </c>
-      <c r="P104" s="24" t="s">
+      <c r="P104" s="23" t="s">
         <v>1094</v>
       </c>
     </row>
@@ -9292,13 +9289,13 @@
       <c r="M105" s="6" t="s">
         <v>433</v>
       </c>
-      <c r="N105" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O105" s="24" t="s">
+      <c r="N105" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O105" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P105" s="24"/>
+      <c r="P105" s="23"/>
     </row>
     <row r="106" spans="1:16" ht="52.8" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="s">
@@ -9340,13 +9337,13 @@
       <c r="M106" s="6" t="s">
         <v>434</v>
       </c>
-      <c r="N106" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O106" s="24" t="s">
+      <c r="N106" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O106" s="23" t="s">
         <v>1066</v>
       </c>
-      <c r="P106" s="24" t="s">
+      <c r="P106" s="23" t="s">
         <v>1095</v>
       </c>
     </row>
@@ -9390,13 +9387,13 @@
       <c r="M107" s="6" t="s">
         <v>435</v>
       </c>
-      <c r="N107" s="29" t="s">
+      <c r="N107" s="28" t="s">
         <v>754</v>
       </c>
-      <c r="O107" s="24" t="s">
+      <c r="O107" s="23" t="s">
         <v>1025</v>
       </c>
-      <c r="P107" s="24" t="s">
+      <c r="P107" s="23" t="s">
         <v>1024</v>
       </c>
     </row>
@@ -9440,11 +9437,11 @@
       <c r="M108" s="6" t="s">
         <v>436</v>
       </c>
-      <c r="N108" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O108" s="25"/>
-      <c r="P108" s="24" t="s">
+      <c r="N108" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O108" s="24"/>
+      <c r="P108" s="23" t="s">
         <v>1096</v>
       </c>
     </row>
@@ -9488,13 +9485,13 @@
       <c r="M109" s="6" t="s">
         <v>437</v>
       </c>
-      <c r="N109" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O109" s="24" t="s">
+      <c r="N109" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O109" s="23" t="s">
         <v>1023</v>
       </c>
-      <c r="P109" s="24" t="s">
+      <c r="P109" s="23" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9538,13 +9535,13 @@
       <c r="M110" s="6" t="s">
         <v>438</v>
       </c>
-      <c r="N110" s="29" t="s">
+      <c r="N110" s="28" t="s">
         <v>755</v>
       </c>
-      <c r="O110" s="24" t="s">
+      <c r="O110" s="23" t="s">
         <v>1029</v>
       </c>
-      <c r="P110" s="24"/>
+      <c r="P110" s="23"/>
     </row>
     <row r="111" spans="1:16" ht="92.4" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="s">
@@ -9586,11 +9583,11 @@
       <c r="M111" s="6" t="s">
         <v>439</v>
       </c>
-      <c r="N111" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O111" s="24"/>
-      <c r="P111" s="24" t="s">
+      <c r="N111" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O111" s="23"/>
+      <c r="P111" s="23" t="s">
         <v>1097</v>
       </c>
     </row>
@@ -9634,13 +9631,13 @@
       <c r="M112" s="6" t="s">
         <v>440</v>
       </c>
-      <c r="N112" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O112" s="24" t="s">
+      <c r="N112" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O112" s="23" t="s">
         <v>1098</v>
       </c>
-      <c r="P112" s="24" t="s">
+      <c r="P112" s="23" t="s">
         <v>1099</v>
       </c>
     </row>
@@ -9684,7 +9681,7 @@
       <c r="M113" s="13" t="s">
         <v>440</v>
       </c>
-      <c r="N113" s="29" t="s">
+      <c r="N113" s="28" t="s">
         <v>756</v>
       </c>
       <c r="O113" s="13"/>
@@ -9730,11 +9727,11 @@
       <c r="M114" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="N114" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O114" s="24"/>
-      <c r="P114" s="24" t="s">
+      <c r="N114" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O114" s="23"/>
+      <c r="P114" s="23" t="s">
         <v>1100</v>
       </c>
     </row>
@@ -9778,13 +9775,13 @@
       <c r="M115" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="N115" s="29" t="s">
-        <v>106</v>
-      </c>
-      <c r="O115" s="24" t="s">
+      <c r="N115" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="O115" s="23" t="s">
         <v>1101</v>
       </c>
-      <c r="P115" s="24" t="s">
+      <c r="P115" s="23" t="s">
         <v>107</v>
       </c>
     </row>
@@ -9828,11 +9825,11 @@
       <c r="M116" s="6" t="s">
         <v>442</v>
       </c>
-      <c r="N116" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="O116" s="25"/>
-      <c r="P116" s="24"/>
+      <c r="N116" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="O116" s="24"/>
+      <c r="P116" s="23"/>
     </row>
     <row r="117" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A117" s="12" t="s">
@@ -9847,13 +9844,13 @@
       <c r="D117" s="11" t="s">
         <v>686</v>
       </c>
-      <c r="E117" s="20" t="s">
+      <c r="E117" s="19" t="s">
         <v>986</v>
       </c>
       <c r="F117" s="12" t="s">
         <v>106</v>
       </c>
-      <c r="G117" s="21"/>
+      <c r="G117" s="20"/>
       <c r="H117" s="12" t="s">
         <v>106</v>
       </c>
@@ -9872,7 +9869,7 @@
       <c r="M117" s="8" t="s">
         <v>106</v>
       </c>
-      <c r="N117" s="34" t="s">
+      <c r="N117" s="33" t="s">
         <v>106</v>
       </c>
       <c r="O117" s="8"/>

</xml_diff>

<commit_message>
Arpita maam photo changed and Ronak sir updation
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\motat\OneDrive\Desktop\CSPIT_NEW_2024\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72963D7-1F1B-4E2C-8FAB-C5890ED098A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4C1597E-B4F9-4D48-A651-C6C1825F186B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="1104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1827" uniqueCount="1105">
   <si>
     <t>Name</t>
   </si>
@@ -3534,6 +3534,9 @@
   </si>
   <si>
     <t>Certification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mr. RonakKumar Patel  </t>
   </si>
 </sst>
 </file>
@@ -8709,7 +8712,7 @@
     </row>
     <row r="94" spans="1:16" ht="39.6" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="s">
-        <v>959</v>
+        <v>1104</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>108</v>

</xml_diff>

<commit_message>
parth sir content updated
</commit_message>
<xml_diff>
--- a/faculty_data.xlsx
+++ b/faculty_data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23145" windowHeight="8520"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23148" windowHeight="8520"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2187,9 +2187,6 @@
     <t xml:space="preserve">Machine Learning, Deep Learning, MultiNAModal Information Retrieval </t>
   </si>
   <si>
-    <t xml:space="preserve">PrivacyNAPreserving, </t>
-  </si>
-  <si>
     <t>Python Programming,Machine Learning, Embedded System</t>
   </si>
   <si>
@@ -3536,6 +3533,9 @@
   </si>
   <si>
     <t>https://learnwithparth.in/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Privacy Preserving </t>
   </si>
 </sst>
 </file>
@@ -4097,22 +4097,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K106" sqref="K106"/>
+    <sheetView tabSelected="1" topLeftCell="A75" zoomScale="79" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="4" width="25.85546875" style="21"/>
-    <col min="5" max="5" width="24.7109375" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="21"/>
-    <col min="8" max="10" width="25.85546875" style="21"/>
-    <col min="11" max="11" width="24.7109375" style="21" customWidth="1"/>
-    <col min="12" max="12" width="34.85546875" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="43.28515625" style="21" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" style="21"/>
-    <col min="15" max="16" width="27.140625" style="14" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="4" width="25.88671875" style="21"/>
+    <col min="5" max="5" width="24.6640625" customWidth="1"/>
+    <col min="6" max="6" width="25.88671875" style="21"/>
+    <col min="8" max="10" width="25.88671875" style="21"/>
+    <col min="11" max="11" width="24.6640625" style="21" customWidth="1"/>
+    <col min="12" max="12" width="34.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.33203125" style="21" customWidth="1"/>
+    <col min="14" max="14" width="25.88671875" style="21"/>
+    <col min="15" max="16" width="27.109375" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="20" customFormat="1">
@@ -4132,7 +4132,7 @@
         <v>10</v>
       </c>
       <c r="F1" s="16" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="G1" s="16" t="s">
         <v>6</v>
@@ -4156,18 +4156,18 @@
         <v>676</v>
       </c>
       <c r="N1" s="25" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="O1" s="9" t="s">
+        <v>1098</v>
+      </c>
+      <c r="P1" s="9" t="s">
         <v>1099</v>
       </c>
-      <c r="P1" s="9" t="s">
-        <v>1100</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="45">
+    </row>
+    <row r="2" spans="1:16" ht="43.2">
       <c r="A2" s="1" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>108</v>
@@ -4179,7 +4179,7 @@
         <v>114</v>
       </c>
       <c r="E2" s="17" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>240</v>
@@ -4194,7 +4194,7 @@
         <v>137</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="K2" s="10" t="s">
         <v>106</v>
@@ -4209,15 +4209,15 @@
         <v>106</v>
       </c>
       <c r="O2" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="P2" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="114.75">
+    <row r="3" spans="1:16" ht="118.8">
       <c r="A3" s="1" t="s">
-        <v>982</v>
+        <v>981</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>108</v>
@@ -4229,7 +4229,7 @@
         <v>13</v>
       </c>
       <c r="E3" s="17" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>241</v>
@@ -4244,7 +4244,7 @@
         <v>139</v>
       </c>
       <c r="J3" s="6" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>106</v>
@@ -4256,7 +4256,7 @@
         <v>352</v>
       </c>
       <c r="N3" s="27" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="O3" s="22" t="s">
         <v>106</v>
@@ -4265,9 +4265,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="63.75">
+    <row r="4" spans="1:16" ht="52.8">
       <c r="A4" s="1" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>108</v>
@@ -4279,7 +4279,7 @@
         <v>26</v>
       </c>
       <c r="E4" s="17" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="F4" s="3" t="s">
         <v>242</v>
@@ -4294,7 +4294,7 @@
         <v>138</v>
       </c>
       <c r="J4" s="6" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="K4" s="6" t="s">
         <v>527</v>
@@ -4309,15 +4309,15 @@
         <v>106</v>
       </c>
       <c r="O4" s="22" t="s">
+        <v>1010</v>
+      </c>
+      <c r="P4" s="22" t="s">
         <v>1011</v>
       </c>
-      <c r="P4" s="22" t="s">
-        <v>1012</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" ht="76.5">
+    </row>
+    <row r="5" spans="1:16" ht="79.2">
       <c r="A5" s="1" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>108</v>
@@ -4329,7 +4329,7 @@
         <v>68</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>243</v>
@@ -4344,7 +4344,7 @@
         <v>140</v>
       </c>
       <c r="J5" s="6" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="K5" s="10" t="s">
         <v>106</v>
@@ -4365,9 +4365,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:16" ht="63.75">
+    <row r="6" spans="1:16" ht="66">
       <c r="A6" s="1" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>108</v>
@@ -4379,7 +4379,7 @@
         <v>44</v>
       </c>
       <c r="E6" s="17" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="F6" s="3" t="s">
         <v>244</v>
@@ -4394,7 +4394,7 @@
         <v>141</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>106</v>
@@ -4412,15 +4412,15 @@
         <v>106</v>
       </c>
       <c r="P6" s="22" t="s">
-        <v>1014</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" ht="409.5">
+        <v>1013</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="409.6">
       <c r="A7" s="1" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>987</v>
+        <v>986</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>5</v>
@@ -4429,7 +4429,7 @@
         <v>115</v>
       </c>
       <c r="E7" s="17" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>245</v>
@@ -4444,7 +4444,7 @@
         <v>143</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="K7" s="10" t="s">
         <v>106</v>
@@ -4456,18 +4456,18 @@
         <v>356</v>
       </c>
       <c r="N7" s="27" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="O7" s="22" t="s">
+        <v>1014</v>
+      </c>
+      <c r="P7" s="22" t="s">
         <v>1015</v>
       </c>
-      <c r="P7" s="22" t="s">
-        <v>1016</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" ht="45">
+    </row>
+    <row r="8" spans="1:16" ht="43.2">
       <c r="A8" s="1" t="s">
-        <v>996</v>
+        <v>995</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>108</v>
@@ -4479,7 +4479,7 @@
         <v>116</v>
       </c>
       <c r="E8" s="17" t="s">
-        <v>985</v>
+        <v>984</v>
       </c>
       <c r="F8" s="4" t="s">
         <v>246</v>
@@ -4494,7 +4494,7 @@
         <v>142</v>
       </c>
       <c r="J8" s="6" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="K8" s="10" t="s">
         <v>106</v>
@@ -4510,12 +4510,12 @@
       </c>
       <c r="O8" s="23"/>
       <c r="P8" s="22" t="s">
-        <v>1017</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="102">
+        <v>1016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="92.4">
       <c r="A9" s="1" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>108</v>
@@ -4527,7 +4527,7 @@
         <v>36</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="F9" s="3" t="s">
         <v>247</v>
@@ -4542,7 +4542,7 @@
         <v>144</v>
       </c>
       <c r="J9" s="6" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>106</v>
@@ -4554,18 +4554,18 @@
         <v>357</v>
       </c>
       <c r="N9" s="27" t="s">
-        <v>720</v>
+        <v>719</v>
       </c>
       <c r="O9" s="22" t="s">
+        <v>1017</v>
+      </c>
+      <c r="P9" s="22" t="s">
         <v>1018</v>
       </c>
-      <c r="P9" s="22" t="s">
-        <v>1019</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" ht="63.75">
+    </row>
+    <row r="10" spans="1:16" ht="66">
       <c r="A10" s="1" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>108</v>
@@ -4577,7 +4577,7 @@
         <v>63</v>
       </c>
       <c r="E10" s="17" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>248</v>
@@ -4592,7 +4592,7 @@
         <v>145</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>106</v>
@@ -4607,15 +4607,15 @@
         <v>106</v>
       </c>
       <c r="O10" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P10" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:16" ht="153">
+    <row r="11" spans="1:16" ht="145.19999999999999">
       <c r="A11" s="1" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>108</v>
@@ -4627,10 +4627,10 @@
         <v>117</v>
       </c>
       <c r="E11" s="17" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>106</v>
@@ -4657,15 +4657,15 @@
         <v>106</v>
       </c>
       <c r="O11" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P11" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="204">
+    <row r="12" spans="1:16" ht="198">
       <c r="A12" s="1" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>108</v>
@@ -4677,7 +4677,7 @@
         <v>38</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="F12" s="3" t="s">
         <v>249</v>
@@ -4686,7 +4686,7 @@
         <v>106</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="I12" s="8" t="s">
         <v>556</v>
@@ -4704,18 +4704,18 @@
         <v>359</v>
       </c>
       <c r="N12" s="27" t="s">
-        <v>721</v>
+        <v>720</v>
       </c>
       <c r="O12" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="P12" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="13" spans="1:16" ht="120">
+    <row r="13" spans="1:16" ht="105.6">
       <c r="A13" s="1" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>110</v>
@@ -4727,7 +4727,7 @@
         <v>81</v>
       </c>
       <c r="E13" s="17" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="F13" s="3" t="s">
         <v>250</v>
@@ -4754,18 +4754,18 @@
         <v>358</v>
       </c>
       <c r="N13" s="27" t="s">
-        <v>722</v>
+        <v>721</v>
       </c>
       <c r="O13" s="22" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="P13" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="14" spans="1:16" ht="409.5">
+    <row r="14" spans="1:16" ht="409.6">
       <c r="A14" s="1" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>109</v>
@@ -4777,7 +4777,7 @@
         <v>28</v>
       </c>
       <c r="E14" s="17" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>251</v>
@@ -4786,7 +4786,7 @@
         <v>106</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="I14" s="1" t="s">
         <v>147</v>
@@ -4804,18 +4804,18 @@
         <v>360</v>
       </c>
       <c r="N14" s="27" t="s">
-        <v>723</v>
+        <v>722</v>
       </c>
       <c r="O14" s="22" t="s">
+        <v>1023</v>
+      </c>
+      <c r="P14" s="22" t="s">
         <v>1024</v>
       </c>
-      <c r="P14" s="22" t="s">
-        <v>1025</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" ht="102">
+    </row>
+    <row r="15" spans="1:16" ht="92.4">
       <c r="A15" s="1" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>108</v>
@@ -4827,7 +4827,7 @@
         <v>86</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="F15" s="3" t="s">
         <v>252</v>
@@ -4857,15 +4857,15 @@
         <v>106</v>
       </c>
       <c r="O15" s="22" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="P15" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="16" spans="1:16" ht="30">
+    <row r="16" spans="1:16" ht="28.8">
       <c r="A16" s="1" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>108</v>
@@ -4877,7 +4877,7 @@
         <v>118</v>
       </c>
       <c r="E16" s="17" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="F16" s="3" t="s">
         <v>253</v>
@@ -4913,9 +4913,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="17" spans="1:16" ht="216.75">
+    <row r="17" spans="1:16" ht="211.2">
       <c r="A17" s="1" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>108</v>
@@ -4927,16 +4927,16 @@
         <v>30</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>106</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="I17" s="1" t="s">
         <v>106</v>
@@ -4954,18 +4954,18 @@
         <v>362</v>
       </c>
       <c r="N17" s="27" t="s">
-        <v>724</v>
+        <v>723</v>
       </c>
       <c r="O17" s="22" t="s">
-        <v>1027</v>
+        <v>1026</v>
       </c>
       <c r="P17" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="18" spans="1:16" ht="114.75">
+    <row r="18" spans="1:16" ht="118.8">
       <c r="A18" s="1" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>108</v>
@@ -4977,7 +4977,7 @@
         <v>15</v>
       </c>
       <c r="E18" s="17" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="F18" s="3" t="s">
         <v>254</v>
@@ -5004,7 +5004,7 @@
         <v>363</v>
       </c>
       <c r="N18" s="27" t="s">
-        <v>725</v>
+        <v>724</v>
       </c>
       <c r="O18" s="22" t="s">
         <v>106</v>
@@ -5013,9 +5013,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="1:16" ht="127.5">
+    <row r="19" spans="1:16" ht="132">
       <c r="A19" s="1" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>110</v>
@@ -5027,7 +5027,7 @@
         <v>23</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="F19" s="3" t="s">
         <v>255</v>
@@ -5054,18 +5054,18 @@
         <v>364</v>
       </c>
       <c r="N19" s="27" t="s">
-        <v>726</v>
+        <v>725</v>
       </c>
       <c r="O19" s="22" t="s">
+        <v>1027</v>
+      </c>
+      <c r="P19" s="22" t="s">
         <v>1028</v>
       </c>
-      <c r="P19" s="22" t="s">
-        <v>1029</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" ht="89.25">
+    </row>
+    <row r="20" spans="1:16" ht="79.2">
       <c r="A20" s="1" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>108</v>
@@ -5077,7 +5077,7 @@
         <v>69</v>
       </c>
       <c r="E20" s="17" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="F20" s="3" t="s">
         <v>256</v>
@@ -5107,15 +5107,15 @@
         <v>106</v>
       </c>
       <c r="O20" s="22" t="s">
+        <v>1029</v>
+      </c>
+      <c r="P20" s="22" t="s">
         <v>1030</v>
       </c>
-      <c r="P20" s="22" t="s">
-        <v>1031</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="76.5">
+    </row>
+    <row r="21" spans="1:16" ht="66">
       <c r="A21" s="1" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>108</v>
@@ -5127,7 +5127,7 @@
         <v>41</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="F21" s="3" t="s">
         <v>257</v>
@@ -5163,9 +5163,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="22" spans="1:16" ht="76.5">
+    <row r="22" spans="1:16" ht="66">
       <c r="A22" s="1" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>110</v>
@@ -5177,10 +5177,10 @@
         <v>46</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>106</v>
@@ -5207,15 +5207,15 @@
         <v>106</v>
       </c>
       <c r="O22" s="22" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="P22" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="23" spans="1:16" ht="51">
+    <row r="23" spans="1:16" ht="52.8">
       <c r="A23" s="1" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>108</v>
@@ -5227,7 +5227,7 @@
         <v>24</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="F23" s="3" t="s">
         <v>258</v>
@@ -5254,18 +5254,18 @@
         <v>367</v>
       </c>
       <c r="N23" s="27" t="s">
-        <v>727</v>
+        <v>726</v>
       </c>
       <c r="O23" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="P23" s="22" t="s">
-        <v>1032</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" ht="204">
+        <v>1031</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="211.2">
       <c r="A24" s="1" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>108</v>
@@ -5277,7 +5277,7 @@
         <v>50</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="F24" s="3" t="s">
         <v>259</v>
@@ -5307,15 +5307,15 @@
         <v>106</v>
       </c>
       <c r="O24" s="22" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="P24" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="63.75">
+    <row r="25" spans="1:16" ht="66">
       <c r="A25" s="1" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>108</v>
@@ -5327,7 +5327,7 @@
         <v>119</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>260</v>
@@ -5354,18 +5354,18 @@
         <v>106</v>
       </c>
       <c r="N25" s="27" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="O25" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P25" s="22" t="s">
-        <v>1033</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" ht="102">
+        <v>1032</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="92.4">
       <c r="A26" s="1" t="s">
-        <v>981</v>
+        <v>980</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>110</v>
@@ -5377,7 +5377,7 @@
         <v>51</v>
       </c>
       <c r="E26" s="17" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="F26" s="3" t="s">
         <v>261</v>
@@ -5386,7 +5386,7 @@
         <v>106</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="I26" s="1" t="s">
         <v>157</v>
@@ -5407,15 +5407,15 @@
         <v>106</v>
       </c>
       <c r="O26" s="22" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="P26" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="89.25">
+    <row r="27" spans="1:16" ht="92.4">
       <c r="A27" s="1" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>108</v>
@@ -5427,7 +5427,7 @@
         <v>57</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="F27" s="3" t="s">
         <v>262</v>
@@ -5454,18 +5454,18 @@
         <v>370</v>
       </c>
       <c r="N27" s="27" t="s">
-        <v>729</v>
+        <v>728</v>
       </c>
       <c r="O27" s="22" t="s">
-        <v>1034</v>
+        <v>1033</v>
       </c>
       <c r="P27" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="28" spans="1:16" ht="63.75">
+    <row r="28" spans="1:16" ht="66">
       <c r="A28" s="1" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>108</v>
@@ -5477,7 +5477,7 @@
         <v>42</v>
       </c>
       <c r="E28" s="17" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="F28" s="3" t="s">
         <v>263</v>
@@ -5504,18 +5504,18 @@
         <v>359</v>
       </c>
       <c r="N28" s="27" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="O28" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="P28" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="29" spans="1:16" ht="45">
+    <row r="29" spans="1:16" ht="39.6">
       <c r="A29" s="1" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>108</v>
@@ -5527,7 +5527,7 @@
         <v>32</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="F29" s="3" t="s">
         <v>264</v>
@@ -5557,15 +5557,15 @@
         <v>106</v>
       </c>
       <c r="O29" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P29" s="22" t="s">
-        <v>1035</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" ht="105">
+        <v>1034</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="92.4">
       <c r="A30" s="1" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>108</v>
@@ -5577,7 +5577,7 @@
         <v>120</v>
       </c>
       <c r="E30" s="17" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="F30" s="3" t="s">
         <v>265</v>
@@ -5613,9 +5613,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="31" spans="1:16" ht="255">
+    <row r="31" spans="1:16" ht="264">
       <c r="A31" s="1" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>110</v>
@@ -5627,7 +5627,7 @@
         <v>35</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="F31" s="3" t="s">
         <v>266</v>
@@ -5657,15 +5657,15 @@
         <v>106</v>
       </c>
       <c r="O31" s="24" t="s">
-        <v>1036</v>
+        <v>1035</v>
       </c>
       <c r="P31" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="32" spans="1:16" ht="191.25">
+    <row r="32" spans="1:16" ht="198">
       <c r="A32" s="1" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>108</v>
@@ -5677,7 +5677,7 @@
         <v>121</v>
       </c>
       <c r="E32" s="17" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="F32" s="3" t="s">
         <v>267</v>
@@ -5704,16 +5704,16 @@
         <v>674</v>
       </c>
       <c r="N32" s="27" t="s">
-        <v>731</v>
+        <v>730</v>
       </c>
       <c r="O32" s="23"/>
       <c r="P32" s="22" t="s">
-        <v>1037</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" ht="51">
+        <v>1036</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="52.8">
       <c r="A33" s="1" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>108</v>
@@ -5725,7 +5725,7 @@
         <v>66</v>
       </c>
       <c r="E33" s="17" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="F33" s="3" t="s">
         <v>268</v>
@@ -5734,7 +5734,7 @@
         <v>106</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="I33" s="1" t="s">
         <v>162</v>
@@ -5756,12 +5756,12 @@
       </c>
       <c r="O33" s="22"/>
       <c r="P33" s="22" t="s">
-        <v>1038</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" ht="63.75">
+        <v>1037</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="66">
       <c r="A34" s="1" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>108</v>
@@ -5773,7 +5773,7 @@
         <v>31</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="F34" s="3" t="s">
         <v>269</v>
@@ -5809,9 +5809,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="35" spans="1:16" ht="89.25">
+    <row r="35" spans="1:16" ht="92.4">
       <c r="A35" s="1" t="s">
-        <v>980</v>
+        <v>979</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>110</v>
@@ -5823,7 +5823,7 @@
         <v>677</v>
       </c>
       <c r="E35" s="17" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="F35" s="3" t="s">
         <v>270</v>
@@ -5850,18 +5850,18 @@
         <v>374</v>
       </c>
       <c r="N35" s="27" t="s">
-        <v>732</v>
+        <v>731</v>
       </c>
       <c r="O35" s="22" t="s">
-        <v>1023</v>
+        <v>1022</v>
       </c>
       <c r="P35" s="22" t="s">
-        <v>1039</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" ht="76.5">
+        <v>1038</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="79.2">
       <c r="A36" s="1" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>108</v>
@@ -5873,7 +5873,7 @@
         <v>94</v>
       </c>
       <c r="E36" s="17" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="F36" s="3" t="s">
         <v>271</v>
@@ -5903,15 +5903,15 @@
         <v>106</v>
       </c>
       <c r="O36" s="22" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="P36" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="127.5">
+    <row r="37" spans="1:16" ht="132">
       <c r="A37" s="1" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>108</v>
@@ -5923,10 +5923,10 @@
         <v>40</v>
       </c>
       <c r="E37" s="17" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="G37" s="1" t="s">
         <v>106</v>
@@ -5953,15 +5953,15 @@
         <v>106</v>
       </c>
       <c r="O37" s="22" t="s">
-        <v>1041</v>
+        <v>1040</v>
       </c>
       <c r="P37" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="38" spans="1:16" ht="114.75">
+    <row r="38" spans="1:16" ht="118.8">
       <c r="A38" s="1" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>108</v>
@@ -5973,7 +5973,7 @@
         <v>47</v>
       </c>
       <c r="E38" s="17" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="F38" s="3" t="s">
         <v>272</v>
@@ -6003,15 +6003,15 @@
         <v>106</v>
       </c>
       <c r="O38" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="P38" s="22" t="s">
-        <v>1042</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" ht="76.5">
+        <v>1041</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="79.2">
       <c r="A39" s="1" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>108</v>
@@ -6023,7 +6023,7 @@
         <v>77</v>
       </c>
       <c r="E39" s="17" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="F39" s="3" t="s">
         <v>273</v>
@@ -6059,9 +6059,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="40" spans="1:16" ht="51">
+    <row r="40" spans="1:16" ht="52.8">
       <c r="A40" s="1" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>108</v>
@@ -6073,7 +6073,7 @@
         <v>59</v>
       </c>
       <c r="E40" s="17" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="F40" s="3" t="s">
         <v>274</v>
@@ -6082,7 +6082,7 @@
         <v>106</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="I40" s="1" t="s">
         <v>168</v>
@@ -6103,15 +6103,15 @@
         <v>106</v>
       </c>
       <c r="O40" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P40" s="22" t="s">
-        <v>1043</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" ht="45">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="43.2">
       <c r="A41" s="1" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>108</v>
@@ -6123,7 +6123,7 @@
         <v>48</v>
       </c>
       <c r="E41" s="17" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="F41" s="3" t="s">
         <v>275</v>
@@ -6159,9 +6159,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="42" spans="1:16" ht="63.75">
+    <row r="42" spans="1:16" ht="66">
       <c r="A42" s="1" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>108</v>
@@ -6173,7 +6173,7 @@
         <v>70</v>
       </c>
       <c r="E42" s="17" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="F42" s="3" t="s">
         <v>276</v>
@@ -6200,18 +6200,18 @@
         <v>380</v>
       </c>
       <c r="N42" s="27" t="s">
-        <v>733</v>
+        <v>732</v>
       </c>
       <c r="O42" s="22" t="s">
+        <v>1043</v>
+      </c>
+      <c r="P42" s="22" t="s">
         <v>1044</v>
       </c>
-      <c r="P42" s="22" t="s">
-        <v>1045</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" ht="178.5">
+    </row>
+    <row r="43" spans="1:16" ht="171.6">
       <c r="A43" s="1" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>108</v>
@@ -6223,7 +6223,7 @@
         <v>90</v>
       </c>
       <c r="E43" s="17" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="F43" s="3" t="s">
         <v>277</v>
@@ -6254,12 +6254,12 @@
       </c>
       <c r="O43" s="22"/>
       <c r="P43" s="22" t="s">
-        <v>1046</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" ht="45">
+        <v>1045</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="43.2">
       <c r="A44" s="1" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>108</v>
@@ -6271,7 +6271,7 @@
         <v>82</v>
       </c>
       <c r="E44" s="17" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="F44" s="3" t="s">
         <v>278</v>
@@ -6301,15 +6301,15 @@
         <v>106</v>
       </c>
       <c r="O44" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P44" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="45" spans="1:16" ht="293.25">
+    <row r="45" spans="1:16" ht="290.39999999999998">
       <c r="A45" s="1" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>108</v>
@@ -6321,7 +6321,7 @@
         <v>72</v>
       </c>
       <c r="E45" s="17" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="F45" s="3" t="s">
         <v>279</v>
@@ -6352,12 +6352,12 @@
       </c>
       <c r="O45" s="22"/>
       <c r="P45" s="22" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" ht="114.75">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="118.8">
       <c r="A46" s="1" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>108</v>
@@ -6369,7 +6369,7 @@
         <v>88</v>
       </c>
       <c r="E46" s="17" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="F46" s="3" t="s">
         <v>280</v>
@@ -6405,9 +6405,9 @@
         <v>107</v>
       </c>
     </row>
-    <row r="47" spans="1:16" ht="63.75">
+    <row r="47" spans="1:16" ht="66">
       <c r="A47" s="1" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>110</v>
@@ -6419,7 +6419,7 @@
         <v>62</v>
       </c>
       <c r="E47" s="17" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="F47" s="3" t="s">
         <v>281</v>
@@ -6449,15 +6449,15 @@
         <v>106</v>
       </c>
       <c r="O47" s="22" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="P47" s="22" t="s">
-        <v>1013</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" ht="102">
+        <v>1012</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="105.6">
       <c r="A48" s="1" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>108</v>
@@ -6469,7 +6469,7 @@
         <v>16</v>
       </c>
       <c r="E48" s="17" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="F48" s="3" t="s">
         <v>282</v>
@@ -6496,18 +6496,18 @@
         <v>384</v>
       </c>
       <c r="N48" s="27" t="s">
-        <v>734</v>
+        <v>733</v>
       </c>
       <c r="O48" s="22" t="s">
+        <v>1046</v>
+      </c>
+      <c r="P48" s="22" t="s">
         <v>1047</v>
       </c>
-      <c r="P48" s="22" t="s">
-        <v>1048</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" ht="153">
+    </row>
+    <row r="49" spans="1:16" ht="158.4">
       <c r="A49" s="1" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>108</v>
@@ -6519,7 +6519,7 @@
         <v>22</v>
       </c>
       <c r="E49" s="17" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="F49" s="3" t="s">
         <v>283</v>
@@ -6528,7 +6528,7 @@
         <v>106</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="I49" s="8" t="s">
         <v>176</v>
@@ -6546,18 +6546,18 @@
         <v>385</v>
       </c>
       <c r="N49" s="27" t="s">
-        <v>735</v>
+        <v>734</v>
       </c>
       <c r="O49" s="22" t="s">
-        <v>1040</v>
+        <v>1039</v>
       </c>
       <c r="P49" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="50" spans="1:16" ht="165.75">
+    <row r="50" spans="1:16" ht="171.6">
       <c r="A50" s="1" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>110</v>
@@ -6569,7 +6569,7 @@
         <v>678</v>
       </c>
       <c r="E50" s="17" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="F50" s="3" t="s">
         <v>284</v>
@@ -6578,7 +6578,7 @@
         <v>106</v>
       </c>
       <c r="H50" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="I50" s="1" t="s">
         <v>177</v>
@@ -6599,15 +6599,15 @@
         <v>106</v>
       </c>
       <c r="O50" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P50" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="51" spans="1:16" ht="51">
+    <row r="51" spans="1:16" ht="52.8">
       <c r="A51" s="1" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>108</v>
@@ -6616,10 +6616,10 @@
         <v>5</v>
       </c>
       <c r="D51" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="E51" s="17" t="s">
         <v>1005</v>
-      </c>
-      <c r="E51" s="17" t="s">
-        <v>1006</v>
       </c>
       <c r="F51" s="3"/>
       <c r="G51" s="1" t="s">
@@ -6627,7 +6627,7 @@
       </c>
       <c r="H51" s="3"/>
       <c r="I51" s="15" t="s">
-        <v>1007</v>
+        <v>1006</v>
       </c>
       <c r="J51" s="6"/>
       <c r="K51" s="7" t="s">
@@ -6639,9 +6639,9 @@
       <c r="O51" s="6"/>
       <c r="P51" s="6"/>
     </row>
-    <row r="52" spans="1:16" ht="45">
+    <row r="52" spans="1:16" ht="43.2">
       <c r="A52" s="1" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>108</v>
@@ -6653,7 +6653,7 @@
         <v>26</v>
       </c>
       <c r="E52" s="17" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="F52" s="3" t="s">
         <v>285</v>
@@ -6687,9 +6687,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="53" spans="1:16" ht="89.25">
+    <row r="53" spans="1:16" ht="92.4">
       <c r="A53" s="1" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>110</v>
@@ -6701,7 +6701,7 @@
         <v>54</v>
       </c>
       <c r="E53" s="17" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="F53" s="3" t="s">
         <v>286</v>
@@ -6731,15 +6731,15 @@
         <v>106</v>
       </c>
       <c r="O53" s="22" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="P53" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:16" ht="89.25">
+    <row r="54" spans="1:16" ht="92.4">
       <c r="A54" s="1" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>108</v>
@@ -6751,7 +6751,7 @@
         <v>58</v>
       </c>
       <c r="E54" s="17" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="F54" s="3" t="s">
         <v>287</v>
@@ -6760,7 +6760,7 @@
         <v>106</v>
       </c>
       <c r="H54" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="I54" s="1" t="s">
         <v>181</v>
@@ -6784,12 +6784,12 @@
         <v>106</v>
       </c>
       <c r="P54" s="22" t="s">
-        <v>1049</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" ht="76.5">
+        <v>1048</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" ht="79.2">
       <c r="A55" s="1" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>108</v>
@@ -6801,7 +6801,7 @@
         <v>122</v>
       </c>
       <c r="E55" s="17" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>288</v>
@@ -6810,7 +6810,7 @@
         <v>106</v>
       </c>
       <c r="H55" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="I55" s="1" t="s">
         <v>180</v>
@@ -6828,18 +6828,18 @@
         <v>388</v>
       </c>
       <c r="N55" s="27" t="s">
-        <v>736</v>
+        <v>735</v>
       </c>
       <c r="O55" s="22" t="s">
+        <v>1049</v>
+      </c>
+      <c r="P55" s="22" t="s">
         <v>1050</v>
       </c>
-      <c r="P55" s="22" t="s">
-        <v>1051</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="165.75">
+    </row>
+    <row r="56" spans="1:16" ht="171.6">
       <c r="A56" s="1" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>108</v>
@@ -6851,10 +6851,10 @@
         <v>87</v>
       </c>
       <c r="E56" s="17" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="F56" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="G56" s="1" t="s">
         <v>106</v>
@@ -6881,15 +6881,15 @@
         <v>106</v>
       </c>
       <c r="O56" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P56" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="57" spans="1:16" ht="127.5">
+    <row r="57" spans="1:16" ht="118.8">
       <c r="A57" s="1" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>108</v>
@@ -6901,7 +6901,7 @@
         <v>679</v>
       </c>
       <c r="E57" s="17" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="F57" s="3" t="s">
         <v>289</v>
@@ -6910,7 +6910,7 @@
         <v>106</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="I57" s="1" t="s">
         <v>183</v>
@@ -6928,18 +6928,18 @@
         <v>390</v>
       </c>
       <c r="N57" s="27" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="O57" s="22" t="s">
+        <v>1051</v>
+      </c>
+      <c r="P57" s="22" t="s">
         <v>1052</v>
       </c>
-      <c r="P57" s="22" t="s">
-        <v>1053</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" ht="127.5">
+    </row>
+    <row r="58" spans="1:16" ht="132">
       <c r="A58" s="1" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>108</v>
@@ -6951,7 +6951,7 @@
         <v>123</v>
       </c>
       <c r="E58" s="17" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>290</v>
@@ -6960,7 +6960,7 @@
         <v>106</v>
       </c>
       <c r="H58" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="I58" s="1" t="s">
         <v>184</v>
@@ -6981,15 +6981,15 @@
         <v>106</v>
       </c>
       <c r="O58" s="22" t="s">
-        <v>1054</v>
+        <v>1053</v>
       </c>
       <c r="P58" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="59" spans="1:16" ht="357">
+    <row r="59" spans="1:16" ht="356.4">
       <c r="A59" s="1" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>108</v>
@@ -7001,7 +7001,7 @@
         <v>79</v>
       </c>
       <c r="E59" s="17" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="F59" s="3" t="s">
         <v>291</v>
@@ -7010,7 +7010,7 @@
         <v>106</v>
       </c>
       <c r="H59" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="I59" s="1" t="s">
         <v>185</v>
@@ -7031,15 +7031,15 @@
         <v>106</v>
       </c>
       <c r="O59" s="22" t="s">
-        <v>1055</v>
+        <v>1054</v>
       </c>
       <c r="P59" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="60" spans="1:16" ht="153">
+    <row r="60" spans="1:16" ht="158.4">
       <c r="A60" s="1" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>108</v>
@@ -7051,7 +7051,7 @@
         <v>124</v>
       </c>
       <c r="E60" s="17" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="F60" s="3" t="s">
         <v>292</v>
@@ -7078,18 +7078,18 @@
         <v>393</v>
       </c>
       <c r="N60" s="27" t="s">
-        <v>738</v>
+        <v>737</v>
       </c>
       <c r="O60" s="22" t="s">
+        <v>1055</v>
+      </c>
+      <c r="P60" s="22" t="s">
         <v>1056</v>
       </c>
-      <c r="P60" s="22" t="s">
-        <v>1057</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" ht="409.5">
+    </row>
+    <row r="61" spans="1:16" ht="409.6">
       <c r="A61" s="1" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>109</v>
@@ -7101,16 +7101,16 @@
         <v>64</v>
       </c>
       <c r="E61" s="17" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="F61" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>106</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="I61" s="1" t="s">
         <v>187</v>
@@ -7131,15 +7131,15 @@
         <v>106</v>
       </c>
       <c r="O61" s="22" t="s">
-        <v>1058</v>
+        <v>1057</v>
       </c>
       <c r="P61" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="62" spans="1:16" ht="76.5">
+    <row r="62" spans="1:16" ht="79.2">
       <c r="A62" s="1" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>108</v>
@@ -7151,7 +7151,7 @@
         <v>61</v>
       </c>
       <c r="E62" s="17" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>293</v>
@@ -7181,15 +7181,15 @@
         <v>106</v>
       </c>
       <c r="O62" s="22" t="s">
+        <v>1058</v>
+      </c>
+      <c r="P62" s="22" t="s">
         <v>1059</v>
       </c>
-      <c r="P62" s="22" t="s">
-        <v>1060</v>
-      </c>
-    </row>
-    <row r="63" spans="1:16" ht="63.75">
+    </row>
+    <row r="63" spans="1:16" ht="66">
       <c r="A63" s="1" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>108</v>
@@ -7201,7 +7201,7 @@
         <v>680</v>
       </c>
       <c r="E63" s="17" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="F63" s="3" t="s">
         <v>294</v>
@@ -7232,12 +7232,12 @@
       </c>
       <c r="O63" s="22"/>
       <c r="P63" s="22" t="s">
-        <v>1061</v>
-      </c>
-    </row>
-    <row r="64" spans="1:16" ht="127.5">
+        <v>1060</v>
+      </c>
+    </row>
+    <row r="64" spans="1:16" ht="132">
       <c r="A64" s="1" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>108</v>
@@ -7249,7 +7249,7 @@
         <v>74</v>
       </c>
       <c r="E64" s="17" t="s">
-        <v>986</v>
+        <v>985</v>
       </c>
       <c r="F64" s="3" t="s">
         <v>295</v>
@@ -7276,18 +7276,18 @@
         <v>358</v>
       </c>
       <c r="N64" s="27" t="s">
-        <v>730</v>
+        <v>729</v>
       </c>
       <c r="O64" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P64" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="65" spans="1:16" ht="114.75">
+    <row r="65" spans="1:16" ht="118.8">
       <c r="A65" s="1" t="s">
-        <v>934</v>
+        <v>933</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>108</v>
@@ -7299,7 +7299,7 @@
         <v>65</v>
       </c>
       <c r="E65" s="17" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>296</v>
@@ -7308,7 +7308,7 @@
         <v>106</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="I65" s="1" t="s">
         <v>191</v>
@@ -7333,9 +7333,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="66" spans="1:16" ht="76.5">
+    <row r="66" spans="1:16" ht="79.2">
       <c r="A66" s="1" t="s">
-        <v>935</v>
+        <v>934</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>108</v>
@@ -7347,7 +7347,7 @@
         <v>95</v>
       </c>
       <c r="E66" s="17" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="F66" s="3" t="s">
         <v>297</v>
@@ -7374,18 +7374,18 @@
         <v>398</v>
       </c>
       <c r="N66" s="27" t="s">
-        <v>739</v>
+        <v>738</v>
       </c>
       <c r="O66" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P66" s="22" t="s">
-        <v>1062</v>
-      </c>
-    </row>
-    <row r="67" spans="1:16" ht="267.75">
+        <v>1061</v>
+      </c>
+    </row>
+    <row r="67" spans="1:16" ht="277.2">
       <c r="A67" s="1" t="s">
-        <v>936</v>
+        <v>935</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>108</v>
@@ -7397,7 +7397,7 @@
         <v>34</v>
       </c>
       <c r="E67" s="17" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="F67" s="3" t="s">
         <v>298</v>
@@ -7406,7 +7406,7 @@
         <v>106</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="I67" s="1" t="s">
         <v>193</v>
@@ -7427,15 +7427,15 @@
         <v>106</v>
       </c>
       <c r="O67" s="22" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="P67" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="68" spans="1:16" ht="45">
+    <row r="68" spans="1:16" ht="39.6">
       <c r="A68" s="1" t="s">
-        <v>937</v>
+        <v>936</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>108</v>
@@ -7447,7 +7447,7 @@
         <v>19</v>
       </c>
       <c r="E68" s="17" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="F68" s="3" t="s">
         <v>299</v>
@@ -7477,15 +7477,15 @@
         <v>106</v>
       </c>
       <c r="O68" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="P68" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="69" spans="1:16" ht="45">
+    <row r="69" spans="1:16" ht="43.2">
       <c r="A69" s="1" t="s">
-        <v>938</v>
+        <v>937</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>108</v>
@@ -7497,7 +7497,7 @@
         <v>125</v>
       </c>
       <c r="E69" s="17" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="F69" s="3" t="s">
         <v>300</v>
@@ -7533,9 +7533,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="70" spans="1:16" ht="178.5">
+    <row r="70" spans="1:16" ht="184.8">
       <c r="A70" s="1" t="s">
-        <v>939</v>
+        <v>938</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>108</v>
@@ -7547,10 +7547,10 @@
         <v>45</v>
       </c>
       <c r="E70" s="17" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="F70" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="G70" s="1" t="s">
         <v>106</v>
@@ -7574,19 +7574,19 @@
         <v>401</v>
       </c>
       <c r="N70" s="27" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
       <c r="O70" s="22" t="s">
-        <v>1064</v>
+        <v>1063</v>
       </c>
       <c r="P70" s="22"/>
     </row>
-    <row r="71" spans="1:16" ht="89.25">
+    <row r="71" spans="1:16" ht="79.2">
       <c r="A71" s="1" t="s">
-        <v>979</v>
+        <v>978</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>989</v>
+        <v>988</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>5</v>
@@ -7595,7 +7595,7 @@
         <v>681</v>
       </c>
       <c r="E71" s="17" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="F71" s="3" t="s">
         <v>301</v>
@@ -7625,16 +7625,16 @@
         <v>106</v>
       </c>
       <c r="O71" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P71" s="22"/>
     </row>
-    <row r="72" spans="1:16" ht="114.75">
+    <row r="72" spans="1:16" ht="118.8">
       <c r="A72" s="1" t="s">
-        <v>940</v>
+        <v>939</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>990</v>
+        <v>989</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>5</v>
@@ -7643,7 +7643,7 @@
         <v>12</v>
       </c>
       <c r="E72" s="17" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="F72" s="3" t="s">
         <v>302</v>
@@ -7652,7 +7652,7 @@
         <v>106</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="I72" s="1" t="s">
         <v>198</v>
@@ -7673,18 +7673,18 @@
         <v>106</v>
       </c>
       <c r="O72" s="22" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="P72" s="22" t="s">
-        <v>1065</v>
-      </c>
-    </row>
-    <row r="73" spans="1:16" ht="178.5">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="184.8">
       <c r="A73" s="1" t="s">
-        <v>941</v>
+        <v>940</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>991</v>
+        <v>990</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>5</v>
@@ -7693,7 +7693,7 @@
         <v>126</v>
       </c>
       <c r="E73" s="17" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="F73" s="3" t="s">
         <v>303</v>
@@ -7702,7 +7702,7 @@
         <v>106</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="I73" s="1" t="s">
         <v>199</v>
@@ -7720,18 +7720,18 @@
         <v>404</v>
       </c>
       <c r="N73" s="27" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="O73" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P73" s="22" t="s">
-        <v>1066</v>
-      </c>
-    </row>
-    <row r="74" spans="1:16" ht="408">
+        <v>1065</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16" ht="409.6">
       <c r="A74" s="1" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>108</v>
@@ -7743,10 +7743,10 @@
         <v>92</v>
       </c>
       <c r="E74" s="17" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="F74" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="G74" s="1" t="s">
         <v>106</v>
@@ -7770,16 +7770,16 @@
         <v>405</v>
       </c>
       <c r="N74" s="27" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="O74" s="22"/>
       <c r="P74" s="22" t="s">
-        <v>1067</v>
-      </c>
-    </row>
-    <row r="75" spans="1:16" ht="51">
+        <v>1066</v>
+      </c>
+    </row>
+    <row r="75" spans="1:16" ht="52.8">
       <c r="A75" s="1" t="s">
-        <v>943</v>
+        <v>942</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>108</v>
@@ -7791,7 +7791,7 @@
         <v>67</v>
       </c>
       <c r="E75" s="17" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="F75" s="3" t="s">
         <v>304</v>
@@ -7827,9 +7827,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="76" spans="1:16" ht="51">
+    <row r="76" spans="1:16" ht="52.8">
       <c r="A76" s="1" t="s">
-        <v>944</v>
+        <v>943</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>108</v>
@@ -7841,7 +7841,7 @@
         <v>127</v>
       </c>
       <c r="E76" s="17" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="F76" s="3" t="s">
         <v>305</v>
@@ -7868,18 +7868,18 @@
         <v>406</v>
       </c>
       <c r="N76" s="27" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="O76" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P76" s="22" t="s">
-        <v>1068</v>
-      </c>
-    </row>
-    <row r="77" spans="1:16" ht="63.75">
+        <v>1067</v>
+      </c>
+    </row>
+    <row r="77" spans="1:16" ht="52.8">
       <c r="A77" s="1" t="s">
-        <v>945</v>
+        <v>944</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>108</v>
@@ -7891,7 +7891,7 @@
         <v>33</v>
       </c>
       <c r="E77" s="17" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="F77" s="3" t="s">
         <v>306</v>
@@ -7925,9 +7925,9 @@
         <v>106</v>
       </c>
     </row>
-    <row r="78" spans="1:16" ht="51">
+    <row r="78" spans="1:16" ht="52.8">
       <c r="A78" s="1" t="s">
-        <v>946</v>
+        <v>945</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>108</v>
@@ -7939,7 +7939,7 @@
         <v>25</v>
       </c>
       <c r="E78" s="17" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>307</v>
@@ -7973,21 +7973,21 @@
         <v>106</v>
       </c>
     </row>
-    <row r="79" spans="1:16" ht="51">
+    <row r="79" spans="1:16" ht="52.8">
       <c r="A79" s="1" t="s">
-        <v>978</v>
+        <v>977</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>988</v>
+        <v>987</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>5</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>682</v>
+        <v>1104</v>
       </c>
       <c r="E79" s="17" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="F79" s="3" t="s">
         <v>308</v>
@@ -8005,7 +8005,7 @@
         <v>499</v>
       </c>
       <c r="K79" s="6" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="L79" s="6" t="s">
         <v>636</v>
@@ -8017,15 +8017,15 @@
         <v>106</v>
       </c>
       <c r="O79" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P79" s="22" t="s">
-        <v>1069</v>
-      </c>
-    </row>
-    <row r="80" spans="1:16" ht="38.25">
+        <v>1068</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16" ht="39.6">
       <c r="A80" s="1" t="s">
-        <v>947</v>
+        <v>946</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>108</v>
@@ -8037,7 +8037,7 @@
         <v>29</v>
       </c>
       <c r="E80" s="17" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="F80" s="3" t="s">
         <v>309</v>
@@ -8067,15 +8067,15 @@
         <v>106</v>
       </c>
       <c r="O80" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P80" s="22" t="s">
-        <v>1070</v>
-      </c>
-    </row>
-    <row r="81" spans="1:16" ht="140.25">
+        <v>1069</v>
+      </c>
+    </row>
+    <row r="81" spans="1:16" ht="145.19999999999999">
       <c r="A81" s="1" t="s">
-        <v>948</v>
+        <v>947</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>108</v>
@@ -8087,10 +8087,10 @@
         <v>55</v>
       </c>
       <c r="E81" s="17" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="F81" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="G81" s="1" t="s">
         <v>106</v>
@@ -8114,16 +8114,16 @@
         <v>410</v>
       </c>
       <c r="N81" s="27" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="O81" s="22" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="P81" s="22"/>
     </row>
-    <row r="82" spans="1:16" ht="63.75">
+    <row r="82" spans="1:16" ht="66">
       <c r="A82" s="1" t="s">
-        <v>949</v>
+        <v>948</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>108</v>
@@ -8135,7 +8135,7 @@
         <v>128</v>
       </c>
       <c r="E82" s="17" t="s">
-        <v>984</v>
+        <v>983</v>
       </c>
       <c r="F82" s="3" t="s">
         <v>310</v>
@@ -8165,15 +8165,15 @@
         <v>106</v>
       </c>
       <c r="O82" s="22" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="P82" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="83" spans="1:16" ht="114.75">
+    <row r="83" spans="1:16" ht="118.8">
       <c r="A83" s="1" t="s">
-        <v>977</v>
+        <v>976</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>108</v>
@@ -8185,7 +8185,7 @@
         <v>14</v>
       </c>
       <c r="E83" s="17" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="F83" s="3" t="s">
         <v>311</v>
@@ -8215,13 +8215,13 @@
         <v>106</v>
       </c>
       <c r="O83" s="22" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="P83" s="22"/>
     </row>
-    <row r="84" spans="1:16" ht="140.25">
+    <row r="84" spans="1:16" ht="145.19999999999999">
       <c r="A84" s="1" t="s">
-        <v>950</v>
+        <v>949</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>108</v>
@@ -8233,7 +8233,7 @@
         <v>76</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="F84" s="3" t="s">
         <v>312</v>
@@ -8263,13 +8263,13 @@
         <v>106</v>
       </c>
       <c r="O84" s="22" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="P84" s="22"/>
     </row>
-    <row r="85" spans="1:16" ht="75">
+    <row r="85" spans="1:16" ht="57.6">
       <c r="A85" s="1" t="s">
-        <v>997</v>
+        <v>996</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>108</v>
@@ -8281,7 +8281,7 @@
         <v>129</v>
       </c>
       <c r="E85" s="17" t="s">
-        <v>1003</v>
+        <v>1002</v>
       </c>
       <c r="F85" s="3" t="s">
         <v>313</v>
@@ -8311,13 +8311,13 @@
         <v>106</v>
       </c>
       <c r="O85" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P85" s="22"/>
     </row>
-    <row r="86" spans="1:16" ht="331.5">
+    <row r="86" spans="1:16" ht="330">
       <c r="A86" s="1" t="s">
-        <v>995</v>
+        <v>994</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>108</v>
@@ -8329,7 +8329,7 @@
         <v>27</v>
       </c>
       <c r="E86" s="17" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>314</v>
@@ -8356,18 +8356,18 @@
         <v>415</v>
       </c>
       <c r="N86" s="27" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="O86" s="22" t="s">
+        <v>1074</v>
+      </c>
+      <c r="P86" s="22" t="s">
         <v>1075</v>
       </c>
-      <c r="P86" s="22" t="s">
-        <v>1076</v>
-      </c>
-    </row>
-    <row r="87" spans="1:16" ht="89.25">
+    </row>
+    <row r="87" spans="1:16" ht="79.2">
       <c r="A87" s="1" t="s">
-        <v>951</v>
+        <v>950</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>108</v>
@@ -8379,7 +8379,7 @@
         <v>93</v>
       </c>
       <c r="E87" s="17" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="F87" s="3" t="s">
         <v>315</v>
@@ -8388,7 +8388,7 @@
         <v>106</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="I87" s="1" t="s">
         <v>212</v>
@@ -8406,18 +8406,18 @@
         <v>675</v>
       </c>
       <c r="N87" s="27" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="O87" s="22" t="s">
-        <v>1015</v>
+        <v>1014</v>
       </c>
       <c r="P87" s="22" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="88" spans="1:16" ht="76.5">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="88" spans="1:16" ht="79.2">
       <c r="A88" s="1" t="s">
-        <v>998</v>
+        <v>997</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>108</v>
@@ -8429,7 +8429,7 @@
         <v>130</v>
       </c>
       <c r="E88" s="17" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="F88" s="3" t="s">
         <v>316</v>
@@ -8459,13 +8459,13 @@
         <v>106</v>
       </c>
       <c r="O88" s="22" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="P88" s="22"/>
     </row>
-    <row r="89" spans="1:16" ht="76.5">
+    <row r="89" spans="1:16" ht="79.2">
       <c r="A89" s="1" t="s">
-        <v>976</v>
+        <v>975</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>108</v>
@@ -8477,7 +8477,7 @@
         <v>91</v>
       </c>
       <c r="E89" s="17" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="F89" s="3" t="s">
         <v>317</v>
@@ -8507,15 +8507,15 @@
         <v>106</v>
       </c>
       <c r="O89" s="22" t="s">
+        <v>1077</v>
+      </c>
+      <c r="P89" s="22" t="s">
         <v>1078</v>
       </c>
-      <c r="P89" s="22" t="s">
-        <v>1079</v>
-      </c>
-    </row>
-    <row r="90" spans="1:16" ht="267.75">
+    </row>
+    <row r="90" spans="1:16" ht="264">
       <c r="A90" s="1" t="s">
-        <v>952</v>
+        <v>951</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>108</v>
@@ -8527,7 +8527,7 @@
         <v>52</v>
       </c>
       <c r="E90" s="17" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="F90" s="3" t="s">
         <v>318</v>
@@ -8554,18 +8554,18 @@
         <v>418</v>
       </c>
       <c r="N90" s="27" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="O90" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P90" s="22" t="s">
-        <v>1080</v>
-      </c>
-    </row>
-    <row r="91" spans="1:16" ht="45">
+        <v>1079</v>
+      </c>
+    </row>
+    <row r="91" spans="1:16" ht="28.8">
       <c r="A91" s="1" t="s">
-        <v>953</v>
+        <v>952</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>108</v>
@@ -8577,7 +8577,7 @@
         <v>20</v>
       </c>
       <c r="E91" s="17" t="s">
-        <v>1002</v>
+        <v>1001</v>
       </c>
       <c r="F91" s="3" t="s">
         <v>319</v>
@@ -8586,7 +8586,7 @@
         <v>106</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="I91" s="1" t="s">
         <v>215</v>
@@ -8607,15 +8607,15 @@
         <v>106</v>
       </c>
       <c r="O91" s="22" t="s">
+        <v>1080</v>
+      </c>
+      <c r="P91" s="22" t="s">
         <v>1081</v>
       </c>
-      <c r="P91" s="22" t="s">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="92" spans="1:16" ht="45">
+    </row>
+    <row r="92" spans="1:16" ht="43.2">
       <c r="A92" s="1" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>108</v>
@@ -8627,7 +8627,7 @@
         <v>17</v>
       </c>
       <c r="E92" s="17" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="F92" s="3" t="s">
         <v>320</v>
@@ -8659,9 +8659,9 @@
       <c r="O92" s="6"/>
       <c r="P92" s="6"/>
     </row>
-    <row r="93" spans="1:16" ht="255">
+    <row r="93" spans="1:16" ht="250.8">
       <c r="A93" s="1" t="s">
-        <v>955</v>
+        <v>954</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>109</v>
@@ -8673,7 +8673,7 @@
         <v>131</v>
       </c>
       <c r="E93" s="17" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="F93" s="3" t="s">
         <v>321</v>
@@ -8682,7 +8682,7 @@
         <v>106</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="I93" s="1" t="s">
         <v>217</v>
@@ -8700,18 +8700,18 @@
         <v>421</v>
       </c>
       <c r="N93" s="27" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="O93" s="22" t="s">
+        <v>1082</v>
+      </c>
+      <c r="P93" s="22" t="s">
         <v>1083</v>
       </c>
-      <c r="P93" s="22" t="s">
-        <v>1084</v>
-      </c>
-    </row>
-    <row r="94" spans="1:16" ht="45">
+    </row>
+    <row r="94" spans="1:16" ht="39.6">
       <c r="A94" s="1" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>108</v>
@@ -8723,7 +8723,7 @@
         <v>85</v>
       </c>
       <c r="E94" s="17" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="F94" s="3" t="s">
         <v>322</v>
@@ -8753,13 +8753,13 @@
         <v>106</v>
       </c>
       <c r="O94" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P94" s="22"/>
     </row>
-    <row r="95" spans="1:16" ht="51">
+    <row r="95" spans="1:16" ht="52.8">
       <c r="A95" s="1" t="s">
-        <v>956</v>
+        <v>955</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>108</v>
@@ -8771,7 +8771,7 @@
         <v>21</v>
       </c>
       <c r="E95" s="17" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="F95" s="3" t="s">
         <v>323</v>
@@ -8798,18 +8798,18 @@
         <v>423</v>
       </c>
       <c r="N95" s="27" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="O95" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="P95" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="96" spans="1:16" ht="127.5">
+    <row r="96" spans="1:16" ht="132">
       <c r="A96" s="1" t="s">
-        <v>957</v>
+        <v>956</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>110</v>
@@ -8821,7 +8821,7 @@
         <v>75</v>
       </c>
       <c r="E96" s="17" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="F96" s="3" t="s">
         <v>324</v>
@@ -8830,7 +8830,7 @@
         <v>106</v>
       </c>
       <c r="H96" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="I96" s="1" t="s">
         <v>220</v>
@@ -8848,18 +8848,18 @@
         <v>424</v>
       </c>
       <c r="N96" s="27" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="O96" s="22" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="P96" s="22" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="97" spans="1:16" ht="140.25">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="97" spans="1:16" ht="132">
       <c r="A97" s="1" t="s">
-        <v>1008</v>
+        <v>1007</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>110</v>
@@ -8871,7 +8871,7 @@
         <v>43</v>
       </c>
       <c r="E97" s="17" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="F97" s="3" t="s">
         <v>325</v>
@@ -8880,13 +8880,13 @@
         <v>106</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="I97" s="1" t="s">
         <v>221</v>
       </c>
       <c r="J97" s="6" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="K97" s="10" t="s">
         <v>106</v>
@@ -8898,16 +8898,16 @@
         <v>425</v>
       </c>
       <c r="N97" s="27" t="s">
-        <v>737</v>
+        <v>736</v>
       </c>
       <c r="O97" s="22" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="P97" s="22"/>
     </row>
-    <row r="98" spans="1:16" ht="89.25">
+    <row r="98" spans="1:16" ht="92.4">
       <c r="A98" s="1" t="s">
-        <v>999</v>
+        <v>998</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>108</v>
@@ -8919,7 +8919,7 @@
         <v>53</v>
       </c>
       <c r="E98" s="17" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="F98" s="3" t="s">
         <v>326</v>
@@ -8934,7 +8934,7 @@
         <v>222</v>
       </c>
       <c r="J98" s="6" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="K98" s="6" t="s">
         <v>544</v>
@@ -8946,18 +8946,18 @@
         <v>426</v>
       </c>
       <c r="N98" s="27" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="O98" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P98" s="22" t="s">
-        <v>1087</v>
-      </c>
-    </row>
-    <row r="99" spans="1:16" ht="63.75">
+        <v>1086</v>
+      </c>
+    </row>
+    <row r="99" spans="1:16" ht="66">
       <c r="A99" s="1" t="s">
-        <v>958</v>
+        <v>957</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>108</v>
@@ -8969,7 +8969,7 @@
         <v>80</v>
       </c>
       <c r="E99" s="17" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="F99" s="3" t="s">
         <v>327</v>
@@ -8999,13 +8999,13 @@
         <v>106</v>
       </c>
       <c r="O99" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P99" s="22"/>
     </row>
-    <row r="100" spans="1:16" ht="51">
+    <row r="100" spans="1:16" ht="39.6">
       <c r="A100" s="1" t="s">
-        <v>959</v>
+        <v>958</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>108</v>
@@ -9017,7 +9017,7 @@
         <v>132</v>
       </c>
       <c r="E100" s="17" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>328</v>
@@ -9050,12 +9050,12 @@
         <v>106</v>
       </c>
       <c r="P100" s="22" t="s">
-        <v>1088</v>
-      </c>
-    </row>
-    <row r="101" spans="1:16" ht="89.25">
+        <v>1087</v>
+      </c>
+    </row>
+    <row r="101" spans="1:16" ht="79.2">
       <c r="A101" s="1" t="s">
-        <v>960</v>
+        <v>959</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>108</v>
@@ -9067,7 +9067,7 @@
         <v>39</v>
       </c>
       <c r="E101" s="17" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="F101" s="3" t="s">
         <v>329</v>
@@ -9097,27 +9097,27 @@
         <v>106</v>
       </c>
       <c r="O101" s="22" t="s">
-        <v>1010</v>
+        <v>1009</v>
       </c>
       <c r="P101" s="22" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="102" spans="1:16" ht="60">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="102" spans="1:16" ht="43.2">
       <c r="A102" s="1" t="s">
-        <v>1000</v>
+        <v>999</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>108</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>1001</v>
+        <v>1000</v>
       </c>
       <c r="D102" s="3" t="s">
         <v>49</v>
       </c>
       <c r="E102" s="17" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>330</v>
@@ -9147,15 +9147,15 @@
         <v>106</v>
       </c>
       <c r="O102" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P102" s="22" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="103" spans="1:16" ht="90">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="103" spans="1:16" ht="86.4">
       <c r="A103" s="1" t="s">
-        <v>961</v>
+        <v>960</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>108</v>
@@ -9167,7 +9167,7 @@
         <v>84</v>
       </c>
       <c r="E103" s="17" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="F103" s="3" t="s">
         <v>331</v>
@@ -9198,12 +9198,12 @@
       </c>
       <c r="O103" s="22"/>
       <c r="P103" s="22" t="s">
-        <v>1089</v>
-      </c>
-    </row>
-    <row r="104" spans="1:16" ht="51">
+        <v>1088</v>
+      </c>
+    </row>
+    <row r="104" spans="1:16" ht="52.8">
       <c r="A104" s="1" t="s">
-        <v>962</v>
+        <v>961</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>108</v>
@@ -9215,7 +9215,7 @@
         <v>89</v>
       </c>
       <c r="E104" s="17" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>332</v>
@@ -9245,15 +9245,15 @@
         <v>106</v>
       </c>
       <c r="O104" s="22" t="s">
+        <v>1089</v>
+      </c>
+      <c r="P104" s="22" t="s">
         <v>1090</v>
       </c>
-      <c r="P104" s="22" t="s">
-        <v>1091</v>
-      </c>
-    </row>
-    <row r="105" spans="1:16" ht="51">
+    </row>
+    <row r="105" spans="1:16" ht="52.8">
       <c r="A105" s="1" t="s">
-        <v>963</v>
+        <v>962</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>108</v>
@@ -9265,7 +9265,7 @@
         <v>83</v>
       </c>
       <c r="E105" s="17" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="F105" s="3" t="s">
         <v>333</v>
@@ -9295,16 +9295,16 @@
         <v>106</v>
       </c>
       <c r="O105" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P105" s="22"/>
     </row>
-    <row r="106" spans="1:16" ht="51">
+    <row r="106" spans="1:16" ht="52.8">
       <c r="A106" s="1" t="s">
-        <v>964</v>
+        <v>963</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>994</v>
+        <v>993</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>5</v>
@@ -9313,7 +9313,7 @@
         <v>18</v>
       </c>
       <c r="E106" s="17" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="F106" s="3" t="s">
         <v>334</v>
@@ -9322,7 +9322,7 @@
         <v>106</v>
       </c>
       <c r="H106" s="33" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="I106" s="1" t="s">
         <v>229</v>
@@ -9331,7 +9331,7 @@
         <v>96</v>
       </c>
       <c r="K106" s="6" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="L106" s="6" t="s">
         <v>662</v>
@@ -9343,18 +9343,18 @@
         <v>106</v>
       </c>
       <c r="O106" s="22" t="s">
-        <v>1063</v>
+        <v>1062</v>
       </c>
       <c r="P106" s="22" t="s">
-        <v>1092</v>
-      </c>
-    </row>
-    <row r="107" spans="1:16" ht="89.25">
+        <v>1091</v>
+      </c>
+    </row>
+    <row r="107" spans="1:16" ht="92.4">
       <c r="A107" s="1" t="s">
-        <v>965</v>
+        <v>964</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>993</v>
+        <v>992</v>
       </c>
       <c r="C107" s="1" t="s">
         <v>5</v>
@@ -9363,7 +9363,7 @@
         <v>133</v>
       </c>
       <c r="E107" s="17" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>335</v>
@@ -9390,18 +9390,18 @@
         <v>434</v>
       </c>
       <c r="N107" s="27" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="O107" s="22" t="s">
-        <v>1022</v>
+        <v>1021</v>
       </c>
       <c r="P107" s="22" t="s">
-        <v>1021</v>
-      </c>
-    </row>
-    <row r="108" spans="1:16" ht="45">
+        <v>1020</v>
+      </c>
+    </row>
+    <row r="108" spans="1:16" ht="43.2">
       <c r="A108" s="1" t="s">
-        <v>966</v>
+        <v>965</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>108</v>
@@ -9413,7 +9413,7 @@
         <v>134</v>
       </c>
       <c r="E108" s="17" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="F108" s="3" t="s">
         <v>336</v>
@@ -9444,12 +9444,12 @@
       </c>
       <c r="O108" s="23"/>
       <c r="P108" s="22" t="s">
-        <v>1093</v>
-      </c>
-    </row>
-    <row r="109" spans="1:16" ht="51">
+        <v>1092</v>
+      </c>
+    </row>
+    <row r="109" spans="1:16" ht="52.8">
       <c r="A109" s="1" t="s">
-        <v>967</v>
+        <v>966</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>108</v>
@@ -9461,7 +9461,7 @@
         <v>71</v>
       </c>
       <c r="E109" s="17" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="F109" s="3" t="s">
         <v>71</v>
@@ -9491,15 +9491,15 @@
         <v>106</v>
       </c>
       <c r="O109" s="22" t="s">
-        <v>1020</v>
+        <v>1019</v>
       </c>
       <c r="P109" s="22" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="110" spans="1:16" ht="135">
+    <row r="110" spans="1:16" ht="129.6">
       <c r="A110" s="1" t="s">
-        <v>968</v>
+        <v>967</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>108</v>
@@ -9511,7 +9511,7 @@
         <v>78</v>
       </c>
       <c r="E110" s="17" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="F110" s="3" t="s">
         <v>337</v>
@@ -9538,16 +9538,16 @@
         <v>437</v>
       </c>
       <c r="N110" s="27" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="O110" s="22" t="s">
-        <v>1026</v>
+        <v>1025</v>
       </c>
       <c r="P110" s="22"/>
     </row>
-    <row r="111" spans="1:16" ht="89.25">
+    <row r="111" spans="1:16" ht="92.4">
       <c r="A111" s="1" t="s">
-        <v>969</v>
+        <v>968</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>108</v>
@@ -9559,7 +9559,7 @@
         <v>56</v>
       </c>
       <c r="E111" s="17" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="F111" s="3" t="s">
         <v>338</v>
@@ -9590,15 +9590,15 @@
       </c>
       <c r="O111" s="22"/>
       <c r="P111" s="22" t="s">
-        <v>1094</v>
-      </c>
-    </row>
-    <row r="112" spans="1:16" ht="76.5">
+        <v>1093</v>
+      </c>
+    </row>
+    <row r="112" spans="1:16" ht="79.2">
       <c r="A112" s="1" t="s">
-        <v>975</v>
+        <v>974</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>1009</v>
+        <v>1008</v>
       </c>
       <c r="C112" s="1" t="s">
         <v>5</v>
@@ -9607,7 +9607,7 @@
         <v>60</v>
       </c>
       <c r="E112" s="17" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="F112" s="3" t="s">
         <v>339</v>
@@ -9616,7 +9616,7 @@
         <v>106</v>
       </c>
       <c r="H112" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>235</v>
@@ -9637,18 +9637,18 @@
         <v>106</v>
       </c>
       <c r="O112" s="22" t="s">
+        <v>1094</v>
+      </c>
+      <c r="P112" s="22" t="s">
         <v>1095</v>
       </c>
-      <c r="P112" s="22" t="s">
-        <v>1096</v>
-      </c>
-    </row>
-    <row r="113" spans="1:16" ht="45">
+    </row>
+    <row r="113" spans="1:16" ht="28.8">
       <c r="A113" s="1" t="s">
-        <v>970</v>
+        <v>969</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>992</v>
+        <v>991</v>
       </c>
       <c r="C113" s="1" t="s">
         <v>5</v>
@@ -9657,7 +9657,7 @@
         <v>73</v>
       </c>
       <c r="E113" s="17" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="F113" s="3" t="s">
         <v>340</v>
@@ -9684,14 +9684,14 @@
         <v>439</v>
       </c>
       <c r="N113" s="27" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="O113" s="13"/>
       <c r="P113" s="13"/>
     </row>
-    <row r="114" spans="1:16" ht="178.5">
+    <row r="114" spans="1:16" ht="184.8">
       <c r="A114" s="1" t="s">
-        <v>971</v>
+        <v>970</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>108</v>
@@ -9703,7 +9703,7 @@
         <v>37</v>
       </c>
       <c r="E114" s="17" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="F114" s="3" t="s">
         <v>341</v>
@@ -9734,12 +9734,12 @@
       </c>
       <c r="O114" s="22"/>
       <c r="P114" s="22" t="s">
-        <v>1097</v>
-      </c>
-    </row>
-    <row r="115" spans="1:16" ht="63.75">
+        <v>1096</v>
+      </c>
+    </row>
+    <row r="115" spans="1:16" ht="66">
       <c r="A115" s="1" t="s">
-        <v>972</v>
+        <v>971</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>108</v>
@@ -9751,10 +9751,10 @@
         <v>135</v>
       </c>
       <c r="E115" s="17" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>106</v>
@@ -9781,15 +9781,15 @@
         <v>106</v>
       </c>
       <c r="O115" s="22" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="P115" s="22" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="116" spans="1:16" ht="76.5">
+    <row r="116" spans="1:16" ht="79.2">
       <c r="A116" s="1" t="s">
-        <v>973</v>
+        <v>972</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>108</v>
@@ -9801,7 +9801,7 @@
         <v>136</v>
       </c>
       <c r="E116" s="17" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="F116" s="3" t="s">
         <v>342</v>
@@ -9833,9 +9833,9 @@
       <c r="O116" s="23"/>
       <c r="P116" s="22"/>
     </row>
-    <row r="117" spans="1:16" ht="30">
+    <row r="117" spans="1:16" ht="28.8">
       <c r="A117" s="12" t="s">
-        <v>974</v>
+        <v>973</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>108</v>
@@ -9844,10 +9844,10 @@
         <v>555</v>
       </c>
       <c r="D117" s="11" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E117" s="18" t="s">
-        <v>983</v>
+        <v>982</v>
       </c>
       <c r="F117" s="12" t="s">
         <v>106</v>
@@ -10345,7 +10345,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -10357,7 +10357,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>